<commit_message>
Introduce caste groups. - UNSPECIALIZED <- ROGUE - WARRIOR <- FIGHTER, PALADIN, GRANDMASTER, TITAN Limiting attributes (max 100). Refactor calculation method to avoid an occurrence of a magic float number.
</commit_message>
<xml_diff>
--- a/doc/caste_system.xlsx
+++ b/doc/caste_system.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/349dfb9748b30a92/Asztali gép/ataliasflame_2.0/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2994" documentId="8_{652F4476-B36F-42CD-831D-0D71B9923ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{629547AE-38BA-4985-82D2-2671EAF1F6D6}"/>
+  <xr:revisionPtr revIDLastSave="3120" documentId="8_{652F4476-B36F-42CD-831D-0D71B9923ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB6E6382-5F31-4752-BCE9-58702A0BBA31}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{CAF51EC3-63EC-48CD-AA7B-C21B3D5D222B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CAF51EC3-63EC-48CD-AA7B-C21B3D5D222B}"/>
   </bookViews>
   <sheets>
     <sheet name="caste list" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,31 @@
     <author>Mikló Attila</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{78271437-06AD-4FA1-9A52-939A4B175A43}">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{3C6D7914-9ECF-4C54-97EA-A97734447BA7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mikló Attila:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+unspecialized</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{78271437-06AD-4FA1-9A52-939A4B175A43}">
       <text>
         <r>
           <rPr>
@@ -71,7 +95,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{7D096874-F439-4A5D-946D-DBD464B95DD0}">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{5F3CB805-931A-4350-B6D0-041B7D7E5B9E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mikló Attila:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+magician</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{7D096874-F439-4A5D-946D-DBD464B95DD0}">
       <text>
         <r>
           <rPr>
@@ -95,7 +143,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{38194860-923D-4148-A97E-A818B9AA2646}">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{38194860-923D-4148-A97E-A818B9AA2646}">
       <text>
         <r>
           <rPr>
@@ -119,7 +167,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{D1466D25-BCCE-4BF1-B2E8-D45A5998F7B5}">
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{D1466D25-BCCE-4BF1-B2E8-D45A5998F7B5}">
       <text>
         <r>
           <rPr>
@@ -143,7 +191,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{E196D7E0-8288-4797-B736-7A79201C9F0D}">
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{E196D7E0-8288-4797-B736-7A79201C9F0D}">
       <text>
         <r>
           <rPr>
@@ -167,7 +215,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{40CFFF93-F61F-4BEA-84F8-E4E701A68F86}">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{40CFFF93-F61F-4BEA-84F8-E4E701A68F86}">
       <text>
         <r>
           <rPr>
@@ -191,7 +239,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{7C9B282B-EA35-4971-AAFB-23837FA7AAEF}">
+    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{CDC031F3-CBAF-46AE-929F-AEA4F11DA89C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mikló Attila:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+warrior</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{7C9B282B-EA35-4971-AAFB-23837FA7AAEF}">
       <text>
         <r>
           <rPr>
@@ -215,7 +287,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{9BD77CCB-3A24-4AE4-B43E-FBE10BC16D53}">
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{9BD77CCB-3A24-4AE4-B43E-FBE10BC16D53}">
       <text>
         <r>
           <rPr>
@@ -239,7 +311,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{91B43E26-B33C-454E-BEAD-29F8407C2340}">
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{91B43E26-B33C-454E-BEAD-29F8407C2340}">
       <text>
         <r>
           <rPr>
@@ -263,7 +335,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{1C8E939D-3AF5-4371-97F4-0ED5A6A4C16C}">
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{1C8E939D-3AF5-4371-97F4-0ED5A6A4C16C}">
       <text>
         <r>
           <rPr>
@@ -287,7 +359,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="A12" authorId="0" shapeId="0" xr:uid="{DF9BB6E1-A51E-4924-B0C7-8E424E30F2D3}">
+    <comment ref="A12" authorId="0" shapeId="0" xr:uid="{ADADEC99-8F35-4F4E-98C5-D5F6F25285C2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mikló Attila:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+wanderer</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{DF9BB6E1-A51E-4924-B0C7-8E424E30F2D3}">
       <text>
         <r>
           <rPr>
@@ -311,7 +407,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A13" authorId="0" shapeId="0" xr:uid="{C321B913-EB30-43DE-87D1-B295FECC6FC2}">
+    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{C321B913-EB30-43DE-87D1-B295FECC6FC2}">
       <text>
         <r>
           <rPr>
@@ -335,7 +431,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A14" authorId="0" shapeId="0" xr:uid="{59B1B662-5259-41F0-8FD8-4361C6875AF5}">
+    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{59B1B662-5259-41F0-8FD8-4361C6875AF5}">
       <text>
         <r>
           <rPr>
@@ -359,7 +455,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A15" authorId="0" shapeId="0" xr:uid="{318FA5FA-0DB7-4219-B1E0-0004BC31B0C7}">
+    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{318FA5FA-0DB7-4219-B1E0-0004BC31B0C7}">
       <text>
         <r>
           <rPr>
@@ -383,7 +479,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="A16" authorId="0" shapeId="0" xr:uid="{F12B9F38-E667-4D3F-8C03-DBDC2EC579AE}">
+    <comment ref="A16" authorId="0" shapeId="0" xr:uid="{CEDF0E1C-FAE7-4EA7-8F0F-A62697734D2C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mikló Attila:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+nature dweller</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B16" authorId="0" shapeId="0" xr:uid="{F12B9F38-E667-4D3F-8C03-DBDC2EC579AE}">
       <text>
         <r>
           <rPr>
@@ -407,7 +527,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A17" authorId="0" shapeId="0" xr:uid="{540767F7-80F6-47BC-B78E-2594ED20CC2E}">
+    <comment ref="B17" authorId="0" shapeId="0" xr:uid="{540767F7-80F6-47BC-B78E-2594ED20CC2E}">
       <text>
         <r>
           <rPr>
@@ -431,7 +551,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A18" authorId="0" shapeId="0" xr:uid="{94CF7A54-37EB-4378-B6EA-8AD39E6CDFCC}">
+    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{94CF7A54-37EB-4378-B6EA-8AD39E6CDFCC}">
       <text>
         <r>
           <rPr>
@@ -455,7 +575,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A19" authorId="0" shapeId="0" xr:uid="{181AD8F3-0232-426B-B8FB-7408DFB3721F}">
+    <comment ref="B19" authorId="0" shapeId="0" xr:uid="{181AD8F3-0232-426B-B8FB-7408DFB3721F}">
       <text>
         <r>
           <rPr>
@@ -479,7 +599,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="A20" authorId="0" shapeId="0" xr:uid="{B046AC2F-09DE-420E-9685-9DD89EC21152}">
+    <comment ref="A20" authorId="0" shapeId="0" xr:uid="{682B2CAC-DCE6-4EB3-A127-38375F25FC2D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mikló Attila:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+cleric</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B20" authorId="0" shapeId="0" xr:uid="{B046AC2F-09DE-420E-9685-9DD89EC21152}">
       <text>
         <r>
           <rPr>
@@ -503,7 +647,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A21" authorId="0" shapeId="0" xr:uid="{222C7712-FC3E-44F8-A634-812001C75FE4}">
+    <comment ref="B21" authorId="0" shapeId="0" xr:uid="{222C7712-FC3E-44F8-A634-812001C75FE4}">
       <text>
         <r>
           <rPr>
@@ -527,7 +671,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A22" authorId="0" shapeId="0" xr:uid="{2834CA0C-6517-405B-97C4-6C7320890086}">
+    <comment ref="B22" authorId="0" shapeId="0" xr:uid="{2834CA0C-6517-405B-97C4-6C7320890086}">
       <text>
         <r>
           <rPr>
@@ -551,7 +695,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A23" authorId="0" shapeId="0" xr:uid="{C8E97A63-84F4-41D0-BECE-2F8E77BEE634}">
+    <comment ref="B23" authorId="0" shapeId="0" xr:uid="{C8E97A63-84F4-41D0-BECE-2F8E77BEE634}">
       <text>
         <r>
           <rPr>
@@ -1562,7 +1706,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="84">
   <si>
     <t>csavargó</t>
   </si>
@@ -1803,12 +1947,24 @@
   <si>
     <t>Arimaszpó</t>
   </si>
+  <si>
+    <t>specializálatlan</t>
+  </si>
+  <si>
+    <t>vándor</t>
+  </si>
+  <si>
+    <t>természet lakó</t>
+  </si>
+  <si>
+    <t>klerikus</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1876,14 +2032,6 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FFFFFF00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1917,7 +2065,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -2011,12 +2159,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2057,11 +2214,51 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -2381,88 +2578,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E471BE-CB76-416C-8A0D-8BCD59B0033A}">
-  <dimension ref="A1:Q23"/>
+  <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
-      <c r="B1" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B1" s="1"/>
+      <c r="C1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>24</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>25</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>26</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>27</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>28</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>29</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>32</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>33</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>34</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>35</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>39</v>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>39</v>
@@ -2488,10 +2688,10 @@
       <c r="J2" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="K2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>39</v>
       </c>
       <c r="M2" t="s">
@@ -2506,16 +2706,19 @@
       <c r="P2" t="s">
         <v>39</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="Q2" t="s">
+        <v>39</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>39</v>
+      <c r="B3" s="33" t="s">
+        <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>39</v>
@@ -2527,7 +2730,7 @@
         <v>39</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>40</v>
@@ -2539,12 +2742,12 @@
         <v>40</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L3" s="4" t="s">
         <v>39</v>
       </c>
       <c r="M3" s="5" t="s">
@@ -2557,19 +2760,20 @@
         <v>39</v>
       </c>
       <c r="P3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q3" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="Q3" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="R3" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="39"/>
+      <c r="B4" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="C4" s="5" t="s">
         <v>39</v>
       </c>
@@ -2580,7 +2784,7 @@
         <v>39</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>40</v>
@@ -2592,12 +2796,12 @@
         <v>40</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L4" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" s="4" t="s">
         <v>39</v>
       </c>
       <c r="M4" s="5" t="s">
@@ -2610,19 +2814,20 @@
         <v>39</v>
       </c>
       <c r="P4" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="Q4" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="R4" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="39"/>
+      <c r="B5" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="C5" s="5" t="s">
         <v>39</v>
       </c>
@@ -2633,7 +2838,7 @@
         <v>39</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>40</v>
@@ -2645,12 +2850,12 @@
         <v>40</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" s="4" t="s">
         <v>39</v>
       </c>
       <c r="M5" s="5" t="s">
@@ -2663,19 +2868,20 @@
         <v>39</v>
       </c>
       <c r="P5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q5" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="Q5" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="R5" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" s="39"/>
+      <c r="B6" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="C6" s="5" t="s">
         <v>39</v>
       </c>
@@ -2686,7 +2892,7 @@
         <v>39</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>40</v>
@@ -2698,12 +2904,12 @@
         <v>40</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L6" s="4" t="s">
         <v>39</v>
       </c>
       <c r="M6" s="5" t="s">
@@ -2716,19 +2922,20 @@
         <v>39</v>
       </c>
       <c r="P6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q6" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="Q6" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="R6" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="40"/>
+      <c r="B7" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="C7" s="5" t="s">
         <v>39</v>
       </c>
@@ -2739,7 +2946,7 @@
         <v>39</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>40</v>
@@ -2751,12 +2958,12 @@
         <v>40</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L7" s="4" t="s">
         <v>39</v>
       </c>
       <c r="M7" s="5" t="s">
@@ -2769,18 +2976,21 @@
         <v>39</v>
       </c>
       <c r="P7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q7" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="Q7" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="R7" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
-        <v>39</v>
+      <c r="B8" s="35" t="s">
+        <v>5</v>
       </c>
       <c r="C8" t="s">
         <v>39</v>
@@ -2804,12 +3014,12 @@
         <v>39</v>
       </c>
       <c r="J8" t="s">
+        <v>39</v>
+      </c>
+      <c r="K8" t="s">
         <v>40</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L8" t="s">
+      <c r="L8" s="1" t="s">
         <v>39</v>
       </c>
       <c r="M8" t="s">
@@ -2824,176 +3034,182 @@
       <c r="P8" t="s">
         <v>39</v>
       </c>
-      <c r="Q8" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="32" t="s">
+      <c r="Q8" t="s">
+        <v>39</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="42"/>
+      <c r="B9" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="I9" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="J9" s="33" t="s">
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J9" t="s">
+        <v>39</v>
+      </c>
+      <c r="K9" t="s">
         <v>40</v>
       </c>
-      <c r="K9" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="L9" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="M9" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="N9" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="O9" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="P9" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q9" s="32" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="32" t="s">
+      <c r="L9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M9" t="s">
+        <v>39</v>
+      </c>
+      <c r="N9" t="s">
+        <v>39</v>
+      </c>
+      <c r="O9" t="s">
+        <v>39</v>
+      </c>
+      <c r="P9" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>39</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" s="42"/>
+      <c r="B10" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="H10" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="I10" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="J10" s="33" t="s">
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10" t="s">
+        <v>39</v>
+      </c>
+      <c r="K10" t="s">
         <v>40</v>
       </c>
-      <c r="K10" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="L10" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="M10" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="N10" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="O10" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="P10" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q10" s="32" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="34" t="s">
+      <c r="L10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M10" t="s">
+        <v>39</v>
+      </c>
+      <c r="N10" t="s">
+        <v>39</v>
+      </c>
+      <c r="O10" t="s">
+        <v>39</v>
+      </c>
+      <c r="P10" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>39</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="43"/>
+      <c r="B11" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="H11" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="I11" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="J11" s="33" t="s">
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" t="s">
+        <v>39</v>
+      </c>
+      <c r="J11" t="s">
+        <v>39</v>
+      </c>
+      <c r="K11" t="s">
         <v>40</v>
       </c>
-      <c r="K11" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="L11" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="M11" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="N11" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="O11" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="P11" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q11" s="32" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="L11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M11" t="s">
+        <v>39</v>
+      </c>
+      <c r="N11" t="s">
+        <v>39</v>
+      </c>
+      <c r="O11" t="s">
+        <v>39</v>
+      </c>
+      <c r="P11" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>39</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="C12" s="3" t="s">
         <v>39</v>
       </c>
@@ -3016,12 +3232,12 @@
         <v>39</v>
       </c>
       <c r="J12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K12" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="K12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L12" s="3" t="s">
+      <c r="L12" s="2" t="s">
         <v>39</v>
       </c>
       <c r="M12" s="3" t="s">
@@ -3036,17 +3252,18 @@
       <c r="P12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="Q12" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="Q12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="45"/>
+      <c r="B13" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="C13" s="5" t="s">
         <v>39</v>
       </c>
@@ -3069,12 +3286,12 @@
         <v>39</v>
       </c>
       <c r="J13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="K13" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="K13" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L13" s="5" t="s">
+      <c r="L13" s="4" t="s">
         <v>39</v>
       </c>
       <c r="M13" s="5" t="s">
@@ -3089,17 +3306,18 @@
       <c r="P13" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="Q13" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+      <c r="Q13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="R13" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" s="45"/>
+      <c r="B14" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="C14" s="5" t="s">
         <v>39</v>
       </c>
@@ -3122,12 +3340,12 @@
         <v>39</v>
       </c>
       <c r="J14" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="K14" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="K14" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L14" s="5" t="s">
+      <c r="L14" s="4" t="s">
         <v>39</v>
       </c>
       <c r="M14" s="5" t="s">
@@ -3142,17 +3360,18 @@
       <c r="P14" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="Q14" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
+      <c r="Q14" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" s="46"/>
+      <c r="B15" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="C15" s="5" t="s">
         <v>39</v>
       </c>
@@ -3175,12 +3394,12 @@
         <v>39</v>
       </c>
       <c r="J15" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="K15" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="K15" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L15" s="5" t="s">
+      <c r="L15" s="4" t="s">
         <v>39</v>
       </c>
       <c r="M15" s="5" t="s">
@@ -3195,17 +3414,20 @@
       <c r="P15" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="Q15" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="Q15" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="R15" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="C16" s="3" t="s">
         <v>39</v>
       </c>
@@ -3230,10 +3452,10 @@
       <c r="J16" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="K16" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L16" s="3" t="s">
+      <c r="K16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L16" s="2" t="s">
         <v>39</v>
       </c>
       <c r="M16" s="3" t="s">
@@ -3248,17 +3470,18 @@
       <c r="P16" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="Q16" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+      <c r="Q16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A17" s="45"/>
+      <c r="B17" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="C17" s="5" t="s">
         <v>39</v>
       </c>
@@ -3283,10 +3506,10 @@
       <c r="J17" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="K17" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L17" s="5" t="s">
+      <c r="K17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L17" s="4" t="s">
         <v>39</v>
       </c>
       <c r="M17" s="5" t="s">
@@ -3301,17 +3524,18 @@
       <c r="P17" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="Q17" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+      <c r="Q17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="R17" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A18" s="45"/>
+      <c r="B18" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="C18" s="5" t="s">
         <v>39</v>
       </c>
@@ -3336,10 +3560,10 @@
       <c r="J18" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="K18" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L18" s="5" t="s">
+      <c r="K18" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L18" s="4" t="s">
         <v>39</v>
       </c>
       <c r="M18" s="5" t="s">
@@ -3354,17 +3578,18 @@
       <c r="P18" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="Q18" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
+      <c r="Q18" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="R18" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19" s="46"/>
+      <c r="B19" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="C19" s="5" t="s">
         <v>39</v>
       </c>
@@ -3389,10 +3614,10 @@
       <c r="J19" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="K19" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L19" s="5" t="s">
+      <c r="K19" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L19" s="4" t="s">
         <v>39</v>
       </c>
       <c r="M19" s="5" t="s">
@@ -3407,17 +3632,20 @@
       <c r="P19" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="Q19" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+      <c r="Q19" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="R19" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A20" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="C20" s="5" t="s">
         <v>39</v>
       </c>
@@ -3434,18 +3662,18 @@
         <v>39</v>
       </c>
       <c r="H20" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I20" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="I20" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="J20" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="K20" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L20" s="5" t="s">
+      <c r="K20" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L20" s="4" t="s">
         <v>39</v>
       </c>
       <c r="M20" s="5" t="s">
@@ -3460,17 +3688,18 @@
       <c r="P20" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="Q20" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
+      <c r="Q20" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="R20" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A21" s="39"/>
+      <c r="B21" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="C21" s="5" t="s">
         <v>39</v>
       </c>
@@ -3487,18 +3716,18 @@
         <v>39</v>
       </c>
       <c r="H21" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I21" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="I21" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="J21" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="K21" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L21" s="5" t="s">
+      <c r="K21" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L21" s="4" t="s">
         <v>39</v>
       </c>
       <c r="M21" s="5" t="s">
@@ -3513,17 +3742,18 @@
       <c r="P21" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="Q21" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+      <c r="Q21" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="R21" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A22" s="39"/>
+      <c r="B22" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="C22" s="5" t="s">
         <v>39</v>
       </c>
@@ -3540,18 +3770,18 @@
         <v>39</v>
       </c>
       <c r="H22" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I22" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="I22" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="J22" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="K22" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L22" s="5" t="s">
+      <c r="K22" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L22" s="4" t="s">
         <v>39</v>
       </c>
       <c r="M22" s="5" t="s">
@@ -3566,17 +3796,18 @@
       <c r="P22" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="Q22" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A23" s="6" t="s">
+      <c r="Q22" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="R22" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A23" s="40"/>
+      <c r="B23" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="C23" s="5" t="s">
         <v>39</v>
       </c>
@@ -3593,18 +3824,18 @@
         <v>39</v>
       </c>
       <c r="H23" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I23" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="I23" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="J23" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="K23" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L23" s="5" t="s">
+      <c r="K23" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L23" s="4" t="s">
         <v>39</v>
       </c>
       <c r="M23" s="5" t="s">
@@ -3619,11 +3850,21 @@
       <c r="P23" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="Q23" s="4" t="s">
+      <c r="Q23" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="R23" s="4" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A23"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -4079,46 +4320,46 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="I9" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="J9" s="33">
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J9">
         <v>5</v>
       </c>
-      <c r="K9" s="33">
+      <c r="K9">
         <v>5</v>
       </c>
-      <c r="L9" s="33">
+      <c r="L9">
         <v>5</v>
       </c>
-      <c r="M9" s="33">
+      <c r="M9">
         <v>5</v>
       </c>
-      <c r="N9" s="33">
+      <c r="N9">
         <v>-1</v>
       </c>
       <c r="O9" s="5">
@@ -4290,7 +4531,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B2" s="17">
@@ -4435,7 +4676,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="16" t="s">
         <v>37</v>
       </c>
       <c r="B7" s="17">
@@ -4576,13 +4817,13 @@
       <c r="M1" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="33" t="s">
+      <c r="N1" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="33" t="s">
+      <c r="O1" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="32" t="s">
+      <c r="P1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="Q1" s="3" t="s">
@@ -4668,13 +4909,13 @@
       <c r="M2">
         <v>5</v>
       </c>
-      <c r="N2" s="33">
+      <c r="N2">
         <v>20</v>
       </c>
-      <c r="O2" s="33">
+      <c r="O2">
         <v>50</v>
       </c>
-      <c r="P2" s="32">
+      <c r="P2" s="1">
         <v>100</v>
       </c>
       <c r="Q2" s="3">
@@ -4761,13 +5002,13 @@
       <c r="M3">
         <v>5</v>
       </c>
-      <c r="N3" s="33">
+      <c r="N3">
         <v>20</v>
       </c>
-      <c r="O3" s="33">
+      <c r="O3">
         <v>50</v>
       </c>
-      <c r="P3" s="32">
+      <c r="P3" s="1">
         <v>100</v>
       </c>
       <c r="Q3" s="3">
@@ -4854,13 +5095,13 @@
       <c r="M4">
         <v>5</v>
       </c>
-      <c r="N4" s="33">
+      <c r="N4">
         <v>20</v>
       </c>
-      <c r="O4" s="33">
+      <c r="O4">
         <v>50</v>
       </c>
-      <c r="P4" s="32">
+      <c r="P4" s="1">
         <v>100</v>
       </c>
       <c r="Q4" s="3">
@@ -4947,13 +5188,13 @@
       <c r="M5">
         <v>5</v>
       </c>
-      <c r="N5" s="33">
+      <c r="N5">
         <v>20</v>
       </c>
-      <c r="O5" s="33">
+      <c r="O5">
         <v>50</v>
       </c>
-      <c r="P5" s="32">
+      <c r="P5" s="1">
         <v>100</v>
       </c>
       <c r="Q5" s="3">
@@ -5040,13 +5281,13 @@
       <c r="M6">
         <v>2</v>
       </c>
-      <c r="N6" s="33">
+      <c r="N6">
         <v>7</v>
       </c>
-      <c r="O6" s="33">
+      <c r="O6">
         <v>20</v>
       </c>
-      <c r="P6" s="32">
+      <c r="P6" s="1">
         <v>40</v>
       </c>
       <c r="Q6" s="3">
@@ -6560,8 +6801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D8DF294-C85C-47A3-9A81-4E26EFDC10EC}">
   <dimension ref="A1:BK54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="BF40" sqref="BF40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="BF29" sqref="BF29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -6615,13 +6856,13 @@
     <col min="48" max="48" width="9" style="18" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="5" style="18" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="8.88671875" style="18"/>
-    <col min="51" max="51" width="7.88671875" style="35" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="6.109375" style="35" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="5.77734375" style="35" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="4.77734375" style="35" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="9" style="35" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="5" style="35" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="8.88671875" style="35"/>
+    <col min="51" max="51" width="7.88671875" style="18" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="6.109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="5.77734375" style="18" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="4.77734375" style="18" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="9" style="18" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="5" style="18" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="8.88671875" style="18"/>
     <col min="58" max="58" width="7.88671875" style="18" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="6.109375" style="18" bestFit="1" customWidth="1"/>
     <col min="60" max="60" width="5.77734375" style="18" bestFit="1" customWidth="1"/>
@@ -7067,7 +7308,6 @@
         <f>ROUND($B$10*(1+$Q$2*(1+F2+L2)*E2+$Q$3*(1+F3+L3)*E3+$Q$4*(1+F4+L4)*E4+$Q$5*(1+F5+L5)*E5+$Q$6*(1+F6+L6)*E6),0)</f>
         <v>110</v>
       </c>
-      <c r="AC4" s="35"/>
       <c r="AD4" s="20" t="s">
         <v>32</v>
       </c>
@@ -7091,7 +7331,6 @@
         <f>ROUND($B$10*(1+$Q$2*(1+G2+L2)*E2+$Q$3*(1+G3+L3)*E3+ROUND($Q$4*(1+G4+L4),0)*E4+$Q$5*(1+G5+L5)*E5+$Q$6*(1+G6+L6)*E6),0)</f>
         <v>110</v>
       </c>
-      <c r="AJ4" s="35"/>
       <c r="AK4" s="20" t="s">
         <v>32</v>
       </c>
@@ -7115,7 +7354,6 @@
         <f>ROUND($B$10*(1+$Q$2*(1+H2+L2)*E2+$Q$3*(1+H3+L3)*E3+ROUND($Q$4*(1+H4+L4),0)*E4+$Q$5*(1+H5+L5)*E5+$Q$6*(1+H6+L6)*E6),0)</f>
         <v>110</v>
       </c>
-      <c r="AQ4" s="35"/>
       <c r="AR4" s="20" t="s">
         <v>32</v>
       </c>
@@ -7139,7 +7377,6 @@
         <f>ROUND($B$10*(1+$Q$2*(1+I2+L2)*E2+$Q$3*(1+I3+L3)*E3+ROUND($Q$4*(1+I4+L4),0)*E4+$Q$5*(1+I5+L5)*E5+$Q$6*(1+I6+L6)*E6),0)</f>
         <v>110</v>
       </c>
-      <c r="AX4" s="35"/>
       <c r="AY4" s="20" t="s">
         <v>32</v>
       </c>
@@ -8084,7 +8321,6 @@
         <f>ROUND($B$10*(1+$R$2*(1+F2+L2)*E2+$R$3*(1+F3+L3)*E3+ROUND($R$4*(1+F4+L4),0)*E4+$R$5*(1+F5+L5)*E5+$R$6*(1+F6+L6)*E6),0)</f>
         <v>150</v>
       </c>
-      <c r="AC11" s="35"/>
       <c r="AD11" s="20" t="s">
         <v>32</v>
       </c>
@@ -8108,7 +8344,6 @@
         <f>ROUND($B$10*(1+$R$2*(1+G2+L2)*E2+$R$3*(1+G3+L3)*E3+ROUND($R$4*(1+G4+L4),0)*E4+$R$5*(1+G5+L5)*E5+$R$6*(1+G6+L6)*E6),0)</f>
         <v>150</v>
       </c>
-      <c r="AJ11" s="35"/>
       <c r="AK11" s="20" t="s">
         <v>32</v>
       </c>
@@ -8132,7 +8367,6 @@
         <f>ROUND($B$10*(1+$R$2*(1+H2+L2)*E2+$R$3*(1+H3+L3)*E3+ROUND($R$4*(1+H4+L4),0)*E4+$R$5*(1+H5+L5)*E5+$R$6*(1+H6+L6)*E6),0)</f>
         <v>150</v>
       </c>
-      <c r="AQ11" s="35"/>
       <c r="AR11" s="20" t="s">
         <v>32</v>
       </c>
@@ -8156,7 +8390,6 @@
         <f>ROUND($B$10*(1+$R$2*(1+I2+L2)*E2+$R$3*(1+I3+L3)*E3+ROUND($R$4*(1+I4+L4),0)*E4+$R$5*(1+I5+L5)*E5+$R$6*(1+I6+L6)*E6),0)</f>
         <v>150</v>
       </c>
-      <c r="AX11" s="35"/>
       <c r="AY11" s="20" t="s">
         <v>32</v>
       </c>
@@ -8919,7 +9152,6 @@
         <f>ROUND($B$10*(1+$S$2*(1+F2+L2)*E2+$S$3*(1+F3+L3)*E3+ROUND($S$4*(1+F4+L4),0)*E4+$S$5*(1+F5+L5)*E5+$S$6*(1+F6+L6)*E6),0)</f>
         <v>300</v>
       </c>
-      <c r="AC18" s="35"/>
       <c r="AD18" s="20" t="s">
         <v>32</v>
       </c>
@@ -8943,7 +9175,6 @@
         <f>ROUND($B$10*(1+$S$2*(1+G2+L2)*E2+$S$3*(1+G3+L3)*E3+ROUND($S$4*(1+G4+L4),0)*E4+$S$5*(1+G5+L5)*E5+$S$6*(1+G6+L6)*E6),0)</f>
         <v>280</v>
       </c>
-      <c r="AJ18" s="35"/>
       <c r="AK18" s="20" t="s">
         <v>32</v>
       </c>
@@ -8967,7 +9198,6 @@
         <f>ROUND($B$10*(1+$S$2*(1+H2+L2)*E2+$S$3*(1+H3+L3)*E3+ROUND($S$4*(1+H4+L4),0)*E4+$S$5*(1+H5+L5)*E5+$S$6*(1+H6+L6)*E6),0)</f>
         <v>290</v>
       </c>
-      <c r="AQ18" s="35"/>
       <c r="AR18" s="20" t="s">
         <v>32</v>
       </c>
@@ -8991,7 +9221,6 @@
         <f>ROUND($B$10*(1+$S$2*(1+I2+L2)*E2+$S$3*(1+I3+L3)*E3+ROUND($S$4*(1+I4+L4),0)*E4+$S$5*(1+I5+L5)*E5+$S$6*(1+I6+L6)*E6),0)</f>
         <v>300</v>
       </c>
-      <c r="AX18" s="35"/>
       <c r="AY18" s="20" t="s">
         <v>32</v>
       </c>
@@ -9733,7 +9962,6 @@
         <f>ROUND($B$10*(1+$T$2*(1+F2+L2)*E2+$T$3*(1+F3+L3)*E3+ROUND($T$4*(1+F4+L4),0)*E4+$T$5*(1+F5+L5)*E5+$T$6*(1+F6+L6)*E6),0)</f>
         <v>600</v>
       </c>
-      <c r="AC25" s="35"/>
       <c r="AD25" s="20" t="s">
         <v>32</v>
       </c>
@@ -9757,7 +9985,6 @@
         <f>ROUND($B$10*(1+$T$2*(1+G2+L2)*E2+$T$3*(1+G3+L3)*E3+ROUND($T$4*(1+G4+L4),0)*E4+$T$5*(1+G5+L5)*E5+$T$6*(1+G6+L6)*E6),0)</f>
         <v>550</v>
       </c>
-      <c r="AJ25" s="35"/>
       <c r="AK25" s="20" t="s">
         <v>32</v>
       </c>
@@ -9781,7 +10008,6 @@
         <f>ROUND($B$10*(1+$T$2*(1+H2+L2)*E2+$T$3*(1+H3+L3)*E3+ROUND($T$4*(1+H4+L4),0)*E4+$T$5*(1+H5+L5)*E5+$T$6*(1+H6+L6)*E6),0)</f>
         <v>580</v>
       </c>
-      <c r="AQ25" s="35"/>
       <c r="AR25" s="20" t="s">
         <v>32</v>
       </c>
@@ -9805,35 +10031,34 @@
         <f>ROUND($B$10*(1+$T$2*(1+I2+L2)*E2+$T$3*(1+I3+L3)*E3+ROUND($T$4*(1+I4+L4),0)*E4+$T$5*(1+I5+L5)*E5+$T$6*(1+I6+L6)*E6),0)</f>
         <v>600</v>
       </c>
-      <c r="AX25" s="35"/>
       <c r="AY25" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="AZ25" s="36">
-        <f>ROUND($B$8*(1+$T$2*(1+J2+L2)*B2+ROUNDDOWN($T$3*(1+J3+L3),0)*B3+$T$4*(1+J4+L4)*B4+$T$5*(1+J5+L5)*B5+$T$6*(1+J6+L6)*B6),0)</f>
-        <v>205</v>
-      </c>
-      <c r="BA25" s="36">
-        <f>ROUND($B$9*(1+ROUNDDOWN($T$2*(1+J2+L2),0)*C2+$T$3*(1+J3+L3)*C3+$T$4*(1+J4+L4)*C4+$T$5*(1+J5+L5)*C5+$T$6*(1+J6+L6)*C6),0)</f>
-        <v>51</v>
+      <c r="AZ25" s="21">
+        <f>ROUND($B$8*(1+$T$2*(1+J2+L2)*B2+ROUND($T$3*(1+J3+L3),0)*B3+$T$4*(1+J4+L4)*B4+ROUND($T$5*(1+J5+L5),0)*B5+$T$6*(1+J6+L6)*B6),0)</f>
+        <v>207</v>
+      </c>
+      <c r="BA25" s="20">
+        <f>ROUND($B$9*(1+$T$2*(1+J2+L2)*C2+$T$3*(1+J3+L3)*C3+$T$4*(1+J4+L4)*C4+$T$5*(1+J5+L5)*C5+$T$6*(1+J6+L6)*C6),0)</f>
+        <v>52</v>
       </c>
       <c r="BB25" s="20">
         <f t="shared" ref="BB25:BB29" si="22">ROUND($B$12*(1+BC25),0)</f>
         <v>13</v>
       </c>
-      <c r="BC25" s="36">
-        <f>ROUND($B$11+ROUNDDOWN($T$2*(1+J2+L2),0)*D2+ROUNDDOWN($T$3*(1+J3+L3),0)*D3+$T$4*(1+J4+L4)*D4+$T$5*(1+J5+L5)*D5+$T$6*(1+J6+L6)*D6,2)</f>
-        <v>1.56</v>
-      </c>
-      <c r="BD25" s="36">
-        <f>ROUND($B$10*(1+$T$2*(1+J2+L2)*E2+$T$3*(1+J3+L3)*E3+ROUNDDOWN($T$4*(1+J4+L4),0)*E4+$T$5*(1+J5+L5)*E5+$T$6*(1+J6+L6)*E6),0)</f>
-        <v>620</v>
+      <c r="BC25" s="21">
+        <f>ROUND($B$11+ROUND($T$2*(1+J2+L2),0)*D2+$T$3*(1+J3+L3)*D3+$T$4*(1+J4+L4)*D4+$T$5*(1+J5+L5)*D5+$T$6*(1+J6+L6)*D6,2)</f>
+        <v>1.59</v>
+      </c>
+      <c r="BD25" s="21">
+        <f>ROUND($B$10*(1+$T$2*(1+J2+L2)*E2+$T$3*(1+J3+L3)*E3+ROUND($T$4*(1+J4+L4),0)*E4+$T$5*(1+J5+L5)*E5+$T$6*(1+J6+L6)*E6),0)</f>
+        <v>630</v>
       </c>
       <c r="BF25" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="BG25" s="20">
-        <f>ROUND($B$8*(1+$T$2*(1+K2+L2)*B2+$T$3*(1+K3+L3)*B3+$T$4*(1+K4+L4)*B4+$T$5*(1+K5+L5)*B5+$T$6*(1+K6+L6)*B6),0)</f>
+      <c r="BG25" s="21">
+        <f>ROUND($B$8*(1+$T$2*(1+K2+L2)*B2+ROUND($T$3*(1+K3+L3),0)*B3+$T$4*(1+K4+L4)*B4+ROUND($T$5*(1+K5+L5),0)*B5+$T$6*(1+K6+L6)*B6),0)</f>
         <v>238</v>
       </c>
       <c r="BH25" s="20">
@@ -9949,31 +10174,31 @@
       <c r="AY26" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="AZ26" s="36">
-        <f>ROUND($B$8*(1+$T$2*(1+J2+M2)*B2+ROUNDDOWN($T$3*(1+J3+M3),0)*B3+$T$4*(1+J4+M4)*B4+$T$5*(1+J5+M5)*B5+$T$6*(1+J6+M6)*B6),0)</f>
-        <v>205</v>
-      </c>
-      <c r="BA26" s="36">
-        <f>ROUND($B$9*(1+ROUNDDOWN($T$2*(1+J2+M2),0)*C2+$T$3*(1+J3+M3)*C3+$T$4*(1+J4+M4)*C4+$T$5*(1+J5+M5)*C5+$T$6*(1+J6+M6)*C6),0)</f>
-        <v>51</v>
+      <c r="AZ26" s="21">
+        <f>ROUND($B$8*(1+$T$2*(1+J2+M2)*B2+ROUND($T$3*(1+J3+M3),0)*B3+$T$4*(1+J4+M4)*B4+ROUND($T$5*(1+J5+M5),0)*B5+$T$6*(1+J6+M6)*B6),0)</f>
+        <v>207</v>
+      </c>
+      <c r="BA26" s="20">
+        <f>ROUND($B$9*(1+$T$2*(1+J2+M2)*C2+$T$3*(1+J3+M3)*C3+$T$4*(1+J4+M4)*C4+$T$5*(1+J5+M5)*C5+$T$6*(1+J6+M6)*C6),0)</f>
+        <v>52</v>
       </c>
       <c r="BB26" s="20">
         <f t="shared" si="22"/>
         <v>13</v>
       </c>
-      <c r="BC26" s="36">
-        <f>ROUND($B$11+ROUNDDOWN($T$2*(1+J2+M2),0)*D2+ROUNDDOWN($T$3*(1+J3+M3),0)*D3+$T$4*(1+J4+M4)*D4+$T$5*(1+J5+M5)*D5+$T$6*(1+J6+M6)*D6,2)</f>
-        <v>1.56</v>
-      </c>
-      <c r="BD26" s="36">
-        <f>ROUND($B$10*(1+$T$2*(1+J2+M2)*E2+$T$3*(1+J3+M3)*E3+ROUNDDOWN($T$4*(1+J4+M4),0)*E4+$T$5*(1+J5+M5)*E5+$T$6*(1+J6+M6)*E6),0)</f>
+      <c r="BC26" s="21">
+        <f>ROUND($B$11+ROUND($T$2*(1+J2+M2),0)*D2+$T$3*(1+J3+M3)*D3+$T$4*(1+J4+M4)*D4+$T$5*(1+J5+M5)*D5+$T$6*(1+J6+M6)*D6,2)</f>
+        <v>1.59</v>
+      </c>
+      <c r="BD26" s="21">
+        <f>ROUND($B$10*(1+$T$2*(1+J2+M2)*E2+$T$3*(1+J3+M3)*E3+ROUND($T$4*(1+J4+M4),0)*E4+$T$5*(1+J5+M5)*E5+$T$6*(1+J6+M6)*E6),0)</f>
         <v>630</v>
       </c>
       <c r="BF26" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="BG26" s="20">
-        <f>ROUND($B$8*(1+$T$2*(1+K2+M2)*B2+$T$3*(1+K3+M3)*B3+$T$4*(1+K4+M4)*B4+$T$5*(1+K5+M5)*B5+$T$6*(1+K6+M6)*B6),0)</f>
+      <c r="BG26" s="21">
+        <f>ROUND($B$8*(1+$T$2*(1+K2+M2)*B2+ROUND($T$3*(1+K3+M3),0)*B3+$T$4*(1+K4+M4)*B4+ROUND($T$5*(1+K5+M5),0)*B5+$T$6*(1+K6+M6)*B6),0)</f>
         <v>238</v>
       </c>
       <c r="BH26" s="20">
@@ -10089,31 +10314,31 @@
       <c r="AY27" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="AZ27" s="36">
-        <f>ROUND($B$8*(1+$T$2*(1+J2+N2)*B2+ROUNDDOWN($T$3*(1+J3+N3),0)*B3+$T$4*(1+J4+N4)*B4+$T$5*(1+J5+N5)*B5+$T$6*(1+J6+N6)*B6),0)</f>
-        <v>205</v>
-      </c>
-      <c r="BA27" s="36">
-        <f>ROUND($B$9*(1+ROUNDDOWN($T$2*(1+J2+N2),0)*C2+$T$3*(1+J3+N3)*C3+$T$4*(1+J4+N4)*C4+$T$5*(1+J5+N5)*C5+$T$6*(1+J6+N6)*C6),0)</f>
+      <c r="AZ27" s="21">
+        <f>ROUND($B$8*(1+$T$2*(1+J2+N2)*B2+ROUND($T$3*(1+J3+N3),0)*B3+$T$4*(1+J4+N4)*B4+ROUND($T$5*(1+J5+N5),0)*B5+$T$6*(1+J6+N6)*B6),0)</f>
+        <v>207</v>
+      </c>
+      <c r="BA27" s="20">
+        <f>ROUND($B$9*(1+$T$2*(1+J2+N2)*C2+$T$3*(1+J3+N3)*C3+$T$4*(1+J4+N4)*C4+$T$5*(1+J5+N5)*C5+$T$6*(1+J6+N6)*C6),0)</f>
         <v>52</v>
       </c>
       <c r="BB27" s="20">
         <f t="shared" si="22"/>
         <v>13</v>
       </c>
-      <c r="BC27" s="36">
-        <f>ROUND($B$11+ROUNDDOWN($T$2*(1+J2+N2),0)*D2+ROUNDDOWN($T$3*(1+J3+N3),0)*D3+$T$4*(1+J4+N4)*D4+$T$5*(1+J5+N5)*D5+$T$6*(1+J6+N6)*D6,2)</f>
-        <v>1.6</v>
-      </c>
-      <c r="BD27" s="36">
-        <f>ROUND($B$10*(1+$T$2*(1+J2+N2)*E2+$T$3*(1+J3+N3)*E3+ROUNDDOWN($T$4*(1+J4+N4),0)*E4+$T$5*(1+J5+N5)*E5+$T$6*(1+J6+N6)*E6),0)</f>
-        <v>620</v>
+      <c r="BC27" s="21">
+        <f>ROUND($B$11+ROUND($T$2*(1+J2+N2),0)*D2+$T$3*(1+J3+N3)*D3+$T$4*(1+J4+N4)*D4+$T$5*(1+J5+N5)*D5+$T$6*(1+J6+N6)*D6,2)</f>
+        <v>1.61</v>
+      </c>
+      <c r="BD27" s="21">
+        <f>ROUND($B$10*(1+$T$2*(1+J2+N2)*E2+$T$3*(1+J3+N3)*E3+ROUND($T$4*(1+J4+N4),0)*E4+$T$5*(1+J5+N5)*E5+$T$6*(1+J6+N6)*E6),0)</f>
+        <v>630</v>
       </c>
       <c r="BF27" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="BG27" s="20">
-        <f>ROUND($B$8*(1+$T$2*(1+K2+N2)*B2+$T$3*(1+K3+N3)*B3+$T$4*(1+K4+N4)*B4+$T$5*(1+K5+N5)*B5+$T$6*(1+K6+N6)*B6),0)</f>
+      <c r="BG27" s="21">
+        <f>ROUND($B$8*(1+$T$2*(1+K2+N2)*B2+ROUND($T$3*(1+K3+N3),0)*B3+$T$4*(1+K4+N4)*B4+ROUND($T$5*(1+K5+N5),0)*B5+$T$6*(1+K6+N6)*B6),0)</f>
         <v>238</v>
       </c>
       <c r="BH27" s="20">
@@ -10229,31 +10454,31 @@
       <c r="AY28" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="AZ28" s="36">
-        <f>ROUND($B$8*(1+$T$2*(1+J2+O2)*B2+ROUNDDOWN($T$3*(1+J3+O3),0)*B3+$T$4*(1+J4+O4)*B4+$T$5*(1+J5+O5)*B5+$T$6*(1+J6+O6)*B6),0)</f>
-        <v>205</v>
-      </c>
-      <c r="BA28" s="36">
-        <f>ROUND($B$9*(1+ROUNDDOWN($T$2*(1+J2+O2),0)*C2+$T$3*(1+J3+O3)*C3+$T$4*(1+J4+O4)*C4+$T$5*(1+J5+O5)*C5+$T$6*(1+J6+O6)*C6),0)</f>
-        <v>51</v>
+      <c r="AZ28" s="21">
+        <f>ROUND($B$8*(1+$T$2*(1+J2+O2)*B2+ROUND($T$3*(1+J3+O3),0)*B3+$T$4*(1+J4+O4)*B4+ROUND($T$5*(1+J5+O5),0)*B5+$T$6*(1+J6+O6)*B6),0)</f>
+        <v>207</v>
+      </c>
+      <c r="BA28" s="20">
+        <f>ROUND($B$9*(1+$T$2*(1+J2+O2)*C2+$T$3*(1+J3+O3)*C3+$T$4*(1+J4+O4)*C4+$T$5*(1+J5+O5)*C5+$T$6*(1+J6+O6)*C6),0)</f>
+        <v>52</v>
       </c>
       <c r="BB28" s="20">
         <f t="shared" si="22"/>
         <v>13</v>
       </c>
-      <c r="BC28" s="36">
-        <f>ROUND($B$11+ROUNDDOWN($T$2*(1+J2+O2),0)*D2+ROUNDDOWN($T$3*(1+J3+O3),0)*D3+$T$4*(1+J4+O4)*D4+$T$5*(1+J5+O5)*D5+$T$6*(1+J6+O6)*D6,2)</f>
-        <v>1.56</v>
-      </c>
-      <c r="BD28" s="36">
-        <f>ROUND($B$10*(1+$T$2*(1+J2+O2)*E2+$T$3*(1+J3+O3)*E3+ROUNDDOWN($T$4*(1+J4+O4),0)*E4+$T$5*(1+J5+O5)*E5+$T$6*(1+J6+O6)*E6),0)</f>
-        <v>620</v>
+      <c r="BC28" s="21">
+        <f>ROUND($B$11+ROUND($T$2*(1+J2+O2),0)*D2+$T$3*(1+J3+O3)*D3+$T$4*(1+J4+O4)*D4+$T$5*(1+J5+O5)*D5+$T$6*(1+J6+O6)*D6,2)</f>
+        <v>1.59</v>
+      </c>
+      <c r="BD28" s="21">
+        <f>ROUND($B$10*(1+$T$2*(1+J2+O2)*E2+$T$3*(1+J3+O3)*E3+ROUND($T$4*(1+J4+O4),0)*E4+$T$5*(1+J5+O5)*E5+$T$6*(1+J6+O6)*E6),0)</f>
+        <v>630</v>
       </c>
       <c r="BF28" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="BG28" s="20">
-        <f>ROUND($B$8*(1+$T$2*(1+K2+O2)*B2+$T$3*(1+K3+O3)*B3+$T$4*(1+K4+O4)*B4+$T$5*(1+K5+O5)*B5+$T$6*(1+K6+O6)*B6),0)</f>
+      <c r="BG28" s="21">
+        <f>ROUND($B$8*(1+$T$2*(1+K2+O2)*B2+ROUND($T$3*(1+K3+O3),0)*B3+$T$4*(1+K4+O4)*B4+ROUND($T$5*(1+K5+O5),0)*B5+$T$6*(1+K6+O6)*B6),0)</f>
         <v>238</v>
       </c>
       <c r="BH28" s="20">
@@ -10369,25 +10594,25 @@
       <c r="AY29" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="AZ29" s="36">
-        <f>ROUND($B$8*(1+$T$2*(1+J2+P2)*B2+ROUNDDOWN($T$3*(1+J3+P3),0)*B3+$T$4*(1+J4+P4)*B4+$T$5*(1+J5+P5)*B5+$T$6*(1+J6+P6)*B6),0)</f>
-        <v>208</v>
-      </c>
-      <c r="BA29" s="36">
-        <f>ROUND($B$9*(1+ROUNDDOWN($T$2*(1+J2+P2),0)*C2+$T$3*(1+J3+P3)*C3+$T$4*(1+J4+P4)*C4+$T$5*(1+J5+P5)*C5+$T$6*(1+J6+P6)*C6),0)</f>
+      <c r="AZ29" s="21">
+        <f>ROUND($B$8*(1+$T$2*(1+J2+P2)*B2+ROUND($T$3*(1+J3+P3),0)*B3+$T$4*(1+J4+P4)*B4+ROUND($T$5*(1+J5+P5),0)*B5+$T$6*(1+J6+P6)*B6),0)</f>
+        <v>209</v>
+      </c>
+      <c r="BA29" s="20">
+        <f>ROUND($B$9*(1+$T$2*(1+J2+P2)*C2+$T$3*(1+J3+P3)*C3+$T$4*(1+J4+P4)*C4+$T$5*(1+J5+P5)*C5+$T$6*(1+J6+P6)*C6),0)</f>
         <v>52</v>
       </c>
       <c r="BB29" s="20">
         <f t="shared" si="22"/>
         <v>13</v>
       </c>
-      <c r="BC29" s="36">
-        <f>ROUND($B$11+ROUNDDOWN($T$2*(1+J2+P2),0)*D2+ROUNDDOWN($T$3*(1+J3+P3),0)*D3+$T$4*(1+J4+P4)*D4+$T$5*(1+J5+P5)*D5+$T$6*(1+J6+P6)*D6,2)</f>
-        <v>1.58</v>
-      </c>
-      <c r="BD29" s="36">
-        <f>ROUND($B$10*(1+$T$2*(1+J2+P2)*E2+$T$3*(1+J3+P3)*E3+ROUNDDOWN($T$4*(1+J4+P4),0)*E4+$T$5*(1+J5+P5)*E5+$T$6*(1+J6+P6)*E6),0)</f>
-        <v>620</v>
+      <c r="BC29" s="21">
+        <f>ROUND($B$11+ROUND($T$2*(1+J2+P2),0)*D2+$T$3*(1+J3+P3)*D3+$T$4*(1+J4+P4)*D4+$T$5*(1+J5+P5)*D5+$T$6*(1+J6+P6)*D6,2)</f>
+        <v>1.6</v>
+      </c>
+      <c r="BD29" s="21">
+        <f>ROUND($B$10*(1+$T$2*(1+J2+P2)*E2+$T$3*(1+J3+P3)*E3+ROUND($T$4*(1+J4+P4),0)*E4+$T$5*(1+J5+P5)*E5+$T$6*(1+J6+P6)*E6),0)</f>
+        <v>630</v>
       </c>
       <c r="BF29" s="20" t="s">
         <v>36</v>
@@ -10547,7 +10772,6 @@
         <f>ROUND($B$10*(1+$U$2*(1+F2+L2)*E2+$U$3*(1+F3+L3)*E3+$U$4*(1+F4+L4)*E4+$U$5*(1+F5+L5)*E5+$U$6*(1+F6+L6)*E6),0)</f>
         <v>1100</v>
       </c>
-      <c r="AC32" s="35"/>
       <c r="AD32" s="20" t="s">
         <v>32</v>
       </c>
@@ -10571,7 +10795,6 @@
         <f>ROUND($B$10*(1+$U$2*(1+G2+L2)*E2+$U$3*(1+G3+L3)*E3+$U$4*(1+G4+L4)*E4+$U$5*(1+G5+L5)*E5+$U$6*(1+G6+L6)*E6),0)</f>
         <v>1000</v>
       </c>
-      <c r="AJ32" s="35"/>
       <c r="AK32" s="20" t="s">
         <v>32</v>
       </c>
@@ -10595,7 +10818,6 @@
         <f>ROUND($B$10*(1+$U$2*(1+H2+L2)*E2+$U$3*(1+H3+L3)*E3+$U$4*(1+H4+L4)*E4+$U$5*(1+H5+L5)*E5+$U$6*(1+H6+L6)*E6),0)</f>
         <v>1050</v>
       </c>
-      <c r="AQ32" s="35"/>
       <c r="AR32" s="20" t="s">
         <v>32</v>
       </c>
@@ -10619,7 +10841,6 @@
         <f>ROUND($B$10*(1+$U$2*(1+I2+L2)*E2+$U$3*(1+I3+L3)*E3+$U$4*(1+I4+L4)*E4+$U$5*(1+I5+L5)*E5+$U$6*(1+I6+L6)*E6),0)</f>
         <v>1090</v>
       </c>
-      <c r="AX32" s="35"/>
       <c r="AY32" s="20" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
Introduce weapons: - FIST - STAFF - DAGGER - SPEAR - SWORD Character gaines random weapon at start. Damage and defense are determined based on the gained weapon.
</commit_message>
<xml_diff>
--- a/doc/caste_system.xlsx
+++ b/doc/caste_system.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/349dfb9748b30a92/Asztali gép/ataliasflame_2.0/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3326" documentId="8_{652F4476-B36F-42CD-831D-0D71B9923ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC41C551-48E2-45A6-814F-CAD97E5C04B9}"/>
+  <xr:revisionPtr revIDLastSave="3353" documentId="8_{652F4476-B36F-42CD-831D-0D71B9923ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A55BE310-870A-49C8-A2B0-99EA6CE4ABB0}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="12744" yWindow="10956" windowWidth="2388" windowHeight="564" activeTab="7" xr2:uid="{CAF51EC3-63EC-48CD-AA7B-C21B3D5D222B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{CAF51EC3-63EC-48CD-AA7B-C21B3D5D222B}"/>
   </bookViews>
   <sheets>
     <sheet name="caste list" sheetId="1" r:id="rId1"/>
@@ -1699,6 +1699,64 @@
           </rPr>
           <t xml:space="preserve">
 magic</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Mikló Attila</author>
+  </authors>
+  <commentList>
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{79C556D0-7010-4305-9BDB-E919A439FE16}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mikló Attila:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+dagger +1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{0259C8DD-5A70-4A6D-81DD-88341699A6CF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mikló Attila:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+dagger +5</t>
         </r>
       </text>
     </comment>
@@ -1898,9 +1956,6 @@
     <t>realmax</t>
   </si>
   <si>
-    <t>pusztakezes sebzés</t>
-  </si>
-  <si>
     <t>sebzés szorzó</t>
   </si>
   <si>
@@ -1962,6 +2017,9 @@
   </si>
   <si>
     <t>-&gt;</t>
+  </si>
+  <si>
+    <t>élterő</t>
   </si>
 </sst>
 </file>
@@ -2177,7 +2235,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2232,6 +2290,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2653,7 +2713,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>0</v>
@@ -2708,7 +2768,7 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="38" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="30" t="s">
@@ -2764,7 +2824,7 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="37"/>
+      <c r="A4" s="39"/>
       <c r="B4" s="30" t="s">
         <v>2</v>
       </c>
@@ -2818,7 +2878,7 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="37"/>
+      <c r="A5" s="39"/>
       <c r="B5" s="30" t="s">
         <v>3</v>
       </c>
@@ -2872,7 +2932,7 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="37"/>
+      <c r="A6" s="39"/>
       <c r="B6" s="30" t="s">
         <v>21</v>
       </c>
@@ -2926,7 +2986,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="38"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="31" t="s">
         <v>4</v>
       </c>
@@ -2980,7 +3040,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="41" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="32" t="s">
@@ -3036,7 +3096,7 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="40"/>
+      <c r="A9" s="42"/>
       <c r="B9" s="32" t="s">
         <v>6</v>
       </c>
@@ -3090,7 +3150,7 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="40"/>
+      <c r="A10" s="42"/>
       <c r="B10" s="32" t="s">
         <v>7</v>
       </c>
@@ -3144,7 +3204,7 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="41"/>
+      <c r="A11" s="43"/>
       <c r="B11" s="29" t="s">
         <v>8</v>
       </c>
@@ -3198,8 +3258,8 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="39" t="s">
-        <v>81</v>
+      <c r="A12" s="41" t="s">
+        <v>80</v>
       </c>
       <c r="B12" s="32" t="s">
         <v>9</v>
@@ -3254,7 +3314,7 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="40"/>
+      <c r="A13" s="42"/>
       <c r="B13" s="30" t="s">
         <v>10</v>
       </c>
@@ -3308,7 +3368,7 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="40"/>
+      <c r="A14" s="42"/>
       <c r="B14" s="30" t="s">
         <v>11</v>
       </c>
@@ -3362,7 +3422,7 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="41"/>
+      <c r="A15" s="43"/>
       <c r="B15" s="31" t="s">
         <v>12</v>
       </c>
@@ -3416,8 +3476,8 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="39" t="s">
-        <v>82</v>
+      <c r="A16" s="41" t="s">
+        <v>81</v>
       </c>
       <c r="B16" s="32" t="s">
         <v>13</v>
@@ -3472,7 +3532,7 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="40"/>
+      <c r="A17" s="42"/>
       <c r="B17" s="30" t="s">
         <v>14</v>
       </c>
@@ -3526,7 +3586,7 @@
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" s="40"/>
+      <c r="A18" s="42"/>
       <c r="B18" s="30" t="s">
         <v>15</v>
       </c>
@@ -3580,7 +3640,7 @@
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" s="41"/>
+      <c r="A19" s="43"/>
       <c r="B19" s="31" t="s">
         <v>16</v>
       </c>
@@ -3634,8 +3694,8 @@
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="36" t="s">
-        <v>83</v>
+      <c r="A20" s="38" t="s">
+        <v>82</v>
       </c>
       <c r="B20" s="30" t="s">
         <v>17</v>
@@ -3690,7 +3750,7 @@
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21" s="37"/>
+      <c r="A21" s="39"/>
       <c r="B21" s="30" t="s">
         <v>18</v>
       </c>
@@ -3744,7 +3804,7 @@
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22" s="37"/>
+      <c r="A22" s="39"/>
       <c r="B22" s="30" t="s">
         <v>19</v>
       </c>
@@ -3798,7 +3858,7 @@
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23" s="38"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="31" t="s">
         <v>20</v>
       </c>
@@ -5779,7 +5839,7 @@
   <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5980,13 +6040,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" t="s">
         <v>77</v>
       </c>
-      <c r="B1" t="s">
-        <v>78</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -5997,7 +6057,7 @@
         <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -6796,11 +6856,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D8DF294-C85C-47A3-9A81-4E26EFDC10EC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D8DF294-C85C-47A3-9A81-4E26EFDC10EC}">
   <dimension ref="A1:BK54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="BF29" sqref="BF29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -6932,54 +6992,54 @@
       <c r="U1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="W1" s="42" t="s">
+      <c r="W1" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="X1" s="44"/>
+      <c r="Y1" s="44"/>
+      <c r="Z1" s="44"/>
+      <c r="AA1" s="44"/>
+      <c r="AB1" s="44"/>
+      <c r="AD1" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="X1" s="42"/>
-      <c r="Y1" s="42"/>
-      <c r="Z1" s="42"/>
-      <c r="AA1" s="42"/>
-      <c r="AB1" s="42"/>
-      <c r="AD1" s="42" t="s">
+      <c r="AE1" s="44"/>
+      <c r="AF1" s="44"/>
+      <c r="AG1" s="44"/>
+      <c r="AH1" s="44"/>
+      <c r="AI1" s="44"/>
+      <c r="AK1" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="AE1" s="42"/>
-      <c r="AF1" s="42"/>
-      <c r="AG1" s="42"/>
-      <c r="AH1" s="42"/>
-      <c r="AI1" s="42"/>
-      <c r="AK1" s="42" t="s">
+      <c r="AL1" s="44"/>
+      <c r="AM1" s="44"/>
+      <c r="AN1" s="44"/>
+      <c r="AO1" s="44"/>
+      <c r="AP1" s="44"/>
+      <c r="AR1" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="AL1" s="42"/>
-      <c r="AM1" s="42"/>
-      <c r="AN1" s="42"/>
-      <c r="AO1" s="42"/>
-      <c r="AP1" s="42"/>
-      <c r="AR1" s="42" t="s">
+      <c r="AS1" s="44"/>
+      <c r="AT1" s="44"/>
+      <c r="AU1" s="44"/>
+      <c r="AV1" s="44"/>
+      <c r="AW1" s="44"/>
+      <c r="AY1" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="AZ1" s="44"/>
+      <c r="BA1" s="44"/>
+      <c r="BB1" s="44"/>
+      <c r="BC1" s="44"/>
+      <c r="BD1" s="44"/>
+      <c r="BF1" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="AS1" s="42"/>
-      <c r="AT1" s="42"/>
-      <c r="AU1" s="42"/>
-      <c r="AV1" s="42"/>
-      <c r="AW1" s="42"/>
-      <c r="AY1" s="42" t="s">
-        <v>79</v>
-      </c>
-      <c r="AZ1" s="42"/>
-      <c r="BA1" s="42"/>
-      <c r="BB1" s="42"/>
-      <c r="BC1" s="42"/>
-      <c r="BD1" s="42"/>
-      <c r="BF1" s="42" t="s">
-        <v>74</v>
-      </c>
-      <c r="BG1" s="42"/>
-      <c r="BH1" s="42"/>
-      <c r="BI1" s="42"/>
-      <c r="BJ1" s="42"/>
-      <c r="BK1" s="42"/>
+      <c r="BG1" s="44"/>
+      <c r="BH1" s="44"/>
+      <c r="BI1" s="44"/>
+      <c r="BJ1" s="44"/>
+      <c r="BK1" s="44"/>
     </row>
     <row r="2" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
@@ -7111,7 +7171,7 @@
         <v>100</v>
       </c>
       <c r="W3" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="X3" s="18" t="s">
         <v>43</v>
@@ -7123,13 +7183,13 @@
         <v>54</v>
       </c>
       <c r="AA3" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AB3" s="18" t="s">
         <v>55</v>
       </c>
       <c r="AD3" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AE3" s="18" t="s">
         <v>43</v>
@@ -7141,13 +7201,13 @@
         <v>54</v>
       </c>
       <c r="AH3" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AI3" s="18" t="s">
         <v>55</v>
       </c>
       <c r="AK3" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AL3" s="18" t="s">
         <v>43</v>
@@ -7159,13 +7219,13 @@
         <v>54</v>
       </c>
       <c r="AO3" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AP3" s="18" t="s">
         <v>55</v>
       </c>
       <c r="AR3" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AS3" s="18" t="s">
         <v>43</v>
@@ -7177,13 +7237,13 @@
         <v>54</v>
       </c>
       <c r="AV3" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AW3" s="18" t="s">
         <v>55</v>
       </c>
       <c r="AY3" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AZ3" s="18" t="s">
         <v>43</v>
@@ -7195,13 +7255,13 @@
         <v>54</v>
       </c>
       <c r="BC3" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BD3" s="18" t="s">
         <v>55</v>
       </c>
       <c r="BF3" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="BG3" s="18" t="s">
         <v>43</v>
@@ -7213,7 +7273,7 @@
         <v>54</v>
       </c>
       <c r="BJ3" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BK3" s="18" t="s">
         <v>55</v>
@@ -7292,7 +7352,7 @@
       </c>
       <c r="Y4" s="18">
         <f>ROUND($B$9*(1+$Q$2*(1+F2+L2)*C2+$Q$3*(1+F3+L3)*C3+$Q$4*(1+F4+L4)*C4+$Q$5*(1+F5+L5)*C5+$Q$6*(1+F6+L6)*C6),0)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Z4" s="18">
         <f>ROUND($B$12*(1+AA4),0)</f>
@@ -7315,7 +7375,7 @@
       </c>
       <c r="AF4" s="18">
         <f>ROUND($B$9*(1+$Q$2*(1+G2+L2)*C2+$Q$3*(1+G3+L3)*C3+$Q$4*(1+G4+L4)*C4+$Q$5*(1+G5+L5)*C5+$Q$6*(1+G6+L6)*C6),0)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AG4" s="18">
         <f>ROUND($B$12*(1+AH4),0)</f>
@@ -7338,7 +7398,7 @@
       </c>
       <c r="AM4" s="18">
         <f>ROUND($B$9*(1+$Q$2*(1+H2+L2)*C2+$Q$3*(1+H3+L3)*C3+$Q$4*(1+H4+L4)*C4+$Q$5*(1+H5+L5)*C5+$Q$6*(1+H6+L6)*C6),0)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AN4" s="18">
         <f>ROUND($B$12*(1+AO4),0)</f>
@@ -7361,7 +7421,7 @@
       </c>
       <c r="AT4" s="18">
         <f>ROUND($B$9*(1+$Q$2*(1+I2+L2)*C2+$Q$3*(1+I3+L3)*C3+$Q$4*(1+I4+L4)*C4+$Q$5*(1+I5+L5)*C5+$Q$6*(1+I6+L6)*C6),0)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AU4" s="18">
         <f>ROUND($B$12*(1+AV4),0)</f>
@@ -7384,7 +7444,7 @@
       </c>
       <c r="BA4" s="18">
         <f>ROUND($B$9*(1+$Q$2*(1+J2+L2)*C2+$Q$3*(1+J3+L3)*C3+$Q$4*(1+J4+L4)*C4+$Q$5*(1+J5+L5)*C5+$Q$6*(1+J6+L6)*C6),0)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="BB4" s="18">
         <f>ROUND($B$12*(1+BC4),0)</f>
@@ -7407,7 +7467,7 @@
       </c>
       <c r="BH4" s="18">
         <f>ROUND($B$9*(1+$Q$2*(1+K2+L2)*C2+$Q$3*(1+K3+L3)*C3+$Q$4*(1+K4+L4)*C4+$Q$5*(1+K5+L5)*C5+$Q$6*(1+K6+L6)*C6),0)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="BI4" s="18">
         <f>ROUND($B$12*(1+BJ4),0)</f>
@@ -7495,7 +7555,7 @@
       </c>
       <c r="Y5" s="18">
         <f>ROUND($B$9*(1+$Q$2*(1+F2+M2)*C2+$Q$3*(1+F3+M3)*C3+$Q$4*(1+F4+M4)*C4+$Q$5*(1+F5+M5)*C5+$Q$6*(1+F6+M6)*C6),0)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Z5" s="18">
         <f>ROUND($B$12*(1+AA5),0)</f>
@@ -7518,7 +7578,7 @@
       </c>
       <c r="AF5" s="18">
         <f>ROUND($B$9*(1+$Q$2*(1+G2+M2)*C2+$Q$3*(1+G3+M3)*C3+$Q$4*(1+G4+M4)*C4+$Q$5*(1+G5+M5)*C5+$Q$6*(1+G6+M6)*C6),0)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AG5" s="18">
         <f>ROUND($B$12*(1+AH5),0)</f>
@@ -7541,7 +7601,7 @@
       </c>
       <c r="AM5" s="18">
         <f>ROUND($B$9*(1+$Q$2*(1+H2+M2)*C2+$Q$3*(1+H3+M3)*C3+$Q$4*(1+H4+M4)*C4+$Q$5*(1+H5+M5)*C5+$Q$6*(1+H6+M6)*C6),0)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AN5" s="18">
         <f>ROUND($B$12*(1+AO5),0)</f>
@@ -7564,7 +7624,7 @@
       </c>
       <c r="AT5" s="18">
         <f>ROUND($B$9*(1+$Q$2*(1+I2+M2)*C2+$Q$3*(1+I3+M3)*C3+$Q$4*(1+I4+M4)*C4+$Q$5*(1+I5+M5)*C5+$Q$6*(1+I6+M6)*C6),0)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AU5" s="18">
         <f>ROUND($B$12*(1+AV5),0)</f>
@@ -7587,7 +7647,7 @@
       </c>
       <c r="BA5" s="18">
         <f>ROUND($B$9*(1+$Q$2*(1+J2+M2)*C2+$Q$3*(1+J3+M3)*C3+$Q$4*(1+J4+M4)*C4+$Q$5*(1+J5+M5)*C5+$Q$6*(1+J6+M6)*C6),0)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="BB5" s="18">
         <f>ROUND($B$12*(1+BC5),0)</f>
@@ -7610,7 +7670,7 @@
       </c>
       <c r="BH5" s="18">
         <f>ROUND($B$9*(1+$Q$2*(1+K2+M2)*C2+$Q$3*(1+K3+M3)*C3+$Q$4*(1+K4+M4)*C4+$Q$5*(1+K5+M5)*C5+$Q$6*(1+K6+M6)*C6),0)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="BI5" s="18">
         <f>ROUND($B$12*(1+BJ5),0)</f>
@@ -7698,7 +7758,7 @@
       </c>
       <c r="Y6" s="18">
         <f>ROUND($B$9*(1+$Q$2*(1+F2+N2)*C2+$Q$3*(1+F3+N3)*C3+$Q$4*(1+F4+N4)*C4+$Q$5*(1+F5+N5)*C5+$Q$6*(1+F6+N6)*C6),0)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Z6" s="18">
         <f>ROUND($B$12*(1+AA6),0)</f>
@@ -7721,7 +7781,7 @@
       </c>
       <c r="AF6" s="18">
         <f>ROUND($B$9*(1+$Q$2*(1+G2+N2)*C2+$Q$3*(1+G3+N3)*C3+$Q$4*(1+G4+N4)*C4+$Q$5*(1+G5+N5)*C5+$Q$6*(1+G6+N6)*C6),0)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AG6" s="18">
         <f t="shared" ref="AG6:AG7" si="0">ROUND($B$12*(1+AH6),0)</f>
@@ -7744,7 +7804,7 @@
       </c>
       <c r="AM6" s="18">
         <f>ROUND($B$9*(1+$Q$2*(1+H2+N2)*C2+$Q$3*(1+H3+N3)*C3+$Q$4*(1+H4+N4)*C4+$Q$5*(1+H5+N5)*C5+$Q$6*(1+H6+N6)*C6),0)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AN6" s="18">
         <f t="shared" ref="AN6:AN8" si="1">ROUND($B$12*(1+AO6),0)</f>
@@ -7767,7 +7827,7 @@
       </c>
       <c r="AT6" s="18">
         <f>ROUND($B$9*(1+$Q$2*(1+I2+N2)*C2+$Q$3*(1+I3+N3)*C3+$Q$4*(1+I4+N4)*C4+$Q$5*(1+I5+N5)*C5+$Q$6*(1+I6+N6)*C6),0)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AU6" s="18">
         <f t="shared" ref="AU6:AU8" si="2">ROUND($B$12*(1+AV6),0)</f>
@@ -7790,7 +7850,7 @@
       </c>
       <c r="BA6" s="18">
         <f>ROUND($B$9*(1+$Q$2*(1+J2+N2)*C2+$Q$3*(1+J3+N3)*C3+$Q$4*(1+J4+N4)*C4+$Q$5*(1+J5+N5)*C5+$Q$6*(1+J6+N6)*C6),0)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="BB6" s="18">
         <f t="shared" ref="BB6:BB8" si="3">ROUND($B$12*(1+BC6),0)</f>
@@ -7813,7 +7873,7 @@
       </c>
       <c r="BH6" s="18">
         <f>ROUND($B$9*(1+$Q$2*(1+K2+N2)*C2+$Q$3*(1+K3+N3)*C3+$Q$4*(1+K4+N4)*C4+$Q$5*(1+K5+N5)*C5+$Q$6*(1+K6+N6)*C6),0)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="BI6" s="18">
         <f t="shared" ref="BI6:BI8" si="4">ROUND($B$12*(1+BJ6),0)</f>
@@ -7838,7 +7898,7 @@
       </c>
       <c r="Y7" s="18">
         <f>ROUND($B$9*(1+$Q$2*(1+F2+O2)*C2+$Q$3*(1+F3+O3)*C3+$Q$4*(1+F4+O4)*C4+$Q$5*(1+F5+O5)*C5+$Q$6*(1+F6+O6)*C6),0)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Z7" s="18">
         <f t="shared" ref="Z7" si="5">ROUND($B$12*(1+AA7),0)</f>
@@ -7861,7 +7921,7 @@
       </c>
       <c r="AF7" s="18">
         <f>ROUND($B$9*(1+$Q$2*(1+G2+O2)*C2+$Q$3*(1+G3+O3)*C3+$Q$4*(1+G4+O4)*C4+$Q$5*(1+G5+O5)*C5+$Q$6*(1+G6+O6)*C6),0)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AG7" s="18">
         <f t="shared" si="0"/>
@@ -7884,7 +7944,7 @@
       </c>
       <c r="AM7" s="18">
         <f>ROUND($B$9*(1+$Q$2*(1+H2+O2)*C2+$Q$3*(1+H3+O3)*C3+$Q$4*(1+H4+O4)*C4+$Q$5*(1+H5+O5)*C5+$Q$6*(1+H6+O6)*C6),0)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AN7" s="18">
         <f t="shared" si="1"/>
@@ -7907,7 +7967,7 @@
       </c>
       <c r="AT7" s="18">
         <f>ROUND($B$9*(1+$Q$2*(1+I2+O2)*C2+$Q$3*(1+I3+O3)*C3+$Q$4*(1+I4+O4)*C4+$Q$5*(1+I5+O5)*C5+$Q$6*(1+I6+O6)*C6),0)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AU7" s="18">
         <f t="shared" si="2"/>
@@ -7930,7 +7990,7 @@
       </c>
       <c r="BA7" s="18">
         <f>ROUND($B$9*(1+$Q$2*(1+J2+O2)*C2+$Q$3*(1+J3+O3)*C3+$Q$4*(1+J4+O4)*C4+$Q$5*(1+J5+O5)*C5+$Q$6*(1+J6+O6)*C6),0)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="BB7" s="18">
         <f t="shared" si="3"/>
@@ -7953,7 +8013,7 @@
       </c>
       <c r="BH7" s="18">
         <f>ROUND($B$9*(1+$Q$2*(1+K2+O2)*C2+$Q$3*(1+K3+O3)*C3+$Q$4*(1+K4+O4)*C4+$Q$5*(1+K5+O5)*C5+$Q$6*(1+K6+O6)*C6),0)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="BI7" s="18">
         <f t="shared" si="4"/>
@@ -7970,7 +8030,7 @@
     </row>
     <row r="8" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="B8" s="21">
         <v>80</v>
@@ -7998,7 +8058,7 @@
       </c>
       <c r="Y8" s="18">
         <f>ROUND($B$9*(1+$Q$2*(1+F2+P2)*C2+$Q$3*(1+F3+P3)*C3+$Q$4*(1+F4+P4)*C4+$Q$5*(1+F5+P5)*C5+$Q$6*(1+F6+P6)*C6),0)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Z8" s="18">
         <f>ROUND($B$12*(1+AA8),0)</f>
@@ -8021,7 +8081,7 @@
       </c>
       <c r="AF8" s="18">
         <f>ROUND($B$9*(1+$Q$2*(1+G2+P2)*C2+$Q$3*(1+G3+P3)*C3+$Q$4*(1+G4+P4)*C4+$Q$5*(1+G5+P5)*C5+$Q$6*(1+G6+P6)*C6),0)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AG8" s="18">
         <f>ROUND($B$12*(1+AH8),0)</f>
@@ -8044,7 +8104,7 @@
       </c>
       <c r="AM8" s="18">
         <f>ROUND($B$9*(1+$Q$2*(1+H2+P2)*C2+$Q$3*(1+H3+P3)*C3+$Q$4*(1+H4+P4)*C4+$Q$5*(1+H5+P5)*C5+$Q$6*(1+H6+P6)*C6),0)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AN8" s="18">
         <f t="shared" si="1"/>
@@ -8067,7 +8127,7 @@
       </c>
       <c r="AT8" s="18">
         <f>ROUND($B$9*(1+$Q$2*(1+I2+P2)*C2+$Q$3*(1+I3+P3)*C3+$Q$4*(1+I4+P4)*C4+$Q$5*(1+I5+P5)*C5+$Q$6*(1+I6+P6)*C6),0)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AU8" s="18">
         <f t="shared" si="2"/>
@@ -8090,7 +8150,7 @@
       </c>
       <c r="BA8" s="18">
         <f>ROUND($B$9*(1+$Q$2*(1+J2+P2)*C2+$Q$3*(1+J3+P3)*C3+$Q$4*(1+J4+P4)*C4+$Q$5*(1+J5+P5)*C5+$Q$6*(1+J6+P6)*C6),0)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="BB8" s="18">
         <f t="shared" si="3"/>
@@ -8113,7 +8173,7 @@
       </c>
       <c r="BH8" s="18">
         <f>ROUND($B$9*(1+$Q$2*(1+K2+P2)*C2+$Q$3*(1+K3+P3)*C3+$Q$4*(1+K4+P4)*C4+$Q$5*(1+K5+P5)*C5+$Q$6*(1+K6+P6)*C6),0)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="BI8" s="18">
         <f t="shared" si="4"/>
@@ -8130,10 +8190,11 @@
     </row>
     <row r="9" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B9" s="21">
-        <v>20</v>
+        <f>20+1</f>
+        <v>21</v>
       </c>
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
@@ -8152,7 +8213,7 @@
     </row>
     <row r="10" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="B10" s="21">
         <v>100</v>
@@ -8172,7 +8233,7 @@
       <c r="O10" s="17"/>
       <c r="P10" s="17"/>
       <c r="W10" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="X10" s="18" t="s">
         <v>43</v>
@@ -8184,13 +8245,13 @@
         <v>54</v>
       </c>
       <c r="AA10" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AB10" s="18" t="s">
         <v>55</v>
       </c>
       <c r="AD10" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AE10" s="18" t="s">
         <v>43</v>
@@ -8202,13 +8263,13 @@
         <v>54</v>
       </c>
       <c r="AH10" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AI10" s="18" t="s">
         <v>55</v>
       </c>
       <c r="AK10" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AL10" s="18" t="s">
         <v>43</v>
@@ -8220,13 +8281,13 @@
         <v>54</v>
       </c>
       <c r="AO10" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AP10" s="18" t="s">
         <v>55</v>
       </c>
       <c r="AR10" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AS10" s="18" t="s">
         <v>43</v>
@@ -8238,13 +8299,13 @@
         <v>54</v>
       </c>
       <c r="AV10" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AW10" s="18" t="s">
         <v>55</v>
       </c>
       <c r="AY10" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AZ10" s="18" t="s">
         <v>43</v>
@@ -8256,13 +8317,13 @@
         <v>54</v>
       </c>
       <c r="BC10" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BD10" s="18" t="s">
         <v>55</v>
       </c>
       <c r="BF10" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="BG10" s="18" t="s">
         <v>43</v>
@@ -8274,7 +8335,7 @@
         <v>54</v>
       </c>
       <c r="BJ10" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BK10" s="18" t="s">
         <v>55</v>
@@ -8282,7 +8343,7 @@
     </row>
     <row r="11" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B11" s="21">
         <v>0</v>
@@ -8305,7 +8366,7 @@
       </c>
       <c r="Y11" s="18">
         <f>ROUND($B$9*(1+$R$2*(1+F2+L2)*C2+$R$3*(1+F3+L3)*C3+$R$4*(1+F4+L4)*C4+$R$5*(1+F5+L5)*C5+$R$6*(1+F6+L6)*C6),0)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Z11" s="18">
         <f>ROUND($B$12*(1+AA11),0)</f>
@@ -8328,7 +8389,7 @@
       </c>
       <c r="AF11" s="18">
         <f>ROUND($B$9*(1+$R$2*(1+G2+L2)*C2+$R$3*(1+G3+L3)*C3+$R$4*(1+G4+L4)*C4+$R$5*(1+G5+L5)*C5+$R$6*(1+G6+L6)*C6),0)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AG11" s="18">
         <f>ROUND($B$12*(1+AH11),0)</f>
@@ -8351,7 +8412,7 @@
       </c>
       <c r="AM11" s="18">
         <f>ROUND($B$9*(1+$R$2*(1+H2+L2)*C2+$R$3*(1+H3+L3)*C3+$R$4*(1+H4+L4)*C4+$R$5*(1+H5+L5)*C5+$R$6*(1+H6+L6)*C6),0)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AN11" s="18">
         <f t="shared" ref="AN11:AN15" si="6">ROUND($B$12*(1+AO11),0)</f>
@@ -8374,7 +8435,7 @@
       </c>
       <c r="AT11" s="18">
         <f>ROUND($B$9*(1+$R$2*(1+I2+L2)*C2+$R$3*(1+I3+L3)*C3+$R$4*(1+I4+L4)*C4+$R$5*(1+I5+L5)*C5+$R$6*(1+I6+L6)*C6),0)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AU11" s="18">
         <f t="shared" ref="AU11:AU15" si="7">ROUND($B$12*(1+AV11),0)</f>
@@ -8397,7 +8458,7 @@
       </c>
       <c r="BA11" s="18">
         <f>ROUND($B$9*(1+$R$2*(1+J2+L2)*C2+$R$3*(1+J3+L3)*C3+$R$4*(1+J4+L4)*C4+$R$5*(1+J5+L5)*C5+$R$6*(1+J6+L6)*C6),0)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="BB11" s="18">
         <f t="shared" ref="BB11:BB15" si="8">ROUND($B$12*(1+BC11),0)</f>
@@ -8420,7 +8481,7 @@
       </c>
       <c r="BH11" s="18">
         <f>ROUND($B$9*(1+$R$2*(1+K2+L2)*C2+$R$3*(1+K3+L3)*C3+$R$4*(1+K4+L4)*C4+$R$5*(1+K5+L5)*C5+$R$6*(1+K6+L6)*C6),0)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="BI11" s="18">
         <f t="shared" ref="BI11:BI15" si="9">ROUND($B$12*(1+BJ11),0)</f>
@@ -8437,9 +8498,10 @@
     </row>
     <row r="12" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B12" s="21">
+        <f>0+5</f>
         <v>5</v>
       </c>
       <c r="C12" s="17"/>
@@ -8460,7 +8522,7 @@
       </c>
       <c r="Y12" s="18">
         <f>ROUND($B$9*(1+$R$2*(1+F2+M2)*C2+$R$3*(1+F3+M3)*C3+$R$4*(1+F4+M4)*C4+$R$5*(1+F5+M5)*C5+$R$6*(1+F6+M6)*C6),0)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Z12" s="18">
         <f>ROUND($B$12*(1+AA12),0)</f>
@@ -8483,7 +8545,7 @@
       </c>
       <c r="AF12" s="18">
         <f>ROUND($B$9*(1+$R$2*(1+G2+M2)*C2+$R$3*(1+G3+M3)*C3+$R$4*(1+G4+M4)*C4+$R$5*(1+G5+M5)*C5+$R$6*(1+G6+M6)*C6),0)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AG12" s="18">
         <f>ROUND($B$12*(1+AH12),0)</f>
@@ -8506,7 +8568,7 @@
       </c>
       <c r="AM12" s="18">
         <f>ROUND($B$9*(1+$R$2*(1+H2+M2)*C2+$R$3*(1+H3+M3)*C3+$R$4*(1+H4+M4)*C4+$R$5*(1+H5+M5)*C5+$R$6*(1+H6+M6)*C6),0)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AN12" s="18">
         <f t="shared" si="6"/>
@@ -8529,7 +8591,7 @@
       </c>
       <c r="AT12" s="18">
         <f>ROUND($B$9*(1+$R$2*(1+I2+M2)*C2+$R$3*(1+I3+M3)*C3+$R$4*(1+I4+M4)*C4+$R$5*(1+I5+M5)*C5+$R$6*(1+I6+M6)*C6),0)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AU12" s="18">
         <f t="shared" si="7"/>
@@ -8552,7 +8614,7 @@
       </c>
       <c r="BA12" s="18">
         <f>ROUND($B$9*(1+$R$2*(1+J2+M2)*C2+$R$3*(1+J3+M3)*C3+$R$4*(1+J4+M4)*C4+$R$5*(1+J5+M5)*C5+$R$6*(1+J6+M6)*C6),0)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="BB12" s="18">
         <f t="shared" si="8"/>
@@ -8575,7 +8637,7 @@
       </c>
       <c r="BH12" s="18">
         <f>ROUND($B$9*(1+$R$2*(1+K2+M2)*C2+$R$3*(1+K3+M3)*C3+$R$4*(1+K4+M4)*C4+$R$5*(1+K5+M5)*C5+$R$6*(1+K6+M6)*C6),0)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="BI12" s="18">
         <f t="shared" si="9"/>
@@ -8601,7 +8663,7 @@
       </c>
       <c r="Y13" s="18">
         <f>ROUND($B$9*(1+$R$2*(1+F2+N2)*C2+$R$3*(1+F3+N3)*C3+$R$4*(1+F4+N4)*C4+$R$5*(1+F5+N5)*C5+$R$6*(1+F6+N6)*C6),0)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Z13" s="18">
         <f t="shared" ref="Z13:Z15" si="10">ROUND($B$12*(1+AA13),0)</f>
@@ -8624,7 +8686,7 @@
       </c>
       <c r="AF13" s="18">
         <f>ROUND($B$9*(1+$R$2*(1+G2+N2)*C2+$R$3*(1+G3+N3)*C3+$R$4*(1+G4+N4)*C4+$R$5*(1+G5+N5)*C5+$R$6*(1+G6+N6)*C6),0)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AG13" s="18">
         <f t="shared" ref="AG13:AG15" si="11">ROUND($B$12*(1+AH13),0)</f>
@@ -8647,7 +8709,7 @@
       </c>
       <c r="AM13" s="18">
         <f>ROUND($B$9*(1+$R$2*(1+H2+N2)*C2+$R$3*(1+H3+N3)*C3+$R$4*(1+H4+N4)*C4+$R$5*(1+H5+N5)*C5+$R$6*(1+H6+N6)*C6),0)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AN13" s="18">
         <f t="shared" si="6"/>
@@ -8670,7 +8732,7 @@
       </c>
       <c r="AT13" s="18">
         <f>ROUND($B$9*(1+$R$2*(1+I2+N2)*C2+$R$3*(1+I3+N3)*C3+$R$4*(1+I4+N4)*C4+$R$5*(1+I5+N5)*C5+$R$6*(1+I6+N6)*C6),0)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AU13" s="18">
         <f t="shared" si="7"/>
@@ -8693,7 +8755,7 @@
       </c>
       <c r="BA13" s="18">
         <f>ROUND($B$9*(1+$R$2*(1+J2+N2)*C2+$R$3*(1+J3+N3)*C3+$R$4*(1+J4+N4)*C4+$R$5*(1+J5+N5)*C5+$R$6*(1+J6+N6)*C6),0)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="BB13" s="18">
         <f t="shared" si="8"/>
@@ -8716,7 +8778,7 @@
       </c>
       <c r="BH13" s="18">
         <f>ROUND($B$9*(1+$R$2*(1+K2+N2)*C2+$R$3*(1+K3+N3)*C3+$R$4*(1+K4+N4)*C4+$R$5*(1+K5+N5)*C5+$R$6*(1+K6+N6)*C6),0)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="BI13" s="18">
         <f t="shared" si="9"/>
@@ -8742,7 +8804,7 @@
       </c>
       <c r="Y14" s="18">
         <f>ROUND($B$9*(1+$R$2*(1+F2+O2)*C2+$R$3*(1+F3+O3)*C3+$R$4*(1+F4+O4)*C4+$R$5*(1+F5+O5)*C5+$R$6*(1+F6+O6)*C6),0)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Z14" s="18">
         <f t="shared" si="10"/>
@@ -8765,7 +8827,7 @@
       </c>
       <c r="AF14" s="18">
         <f>ROUND($B$9*(1+$R$2*(1+G2+O2)*C2+$R$3*(1+G3+O3)*C3+$R$4*(1+G4+O4)*C4+$R$5*(1+G5+O5)*C5+$R$6*(1+G6+O6)*C6),0)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AG14" s="18">
         <f t="shared" si="11"/>
@@ -8788,7 +8850,7 @@
       </c>
       <c r="AM14" s="18">
         <f>ROUND($B$9*(1+$R$2*(1+H2+O2)*C2+$R$3*(1+H3+O3)*C3+$R$4*(1+H4+O4)*C4+$R$5*(1+H5+O5)*C5+$R$6*(1+H6+O6)*C6),0)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AN14" s="18">
         <f t="shared" si="6"/>
@@ -8811,7 +8873,7 @@
       </c>
       <c r="AT14" s="18">
         <f>ROUND($B$9*(1+$R$2*(1+I2+O2)*C2+$R$3*(1+I3+O3)*C3+$R$4*(1+I4+O4)*C4+$R$5*(1+I5+O5)*C5+$R$6*(1+I6+O6)*C6),0)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AU14" s="18">
         <f t="shared" si="7"/>
@@ -8834,7 +8896,7 @@
       </c>
       <c r="BA14" s="18">
         <f>ROUND($B$9*(1+$R$2*(1+J2+O2)*C2+$R$3*(1+J3+O3)*C3+$R$4*(1+J4+O4)*C4+$R$5*(1+J5+O5)*C5+$R$6*(1+J6+O6)*C6),0)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="BB14" s="18">
         <f t="shared" si="8"/>
@@ -8857,7 +8919,7 @@
       </c>
       <c r="BH14" s="18">
         <f>ROUND($B$9*(1+$R$2*(1+K2+O2)*C2+$R$3*(1+K3+O3)*C3+$R$4*(1+K4+O4)*C4+$R$5*(1+K5+O5)*C5+$R$6*(1+K6+O6)*C6),0)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="BI14" s="18">
         <f t="shared" si="9"/>
@@ -8883,7 +8945,7 @@
       </c>
       <c r="Y15" s="18">
         <f>ROUND($B$9*(1+$R$2*(1+F2+P2)*C2+$R$3*(1+F3+P3)*C3+$R$4*(1+F4+P4)*C4+$R$5*(1+F5+P5)*C5+$R$6*(1+F6+P6)*C6),0)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Z15" s="18">
         <f t="shared" si="10"/>
@@ -8906,7 +8968,7 @@
       </c>
       <c r="AF15" s="18">
         <f>ROUND($B$9*(1+$R$2*(1+G2+P2)*C2+$R$3*(1+G3+P3)*C3+$R$4*(1+G4+P4)*C4+$R$5*(1+G5+P5)*C5+$R$6*(1+G6+P6)*C6),0)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AG15" s="18">
         <f t="shared" si="11"/>
@@ -8929,7 +8991,7 @@
       </c>
       <c r="AM15" s="18">
         <f>ROUND($B$9*(1+$R$2*(1+H2+P2)*C2+$R$3*(1+H3+P3)*C3+$R$4*(1+H4+P4)*C4+$R$5*(1+H5+P5)*C5+$R$6*(1+H6+P6)*C6),0)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AN15" s="18">
         <f t="shared" si="6"/>
@@ -8952,7 +9014,7 @@
       </c>
       <c r="AT15" s="18">
         <f>ROUND($B$9*(1+$R$2*(1+I2+P2)*C2+$R$3*(1+I3+P3)*C3+$R$4*(1+I4+P4)*C4+$R$5*(1+I5+P5)*C5+$R$6*(1+I6+P6)*C6),0)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AU15" s="18">
         <f t="shared" si="7"/>
@@ -8975,7 +9037,7 @@
       </c>
       <c r="BA15" s="18">
         <f>ROUND($B$9*(1+$R$2*(1+J2+P2)*C2+$R$3*(1+J3+P3)*C3+$R$4*(1+J4+P4)*C4+$R$5*(1+J5+P5)*C5+$R$6*(1+J6+P6)*C6),0)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="BB15" s="18">
         <f t="shared" si="8"/>
@@ -8998,7 +9060,7 @@
       </c>
       <c r="BH15" s="18">
         <f>ROUND($B$9*(1+$R$2*(1+K2+P2)*C2+$R$3*(1+K3+P3)*C3+$R$4*(1+K4+P4)*C4+$R$5*(1+K5+P5)*C5+$R$6*(1+K6+P6)*C6),0)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="BI15" s="18">
         <f t="shared" si="9"/>
@@ -9018,7 +9080,7 @@
     </row>
     <row r="17" spans="23:63" x14ac:dyDescent="0.2">
       <c r="W17" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="X17" s="18" t="s">
         <v>43</v>
@@ -9030,13 +9092,13 @@
         <v>54</v>
       </c>
       <c r="AA17" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AB17" s="18" t="s">
         <v>55</v>
       </c>
       <c r="AD17" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AE17" s="18" t="s">
         <v>43</v>
@@ -9048,13 +9110,13 @@
         <v>54</v>
       </c>
       <c r="AH17" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AI17" s="18" t="s">
         <v>55</v>
       </c>
       <c r="AK17" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AL17" s="18" t="s">
         <v>43</v>
@@ -9066,13 +9128,13 @@
         <v>54</v>
       </c>
       <c r="AO17" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AP17" s="18" t="s">
         <v>55</v>
       </c>
       <c r="AR17" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AS17" s="18" t="s">
         <v>43</v>
@@ -9084,13 +9146,13 @@
         <v>54</v>
       </c>
       <c r="AV17" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AW17" s="18" t="s">
         <v>55</v>
       </c>
       <c r="AY17" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AZ17" s="18" t="s">
         <v>43</v>
@@ -9102,13 +9164,13 @@
         <v>54</v>
       </c>
       <c r="BC17" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BD17" s="18" t="s">
         <v>55</v>
       </c>
       <c r="BF17" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BG17" s="18" t="s">
         <v>43</v>
@@ -9120,7 +9182,7 @@
         <v>54</v>
       </c>
       <c r="BJ17" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BK17" s="18" t="s">
         <v>55</v>
@@ -9136,7 +9198,7 @@
       </c>
       <c r="Y18" s="18">
         <f>ROUND($B$9*(1+$S$2*(1+F2+L2)*C2+$S$3*(1+F3+L3)*C3+$S$4*(1+F4+L4)*C4+$S$5*(1+F5+L5)*C5+$S$6*(1+F6+L6)*C6),0)</f>
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="Z18" s="18">
         <f>ROUND($B$12*(1+AA18),0)</f>
@@ -9159,7 +9221,7 @@
       </c>
       <c r="AF18" s="18">
         <f>ROUND($B$9*(1+$S$2*(1+G2+L2)*C2+$S$3*(1+G3+L3)*C3+$S$4*(1+G4+L4)*C4+$S$5*(1+G5+L5)*C5+$S$6*(1+G6+L6)*C6),0)</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AG18" s="18">
         <f>ROUND($B$12*(1+AH18),0)</f>
@@ -9182,7 +9244,7 @@
       </c>
       <c r="AM18" s="18">
         <f>ROUND($B$9*(1+$S$2*(1+H2+L2)*C2+$S$3*(1+H3+L3)*C3+$S$4*(1+H4+L4)*C4+$S$5*(1+H5+L5)*C5+$S$6*(1+H6+L6)*C6),0)</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AN18" s="18">
         <f t="shared" ref="AN18:AN22" si="12">ROUND($B$12*(1+AO18),0)</f>
@@ -9205,7 +9267,7 @@
       </c>
       <c r="AT18" s="18">
         <f>ROUND($B$9*(1+$S$2*(1+I2+L2)*C2+$S$3*(1+I3+L3)*C3+$S$4*(1+I4+L4)*C4+$S$5*(1+I5+L5)*C5+$S$6*(1+I6+L6)*C6),0)</f>
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="AU18" s="18">
         <f t="shared" ref="AU18:AU22" si="13">ROUND($B$12*(1+AV18),0)</f>
@@ -9228,7 +9290,7 @@
       </c>
       <c r="BA18" s="18">
         <f>ROUND($B$9*(1+$S$2*(1+J2+L2)*C2+$S$3*(1+J3+L3)*C3+$S$4*(1+J4+L4)*C4+$S$5*(1+J5+L5)*C5+$S$6*(1+J6+L6)*C6),0)</f>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="BB18" s="18">
         <f t="shared" ref="BB18:BB22" si="14">ROUND($B$12*(1+BC18),0)</f>
@@ -9251,7 +9313,7 @@
       </c>
       <c r="BH18" s="18">
         <f>ROUND($B$9*(1+$S$2*(1+K2+L2)*C2+$S$3*(1+K3+L3)*C3+$S$4*(1+K4+L4)*C4+$S$5*(1+K5+L5)*C5+$S$6*(1+K6+L6)*C6),0)</f>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="BI18" s="18">
         <f t="shared" ref="BI18:BI22" si="15">ROUND($B$12*(1+BJ18),0)</f>
@@ -9276,7 +9338,7 @@
       </c>
       <c r="Y19" s="18">
         <f>ROUND($B$9*(1+$S$2*(1+F2+M2)*C2+$S$3*(1+F3+M3)*C3+$S$4*(1+F4+M4)*C4+$S$5*(1+F5+M5)*C5+$S$6*(1+F6+M6)*C6),0)</f>
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="Z19" s="18">
         <f>ROUND($B$12*(1+AA19),0)</f>
@@ -9299,7 +9361,7 @@
       </c>
       <c r="AF19" s="18">
         <f>ROUND($B$9*(1+$S$2*(1+G2+M2)*C2+$S$3*(1+G3+M3)*C3+$S$4*(1+G4+M4)*C4+$S$5*(1+G5+M5)*C5+$S$6*(1+G6+M6)*C6),0)</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AG19" s="18">
         <f>ROUND($B$12*(1+AH19),0)</f>
@@ -9322,7 +9384,7 @@
       </c>
       <c r="AM19" s="18">
         <f>ROUND($B$9*(1+$S$2*(1+H2+M2)*C2+$S$3*(1+H3+M3)*C3+$S$4*(1+H4+M4)*C4+$S$5*(1+H5+M5)*C5+$S$6*(1+H6+M6)*C6),0)</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AN19" s="18">
         <f t="shared" si="12"/>
@@ -9345,7 +9407,7 @@
       </c>
       <c r="AT19" s="18">
         <f>ROUND($B$9*(1+$S$2*(1+I2+M2)*C2+$S$3*(1+I3+M3)*C3+$S$4*(1+I4+M4)*C4+$S$5*(1+I5+M5)*C5+$S$6*(1+I6+M6)*C6),0)</f>
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="AU19" s="18">
         <f t="shared" si="13"/>
@@ -9368,7 +9430,7 @@
       </c>
       <c r="BA19" s="18">
         <f>ROUND($B$9*(1+$S$2*(1+J2+M2)*C2+$S$3*(1+J3+M3)*C3+$S$4*(1+J4+M4)*C4+$S$5*(1+J5+M5)*C5+$S$6*(1+J6+M6)*C6),0)</f>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="BB19" s="18">
         <f t="shared" si="14"/>
@@ -9391,7 +9453,7 @@
       </c>
       <c r="BH19" s="18">
         <f>ROUND($B$9*(1+$S$2*(1+K2+M2)*C2+$S$3*(1+K3+M3)*C3+$S$4*(1+K4+M4)*C4+$S$5*(1+K5+M5)*C5+$S$6*(1+K6+M6)*C6),0)</f>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="BI19" s="18">
         <f t="shared" si="15"/>
@@ -9416,7 +9478,7 @@
       </c>
       <c r="Y20" s="18">
         <f>ROUND($B$9*(1+$S$2*(1+F2+N2)*C2+$S$3*(1+F3+N3)*C3+$S$4*(1+F4+N4)*C4+$S$5*(1+F5+N5)*C5+$S$6*(1+F6+N6)*C6),0)</f>
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="Z20" s="18">
         <f t="shared" ref="Z20:Z22" si="16">ROUND($B$12*(1+AA20),0)</f>
@@ -9439,7 +9501,7 @@
       </c>
       <c r="AF20" s="18">
         <f>ROUND($B$9*(1+$S$2*(1+G2+N2)*C2+$S$3*(1+G3+N3)*C3+$S$4*(1+G4+N4)*C4+$S$5*(1+G5+N5)*C5+$S$6*(1+G6+N6)*C6),0)</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AG20" s="18">
         <f t="shared" ref="AG20:AG22" si="17">ROUND($B$12*(1+AH20),0)</f>
@@ -9462,7 +9524,7 @@
       </c>
       <c r="AM20" s="18">
         <f>ROUND($B$9*(1+$S$2*(1+H2+N2)*C2+$S$3*(1+H3+N3)*C3+$S$4*(1+H4+N4)*C4+$S$5*(1+H5+N5)*C5+$S$6*(1+H6+N6)*C6),0)</f>
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="AN20" s="18">
         <f t="shared" si="12"/>
@@ -9485,7 +9547,7 @@
       </c>
       <c r="AT20" s="18">
         <f>ROUND($B$9*(1+$S$2*(1+I2+N2)*C2+$S$3*(1+I3+N3)*C3+$S$4*(1+I4+N4)*C4+$S$5*(1+I5+N5)*C5+$S$6*(1+I6+N6)*C6),0)</f>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AU20" s="18">
         <f t="shared" si="13"/>
@@ -9508,7 +9570,7 @@
       </c>
       <c r="BA20" s="18">
         <f>ROUND($B$9*(1+$S$2*(1+J2+N2)*C2+$S$3*(1+J3+N3)*C3+$S$4*(1+J4+N4)*C4+$S$5*(1+J5+N5)*C5+$S$6*(1+J6+N6)*C6),0)</f>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="BB20" s="18">
         <f t="shared" si="14"/>
@@ -9531,7 +9593,7 @@
       </c>
       <c r="BH20" s="18">
         <f>ROUND($B$9*(1+$S$2*(1+K2+N2)*C2+$S$3*(1+K3+N3)*C3+$S$4*(1+K4+N4)*C4+$S$5*(1+K5+N5)*C5+$S$6*(1+K6+N6)*C6),0)</f>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="BI20" s="18">
         <f t="shared" si="15"/>
@@ -9556,7 +9618,7 @@
       </c>
       <c r="Y21" s="18">
         <f>ROUND($B$9*(1+$S$2*(1+F2+O2)*C2+$S$3*(1+F3+O3)*C3+$S$4*(1+F4+O4)*C4+$S$5*(1+F5+O5)*C5+$S$6*(1+F6+O6)*C6),0)</f>
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="Z21" s="18">
         <f t="shared" si="16"/>
@@ -9579,7 +9641,7 @@
       </c>
       <c r="AF21" s="18">
         <f>ROUND($B$9*(1+$S$2*(1+G2+O2)*C2+$S$3*(1+G3+O3)*C3+$S$4*(1+G4+O4)*C4+$S$5*(1+G5+O5)*C5+$S$6*(1+G6+O6)*C6),0)</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AG21" s="18">
         <f t="shared" si="17"/>
@@ -9602,7 +9664,7 @@
       </c>
       <c r="AM21" s="18">
         <f>ROUND($B$9*(1+$S$2*(1+H2+O2)*C2+$S$3*(1+H3+O3)*C3+$S$4*(1+H4+O4)*C4+$S$5*(1+H5+O5)*C5+$S$6*(1+H6+O6)*C6),0)</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AN21" s="18">
         <f t="shared" si="12"/>
@@ -9625,7 +9687,7 @@
       </c>
       <c r="AT21" s="18">
         <f>ROUND($B$9*(1+$S$2*(1+I2+O2)*C2+$S$3*(1+I3+O3)*C3+$S$4*(1+I4+O4)*C4+$S$5*(1+I5+O5)*C5+$S$6*(1+I6+O6)*C6),0)</f>
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="AU21" s="18">
         <f t="shared" si="13"/>
@@ -9648,7 +9710,7 @@
       </c>
       <c r="BA21" s="18">
         <f>ROUND($B$9*(1+$S$2*(1+J2+O2)*C2+$S$3*(1+J3+O3)*C3+$S$4*(1+J4+O4)*C4+$S$5*(1+J5+O5)*C5+$S$6*(1+J6+O6)*C6),0)</f>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="BB21" s="18">
         <f t="shared" si="14"/>
@@ -9671,7 +9733,7 @@
       </c>
       <c r="BH21" s="18">
         <f>ROUND($B$9*(1+$S$2*(1+K2+O2)*C2+$S$3*(1+K3+O3)*C3+$S$4*(1+K4+O4)*C4+$S$5*(1+K5+O5)*C5+$S$6*(1+K6+O6)*C6),0)</f>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="BI21" s="18">
         <f t="shared" si="15"/>
@@ -9696,7 +9758,7 @@
       </c>
       <c r="Y22" s="18">
         <f>ROUND($B$9*(1+$S$2*(1+F2+P2)*C2+$S$3*(1+F3+P3)*C3+$S$4*(1+F4+P4)*C4+$S$5*(1+F5+P5)*C5+$S$6*(1+F6+P6)*C6),0)</f>
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="Z22" s="18">
         <f t="shared" si="16"/>
@@ -9719,7 +9781,7 @@
       </c>
       <c r="AF22" s="18">
         <f>ROUND($B$9*(1+$S$2*(1+G2+P2)*C2+$S$3*(1+G3+P3)*C3+$S$4*(1+G4+P4)*C4+$S$5*(1+G5+P5)*C5+$S$6*(1+G6+P6)*C6),0)</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AG22" s="18">
         <f t="shared" si="17"/>
@@ -9742,7 +9804,7 @@
       </c>
       <c r="AM22" s="18">
         <f>ROUND($B$9*(1+$S$2*(1+H2+P2)*C2+$S$3*(1+H3+P3)*C3+$S$4*(1+H4+P4)*C4+$S$5*(1+H5+P5)*C5+$S$6*(1+H6+P6)*C6),0)</f>
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="AN22" s="18">
         <f t="shared" si="12"/>
@@ -9765,7 +9827,7 @@
       </c>
       <c r="AT22" s="18">
         <f>ROUND($B$9*(1+$S$2*(1+I2+P2)*C2+$S$3*(1+I3+P3)*C3+$S$4*(1+I4+P4)*C4+$S$5*(1+I5+P5)*C5+$S$6*(1+I6+P6)*C6),0)</f>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AU22" s="18">
         <f t="shared" si="13"/>
@@ -9788,7 +9850,7 @@
       </c>
       <c r="BA22" s="18">
         <f>ROUND($B$9*(1+$S$2*(1+J2+P2)*C2+$S$3*(1+J3+P3)*C3+$S$4*(1+J4+P4)*C4+$S$5*(1+J5+P5)*C5+$S$6*(1+J6+P6)*C6),0)</f>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="BB22" s="18">
         <f t="shared" si="14"/>
@@ -9811,7 +9873,7 @@
       </c>
       <c r="BH22" s="18">
         <f>ROUND($B$9*(1+$S$2*(1+K2+P2)*C2+$S$3*(1+K3+P3)*C3+$S$4*(1+K4+P4)*C4+$S$5*(1+K5+P5)*C5+$S$6*(1+K6+P6)*C6),0)</f>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="BI22" s="18">
         <f t="shared" si="15"/>
@@ -9828,7 +9890,7 @@
     </row>
     <row r="24" spans="23:63" x14ac:dyDescent="0.2">
       <c r="W24" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="X24" s="18" t="s">
         <v>43</v>
@@ -9840,13 +9902,13 @@
         <v>54</v>
       </c>
       <c r="AA24" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AB24" s="18" t="s">
         <v>55</v>
       </c>
       <c r="AD24" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AE24" s="18" t="s">
         <v>43</v>
@@ -9858,13 +9920,13 @@
         <v>54</v>
       </c>
       <c r="AH24" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AI24" s="18" t="s">
         <v>55</v>
       </c>
       <c r="AK24" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AL24" s="18" t="s">
         <v>43</v>
@@ -9876,13 +9938,13 @@
         <v>54</v>
       </c>
       <c r="AO24" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AP24" s="18" t="s">
         <v>55</v>
       </c>
       <c r="AR24" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AS24" s="18" t="s">
         <v>43</v>
@@ -9894,13 +9956,13 @@
         <v>54</v>
       </c>
       <c r="AV24" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AW24" s="18" t="s">
         <v>55</v>
       </c>
       <c r="AY24" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AZ24" s="18" t="s">
         <v>43</v>
@@ -9912,13 +9974,13 @@
         <v>54</v>
       </c>
       <c r="BC24" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BD24" s="18" t="s">
         <v>55</v>
       </c>
       <c r="BF24" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="BG24" s="18" t="s">
         <v>43</v>
@@ -9930,7 +9992,7 @@
         <v>54</v>
       </c>
       <c r="BJ24" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BK24" s="18" t="s">
         <v>55</v>
@@ -9946,7 +10008,7 @@
       </c>
       <c r="Y25" s="18">
         <f>ROUND($B$9*(1+$T$2*(1+F2+L2)*C2+$T$3*(1+F3+L3)*C3+$T$4*(1+F4+L4)*C4+$T$5*(1+F5+L5)*C5+$T$6*(1+F6+L6)*C6),0)</f>
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="Z25" s="18">
         <f t="shared" ref="Z25:Z29" si="18">ROUND($B$12*(1+AA25),0)</f>
@@ -9969,7 +10031,7 @@
       </c>
       <c r="AF25" s="18">
         <f>ROUND($B$9*(1+$T$2*(1+G2+L2)*C2+$T$3*(1+G3+L3)*C3+$T$4*(1+G4+L4)*C4+$T$5*(1+G5+L5)*C5+$T$6*(1+G6+L6)*C6),0)</f>
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AG25" s="18">
         <f t="shared" ref="AG25:AG29" si="19">ROUND($B$12*(1+AH25),0)</f>
@@ -9992,7 +10054,7 @@
       </c>
       <c r="AM25" s="18">
         <f>ROUND($B$9*(1+$T$2*(1+H2+L2)*C2+$T$3*(1+H3+L3)*C3+$T$4*(1+H4+L4)*C4+$T$5*(1+H5+L5)*C5+$T$6*(1+H6+L6)*C6),0)</f>
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AN25" s="18">
         <f t="shared" ref="AN25:AN29" si="20">ROUND($B$12*(1+AO25),0)</f>
@@ -10015,7 +10077,7 @@
       </c>
       <c r="AT25" s="18">
         <f>ROUND($B$9*(1+$T$2*(1+I2+L2)*C2+$T$3*(1+I3+L3)*C3+$T$4*(1+I4+L4)*C4+$T$5*(1+I5+L5)*C5+$T$6*(1+I6+L6)*C6),0)</f>
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="AU25" s="18">
         <f t="shared" ref="AU25:AU29" si="21">ROUND($B$12*(1+AV25),0)</f>
@@ -10038,7 +10100,7 @@
       </c>
       <c r="BA25" s="18">
         <f>ROUND($B$9*(1+$T$2*(1+J2+L2)*C2+$T$3*(1+J3+L3)*C3+$T$4*(1+J4+L4)*C4+$T$5*(1+J5+L5)*C5+$T$6*(1+J6+L6)*C6),0)</f>
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="BB25" s="18">
         <f t="shared" ref="BB25:BB29" si="22">ROUND($B$12*(1+BC25),0)</f>
@@ -10061,7 +10123,7 @@
       </c>
       <c r="BH25" s="18">
         <f>ROUND($B$9*(1+$T$2*(1+K2+L2)*C2+$T$3*(1+K3+L3)*C3+$T$4*(1+K4+L4)*C4+$T$5*(1+K5+L5)*C5+$T$6*(1+K6+L6)*C6),0)</f>
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="BI25" s="18">
         <f t="shared" ref="BI25:BI29" si="23">ROUND($B$12*(1+BJ25),0)</f>
@@ -10086,7 +10148,7 @@
       </c>
       <c r="Y26" s="18">
         <f>ROUND($B$9*(1+$T$2*(1+F2+M2)*C2+$T$3*(1+F3+M3)*C3+$T$4*(1+F4+M4)*C4+$T$5*(1+F5+M5)*C5+$T$6*(1+F6+M6)*C6),0)</f>
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="Z26" s="18">
         <f t="shared" si="18"/>
@@ -10109,7 +10171,7 @@
       </c>
       <c r="AF26" s="18">
         <f>ROUND($B$9*(1+$T$2*(1+G2+M2)*C2+$T$3*(1+G3+M3)*C3+$T$4*(1+G4+M4)*C4+$T$5*(1+G5+M5)*C5+$T$6*(1+G6+M6)*C6),0)</f>
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AG26" s="18">
         <f t="shared" si="19"/>
@@ -10132,7 +10194,7 @@
       </c>
       <c r="AM26" s="18">
         <f>ROUND($B$9*(1+$T$2*(1+H2+M2)*C2+$T$3*(1+H3+M3)*C3+$T$4*(1+H4+M4)*C4+$T$5*(1+H5+M5)*C5+$T$6*(1+H6+M6)*C6),0)</f>
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AN26" s="18">
         <f t="shared" si="20"/>
@@ -10155,7 +10217,7 @@
       </c>
       <c r="AT26" s="18">
         <f>ROUND($B$9*(1+$T$2*(1+I2+M2)*C2+$T$3*(1+I3+M3)*C3+$T$4*(1+I4+M4)*C4+$T$5*(1+I5+M5)*C5+$T$6*(1+I6+M6)*C6),0)</f>
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="AU26" s="18">
         <f t="shared" si="21"/>
@@ -10178,7 +10240,7 @@
       </c>
       <c r="BA26" s="18">
         <f>ROUND($B$9*(1+$T$2*(1+J2+M2)*C2+$T$3*(1+J3+M3)*C3+$T$4*(1+J4+M4)*C4+$T$5*(1+J5+M5)*C5+$T$6*(1+J6+M6)*C6),0)</f>
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="BB26" s="18">
         <f t="shared" si="22"/>
@@ -10201,7 +10263,7 @@
       </c>
       <c r="BH26" s="18">
         <f>ROUND($B$9*(1+$T$2*(1+K2+M2)*C2+$T$3*(1+K3+M3)*C3+$T$4*(1+K4+M4)*C4+$T$5*(1+K5+M5)*C5+$T$6*(1+K6+M6)*C6),0)</f>
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="BI26" s="18">
         <f t="shared" si="23"/>
@@ -10226,7 +10288,7 @@
       </c>
       <c r="Y27" s="18">
         <f>ROUND($B$9*(1+$T$2*(1+F2+N2)*C2+$T$3*(1+F3+N3)*C3+$T$4*(1+F4+N4)*C4+$T$5*(1+F5+N5)*C5+$T$6*(1+F6+N6)*C6),0)</f>
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="Z27" s="18">
         <f t="shared" si="18"/>
@@ -10249,7 +10311,7 @@
       </c>
       <c r="AF27" s="18">
         <f>ROUND($B$9*(1+$T$2*(1+G2+N2)*C2+$T$3*(1+G3+N3)*C3+$T$4*(1+G4+N4)*C4+$T$5*(1+G5+N5)*C5+$T$6*(1+G6+N6)*C6),0)</f>
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="AG27" s="18">
         <f t="shared" si="19"/>
@@ -10272,7 +10334,7 @@
       </c>
       <c r="AM27" s="18">
         <f>ROUND($B$9*(1+$T$2*(1+H2+N2)*C2+$T$3*(1+H3+N3)*C3+$T$4*(1+H4+N4)*C4+$T$5*(1+H5+N5)*C5+$T$6*(1+H6+N6)*C6),0)</f>
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AN27" s="18">
         <f t="shared" si="20"/>
@@ -10295,7 +10357,7 @@
       </c>
       <c r="AT27" s="18">
         <f>ROUND($B$9*(1+$T$2*(1+I2+N2)*C2+$T$3*(1+I3+N3)*C3+$T$4*(1+I4+N4)*C4+$T$5*(1+I5+N5)*C5+$T$6*(1+I6+N6)*C6),0)</f>
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="AU27" s="18">
         <f t="shared" si="21"/>
@@ -10318,7 +10380,7 @@
       </c>
       <c r="BA27" s="18">
         <f>ROUND($B$9*(1+$T$2*(1+J2+N2)*C2+$T$3*(1+J3+N3)*C3+$T$4*(1+J4+N4)*C4+$T$5*(1+J5+N5)*C5+$T$6*(1+J6+N6)*C6),0)</f>
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="BB27" s="18">
         <f t="shared" si="22"/>
@@ -10341,7 +10403,7 @@
       </c>
       <c r="BH27" s="18">
         <f>ROUND($B$9*(1+$T$2*(1+K2+N2)*C2+$T$3*(1+K3+N3)*C3+$T$4*(1+K4+N4)*C4+$T$5*(1+K5+N5)*C5+$T$6*(1+K6+N6)*C6),0)</f>
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="BI27" s="18">
         <f t="shared" si="23"/>
@@ -10366,7 +10428,7 @@
       </c>
       <c r="Y28" s="18">
         <f>ROUND($B$9*(1+$T$2*(1+F2+O2)*C2+$T$3*(1+F3+O3)*C3+$T$4*(1+F4+O4)*C4+$T$5*(1+F5+O5)*C5+$T$6*(1+F6+O6)*C6),0)</f>
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="Z28" s="18">
         <f t="shared" si="18"/>
@@ -10389,7 +10451,7 @@
       </c>
       <c r="AF28" s="18">
         <f>ROUND($B$9*(1+$T$2*(1+G2+O2)*C2+$T$3*(1+G3+O3)*C3+$T$4*(1+G4+O4)*C4+$T$5*(1+G5+O5)*C5+$T$6*(1+G6+O6)*C6),0)</f>
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AG28" s="18">
         <f t="shared" si="19"/>
@@ -10412,7 +10474,7 @@
       </c>
       <c r="AM28" s="18">
         <f>ROUND($B$9*(1+$T$2*(1+H2+O2)*C2+$T$3*(1+H3+O3)*C3+$T$4*(1+H4+O4)*C4+$T$5*(1+H5+O5)*C5+$T$6*(1+H6+O6)*C6),0)</f>
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AN28" s="18">
         <f t="shared" si="20"/>
@@ -10435,7 +10497,7 @@
       </c>
       <c r="AT28" s="18">
         <f>ROUND($B$9*(1+$T$2*(1+I2+O2)*C2+$T$3*(1+I3+O3)*C3+$T$4*(1+I4+O4)*C4+$T$5*(1+I5+O5)*C5+$T$6*(1+I6+O6)*C6),0)</f>
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="AU28" s="18">
         <f t="shared" si="21"/>
@@ -10458,7 +10520,7 @@
       </c>
       <c r="BA28" s="18">
         <f>ROUND($B$9*(1+$T$2*(1+J2+O2)*C2+$T$3*(1+J3+O3)*C3+$T$4*(1+J4+O4)*C4+$T$5*(1+J5+O5)*C5+$T$6*(1+J6+O6)*C6),0)</f>
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="BB28" s="18">
         <f t="shared" si="22"/>
@@ -10481,7 +10543,7 @@
       </c>
       <c r="BH28" s="18">
         <f>ROUND($B$9*(1+$T$2*(1+K2+O2)*C2+$T$3*(1+K3+O3)*C3+$T$4*(1+K4+O4)*C4+$T$5*(1+K5+O5)*C5+$T$6*(1+K6+O6)*C6),0)</f>
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="BI28" s="18">
         <f t="shared" si="23"/>
@@ -10506,7 +10568,7 @@
       </c>
       <c r="Y29" s="18">
         <f>ROUND($B$9*(1+$T$2*(1+F2+P2)*C2+$T$3*(1+F3+P3)*C3+$T$4*(1+F4+P4)*C4+$T$5*(1+F5+P5)*C5+$T$6*(1+F6+P6)*C6),0)</f>
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="Z29" s="18">
         <f t="shared" si="18"/>
@@ -10529,7 +10591,7 @@
       </c>
       <c r="AF29" s="18">
         <f>ROUND($B$9*(1+$T$2*(1+G2+P2)*C2+$T$3*(1+G3+P3)*C3+$T$4*(1+G4+P4)*C4+$T$5*(1+G5+P5)*C5+$T$6*(1+G6+P6)*C6),0)</f>
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="AG29" s="18">
         <f t="shared" si="19"/>
@@ -10552,7 +10614,7 @@
       </c>
       <c r="AM29" s="18">
         <f>ROUND($B$9*(1+$T$2*(1+H2+P2)*C2+$T$3*(1+H3+P3)*C3+$T$4*(1+H4+P4)*C4+$T$5*(1+H5+P5)*C5+$T$6*(1+H6+P6)*C6),0)</f>
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AN29" s="18">
         <f t="shared" si="20"/>
@@ -10575,7 +10637,7 @@
       </c>
       <c r="AT29" s="18">
         <f>ROUND($B$9*(1+$T$2*(1+I2+P2)*C2+$T$3*(1+I3+P3)*C3+$T$4*(1+I4+P4)*C4+$T$5*(1+I5+P5)*C5+$T$6*(1+I6+P6)*C6),0)</f>
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="AU29" s="18">
         <f t="shared" si="21"/>
@@ -10598,7 +10660,7 @@
       </c>
       <c r="BA29" s="18">
         <f>ROUND($B$9*(1+$T$2*(1+J2+P2)*C2+$T$3*(1+J3+P3)*C3+$T$4*(1+J4+P4)*C4+$T$5*(1+J5+P5)*C5+$T$6*(1+J6+P6)*C6),0)</f>
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="BB29" s="18">
         <f t="shared" si="22"/>
@@ -10621,7 +10683,7 @@
       </c>
       <c r="BH29" s="18">
         <f>ROUND($B$9*(1+$T$2*(1+K2+P2)*C2+$T$3*(1+K3+P3)*C3+$T$4*(1+K4+P4)*C4+$T$5*(1+K5+P5)*C5+$T$6*(1+K6+P6)*C6),0)</f>
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="BI29" s="18">
         <f t="shared" si="23"/>
@@ -10638,7 +10700,7 @@
     </row>
     <row r="31" spans="23:63" x14ac:dyDescent="0.2">
       <c r="W31" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="X31" s="18" t="s">
         <v>43</v>
@@ -10650,13 +10712,13 @@
         <v>54</v>
       </c>
       <c r="AA31" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AB31" s="18" t="s">
         <v>55</v>
       </c>
       <c r="AD31" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AE31" s="18" t="s">
         <v>43</v>
@@ -10668,13 +10730,13 @@
         <v>54</v>
       </c>
       <c r="AH31" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AI31" s="18" t="s">
         <v>55</v>
       </c>
       <c r="AK31" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AL31" s="18" t="s">
         <v>43</v>
@@ -10686,13 +10748,13 @@
         <v>54</v>
       </c>
       <c r="AO31" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AP31" s="18" t="s">
         <v>55</v>
       </c>
       <c r="AR31" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AS31" s="18" t="s">
         <v>43</v>
@@ -10704,13 +10766,13 @@
         <v>54</v>
       </c>
       <c r="AV31" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AW31" s="18" t="s">
         <v>55</v>
       </c>
       <c r="AY31" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AZ31" s="18" t="s">
         <v>43</v>
@@ -10722,13 +10784,13 @@
         <v>54</v>
       </c>
       <c r="BC31" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BD31" s="18" t="s">
         <v>55</v>
       </c>
       <c r="BF31" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BG31" s="18" t="s">
         <v>43</v>
@@ -10740,7 +10802,7 @@
         <v>54</v>
       </c>
       <c r="BJ31" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BK31" s="18" t="s">
         <v>55</v>
@@ -10756,7 +10818,7 @@
       </c>
       <c r="Y32" s="18">
         <f>ROUND($B$9*(1+$U$2*(1+F2+L2)*C2+$U$3*(1+F3+L3)*C3+$U$4*(1+F4+L4)*C4+$U$5*(1+F5+L5)*C5+$U$6*(1+F6+L6)*C6),0)</f>
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="Z32" s="18">
         <f>ROUND($B$12*(1+AA32),0)</f>
@@ -10779,7 +10841,7 @@
       </c>
       <c r="AF32" s="28">
         <f>ROUND($B$9*(1+$U$2*(1+G2+L2)*C2+$U$3*(1+G3+L3)*C3+$U$4*(1+G4+L4)*C4+$U$5*(1+G5+L5)*C5+$U$6*(1+G6+L6)*C6),0)</f>
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="AG32" s="28">
         <f t="shared" ref="AG32:AG35" si="24">ROUND($B$12*(1+AH32),0)</f>
@@ -10802,7 +10864,7 @@
       </c>
       <c r="AM32" s="18">
         <f>ROUND($B$9*(1+$U$2*(1+H2+L2)*C2+$U$3*(1+H3+L3)*C3+$U$4*(1+H4+L4)*C4+$U$5*(1+H5+L5)*C5+$U$6*(1+H6+L6)*C6),0)</f>
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="AN32" s="18">
         <f t="shared" ref="AN32:AN36" si="25">ROUND($B$12*(1+AO32),0)</f>
@@ -10825,7 +10887,7 @@
       </c>
       <c r="AT32" s="18">
         <f>ROUND($B$9*(1+$U$2*(1+I2+L2)*C2+$U$3*(1+I3+L3)*C3+$U$4*(1+I4+L4)*C4+$U$5*(1+I5+L5)*C5+$U$6*(1+I6+L6)*C6),0)</f>
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="AU32" s="27">
         <f t="shared" ref="AU32:AU36" si="26">ROUND($B$12*(1+AV32),0)</f>
@@ -10848,7 +10910,7 @@
       </c>
       <c r="BA32" s="18">
         <f>ROUND($B$9*(1+$U$2*(1+J2+L2)*C2+$U$3*(1+J3+L3)*C3+$U$4*(1+J4+L4)*C4+$U$5*(1+J5+L5)*C5+$U$6*(1+J6+L6)*C6),0)</f>
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="BB32" s="27">
         <f t="shared" ref="BB32:BB36" si="27">ROUND($B$12*(1+BC32),0)</f>
@@ -10871,7 +10933,7 @@
       </c>
       <c r="BH32" s="18">
         <f>ROUND($B$9*(1+$U$2*(1+K2+L2)*C2+$U$3*(1+K3+L3)*C3+$U$4*(1+K4+L4)*C4+$U$5*(1+K5+L5)*C5+$U$6*(1+K6+L6)*C6),0)</f>
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="BI32" s="18">
         <f t="shared" ref="BI32:BI36" si="28">ROUND($B$12*(1+BJ32),0)</f>
@@ -10896,7 +10958,7 @@
       </c>
       <c r="Y33" s="18">
         <f>ROUND($B$9*(1+$U$2*(1+F2+M2)*C2+$U$3*(1+F3+M3)*C3+$U$4*(1+F4+M4)*C4+$U$5*(1+F5+M5)*C5+$U$6*(1+F6+M6)*C6),0)</f>
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="Z33" s="18">
         <f>ROUND($B$12*(1+AA33),0)</f>
@@ -10919,7 +10981,7 @@
       </c>
       <c r="AF33" s="28">
         <f>ROUND($B$9*(1+$U$2*(1+G2+M2)*C2+$U$3*(1+G3+M3)*C3+$U$4*(1+G4+M4)*C4+$U$5*(1+G5+M5)*C5+$U$6*(1+G6+M6)*C6),0)</f>
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="AG33" s="28">
         <f t="shared" si="24"/>
@@ -10942,7 +11004,7 @@
       </c>
       <c r="AM33" s="18">
         <f>ROUND($B$9*(1+$U$2*(1+H2+M2)*C2+$U$3*(1+H3+M3)*C3+$U$4*(1+H4+M4)*C4+$U$5*(1+H5+M5)*C5+$U$6*(1+H6+M6)*C6),0)</f>
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="AN33" s="18">
         <f t="shared" si="25"/>
@@ -10965,7 +11027,7 @@
       </c>
       <c r="AT33" s="18">
         <f>ROUND($B$9*(1+$U$2*(1+I2+M2)*C2+$U$3*(1+I3+M3)*C3+$U$4*(1+I4+M4)*C4+$U$5*(1+I5+M5)*C5+$U$6*(1+I6+M6)*C6),0)</f>
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="AU33" s="27">
         <f t="shared" si="26"/>
@@ -10988,7 +11050,7 @@
       </c>
       <c r="BA33" s="18">
         <f>ROUND($B$9*(1+$U$2*(1+J2+M2)*C2+$U$3*(1+J3+M3)*C3+$U$4*(1+J4+M4)*C4+$U$5*(1+J5+M5)*C5+$U$6*(1+J6+M6)*C6),0)</f>
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="BB33" s="27">
         <f t="shared" si="27"/>
@@ -11011,7 +11073,7 @@
       </c>
       <c r="BH33" s="18">
         <f>ROUND($B$9*(1+$U$2*(1+K2+M2)*C2+$U$3*(1+K3+M3)*C3+$U$4*(1+K4+M4)*C4+$U$5*(1+K5+M5)*C5+$U$6*(1+K6+M6)*C6),0)</f>
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="BI33" s="18">
         <f t="shared" si="28"/>
@@ -11036,7 +11098,7 @@
       </c>
       <c r="Y34" s="18">
         <f>ROUND($B$9*(1+$U$2*(1+F2+N2)*C2+$U$3*(1+F3+N3)*C3+$U$4*(1+F4+N4)*C4+$U$5*(1+F5+N5)*C5+$U$6*(1+F6+N6)*C6),0)</f>
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="Z34" s="18">
         <f t="shared" ref="Z34:Z36" si="29">ROUND($B$12*(1+AA34),0)</f>
@@ -11059,7 +11121,7 @@
       </c>
       <c r="AF34" s="18">
         <f>ROUND($B$9*(1+$U$2*(1+G2+N2)*C2+$U$3*(1+G3+N3)*C3+$U$4*(1+G4+N4)*C4+$U$5*(1+G5+N5)*C5+$U$6*(1+G6+N6)*C6),0)</f>
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="AG34" s="28">
         <f t="shared" si="24"/>
@@ -11082,7 +11144,7 @@
       </c>
       <c r="AM34" s="18">
         <f>ROUND($B$9*(1+$U$2*(1+H2+N2)*C2+$U$3*(1+H3+N3)*C3+$U$4*(1+H4+N4)*C4+$U$5*(1+H5+N5)*C5+$U$6*(1+H6+N6)*C6),0)</f>
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AN34" s="18">
         <f t="shared" si="25"/>
@@ -11105,7 +11167,7 @@
       </c>
       <c r="AT34" s="18">
         <f>ROUND($B$9*(1+$U$2*(1+I2+N2)*C2+$U$3*(1+I3+N3)*C3+$U$4*(1+I4+N4)*C4+$U$5*(1+I5+N5)*C5+$U$6*(1+I6+N6)*C6),0)</f>
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="AU34" s="27">
         <f t="shared" si="26"/>
@@ -11128,7 +11190,7 @@
       </c>
       <c r="BA34" s="27">
         <f>ROUND($B$9*(1+$U$2*(1+J2+N2)*C2+$U$3*(1+J3+N3)*C3+$U$4*(1+J4+N4)*C4+$U$5*(1+J5+N5)*C5+$U$6*(1+J6+N6)*C6),0)</f>
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="BB34" s="27">
         <f t="shared" si="27"/>
@@ -11151,7 +11213,7 @@
       </c>
       <c r="BH34" s="27">
         <f>ROUND($B$9*(1+$U$2*(1+K2+N2)*C2+$U$3*(1+K3+N3)*C3+$U$4*(1+K4+N4)*C4+$U$5*(1+K5+N5)*C5+$U$6*(1+K6+N6)*C6),0)</f>
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="BI34" s="18">
         <f t="shared" si="28"/>
@@ -11176,7 +11238,7 @@
       </c>
       <c r="Y35" s="18">
         <f>ROUND($B$9*(1+$U$2*(1+F2+O2)*C2+$U$3*(1+F3+O3)*C3+$U$4*(1+F4+O4)*C4+$U$5*(1+F5+O5)*C5+$U$6*(1+F6+O6)*C6),0)</f>
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="Z35" s="18">
         <f t="shared" si="29"/>
@@ -11199,7 +11261,7 @@
       </c>
       <c r="AF35" s="28">
         <f>ROUND($B$9*(1+$U$2*(1+G2+O2)*C2+$U$3*(1+G3+O3)*C3+$U$4*(1+G4+O4)*C4+$U$5*(1+G5+O5)*C5+$U$6*(1+G6+O6)*C6),0)</f>
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="AG35" s="28">
         <f t="shared" si="24"/>
@@ -11222,7 +11284,7 @@
       </c>
       <c r="AM35" s="18">
         <f>ROUND($B$9*(1+$U$2*(1+H2+O2)*C2+$U$3*(1+H3+O3)*C3+$U$4*(1+H4+O4)*C4+$U$5*(1+H5+O5)*C5+$U$6*(1+H6+O6)*C6),0)</f>
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="AN35" s="18">
         <f t="shared" si="25"/>
@@ -11245,7 +11307,7 @@
       </c>
       <c r="AT35" s="18">
         <f>ROUND($B$9*(1+$U$2*(1+I2+O2)*C2+$U$3*(1+I3+O3)*C3+$U$4*(1+I4+O4)*C4+$U$5*(1+I5+O5)*C5+$U$6*(1+I6+O6)*C6),0)</f>
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="AU35" s="27">
         <f t="shared" si="26"/>
@@ -11268,7 +11330,7 @@
       </c>
       <c r="BA35" s="18">
         <f>ROUND($B$9*(1+$U$2*(1+J2+O2)*C2+$U$3*(1+J3+O3)*C3+$U$4*(1+J4+O4)*C4+$U$5*(1+J5+O5)*C5+$U$6*(1+J6+O6)*C6),0)</f>
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="BB35" s="27">
         <f t="shared" si="27"/>
@@ -11291,7 +11353,7 @@
       </c>
       <c r="BH35" s="18">
         <f>ROUND($B$9*(1+$U$2*(1+K2+O2)*C2+$U$3*(1+K3+O3)*C3+$U$4*(1+K4+O4)*C4+$U$5*(1+K5+O5)*C5+$U$6*(1+K6+O6)*C6),0)</f>
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="BI35" s="18">
         <f t="shared" si="28"/>
@@ -11316,7 +11378,7 @@
       </c>
       <c r="Y36" s="18">
         <f>ROUND($B$9*(1+$U$2*(1+F2+P2)*C2+$U$3*(1+F3+P3)*C3+$U$4*(1+F4+P4)*C4+$U$5*(1+F5+P5)*C5+$U$6*(1+F6+P6)*C6),0)</f>
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="Z36" s="18">
         <f t="shared" si="29"/>
@@ -11339,7 +11401,7 @@
       </c>
       <c r="AF36" s="18">
         <f>ROUND($B$9*(1+$U$2*(1+G2+P2)*C2+$U$3*(1+G3+P3)*C3+$U$4*(1+G4+P4)*C4+$U$5*(1+G5+P5)*C5+$U$6*(1+G6+P6)*C6),0)</f>
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="AG36" s="28">
         <f>ROUND($B$12*(1+AH36),0)</f>
@@ -11362,7 +11424,7 @@
       </c>
       <c r="AM36" s="18">
         <f>ROUND($B$9*(1+$U$2*(1+H2+P2)*C2+$U$3*(1+H3+P3)*C3+$U$4*(1+H4+P4)*C4+$U$5*(1+H5+P5)*C5+$U$6*(1+H6+P6)*C6),0)</f>
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AN36" s="18">
         <f t="shared" si="25"/>
@@ -11385,7 +11447,7 @@
       </c>
       <c r="AT36" s="18">
         <f>ROUND($B$9*(1+$U$2*(1+I2+P2)*C2+$U$3*(1+I3+P3)*C3+$U$4*(1+I4+P4)*C4+$U$5*(1+I5+P5)*C5+$U$6*(1+I6+P6)*C6),0)</f>
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="AU36" s="27">
         <f t="shared" si="26"/>
@@ -11408,7 +11470,7 @@
       </c>
       <c r="BA36" s="27">
         <f>ROUND($B$9*(1+$U$2*(1+J2+P2)*C2+$U$3*(1+J3+P3)*C3+$U$4*(1+J4+P4)*C4+$U$5*(1+J5+P5)*C5+$U$6*(1+J6+P6)*C6),0)</f>
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="BB36" s="27">
         <f t="shared" si="27"/>
@@ -11431,7 +11493,7 @@
       </c>
       <c r="BH36" s="27">
         <f>ROUND($B$9*(1+$U$2*(1+K2+P2)*C2+$U$3*(1+K3+P3)*C3+$U$4*(1+K4+P4)*C4+$U$5*(1+K5+P5)*C5+$U$6*(1+K6+P6)*C6),0)</f>
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="BI36" s="18">
         <f t="shared" si="28"/>
@@ -11570,23 +11632,23 @@
       </c>
       <c r="X44" s="18">
         <f>ROUND($B$9*(1+Q38*(1+$F$2+$P$2)*$C$2+Q39*(1+$F$3+$P$3)*$C$3+Q40*(1+$F$4+$P$4)*$C$4+Q41*(1+$F$5+$P$5)*$C$5+Q42*(1+$F$6+$P$6)*$C$6),0)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y44" s="18">
         <f>ROUND($B$9*(1+R38*(1+$F$2+$P$2)*$C$2+R39*(1+$F$3+$P$3)*$C$3+R40*(1+$F$4+$P$4)*$C$4+R41*(1+$F$5+$P$5)*$C$5+R42*(1+$F$6+$P$6)*$C$6),0)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Z44" s="18">
         <f>ROUND($B$9*(1+S38*(1+$F$2+$P$2)*$C$2+S39*(1+$F$3+$P$3)*$C$3+S40*(1+$F$4+$P$4)*$C$4+S41*(1+$F$5+$P$5)*$C$5+S42*(1+$F$6+$P$6)*$C$6),0)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="AA44" s="18">
         <f>ROUND($B$9*(1+T38*(1+$F$2+$P$2)*$C$2+T39*(1+$F$3+$P$3)*$C$3+T40*(1+$F$4+$P$4)*$C$4+T41*(1+$F$5+$P$5)*$C$5+T42*(1+$F$6+$P$6)*$C$6),0)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AB44" s="18">
         <f>ROUND($B$9*(1+U38*(1+$F$2+$P$2)*$C$2+U39*(1+$F$3+$P$3)*$C$3+U40*(1+$F$4+$P$4)*$C$4+U41*(1+$F$5+$P$5)*$C$5+U42*(1+$F$6+$P$6)*$C$6),0)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="45" spans="17:63" x14ac:dyDescent="0.2">
@@ -11646,7 +11708,7 @@
         <v>5</v>
       </c>
       <c r="W46" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="X46" s="18">
         <f>ROUND($B$11+Q38*(1+$F$2+$P$2)*$D$2+Q39*(1+$F$3+$P$3)*$D$3+Q40*(1+$F$4+$P$4)*$D$4+Q41*(1+$F$5+$P$5)*$D$5+Q42*(1+$F$6+$P$6)*$D$6,2)</f>
@@ -11782,23 +11844,23 @@
       </c>
       <c r="X51" s="18">
         <f>ROUND($B$9*(1+Q45*(1+$F$2+$P$2)*$C$2+Q46*(1+$F$3+$P$3)*$C$3+Q47*(1+$F$4+$P$4)*$C$4+Q48*(1+$F$5+$P$5)*$C$5+Q49*(1+$F$6+$P$6)*$C$6),0)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y51" s="18">
         <f>ROUND($B$9*(1+R45*(1+$F$2+$P$2)*$C$2+R46*(1+$F$3+$P$3)*$C$3+R47*(1+$F$4+$P$4)*$C$4+R48*(1+$F$5+$P$5)*$C$5+R49*(1+$F$6+$P$6)*$C$6),0)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Z51" s="18">
         <f>ROUND($B$9*(1+S45*(1+$F$2+$P$2)*$C$2+S46*(1+$F$3+$P$3)*$C$3+S47*(1+$F$4+$P$4)*$C$4+S48*(1+$F$5+$P$5)*$C$5+S49*(1+$F$6+$P$6)*$C$6),0)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AA51" s="18">
         <f>ROUND($B$9*(1+T45*(1+$F$2+$P$2)*$C$2+T46*(1+$F$3+$P$3)*$C$3+T47*(1+$F$4+$P$4)*$C$4+T48*(1+$F$5+$P$5)*$C$5+T49*(1+$F$6+$P$6)*$C$6),0)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AB51" s="18">
         <f>ROUND($B$9*(1+U45*(1+$F$2+$P$2)*$C$2+U46*(1+$F$3+$P$3)*$C$3+U47*(1+$F$4+$P$4)*$C$4+U48*(1+$F$5+$P$5)*$C$5+U49*(1+$F$6+$P$6)*$C$6),0)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="52" spans="17:28" x14ac:dyDescent="0.2">
@@ -11828,7 +11890,7 @@
     </row>
     <row r="53" spans="17:28" x14ac:dyDescent="0.2">
       <c r="W53" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="X53" s="18">
         <f>ROUND($B$11+Q45*(1+$F$2+$P$2)*$D$2+Q46*(1+$F$3+$P$3)*$D$3+Q47*(1+$F$4+$P$4)*$D$4+Q48*(1+$F$5+$P$5)*$D$5+Q49*(1+$F$6+$P$6)*$D$6,2)</f>
@@ -11887,6 +11949,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -11894,8 +11957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD573711-C846-40DC-8629-19A685998D3E}">
   <dimension ref="A1:V25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U6" sqref="U6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V10" sqref="V10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11920,63 +11983,63 @@
         <v>0</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L1" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M1" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N1" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O1" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P1" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q1" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="R1" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="S1" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="T1" t="s">
         <v>6</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="36" t="s">
         <v>8</v>
       </c>
     </row>
@@ -12035,13 +12098,16 @@
       <c r="R2">
         <v>19</v>
       </c>
+      <c r="S2">
+        <v>20</v>
+      </c>
       <c r="T2">
         <v>20</v>
       </c>
-      <c r="U2">
+      <c r="U2" s="36">
         <v>50</v>
       </c>
-      <c r="V2">
+      <c r="V2" s="36">
         <v>100</v>
       </c>
     </row>
@@ -12100,13 +12166,16 @@
       <c r="R3">
         <v>19</v>
       </c>
+      <c r="S3">
+        <v>20</v>
+      </c>
       <c r="T3">
         <v>20</v>
       </c>
-      <c r="U3">
+      <c r="U3" s="36">
         <v>50</v>
       </c>
-      <c r="V3">
+      <c r="V3" s="36">
         <v>100</v>
       </c>
     </row>
@@ -12165,13 +12234,16 @@
       <c r="R4">
         <v>20</v>
       </c>
+      <c r="S4">
+        <v>20</v>
+      </c>
       <c r="T4">
         <v>20</v>
       </c>
-      <c r="U4">
+      <c r="U4" s="36">
         <v>50</v>
       </c>
-      <c r="V4">
+      <c r="V4" s="36">
         <v>100</v>
       </c>
     </row>
@@ -12230,13 +12302,16 @@
       <c r="R5">
         <v>19</v>
       </c>
+      <c r="S5">
+        <v>20</v>
+      </c>
       <c r="T5">
         <v>20</v>
       </c>
-      <c r="U5">
+      <c r="U5" s="36">
         <v>50</v>
       </c>
-      <c r="V5">
+      <c r="V5" s="36">
         <v>100</v>
       </c>
     </row>
@@ -12295,14 +12370,16 @@
       <c r="R6" s="34">
         <v>3</v>
       </c>
-      <c r="S6" s="34"/>
+      <c r="S6" s="34">
+        <v>5</v>
+      </c>
       <c r="T6" s="34">
         <v>7</v>
       </c>
-      <c r="U6" s="34">
+      <c r="U6" s="37">
         <v>20</v>
       </c>
-      <c r="V6" s="34">
+      <c r="V6" s="37">
         <v>40</v>
       </c>
     </row>
@@ -12377,17 +12454,17 @@
       </c>
       <c r="S7">
         <f t="shared" ref="S7" si="11">SUM(S2:S6)</f>
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="T7">
         <f t="shared" ref="T7" si="12">SUM(T2:T6)</f>
         <v>87</v>
       </c>
-      <c r="U7">
+      <c r="U7" s="36">
         <f t="shared" ref="U7" si="13">SUM(U2:U6)</f>
         <v>220</v>
       </c>
-      <c r="V7">
+      <c r="V7" s="36">
         <f t="shared" si="0"/>
         <v>440</v>
       </c>
@@ -12397,49 +12474,49 @@
         <v>0</v>
       </c>
       <c r="C10" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F10" t="s">
         <v>9</v>
       </c>
       <c r="G10" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H10" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I10" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J10" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K10" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L10" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M10" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N10" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O10" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P10" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q10" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="R10" s="3" t="s">
         <v>10</v>
@@ -12844,43 +12921,43 @@
         <v>0</v>
       </c>
       <c r="C19" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D19" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E19" t="s">
         <v>13</v>
       </c>
       <c r="F19" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G19" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H19" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I19" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J19" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K19" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L19" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M19" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N19" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O19" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P19" s="3" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Introduce "Level" entity instead of using a mock constant. Use liquibase for schema creation and parameterization (inserting level entities).
</commit_message>
<xml_diff>
--- a/doc/caste_system.xlsx
+++ b/doc/caste_system.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/349dfb9748b30a92/Asztali gép/ataliasflame_2.0/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3353" documentId="8_{652F4476-B36F-42CD-831D-0D71B9923ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A55BE310-870A-49C8-A2B0-99EA6CE4ABB0}"/>
+  <xr:revisionPtr revIDLastSave="3377" documentId="8_{652F4476-B36F-42CD-831D-0D71B9923ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F2553E8-0FC2-4529-AF81-FD0C01569190}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{CAF51EC3-63EC-48CD-AA7B-C21B3D5D222B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{CAF51EC3-63EC-48CD-AA7B-C21B3D5D222B}"/>
   </bookViews>
   <sheets>
     <sheet name="caste list" sheetId="1" r:id="rId1"/>
@@ -2235,7 +2235,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2312,6 +2312,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5838,8 +5841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E471D10E-602D-4E12-A93B-97B72309BCF6}">
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6125,7 +6128,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="45">
         <v>10</v>
       </c>
       <c r="B11">
@@ -6859,7 +6862,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D8DF294-C85C-47A3-9A81-4E26EFDC10EC}">
   <dimension ref="A1:BK54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Introduce sleeping possibility for a character. Sleeping heals an amount of injury. Endurance tests now consider necessity of healing and the character may have a sleep between combats. Warrior development path in the endurance test goes to GRANDMASTER level now.
</commit_message>
<xml_diff>
--- a/doc/caste_system.xlsx
+++ b/doc/caste_system.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/349dfb9748b30a92/Asztali gép/ataliasflame_2.0/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3377" documentId="8_{652F4476-B36F-42CD-831D-0D71B9923ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F2553E8-0FC2-4529-AF81-FD0C01569190}"/>
+  <xr:revisionPtr revIDLastSave="3550" documentId="8_{652F4476-B36F-42CD-831D-0D71B9923ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14B023E6-03DC-442E-9B76-F1BA3DB1AD35}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{CAF51EC3-63EC-48CD-AA7B-C21B3D5D222B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{CAF51EC3-63EC-48CD-AA7B-C21B3D5D222B}"/>
   </bookViews>
   <sheets>
     <sheet name="caste list" sheetId="1" r:id="rId1"/>
@@ -1765,7 +1765,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="85">
   <si>
     <t>csavargó</t>
   </si>
@@ -2235,7 +2235,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2292,6 +2292,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2313,9 +2316,8 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -2332,10 +2334,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2771,7 +2769,7 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="39" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="30" t="s">
@@ -2827,7 +2825,7 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="39"/>
+      <c r="A4" s="40"/>
       <c r="B4" s="30" t="s">
         <v>2</v>
       </c>
@@ -2881,7 +2879,7 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="39"/>
+      <c r="A5" s="40"/>
       <c r="B5" s="30" t="s">
         <v>3</v>
       </c>
@@ -2935,7 +2933,7 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="39"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="30" t="s">
         <v>21</v>
       </c>
@@ -2989,7 +2987,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="40"/>
+      <c r="A7" s="41"/>
       <c r="B7" s="31" t="s">
         <v>4</v>
       </c>
@@ -3043,7 +3041,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="42" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="32" t="s">
@@ -3099,7 +3097,7 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="42"/>
+      <c r="A9" s="43"/>
       <c r="B9" s="32" t="s">
         <v>6</v>
       </c>
@@ -3153,7 +3151,7 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="42"/>
+      <c r="A10" s="43"/>
       <c r="B10" s="32" t="s">
         <v>7</v>
       </c>
@@ -3207,7 +3205,7 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="43"/>
+      <c r="A11" s="44"/>
       <c r="B11" s="29" t="s">
         <v>8</v>
       </c>
@@ -3261,7 +3259,7 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="42" t="s">
         <v>80</v>
       </c>
       <c r="B12" s="32" t="s">
@@ -3317,7 +3315,7 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="42"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="30" t="s">
         <v>10</v>
       </c>
@@ -3371,7 +3369,7 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="42"/>
+      <c r="A14" s="43"/>
       <c r="B14" s="30" t="s">
         <v>11</v>
       </c>
@@ -3425,7 +3423,7 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="43"/>
+      <c r="A15" s="44"/>
       <c r="B15" s="31" t="s">
         <v>12</v>
       </c>
@@ -3479,7 +3477,7 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="41" t="s">
+      <c r="A16" s="42" t="s">
         <v>81</v>
       </c>
       <c r="B16" s="32" t="s">
@@ -3535,7 +3533,7 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="42"/>
+      <c r="A17" s="43"/>
       <c r="B17" s="30" t="s">
         <v>14</v>
       </c>
@@ -3589,7 +3587,7 @@
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" s="42"/>
+      <c r="A18" s="43"/>
       <c r="B18" s="30" t="s">
         <v>15</v>
       </c>
@@ -3643,7 +3641,7 @@
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" s="43"/>
+      <c r="A19" s="44"/>
       <c r="B19" s="31" t="s">
         <v>16</v>
       </c>
@@ -3697,7 +3695,7 @@
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="39" t="s">
         <v>82</v>
       </c>
       <c r="B20" s="30" t="s">
@@ -3753,7 +3751,7 @@
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21" s="39"/>
+      <c r="A21" s="40"/>
       <c r="B21" s="30" t="s">
         <v>18</v>
       </c>
@@ -3807,7 +3805,7 @@
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22" s="39"/>
+      <c r="A22" s="40"/>
       <c r="B22" s="30" t="s">
         <v>19</v>
       </c>
@@ -3861,7 +3859,7 @@
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23" s="40"/>
+      <c r="A23" s="41"/>
       <c r="B23" s="31" t="s">
         <v>20</v>
       </c>
@@ -5841,7 +5839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E471D10E-602D-4E12-A93B-97B72309BCF6}">
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -6128,7 +6126,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="45">
+      <c r="A11" s="38">
         <v>10</v>
       </c>
       <c r="B11">
@@ -6863,7 +6861,7 @@
   <dimension ref="A1:BK54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="BK12" sqref="BK12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -6995,54 +6993,54 @@
       <c r="U1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="W1" s="44" t="s">
+      <c r="W1" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="X1" s="44"/>
-      <c r="Y1" s="44"/>
-      <c r="Z1" s="44"/>
-      <c r="AA1" s="44"/>
-      <c r="AB1" s="44"/>
-      <c r="AD1" s="44" t="s">
+      <c r="X1" s="45"/>
+      <c r="Y1" s="45"/>
+      <c r="Z1" s="45"/>
+      <c r="AA1" s="45"/>
+      <c r="AB1" s="45"/>
+      <c r="AD1" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="AE1" s="44"/>
-      <c r="AF1" s="44"/>
-      <c r="AG1" s="44"/>
-      <c r="AH1" s="44"/>
-      <c r="AI1" s="44"/>
-      <c r="AK1" s="44" t="s">
+      <c r="AE1" s="45"/>
+      <c r="AF1" s="45"/>
+      <c r="AG1" s="45"/>
+      <c r="AH1" s="45"/>
+      <c r="AI1" s="45"/>
+      <c r="AK1" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="AL1" s="44"/>
-      <c r="AM1" s="44"/>
-      <c r="AN1" s="44"/>
-      <c r="AO1" s="44"/>
-      <c r="AP1" s="44"/>
-      <c r="AR1" s="44" t="s">
+      <c r="AL1" s="45"/>
+      <c r="AM1" s="45"/>
+      <c r="AN1" s="45"/>
+      <c r="AO1" s="45"/>
+      <c r="AP1" s="45"/>
+      <c r="AR1" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="AS1" s="44"/>
-      <c r="AT1" s="44"/>
-      <c r="AU1" s="44"/>
-      <c r="AV1" s="44"/>
-      <c r="AW1" s="44"/>
-      <c r="AY1" s="44" t="s">
+      <c r="AS1" s="45"/>
+      <c r="AT1" s="45"/>
+      <c r="AU1" s="45"/>
+      <c r="AV1" s="45"/>
+      <c r="AW1" s="45"/>
+      <c r="AY1" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="AZ1" s="44"/>
-      <c r="BA1" s="44"/>
-      <c r="BB1" s="44"/>
-      <c r="BC1" s="44"/>
-      <c r="BD1" s="44"/>
-      <c r="BF1" s="44" t="s">
+      <c r="AZ1" s="45"/>
+      <c r="BA1" s="45"/>
+      <c r="BB1" s="45"/>
+      <c r="BC1" s="45"/>
+      <c r="BD1" s="45"/>
+      <c r="BF1" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="BG1" s="44"/>
-      <c r="BH1" s="44"/>
-      <c r="BI1" s="44"/>
-      <c r="BJ1" s="44"/>
-      <c r="BK1" s="44"/>
+      <c r="BG1" s="45"/>
+      <c r="BH1" s="45"/>
+      <c r="BI1" s="45"/>
+      <c r="BJ1" s="45"/>
+      <c r="BK1" s="45"/>
     </row>
     <row r="2" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
@@ -11958,10 +11956,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD573711-C846-40DC-8629-19A685998D3E}">
-  <dimension ref="A1:V25"/>
+  <dimension ref="A1:AV25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V10" sqref="V10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="T1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11977,11 +11976,13 @@
     <col min="18" max="18" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="46" width="4" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="4.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -12039,14 +12040,92 @@
       <c r="T1" t="s">
         <v>6</v>
       </c>
-      <c r="U1" s="36" t="s">
+      <c r="U1" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="V1" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="W1" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="X1" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z1" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA1" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB1" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC1" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD1" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="AE1" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="AF1" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="AG1" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH1" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI1" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="AJ1" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="AK1" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="AL1" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="AM1" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN1" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="AO1" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="AP1" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="AQ1" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="AR1" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="AS1" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="AT1" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="AU1" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="V1" s="36" t="s">
+      <c r="AV1" s="36" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>48</v>
       </c>
@@ -12107,14 +12186,92 @@
       <c r="T2">
         <v>20</v>
       </c>
-      <c r="U2" s="36">
+      <c r="U2">
+        <v>21</v>
+      </c>
+      <c r="V2">
+        <v>22</v>
+      </c>
+      <c r="W2">
+        <v>23</v>
+      </c>
+      <c r="X2">
+        <v>24</v>
+      </c>
+      <c r="Y2">
+        <v>25</v>
+      </c>
+      <c r="Z2">
+        <v>27</v>
+      </c>
+      <c r="AA2">
+        <v>28</v>
+      </c>
+      <c r="AB2">
+        <v>29</v>
+      </c>
+      <c r="AC2">
+        <v>30</v>
+      </c>
+      <c r="AD2">
+        <v>31</v>
+      </c>
+      <c r="AE2">
+        <v>33</v>
+      </c>
+      <c r="AF2">
+        <v>34</v>
+      </c>
+      <c r="AG2">
+        <v>35</v>
+      </c>
+      <c r="AH2">
+        <v>36</v>
+      </c>
+      <c r="AI2">
+        <v>37</v>
+      </c>
+      <c r="AJ2">
+        <v>39</v>
+      </c>
+      <c r="AK2">
+        <v>40</v>
+      </c>
+      <c r="AL2">
+        <v>41</v>
+      </c>
+      <c r="AM2">
+        <v>42</v>
+      </c>
+      <c r="AN2">
+        <v>43</v>
+      </c>
+      <c r="AO2">
+        <v>45</v>
+      </c>
+      <c r="AP2">
+        <v>46</v>
+      </c>
+      <c r="AQ2">
+        <v>47</v>
+      </c>
+      <c r="AR2">
+        <v>48</v>
+      </c>
+      <c r="AS2">
+        <v>49</v>
+      </c>
+      <c r="AT2">
         <v>50</v>
       </c>
-      <c r="V2" s="36">
+      <c r="AU2" s="46">
+        <v>50</v>
+      </c>
+      <c r="AV2" s="36">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -12175,14 +12332,92 @@
       <c r="T3">
         <v>20</v>
       </c>
-      <c r="U3" s="36">
+      <c r="U3">
+        <v>21</v>
+      </c>
+      <c r="V3">
+        <v>22</v>
+      </c>
+      <c r="W3">
+        <v>23</v>
+      </c>
+      <c r="X3">
+        <v>25</v>
+      </c>
+      <c r="Y3">
+        <v>26</v>
+      </c>
+      <c r="Z3">
+        <v>27</v>
+      </c>
+      <c r="AA3">
+        <v>28</v>
+      </c>
+      <c r="AB3">
+        <v>29</v>
+      </c>
+      <c r="AC3">
+        <v>30</v>
+      </c>
+      <c r="AD3">
+        <v>32</v>
+      </c>
+      <c r="AE3">
+        <v>33</v>
+      </c>
+      <c r="AF3">
+        <v>34</v>
+      </c>
+      <c r="AG3">
+        <v>35</v>
+      </c>
+      <c r="AH3">
+        <v>36</v>
+      </c>
+      <c r="AI3">
+        <v>38</v>
+      </c>
+      <c r="AJ3">
+        <v>39</v>
+      </c>
+      <c r="AK3">
+        <v>40</v>
+      </c>
+      <c r="AL3">
+        <v>41</v>
+      </c>
+      <c r="AM3">
+        <v>42</v>
+      </c>
+      <c r="AN3">
+        <v>44</v>
+      </c>
+      <c r="AO3">
+        <v>45</v>
+      </c>
+      <c r="AP3">
+        <v>46</v>
+      </c>
+      <c r="AQ3">
+        <v>47</v>
+      </c>
+      <c r="AR3">
+        <v>48</v>
+      </c>
+      <c r="AS3">
+        <v>49</v>
+      </c>
+      <c r="AT3">
         <v>50</v>
       </c>
-      <c r="V3" s="36">
+      <c r="AU3" s="46">
+        <v>50</v>
+      </c>
+      <c r="AV3" s="36">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -12243,14 +12478,92 @@
       <c r="T4">
         <v>20</v>
       </c>
-      <c r="U4" s="36">
+      <c r="U4">
+        <v>21</v>
+      </c>
+      <c r="V4">
+        <v>22</v>
+      </c>
+      <c r="W4">
+        <v>24</v>
+      </c>
+      <c r="X4">
+        <v>25</v>
+      </c>
+      <c r="Y4">
+        <v>26</v>
+      </c>
+      <c r="Z4">
+        <v>27</v>
+      </c>
+      <c r="AA4">
+        <v>28</v>
+      </c>
+      <c r="AB4">
+        <v>30</v>
+      </c>
+      <c r="AC4">
+        <v>31</v>
+      </c>
+      <c r="AD4">
+        <v>32</v>
+      </c>
+      <c r="AE4">
+        <v>33</v>
+      </c>
+      <c r="AF4">
+        <v>34</v>
+      </c>
+      <c r="AG4">
+        <v>35</v>
+      </c>
+      <c r="AH4">
+        <v>37</v>
+      </c>
+      <c r="AI4">
+        <v>38</v>
+      </c>
+      <c r="AJ4">
+        <v>39</v>
+      </c>
+      <c r="AK4">
+        <v>40</v>
+      </c>
+      <c r="AL4">
+        <v>41</v>
+      </c>
+      <c r="AM4">
+        <v>43</v>
+      </c>
+      <c r="AN4">
+        <v>44</v>
+      </c>
+      <c r="AO4">
+        <v>45</v>
+      </c>
+      <c r="AP4">
+        <v>46</v>
+      </c>
+      <c r="AQ4">
+        <v>47</v>
+      </c>
+      <c r="AR4">
+        <v>48</v>
+      </c>
+      <c r="AS4">
+        <v>49</v>
+      </c>
+      <c r="AT4">
         <v>50</v>
       </c>
-      <c r="V4" s="36">
+      <c r="AU4" s="46">
+        <v>50</v>
+      </c>
+      <c r="AV4" s="36">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -12311,14 +12624,92 @@
       <c r="T5">
         <v>20</v>
       </c>
-      <c r="U5" s="36">
+      <c r="U5">
+        <v>20</v>
+      </c>
+      <c r="V5">
+        <v>22</v>
+      </c>
+      <c r="W5">
+        <v>23</v>
+      </c>
+      <c r="X5">
+        <v>24</v>
+      </c>
+      <c r="Y5">
+        <v>25</v>
+      </c>
+      <c r="Z5">
+        <v>26</v>
+      </c>
+      <c r="AA5">
+        <v>28</v>
+      </c>
+      <c r="AB5">
+        <v>29</v>
+      </c>
+      <c r="AC5">
+        <v>30</v>
+      </c>
+      <c r="AD5">
+        <v>31</v>
+      </c>
+      <c r="AE5">
+        <v>32</v>
+      </c>
+      <c r="AF5">
+        <v>34</v>
+      </c>
+      <c r="AG5">
+        <v>35</v>
+      </c>
+      <c r="AH5">
+        <v>36</v>
+      </c>
+      <c r="AI5">
+        <v>37</v>
+      </c>
+      <c r="AJ5">
+        <v>38</v>
+      </c>
+      <c r="AK5">
+        <v>40</v>
+      </c>
+      <c r="AL5">
+        <v>41</v>
+      </c>
+      <c r="AM5">
+        <v>42</v>
+      </c>
+      <c r="AN5">
+        <v>43</v>
+      </c>
+      <c r="AO5">
+        <v>44</v>
+      </c>
+      <c r="AP5">
+        <v>45</v>
+      </c>
+      <c r="AQ5">
+        <v>47</v>
+      </c>
+      <c r="AR5">
+        <v>48</v>
+      </c>
+      <c r="AS5">
+        <v>49</v>
+      </c>
+      <c r="AT5">
         <v>50</v>
       </c>
-      <c r="V5" s="36">
+      <c r="AU5" s="46">
+        <v>50</v>
+      </c>
+      <c r="AV5" s="36">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A6" s="34" t="s">
         <v>49</v>
       </c>
@@ -12379,20 +12770,98 @@
       <c r="T6" s="34">
         <v>7</v>
       </c>
-      <c r="U6" s="37">
+      <c r="U6" s="34">
+        <v>7</v>
+      </c>
+      <c r="V6" s="34">
+        <v>7</v>
+      </c>
+      <c r="W6" s="34">
+        <v>7</v>
+      </c>
+      <c r="X6" s="34">
+        <v>7</v>
+      </c>
+      <c r="Y6" s="34">
+        <v>8</v>
+      </c>
+      <c r="Z6" s="34">
+        <v>8</v>
+      </c>
+      <c r="AA6" s="34">
+        <v>8</v>
+      </c>
+      <c r="AB6" s="34">
+        <v>8</v>
+      </c>
+      <c r="AC6" s="34">
+        <v>9</v>
+      </c>
+      <c r="AD6" s="34">
+        <v>9</v>
+      </c>
+      <c r="AE6" s="34">
+        <v>9</v>
+      </c>
+      <c r="AF6" s="34">
+        <v>9</v>
+      </c>
+      <c r="AG6" s="34">
+        <v>10</v>
+      </c>
+      <c r="AH6" s="34">
+        <v>10</v>
+      </c>
+      <c r="AI6" s="34">
+        <v>10</v>
+      </c>
+      <c r="AJ6" s="34">
+        <v>10</v>
+      </c>
+      <c r="AK6" s="34">
+        <v>10</v>
+      </c>
+      <c r="AL6" s="34">
+        <v>11</v>
+      </c>
+      <c r="AM6" s="34">
+        <v>11</v>
+      </c>
+      <c r="AN6" s="34">
+        <v>11</v>
+      </c>
+      <c r="AO6" s="34">
+        <v>11</v>
+      </c>
+      <c r="AP6" s="34">
+        <v>12</v>
+      </c>
+      <c r="AQ6" s="34">
+        <v>12</v>
+      </c>
+      <c r="AR6" s="34">
+        <v>13</v>
+      </c>
+      <c r="AS6" s="34">
+        <v>14</v>
+      </c>
+      <c r="AT6" s="34">
+        <v>15</v>
+      </c>
+      <c r="AU6" s="47">
         <v>20</v>
       </c>
-      <c r="V6" s="37">
+      <c r="AV6" s="37">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
       <c r="B7">
         <f>SUM(B2:B6)</f>
         <v>5</v>
       </c>
       <c r="C7">
-        <f t="shared" ref="C7:V7" si="0">SUM(C2:C6)</f>
+        <f t="shared" ref="C7:AV7" si="0">SUM(C2:C6)</f>
         <v>10</v>
       </c>
       <c r="D7">
@@ -12460,19 +12929,123 @@
         <v>85</v>
       </c>
       <c r="T7">
-        <f t="shared" ref="T7" si="12">SUM(T2:T6)</f>
+        <f t="shared" ref="T7:U7" si="12">SUM(T2:T6)</f>
         <v>87</v>
       </c>
-      <c r="U7" s="36">
-        <f t="shared" ref="U7" si="13">SUM(U2:U6)</f>
+      <c r="U7">
+        <f t="shared" si="12"/>
+        <v>90</v>
+      </c>
+      <c r="V7">
+        <f t="shared" ref="V7:Y7" si="13">SUM(V2:V6)</f>
+        <v>95</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="13"/>
+        <v>100</v>
+      </c>
+      <c r="X7">
+        <f t="shared" si="13"/>
+        <v>105</v>
+      </c>
+      <c r="Y7">
+        <f t="shared" si="13"/>
+        <v>110</v>
+      </c>
+      <c r="Z7">
+        <f t="shared" ref="Z7:AD7" si="14">SUM(Z2:Z6)</f>
+        <v>115</v>
+      </c>
+      <c r="AA7">
+        <f t="shared" si="14"/>
+        <v>120</v>
+      </c>
+      <c r="AB7">
+        <f t="shared" si="14"/>
+        <v>125</v>
+      </c>
+      <c r="AC7">
+        <f t="shared" si="14"/>
+        <v>130</v>
+      </c>
+      <c r="AD7">
+        <f t="shared" si="14"/>
+        <v>135</v>
+      </c>
+      <c r="AE7">
+        <f t="shared" ref="AE7:AI7" si="15">SUM(AE2:AE6)</f>
+        <v>140</v>
+      </c>
+      <c r="AF7">
+        <f t="shared" si="15"/>
+        <v>145</v>
+      </c>
+      <c r="AG7">
+        <f t="shared" si="15"/>
+        <v>150</v>
+      </c>
+      <c r="AH7">
+        <f t="shared" si="15"/>
+        <v>155</v>
+      </c>
+      <c r="AI7">
+        <f t="shared" si="15"/>
+        <v>160</v>
+      </c>
+      <c r="AJ7">
+        <f t="shared" ref="AJ7:AN7" si="16">SUM(AJ2:AJ6)</f>
+        <v>165</v>
+      </c>
+      <c r="AK7">
+        <f t="shared" si="16"/>
+        <v>170</v>
+      </c>
+      <c r="AL7">
+        <f t="shared" si="16"/>
+        <v>175</v>
+      </c>
+      <c r="AM7">
+        <f t="shared" si="16"/>
+        <v>180</v>
+      </c>
+      <c r="AN7">
+        <f t="shared" si="16"/>
+        <v>185</v>
+      </c>
+      <c r="AO7">
+        <f t="shared" ref="AO7:AT7" si="17">SUM(AO2:AO6)</f>
+        <v>190</v>
+      </c>
+      <c r="AP7">
+        <f t="shared" si="17"/>
+        <v>195</v>
+      </c>
+      <c r="AQ7">
+        <f t="shared" si="17"/>
+        <v>200</v>
+      </c>
+      <c r="AR7">
+        <f t="shared" si="17"/>
+        <v>205</v>
+      </c>
+      <c r="AS7">
+        <f t="shared" ref="AS7" si="18">SUM(AS2:AS6)</f>
+        <v>210</v>
+      </c>
+      <c r="AT7">
+        <f t="shared" si="17"/>
+        <v>215</v>
+      </c>
+      <c r="AU7" s="46">
+        <f t="shared" ref="AU7" si="19">SUM(AU2:AU6)</f>
         <v>220</v>
       </c>
-      <c r="V7" s="36">
+      <c r="AV7" s="36">
         <f t="shared" si="0"/>
         <v>440</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>0</v>
       </c>
@@ -12531,7 +13104,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -12593,7 +13166,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -12655,7 +13228,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>47</v>
       </c>
@@ -12717,7 +13290,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -12779,7 +13352,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A15" s="34" t="s">
         <v>49</v>
       </c>
@@ -12841,81 +13414,81 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.3">
       <c r="B16">
         <f>SUM(B11:B15)</f>
         <v>5</v>
       </c>
       <c r="C16">
-        <f t="shared" ref="C16" si="14">SUM(C11:C15)</f>
+        <f t="shared" ref="C16" si="20">SUM(C11:C15)</f>
         <v>10</v>
       </c>
       <c r="D16">
-        <f t="shared" ref="D16" si="15">SUM(D11:D15)</f>
+        <f t="shared" ref="D16" si="21">SUM(D11:D15)</f>
         <v>15</v>
       </c>
       <c r="E16">
-        <f t="shared" ref="E16" si="16">SUM(E11:E15)</f>
+        <f t="shared" ref="E16" si="22">SUM(E11:E15)</f>
         <v>20</v>
       </c>
       <c r="F16">
-        <f t="shared" ref="F16" si="17">SUM(F11:F15)</f>
+        <f t="shared" ref="F16" si="23">SUM(F11:F15)</f>
         <v>21</v>
       </c>
       <c r="G16">
-        <f t="shared" ref="G16" si="18">SUM(G11:G15)</f>
+        <f t="shared" ref="G16" si="24">SUM(G11:G15)</f>
         <v>25</v>
       </c>
       <c r="H16">
-        <f t="shared" ref="H16" si="19">SUM(H11:H15)</f>
+        <f t="shared" ref="H16" si="25">SUM(H11:H15)</f>
         <v>30</v>
       </c>
       <c r="I16">
-        <f t="shared" ref="I16" si="20">SUM(I11:I15)</f>
+        <f t="shared" ref="I16" si="26">SUM(I11:I15)</f>
         <v>35</v>
       </c>
       <c r="J16">
-        <f t="shared" ref="J16" si="21">SUM(J11:J15)</f>
+        <f t="shared" ref="J16" si="27">SUM(J11:J15)</f>
         <v>40</v>
       </c>
       <c r="K16">
-        <f t="shared" ref="K16" si="22">SUM(K11:K15)</f>
+        <f t="shared" ref="K16" si="28">SUM(K11:K15)</f>
         <v>45</v>
       </c>
       <c r="L16">
-        <f t="shared" ref="L16" si="23">SUM(L11:L15)</f>
+        <f t="shared" ref="L16" si="29">SUM(L11:L15)</f>
         <v>50</v>
       </c>
       <c r="M16">
-        <f t="shared" ref="M16" si="24">SUM(M11:M15)</f>
+        <f t="shared" ref="M16" si="30">SUM(M11:M15)</f>
         <v>55</v>
       </c>
       <c r="N16">
-        <f t="shared" ref="N16" si="25">SUM(N11:N15)</f>
+        <f t="shared" ref="N16" si="31">SUM(N11:N15)</f>
         <v>60</v>
       </c>
       <c r="O16">
-        <f t="shared" ref="O16" si="26">SUM(O11:O15)</f>
+        <f t="shared" ref="O16" si="32">SUM(O11:O15)</f>
         <v>65</v>
       </c>
       <c r="P16">
-        <f t="shared" ref="P16" si="27">SUM(P11:P15)</f>
+        <f t="shared" ref="P16" si="33">SUM(P11:P15)</f>
         <v>70</v>
       </c>
       <c r="Q16">
-        <f t="shared" ref="Q16" si="28">SUM(Q11:Q15)</f>
+        <f t="shared" ref="Q16" si="34">SUM(Q11:Q15)</f>
         <v>75</v>
       </c>
       <c r="R16">
-        <f t="shared" ref="R16" si="29">SUM(R11:R15)</f>
+        <f t="shared" ref="R16" si="35">SUM(R11:R15)</f>
         <v>79</v>
       </c>
       <c r="S16" s="3">
-        <f t="shared" ref="S16" si="30">SUM(S11:S15)</f>
+        <f t="shared" ref="S16" si="36">SUM(S11:S15)</f>
         <v>187</v>
       </c>
       <c r="T16" s="3">
-        <f t="shared" ref="T16" si="31">SUM(T11:T15)</f>
+        <f t="shared" ref="T16" si="37">SUM(T11:T15)</f>
         <v>365</v>
       </c>
     </row>
@@ -13258,67 +13831,67 @@
         <v>5</v>
       </c>
       <c r="C25">
-        <f t="shared" ref="C25" si="32">SUM(C20:C24)</f>
+        <f t="shared" ref="C25" si="38">SUM(C20:C24)</f>
         <v>10</v>
       </c>
       <c r="D25">
-        <f t="shared" ref="D25" si="33">SUM(D20:D24)</f>
+        <f t="shared" ref="D25" si="39">SUM(D20:D24)</f>
         <v>15</v>
       </c>
       <c r="E25">
-        <f t="shared" ref="E25" si="34">SUM(E20:E24)</f>
+        <f t="shared" ref="E25" si="40">SUM(E20:E24)</f>
         <v>17</v>
       </c>
       <c r="F25">
-        <f t="shared" ref="F25" si="35">SUM(F20:F24)</f>
+        <f t="shared" ref="F25" si="41">SUM(F20:F24)</f>
         <v>20</v>
       </c>
       <c r="G25">
-        <f t="shared" ref="G25" si="36">SUM(G20:G24)</f>
+        <f t="shared" ref="G25" si="42">SUM(G20:G24)</f>
         <v>25</v>
       </c>
       <c r="H25">
-        <f t="shared" ref="H25" si="37">SUM(H20:H24)</f>
+        <f t="shared" ref="H25" si="43">SUM(H20:H24)</f>
         <v>30</v>
       </c>
       <c r="I25">
-        <f t="shared" ref="I25" si="38">SUM(I20:I24)</f>
+        <f t="shared" ref="I25" si="44">SUM(I20:I24)</f>
         <v>35</v>
       </c>
       <c r="J25">
-        <f t="shared" ref="J25" si="39">SUM(J20:J24)</f>
+        <f t="shared" ref="J25" si="45">SUM(J20:J24)</f>
         <v>40</v>
       </c>
       <c r="K25">
-        <f t="shared" ref="K25" si="40">SUM(K20:K24)</f>
+        <f t="shared" ref="K25" si="46">SUM(K20:K24)</f>
         <v>45</v>
       </c>
       <c r="L25">
-        <f t="shared" ref="L25" si="41">SUM(L20:L24)</f>
+        <f t="shared" ref="L25" si="47">SUM(L20:L24)</f>
         <v>50</v>
       </c>
       <c r="M25">
-        <f t="shared" ref="M25" si="42">SUM(M20:M24)</f>
+        <f t="shared" ref="M25" si="48">SUM(M20:M24)</f>
         <v>55</v>
       </c>
       <c r="N25">
-        <f t="shared" ref="N25" si="43">SUM(N20:N24)</f>
+        <f t="shared" ref="N25" si="49">SUM(N20:N24)</f>
         <v>60</v>
       </c>
       <c r="O25">
-        <f t="shared" ref="O25" si="44">SUM(O20:O24)</f>
+        <f t="shared" ref="O25" si="50">SUM(O20:O24)</f>
         <v>65</v>
       </c>
       <c r="P25">
-        <f t="shared" ref="P25" si="45">SUM(P20:P24)</f>
+        <f t="shared" ref="P25" si="51">SUM(P20:P24)</f>
         <v>67</v>
       </c>
       <c r="Q25" s="3">
-        <f t="shared" ref="Q25" si="46">SUM(Q20:Q24)</f>
+        <f t="shared" ref="Q25" si="52">SUM(Q20:Q24)</f>
         <v>160</v>
       </c>
       <c r="R25" s="3">
-        <f t="shared" ref="R25" si="47">SUM(R20:R24)</f>
+        <f t="shared" ref="R25" si="53">SUM(R20:R24)</f>
         <v>295</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Introduce looting on monster and a possibility to loot food this way. Food is eaten automatically and restores some health. Warrior development path in the endurance test goes to TITAN level now.
</commit_message>
<xml_diff>
--- a/doc/caste_system.xlsx
+++ b/doc/caste_system.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/349dfb9748b30a92/Asztali gép/ataliasflame_2.0/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3550" documentId="8_{652F4476-B36F-42CD-831D-0D71B9923ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14B023E6-03DC-442E-9B76-F1BA3DB1AD35}"/>
+  <xr:revisionPtr revIDLastSave="3917" documentId="8_{652F4476-B36F-42CD-831D-0D71B9923ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{490079F2-63C5-411E-BA65-10341C0919C1}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{CAF51EC3-63EC-48CD-AA7B-C21B3D5D222B}"/>
   </bookViews>
@@ -1765,7 +1765,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="85">
   <si>
     <t>csavargó</t>
   </si>
@@ -2235,7 +2235,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2290,8 +2290,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2316,6 +2314,9 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -2334,6 +2335,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2769,7 +2774,7 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="37" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="30" t="s">
@@ -2825,7 +2830,7 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="40"/>
+      <c r="A4" s="38"/>
       <c r="B4" s="30" t="s">
         <v>2</v>
       </c>
@@ -2879,7 +2884,7 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="40"/>
+      <c r="A5" s="38"/>
       <c r="B5" s="30" t="s">
         <v>3</v>
       </c>
@@ -2933,7 +2938,7 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="40"/>
+      <c r="A6" s="38"/>
       <c r="B6" s="30" t="s">
         <v>21</v>
       </c>
@@ -2987,7 +2992,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="41"/>
+      <c r="A7" s="39"/>
       <c r="B7" s="31" t="s">
         <v>4</v>
       </c>
@@ -3041,7 +3046,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="40" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="32" t="s">
@@ -3097,7 +3102,7 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="43"/>
+      <c r="A9" s="41"/>
       <c r="B9" s="32" t="s">
         <v>6</v>
       </c>
@@ -3151,7 +3156,7 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="43"/>
+      <c r="A10" s="41"/>
       <c r="B10" s="32" t="s">
         <v>7</v>
       </c>
@@ -3205,7 +3210,7 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="44"/>
+      <c r="A11" s="42"/>
       <c r="B11" s="29" t="s">
         <v>8</v>
       </c>
@@ -3259,7 +3264,7 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="40" t="s">
         <v>80</v>
       </c>
       <c r="B12" s="32" t="s">
@@ -3315,7 +3320,7 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="43"/>
+      <c r="A13" s="41"/>
       <c r="B13" s="30" t="s">
         <v>10</v>
       </c>
@@ -3369,7 +3374,7 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="43"/>
+      <c r="A14" s="41"/>
       <c r="B14" s="30" t="s">
         <v>11</v>
       </c>
@@ -3423,7 +3428,7 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="44"/>
+      <c r="A15" s="42"/>
       <c r="B15" s="31" t="s">
         <v>12</v>
       </c>
@@ -3477,7 +3482,7 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="40" t="s">
         <v>81</v>
       </c>
       <c r="B16" s="32" t="s">
@@ -3533,7 +3538,7 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="43"/>
+      <c r="A17" s="41"/>
       <c r="B17" s="30" t="s">
         <v>14</v>
       </c>
@@ -3587,7 +3592,7 @@
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" s="43"/>
+      <c r="A18" s="41"/>
       <c r="B18" s="30" t="s">
         <v>15</v>
       </c>
@@ -3641,7 +3646,7 @@
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" s="44"/>
+      <c r="A19" s="42"/>
       <c r="B19" s="31" t="s">
         <v>16</v>
       </c>
@@ -3695,7 +3700,7 @@
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="37" t="s">
         <v>82</v>
       </c>
       <c r="B20" s="30" t="s">
@@ -3751,7 +3756,7 @@
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21" s="40"/>
+      <c r="A21" s="38"/>
       <c r="B21" s="30" t="s">
         <v>18</v>
       </c>
@@ -3805,7 +3810,7 @@
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22" s="40"/>
+      <c r="A22" s="38"/>
       <c r="B22" s="30" t="s">
         <v>19</v>
       </c>
@@ -3859,7 +3864,7 @@
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23" s="41"/>
+      <c r="A23" s="39"/>
       <c r="B23" s="31" t="s">
         <v>20</v>
       </c>
@@ -6126,7 +6131,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="38">
+      <c r="A11" s="36">
         <v>10</v>
       </c>
       <c r="B11">
@@ -6860,7 +6865,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D8DF294-C85C-47A3-9A81-4E26EFDC10EC}">
   <dimension ref="A1:BK54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="W1" workbookViewId="0">
       <selection activeCell="BK12" sqref="BK12"/>
     </sheetView>
   </sheetViews>
@@ -6993,54 +6998,54 @@
       <c r="U1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="W1" s="45" t="s">
+      <c r="W1" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="X1" s="45"/>
-      <c r="Y1" s="45"/>
-      <c r="Z1" s="45"/>
-      <c r="AA1" s="45"/>
-      <c r="AB1" s="45"/>
-      <c r="AD1" s="45" t="s">
+      <c r="X1" s="43"/>
+      <c r="Y1" s="43"/>
+      <c r="Z1" s="43"/>
+      <c r="AA1" s="43"/>
+      <c r="AB1" s="43"/>
+      <c r="AD1" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="AE1" s="45"/>
-      <c r="AF1" s="45"/>
-      <c r="AG1" s="45"/>
-      <c r="AH1" s="45"/>
-      <c r="AI1" s="45"/>
-      <c r="AK1" s="45" t="s">
+      <c r="AE1" s="43"/>
+      <c r="AF1" s="43"/>
+      <c r="AG1" s="43"/>
+      <c r="AH1" s="43"/>
+      <c r="AI1" s="43"/>
+      <c r="AK1" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="AL1" s="45"/>
-      <c r="AM1" s="45"/>
-      <c r="AN1" s="45"/>
-      <c r="AO1" s="45"/>
-      <c r="AP1" s="45"/>
-      <c r="AR1" s="45" t="s">
+      <c r="AL1" s="43"/>
+      <c r="AM1" s="43"/>
+      <c r="AN1" s="43"/>
+      <c r="AO1" s="43"/>
+      <c r="AP1" s="43"/>
+      <c r="AR1" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="AS1" s="45"/>
-      <c r="AT1" s="45"/>
-      <c r="AU1" s="45"/>
-      <c r="AV1" s="45"/>
-      <c r="AW1" s="45"/>
-      <c r="AY1" s="45" t="s">
+      <c r="AS1" s="43"/>
+      <c r="AT1" s="43"/>
+      <c r="AU1" s="43"/>
+      <c r="AV1" s="43"/>
+      <c r="AW1" s="43"/>
+      <c r="AY1" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="AZ1" s="45"/>
-      <c r="BA1" s="45"/>
-      <c r="BB1" s="45"/>
-      <c r="BC1" s="45"/>
-      <c r="BD1" s="45"/>
-      <c r="BF1" s="45" t="s">
+      <c r="AZ1" s="43"/>
+      <c r="BA1" s="43"/>
+      <c r="BB1" s="43"/>
+      <c r="BC1" s="43"/>
+      <c r="BD1" s="43"/>
+      <c r="BF1" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="BG1" s="45"/>
-      <c r="BH1" s="45"/>
-      <c r="BI1" s="45"/>
-      <c r="BJ1" s="45"/>
-      <c r="BK1" s="45"/>
+      <c r="BG1" s="43"/>
+      <c r="BH1" s="43"/>
+      <c r="BI1" s="43"/>
+      <c r="BJ1" s="43"/>
+      <c r="BK1" s="43"/>
     </row>
     <row r="2" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
@@ -11956,11 +11961,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD573711-C846-40DC-8629-19A685998D3E}">
-  <dimension ref="A1:AV25"/>
+  <dimension ref="A1:CM25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="T1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="U11" sqref="U11"/>
+      <pane xSplit="1" topLeftCell="CD1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CO11" sqref="CO11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11979,10 +11984,11 @@
     <col min="21" max="22" width="3" bestFit="1" customWidth="1"/>
     <col min="23" max="46" width="4" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="48" max="90" width="4" style="45" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="4.77734375" style="45" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:91" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -12118,14 +12124,143 @@
       <c r="AT1" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="AU1" s="46" t="s">
+      <c r="AU1" t="s">
         <v>7</v>
       </c>
-      <c r="AV1" s="36" t="s">
+      <c r="AV1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="AW1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="AX1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="AY1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="AZ1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="BA1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="BB1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="BC1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="BD1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="BE1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="BF1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="BG1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="BH1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="BI1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="BJ1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="BK1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="BL1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="BM1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="BN1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="BO1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="BP1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="BQ1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="BR1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="BS1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="BT1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="BU1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="BV1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="BW1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="BX1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="BY1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="BZ1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="CA1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="CB1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="CC1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="CD1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="CE1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="CF1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="CG1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="CH1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="CI1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="CJ1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="CK1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="CL1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="CM1" s="45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>48</v>
       </c>
@@ -12264,14 +12399,143 @@
       <c r="AT2">
         <v>50</v>
       </c>
-      <c r="AU2" s="46">
+      <c r="AU2">
         <v>50</v>
       </c>
-      <c r="AV2" s="36">
+      <c r="AV2" s="45">
+        <v>51</v>
+      </c>
+      <c r="AW2" s="45">
+        <v>52</v>
+      </c>
+      <c r="AX2" s="45">
+        <v>54</v>
+      </c>
+      <c r="AY2" s="45">
+        <v>55</v>
+      </c>
+      <c r="AZ2" s="45">
+        <v>56</v>
+      </c>
+      <c r="BA2" s="45">
+        <v>57</v>
+      </c>
+      <c r="BB2" s="45">
+        <v>58</v>
+      </c>
+      <c r="BC2" s="45">
+        <v>59</v>
+      </c>
+      <c r="BD2" s="45">
+        <v>61</v>
+      </c>
+      <c r="BE2" s="45">
+        <v>62</v>
+      </c>
+      <c r="BF2" s="45">
+        <v>63</v>
+      </c>
+      <c r="BG2" s="45">
+        <v>64</v>
+      </c>
+      <c r="BH2" s="45">
+        <v>65</v>
+      </c>
+      <c r="BI2" s="45">
+        <v>67</v>
+      </c>
+      <c r="BJ2" s="45">
+        <v>68</v>
+      </c>
+      <c r="BK2" s="45">
+        <v>69</v>
+      </c>
+      <c r="BL2" s="45">
+        <v>70</v>
+      </c>
+      <c r="BM2" s="45">
+        <v>71</v>
+      </c>
+      <c r="BN2" s="45">
+        <v>72</v>
+      </c>
+      <c r="BO2" s="45">
+        <v>73</v>
+      </c>
+      <c r="BP2" s="45">
+        <v>75</v>
+      </c>
+      <c r="BQ2" s="45">
+        <v>76</v>
+      </c>
+      <c r="BR2" s="45">
+        <v>77</v>
+      </c>
+      <c r="BS2" s="45">
+        <v>78</v>
+      </c>
+      <c r="BT2" s="45">
+        <v>79</v>
+      </c>
+      <c r="BU2" s="45">
+        <v>81</v>
+      </c>
+      <c r="BV2" s="45">
+        <v>82</v>
+      </c>
+      <c r="BW2" s="45">
+        <v>83</v>
+      </c>
+      <c r="BX2" s="45">
+        <v>84</v>
+      </c>
+      <c r="BY2" s="45">
+        <v>85</v>
+      </c>
+      <c r="BZ2" s="45">
+        <v>87</v>
+      </c>
+      <c r="CA2" s="45">
+        <v>88</v>
+      </c>
+      <c r="CB2" s="45">
+        <v>89</v>
+      </c>
+      <c r="CC2" s="45">
+        <v>90</v>
+      </c>
+      <c r="CD2" s="45">
+        <v>91</v>
+      </c>
+      <c r="CE2" s="45">
+        <v>92</v>
+      </c>
+      <c r="CF2" s="45">
+        <v>93</v>
+      </c>
+      <c r="CG2" s="45">
+        <v>94</v>
+      </c>
+      <c r="CH2" s="45">
+        <v>95</v>
+      </c>
+      <c r="CI2" s="45">
+        <v>96</v>
+      </c>
+      <c r="CJ2" s="45">
+        <v>97</v>
+      </c>
+      <c r="CK2" s="45">
+        <v>98</v>
+      </c>
+      <c r="CL2" s="45">
+        <v>99</v>
+      </c>
+      <c r="CM2" s="45">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -12410,14 +12674,143 @@
       <c r="AT3">
         <v>50</v>
       </c>
-      <c r="AU3" s="46">
+      <c r="AU3">
         <v>50</v>
       </c>
-      <c r="AV3" s="36">
+      <c r="AV3" s="45">
+        <v>51</v>
+      </c>
+      <c r="AW3" s="45">
+        <v>53</v>
+      </c>
+      <c r="AX3" s="45">
+        <v>54</v>
+      </c>
+      <c r="AY3" s="45">
+        <v>55</v>
+      </c>
+      <c r="AZ3" s="45">
+        <v>56</v>
+      </c>
+      <c r="BA3" s="45">
+        <v>57</v>
+      </c>
+      <c r="BB3" s="45">
+        <v>59</v>
+      </c>
+      <c r="BC3" s="45">
+        <v>60</v>
+      </c>
+      <c r="BD3" s="45">
+        <v>61</v>
+      </c>
+      <c r="BE3" s="45">
+        <v>62</v>
+      </c>
+      <c r="BF3" s="45">
+        <v>63</v>
+      </c>
+      <c r="BG3" s="45">
+        <v>65</v>
+      </c>
+      <c r="BH3" s="45">
+        <v>66</v>
+      </c>
+      <c r="BI3" s="45">
+        <v>67</v>
+      </c>
+      <c r="BJ3" s="45">
+        <v>68</v>
+      </c>
+      <c r="BK3" s="45">
+        <v>69</v>
+      </c>
+      <c r="BL3" s="45">
+        <v>70</v>
+      </c>
+      <c r="BM3" s="45">
+        <v>71</v>
+      </c>
+      <c r="BN3" s="45">
+        <v>73</v>
+      </c>
+      <c r="BO3" s="45">
+        <v>74</v>
+      </c>
+      <c r="BP3" s="45">
+        <v>75</v>
+      </c>
+      <c r="BQ3" s="45">
+        <v>76</v>
+      </c>
+      <c r="BR3" s="45">
+        <v>77</v>
+      </c>
+      <c r="BS3" s="45">
+        <v>78</v>
+      </c>
+      <c r="BT3" s="45">
+        <v>80</v>
+      </c>
+      <c r="BU3" s="45">
+        <v>81</v>
+      </c>
+      <c r="BV3" s="45">
+        <v>82</v>
+      </c>
+      <c r="BW3" s="45">
+        <v>83</v>
+      </c>
+      <c r="BX3" s="45">
+        <v>84</v>
+      </c>
+      <c r="BY3" s="45">
+        <v>86</v>
+      </c>
+      <c r="BZ3" s="45">
+        <v>87</v>
+      </c>
+      <c r="CA3" s="45">
+        <v>88</v>
+      </c>
+      <c r="CB3" s="45">
+        <v>89</v>
+      </c>
+      <c r="CC3" s="45">
+        <v>90</v>
+      </c>
+      <c r="CD3" s="45">
+        <v>91</v>
+      </c>
+      <c r="CE3" s="45">
+        <v>92</v>
+      </c>
+      <c r="CF3" s="45">
+        <v>93</v>
+      </c>
+      <c r="CG3" s="45">
+        <v>94</v>
+      </c>
+      <c r="CH3" s="45">
+        <v>95</v>
+      </c>
+      <c r="CI3" s="45">
+        <v>96</v>
+      </c>
+      <c r="CJ3" s="45">
+        <v>97</v>
+      </c>
+      <c r="CK3" s="45">
+        <v>98</v>
+      </c>
+      <c r="CL3" s="45">
+        <v>99</v>
+      </c>
+      <c r="CM3" s="45">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -12556,14 +12949,143 @@
       <c r="AT4">
         <v>50</v>
       </c>
-      <c r="AU4" s="46">
+      <c r="AU4">
         <v>50</v>
       </c>
-      <c r="AV4" s="36">
+      <c r="AV4" s="45">
+        <v>52</v>
+      </c>
+      <c r="AW4" s="45">
+        <v>53</v>
+      </c>
+      <c r="AX4" s="45">
+        <v>54</v>
+      </c>
+      <c r="AY4" s="45">
+        <v>55</v>
+      </c>
+      <c r="AZ4" s="45">
+        <v>56</v>
+      </c>
+      <c r="BA4" s="45">
+        <v>58</v>
+      </c>
+      <c r="BB4" s="45">
+        <v>59</v>
+      </c>
+      <c r="BC4" s="45">
+        <v>60</v>
+      </c>
+      <c r="BD4" s="45">
+        <v>61</v>
+      </c>
+      <c r="BE4" s="45">
+        <v>62</v>
+      </c>
+      <c r="BF4" s="45">
+        <v>64</v>
+      </c>
+      <c r="BG4" s="45">
+        <v>65</v>
+      </c>
+      <c r="BH4" s="45">
+        <v>66</v>
+      </c>
+      <c r="BI4" s="45">
+        <v>67</v>
+      </c>
+      <c r="BJ4" s="45">
+        <v>68</v>
+      </c>
+      <c r="BK4" s="45">
+        <v>69</v>
+      </c>
+      <c r="BL4" s="45">
+        <v>70</v>
+      </c>
+      <c r="BM4" s="45">
+        <v>72</v>
+      </c>
+      <c r="BN4" s="45">
+        <v>73</v>
+      </c>
+      <c r="BO4" s="45">
+        <v>74</v>
+      </c>
+      <c r="BP4" s="45">
+        <v>75</v>
+      </c>
+      <c r="BQ4" s="45">
+        <v>76</v>
+      </c>
+      <c r="BR4" s="45">
+        <v>77</v>
+      </c>
+      <c r="BS4" s="45">
+        <v>79</v>
+      </c>
+      <c r="BT4" s="45">
+        <v>80</v>
+      </c>
+      <c r="BU4" s="45">
+        <v>81</v>
+      </c>
+      <c r="BV4" s="45">
+        <v>82</v>
+      </c>
+      <c r="BW4" s="45">
+        <v>83</v>
+      </c>
+      <c r="BX4" s="45">
+        <v>85</v>
+      </c>
+      <c r="BY4" s="45">
+        <v>86</v>
+      </c>
+      <c r="BZ4" s="45">
+        <v>87</v>
+      </c>
+      <c r="CA4" s="45">
+        <v>88</v>
+      </c>
+      <c r="CB4" s="45">
+        <v>89</v>
+      </c>
+      <c r="CC4" s="45">
+        <v>90</v>
+      </c>
+      <c r="CD4" s="45">
+        <v>91</v>
+      </c>
+      <c r="CE4" s="45">
+        <v>92</v>
+      </c>
+      <c r="CF4" s="45">
+        <v>93</v>
+      </c>
+      <c r="CG4" s="45">
+        <v>94</v>
+      </c>
+      <c r="CH4" s="45">
+        <v>95</v>
+      </c>
+      <c r="CI4" s="45">
+        <v>96</v>
+      </c>
+      <c r="CJ4" s="45">
+        <v>97</v>
+      </c>
+      <c r="CK4" s="45">
+        <v>98</v>
+      </c>
+      <c r="CL4" s="45">
+        <v>99</v>
+      </c>
+      <c r="CM4" s="45">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -12702,14 +13224,143 @@
       <c r="AT5">
         <v>50</v>
       </c>
-      <c r="AU5" s="46">
+      <c r="AU5">
         <v>50</v>
       </c>
-      <c r="AV5" s="36">
+      <c r="AV5" s="45">
+        <v>51</v>
+      </c>
+      <c r="AW5" s="45">
+        <v>52</v>
+      </c>
+      <c r="AX5" s="45">
+        <v>53</v>
+      </c>
+      <c r="AY5" s="45">
+        <v>55</v>
+      </c>
+      <c r="AZ5" s="45">
+        <v>56</v>
+      </c>
+      <c r="BA5" s="45">
+        <v>57</v>
+      </c>
+      <c r="BB5" s="45">
+        <v>58</v>
+      </c>
+      <c r="BC5" s="45">
+        <v>59</v>
+      </c>
+      <c r="BD5" s="45">
+        <v>60</v>
+      </c>
+      <c r="BE5" s="45">
+        <v>62</v>
+      </c>
+      <c r="BF5" s="45">
+        <v>63</v>
+      </c>
+      <c r="BG5" s="45">
+        <v>64</v>
+      </c>
+      <c r="BH5" s="45">
+        <v>65</v>
+      </c>
+      <c r="BI5" s="45">
+        <v>66</v>
+      </c>
+      <c r="BJ5" s="45">
+        <v>68</v>
+      </c>
+      <c r="BK5" s="45">
+        <v>69</v>
+      </c>
+      <c r="BL5" s="45">
+        <v>70</v>
+      </c>
+      <c r="BM5" s="45">
+        <v>71</v>
+      </c>
+      <c r="BN5" s="45">
+        <v>72</v>
+      </c>
+      <c r="BO5" s="45">
+        <v>73</v>
+      </c>
+      <c r="BP5" s="45">
+        <v>74</v>
+      </c>
+      <c r="BQ5" s="45">
+        <v>76</v>
+      </c>
+      <c r="BR5" s="45">
+        <v>77</v>
+      </c>
+      <c r="BS5" s="45">
+        <v>78</v>
+      </c>
+      <c r="BT5" s="45">
+        <v>79</v>
+      </c>
+      <c r="BU5" s="45">
+        <v>80</v>
+      </c>
+      <c r="BV5" s="45">
+        <v>82</v>
+      </c>
+      <c r="BW5" s="45">
+        <v>83</v>
+      </c>
+      <c r="BX5" s="45">
+        <v>84</v>
+      </c>
+      <c r="BY5" s="45">
+        <v>85</v>
+      </c>
+      <c r="BZ5" s="45">
+        <v>86</v>
+      </c>
+      <c r="CA5" s="45">
+        <v>88</v>
+      </c>
+      <c r="CB5" s="45">
+        <v>89</v>
+      </c>
+      <c r="CC5" s="45">
+        <v>90</v>
+      </c>
+      <c r="CD5" s="45">
+        <v>91</v>
+      </c>
+      <c r="CE5" s="45">
+        <v>92</v>
+      </c>
+      <c r="CF5" s="45">
+        <v>93</v>
+      </c>
+      <c r="CG5" s="45">
+        <v>94</v>
+      </c>
+      <c r="CH5" s="45">
+        <v>95</v>
+      </c>
+      <c r="CI5" s="45">
+        <v>96</v>
+      </c>
+      <c r="CJ5" s="45">
+        <v>97</v>
+      </c>
+      <c r="CK5" s="45">
+        <v>98</v>
+      </c>
+      <c r="CL5" s="45">
+        <v>99</v>
+      </c>
+      <c r="CM5" s="45">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A6" s="34" t="s">
         <v>49</v>
       </c>
@@ -12848,20 +13499,149 @@
       <c r="AT6" s="34">
         <v>15</v>
       </c>
-      <c r="AU6" s="47">
+      <c r="AU6" s="34">
         <v>20</v>
       </c>
-      <c r="AV6" s="37">
+      <c r="AV6" s="46">
+        <v>20</v>
+      </c>
+      <c r="AW6" s="46">
+        <v>20</v>
+      </c>
+      <c r="AX6" s="46">
+        <v>20</v>
+      </c>
+      <c r="AY6" s="46">
+        <v>20</v>
+      </c>
+      <c r="AZ6" s="46">
+        <v>21</v>
+      </c>
+      <c r="BA6" s="46">
+        <v>21</v>
+      </c>
+      <c r="BB6" s="46">
+        <v>21</v>
+      </c>
+      <c r="BC6" s="46">
+        <v>22</v>
+      </c>
+      <c r="BD6" s="46">
+        <v>22</v>
+      </c>
+      <c r="BE6" s="46">
+        <v>22</v>
+      </c>
+      <c r="BF6" s="46">
+        <v>22</v>
+      </c>
+      <c r="BG6" s="46">
+        <v>22</v>
+      </c>
+      <c r="BH6" s="46">
+        <v>23</v>
+      </c>
+      <c r="BI6" s="46">
+        <v>23</v>
+      </c>
+      <c r="BJ6" s="46">
+        <v>23</v>
+      </c>
+      <c r="BK6" s="46">
+        <v>24</v>
+      </c>
+      <c r="BL6" s="46">
+        <v>25</v>
+      </c>
+      <c r="BM6" s="46">
+        <v>25</v>
+      </c>
+      <c r="BN6" s="46">
+        <v>25</v>
+      </c>
+      <c r="BO6" s="46">
+        <v>26</v>
+      </c>
+      <c r="BP6" s="46">
+        <v>26</v>
+      </c>
+      <c r="BQ6" s="46">
+        <v>26</v>
+      </c>
+      <c r="BR6" s="46">
+        <v>27</v>
+      </c>
+      <c r="BS6" s="46">
+        <v>27</v>
+      </c>
+      <c r="BT6" s="46">
+        <v>27</v>
+      </c>
+      <c r="BU6" s="46">
+        <v>27</v>
+      </c>
+      <c r="BV6" s="46">
+        <v>27</v>
+      </c>
+      <c r="BW6" s="46">
+        <v>28</v>
+      </c>
+      <c r="BX6" s="46">
+        <v>28</v>
+      </c>
+      <c r="BY6" s="46">
+        <v>28</v>
+      </c>
+      <c r="BZ6" s="46">
+        <v>28</v>
+      </c>
+      <c r="CA6" s="46">
+        <v>28</v>
+      </c>
+      <c r="CB6" s="46">
+        <v>29</v>
+      </c>
+      <c r="CC6" s="46">
+        <v>30</v>
+      </c>
+      <c r="CD6" s="46">
+        <v>31</v>
+      </c>
+      <c r="CE6" s="46">
+        <v>32</v>
+      </c>
+      <c r="CF6" s="46">
+        <v>33</v>
+      </c>
+      <c r="CG6" s="46">
+        <v>34</v>
+      </c>
+      <c r="CH6" s="46">
+        <v>35</v>
+      </c>
+      <c r="CI6" s="46">
+        <v>36</v>
+      </c>
+      <c r="CJ6" s="46">
+        <v>37</v>
+      </c>
+      <c r="CK6" s="46">
+        <v>38</v>
+      </c>
+      <c r="CL6" s="46">
+        <v>39</v>
+      </c>
+      <c r="CM6" s="46">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:91" x14ac:dyDescent="0.3">
       <c r="B7">
         <f>SUM(B2:B6)</f>
         <v>5</v>
       </c>
       <c r="C7">
-        <f t="shared" ref="C7:AV7" si="0">SUM(C2:C6)</f>
+        <f t="shared" ref="C7:CM7" si="0">SUM(C2:C6)</f>
         <v>10</v>
       </c>
       <c r="D7">
@@ -13036,16 +13816,188 @@
         <f t="shared" si="17"/>
         <v>215</v>
       </c>
-      <c r="AU7" s="46">
-        <f t="shared" ref="AU7" si="19">SUM(AU2:AU6)</f>
+      <c r="AU7">
+        <f t="shared" ref="AU7:CL7" si="19">SUM(AU2:AU6)</f>
         <v>220</v>
       </c>
-      <c r="AV7" s="36">
+      <c r="AV7" s="45">
+        <f t="shared" si="19"/>
+        <v>225</v>
+      </c>
+      <c r="AW7" s="45">
+        <f t="shared" si="19"/>
+        <v>230</v>
+      </c>
+      <c r="AX7" s="45">
+        <f t="shared" si="19"/>
+        <v>235</v>
+      </c>
+      <c r="AY7" s="45">
+        <f t="shared" si="19"/>
+        <v>240</v>
+      </c>
+      <c r="AZ7" s="45">
+        <f t="shared" si="19"/>
+        <v>245</v>
+      </c>
+      <c r="BA7" s="45">
+        <f t="shared" si="19"/>
+        <v>250</v>
+      </c>
+      <c r="BB7" s="45">
+        <f t="shared" si="19"/>
+        <v>255</v>
+      </c>
+      <c r="BC7" s="45">
+        <f t="shared" si="19"/>
+        <v>260</v>
+      </c>
+      <c r="BD7" s="45">
+        <f t="shared" si="19"/>
+        <v>265</v>
+      </c>
+      <c r="BE7" s="45">
+        <f t="shared" si="19"/>
+        <v>270</v>
+      </c>
+      <c r="BF7" s="45">
+        <f t="shared" si="19"/>
+        <v>275</v>
+      </c>
+      <c r="BG7" s="45">
+        <f t="shared" si="19"/>
+        <v>280</v>
+      </c>
+      <c r="BH7" s="45">
+        <f t="shared" si="19"/>
+        <v>285</v>
+      </c>
+      <c r="BI7" s="45">
+        <f t="shared" si="19"/>
+        <v>290</v>
+      </c>
+      <c r="BJ7" s="45">
+        <f t="shared" si="19"/>
+        <v>295</v>
+      </c>
+      <c r="BK7" s="45">
+        <f t="shared" si="19"/>
+        <v>300</v>
+      </c>
+      <c r="BL7" s="45">
+        <f t="shared" si="19"/>
+        <v>305</v>
+      </c>
+      <c r="BM7" s="45">
+        <f t="shared" si="19"/>
+        <v>310</v>
+      </c>
+      <c r="BN7" s="45">
+        <f t="shared" si="19"/>
+        <v>315</v>
+      </c>
+      <c r="BO7" s="45">
+        <f t="shared" si="19"/>
+        <v>320</v>
+      </c>
+      <c r="BP7" s="45">
+        <f t="shared" si="19"/>
+        <v>325</v>
+      </c>
+      <c r="BQ7" s="45">
+        <f t="shared" si="19"/>
+        <v>330</v>
+      </c>
+      <c r="BR7" s="45">
+        <f t="shared" si="19"/>
+        <v>335</v>
+      </c>
+      <c r="BS7" s="45">
+        <f t="shared" si="19"/>
+        <v>340</v>
+      </c>
+      <c r="BT7" s="45">
+        <f t="shared" si="19"/>
+        <v>345</v>
+      </c>
+      <c r="BU7" s="45">
+        <f t="shared" si="19"/>
+        <v>350</v>
+      </c>
+      <c r="BV7" s="45">
+        <f t="shared" si="19"/>
+        <v>355</v>
+      </c>
+      <c r="BW7" s="45">
+        <f t="shared" si="19"/>
+        <v>360</v>
+      </c>
+      <c r="BX7" s="45">
+        <f t="shared" si="19"/>
+        <v>365</v>
+      </c>
+      <c r="BY7" s="45">
+        <f t="shared" si="19"/>
+        <v>370</v>
+      </c>
+      <c r="BZ7" s="45">
+        <f t="shared" si="19"/>
+        <v>375</v>
+      </c>
+      <c r="CA7" s="45">
+        <f t="shared" si="19"/>
+        <v>380</v>
+      </c>
+      <c r="CB7" s="45">
+        <f t="shared" si="19"/>
+        <v>385</v>
+      </c>
+      <c r="CC7" s="45">
+        <f t="shared" si="19"/>
+        <v>390</v>
+      </c>
+      <c r="CD7" s="45">
+        <f t="shared" si="19"/>
+        <v>395</v>
+      </c>
+      <c r="CE7" s="45">
+        <f t="shared" si="19"/>
+        <v>400</v>
+      </c>
+      <c r="CF7" s="45">
+        <f t="shared" si="19"/>
+        <v>405</v>
+      </c>
+      <c r="CG7" s="45">
+        <f t="shared" si="19"/>
+        <v>410</v>
+      </c>
+      <c r="CH7" s="45">
+        <f t="shared" si="19"/>
+        <v>415</v>
+      </c>
+      <c r="CI7" s="45">
+        <f t="shared" si="19"/>
+        <v>420</v>
+      </c>
+      <c r="CJ7" s="45">
+        <f t="shared" si="19"/>
+        <v>425</v>
+      </c>
+      <c r="CK7" s="45">
+        <f t="shared" si="19"/>
+        <v>430</v>
+      </c>
+      <c r="CL7" s="45">
+        <f t="shared" si="19"/>
+        <v>435</v>
+      </c>
+      <c r="CM7" s="45">
         <f t="shared" si="0"/>
         <v>440</v>
       </c>
     </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:91" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>0</v>
       </c>
@@ -13104,7 +14056,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -13166,7 +14118,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -13228,7 +14180,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>47</v>
       </c>
@@ -13290,7 +14242,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -13352,7 +14304,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:91" x14ac:dyDescent="0.3">
       <c r="A15" s="34" t="s">
         <v>49</v>
       </c>
@@ -13414,7 +14366,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:91" x14ac:dyDescent="0.3">
       <c r="B16">
         <f>SUM(B11:B15)</f>
         <v>5</v>

</xml_diff>

<commit_message>
Introduce new NATURE_DWELLER castes: - DRUID - ARCHDRUID Nature dweller development path in the endurance test goes to ARCHDRUID level now. Introduce limitations among character properties. E.g. The followers of ALATE cannot be WIZARDs.
</commit_message>
<xml_diff>
--- a/doc/caste_system.xlsx
+++ b/doc/caste_system.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/349dfb9748b30a92/Asztali gép/ataliasflame_2.0/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5214" documentId="8_{652F4476-B36F-42CD-831D-0D71B9923ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CFF9D3CF-2612-49BB-8F44-FB68397D59B7}"/>
+  <xr:revisionPtr revIDLastSave="5448" documentId="8_{652F4476-B36F-42CD-831D-0D71B9923ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0590452-0A26-4734-8157-A9B5FEEA1567}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{CAF51EC3-63EC-48CD-AA7B-C21B3D5D222B}"/>
   </bookViews>
@@ -1557,7 +1557,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1168" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1197" uniqueCount="85">
   <si>
     <t>csavargó</t>
   </si>
@@ -2012,7 +2012,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2068,14 +2068,8 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2086,28 +2080,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -2430,7 +2420,7 @@
   <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2469,19 +2459,19 @@
       <c r="F1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J1" t="s">
         <v>29</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L1" s="1" t="s">
@@ -2525,19 +2515,19 @@
       <c r="F2" t="s">
         <v>39</v>
       </c>
-      <c r="G2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="G2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>39</v>
       </c>
       <c r="J2" t="s">
         <v>39</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="3" t="s">
         <v>39</v>
       </c>
       <c r="L2" s="1" t="s">
@@ -2563,22 +2553,22 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="44" t="s">
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" t="s">
         <v>39</v>
       </c>
       <c r="G3" s="3" t="s">
@@ -2590,49 +2580,49 @@
       <c r="I3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="K3" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="L3" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="M3" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="N3" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="O3" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="P3" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q3" s="3" t="s">
+      <c r="K3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" t="s">
+        <v>39</v>
+      </c>
+      <c r="N3" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" t="s">
+        <v>39</v>
+      </c>
+      <c r="P3" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q3" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="R3" s="45" t="s">
+      <c r="R3" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="50"/>
-      <c r="B4" s="48" t="s">
+      <c r="A4" s="39"/>
+      <c r="B4" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="44" t="s">
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" t="s">
         <v>39</v>
       </c>
       <c r="G4" s="3" t="s">
@@ -2644,36 +2634,36 @@
       <c r="I4" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="K4" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="L4" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="M4" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="N4" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="O4" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="P4" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q4" s="3" t="s">
+      <c r="K4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M4" t="s">
+        <v>39</v>
+      </c>
+      <c r="N4" t="s">
+        <v>39</v>
+      </c>
+      <c r="O4" t="s">
+        <v>39</v>
+      </c>
+      <c r="P4" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q4" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="R4" s="45" t="s">
+      <c r="R4" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="50"/>
+      <c r="A5" s="39"/>
       <c r="B5" s="27" t="s">
         <v>3</v>
       </c>
@@ -2727,7 +2717,7 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="50"/>
+      <c r="A6" s="39"/>
       <c r="B6" s="27" t="s">
         <v>21</v>
       </c>
@@ -2781,7 +2771,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="51"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="28" t="s">
         <v>4</v>
       </c>
@@ -2835,7 +2825,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="38" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="29" t="s">
@@ -2853,19 +2843,19 @@
       <c r="F8" t="s">
         <v>39</v>
       </c>
-      <c r="G8" t="s">
-        <v>39</v>
-      </c>
-      <c r="H8" t="s">
-        <v>39</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="G8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>39</v>
       </c>
       <c r="J8" t="s">
         <v>39</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="3" t="s">
         <v>40</v>
       </c>
       <c r="L8" s="1" t="s">
@@ -2891,7 +2881,7 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="41"/>
+      <c r="A9" s="39"/>
       <c r="B9" s="29" t="s">
         <v>6</v>
       </c>
@@ -2907,19 +2897,19 @@
       <c r="F9" t="s">
         <v>39</v>
       </c>
-      <c r="G9" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" t="s">
-        <v>39</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="G9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>39</v>
       </c>
       <c r="J9" t="s">
         <v>39</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="3" t="s">
         <v>40</v>
       </c>
       <c r="L9" s="1" t="s">
@@ -2945,7 +2935,7 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="41"/>
+      <c r="A10" s="39"/>
       <c r="B10" s="29" t="s">
         <v>7</v>
       </c>
@@ -2961,19 +2951,19 @@
       <c r="F10" t="s">
         <v>39</v>
       </c>
-      <c r="G10" t="s">
-        <v>39</v>
-      </c>
-      <c r="H10" t="s">
-        <v>39</v>
-      </c>
-      <c r="I10" t="s">
+      <c r="G10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" s="3" t="s">
         <v>39</v>
       </c>
       <c r="J10" t="s">
         <v>39</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="3" t="s">
         <v>40</v>
       </c>
       <c r="L10" s="1" t="s">
@@ -2999,7 +2989,7 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="42"/>
+      <c r="A11" s="40"/>
       <c r="B11" s="26" t="s">
         <v>8</v>
       </c>
@@ -3015,19 +3005,19 @@
       <c r="F11" t="s">
         <v>39</v>
       </c>
-      <c r="G11" t="s">
-        <v>39</v>
-      </c>
-      <c r="H11" t="s">
-        <v>39</v>
-      </c>
-      <c r="I11" t="s">
+      <c r="G11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" s="3" t="s">
         <v>39</v>
       </c>
       <c r="J11" t="s">
         <v>39</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="3" t="s">
         <v>40</v>
       </c>
       <c r="L11" s="1" t="s">
@@ -3053,7 +3043,7 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="38" t="s">
         <v>79</v>
       </c>
       <c r="B12" s="29" t="s">
@@ -3071,19 +3061,19 @@
       <c r="F12" t="s">
         <v>39</v>
       </c>
-      <c r="G12" t="s">
-        <v>39</v>
-      </c>
-      <c r="H12" t="s">
-        <v>39</v>
-      </c>
-      <c r="I12" t="s">
+      <c r="G12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12" s="3" t="s">
         <v>39</v>
       </c>
       <c r="J12" t="s">
         <v>39</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12" s="3" t="s">
         <v>40</v>
       </c>
       <c r="L12" s="1" t="s">
@@ -3109,7 +3099,7 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="41"/>
+      <c r="A13" s="39"/>
       <c r="B13" s="27" t="s">
         <v>10</v>
       </c>
@@ -3163,7 +3153,7 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="41"/>
+      <c r="A14" s="39"/>
       <c r="B14" s="27" t="s">
         <v>11</v>
       </c>
@@ -3217,7 +3207,7 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="42"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="28" t="s">
         <v>12</v>
       </c>
@@ -3271,7 +3261,7 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="38" t="s">
         <v>80</v>
       </c>
       <c r="B16" s="29" t="s">
@@ -3289,19 +3279,19 @@
       <c r="F16" t="s">
         <v>39</v>
       </c>
-      <c r="G16" t="s">
-        <v>39</v>
-      </c>
-      <c r="H16" t="s">
-        <v>39</v>
-      </c>
-      <c r="I16" t="s">
+      <c r="G16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I16" s="3" t="s">
         <v>39</v>
       </c>
       <c r="J16" t="s">
         <v>39</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K16" s="3" t="s">
         <v>39</v>
       </c>
       <c r="L16" s="1" t="s">
@@ -3327,20 +3317,20 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="41"/>
-      <c r="B17" s="27" t="s">
+      <c r="A17" s="39"/>
+      <c r="B17" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F17" s="3" t="s">
+      <c r="C17" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="45" t="s">
         <v>39</v>
       </c>
       <c r="G17" s="3" t="s">
@@ -3352,49 +3342,49 @@
       <c r="I17" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J17" s="3" t="s">
+      <c r="J17" s="45" t="s">
         <v>39</v>
       </c>
       <c r="K17" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="L17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="N17" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="O17" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="P17" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q17" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="R17" s="2" t="s">
+      <c r="L17" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="M17" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="N17" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="O17" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="P17" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q17" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="R17" s="47" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" s="41"/>
-      <c r="B18" s="27" t="s">
+      <c r="A18" s="39"/>
+      <c r="B18" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" s="3" t="s">
+      <c r="C18" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="45" t="s">
         <v>39</v>
       </c>
       <c r="G18" s="3" t="s">
@@ -3406,36 +3396,36 @@
       <c r="I18" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J18" s="3" t="s">
+      <c r="J18" s="45" t="s">
         <v>39</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="L18" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="N18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="O18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="P18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="R18" s="2" t="s">
+      <c r="L18" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="M18" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="N18" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="O18" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="P18" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q18" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="R18" s="47" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" s="42"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="28" t="s">
         <v>16</v>
       </c>
@@ -3489,7 +3479,7 @@
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="41" t="s">
         <v>81</v>
       </c>
       <c r="B20" s="27" t="s">
@@ -3545,7 +3535,7 @@
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21" s="38"/>
+      <c r="A21" s="42"/>
       <c r="B21" s="27" t="s">
         <v>18</v>
       </c>
@@ -3599,7 +3589,7 @@
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22" s="38"/>
+      <c r="A22" s="42"/>
       <c r="B22" s="27" t="s">
         <v>19</v>
       </c>
@@ -3653,7 +3643,7 @@
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23" s="39"/>
+      <c r="A23" s="43"/>
       <c r="B23" s="28" t="s">
         <v>20</v>
       </c>
@@ -3715,7 +3705,8 @@
     <mergeCell ref="A20:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3724,7 +3715,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="N11" sqref="N11:Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4339,9 +4330,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45FC8AA8-DC1F-4C97-8335-A619D1FCDEA7}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4597,7 +4586,7 @@
   <dimension ref="A1:AC10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H9"/>
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4623,8 +4612,8 @@
     <col min="19" max="19" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.109375" style="45" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.88671875" style="45" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="4" bestFit="1" customWidth="1"/>
@@ -4653,10 +4642,10 @@
       <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="44" t="s">
+      <c r="H1" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="44" t="s">
+      <c r="I1" t="s">
         <v>2</v>
       </c>
       <c r="J1" s="3" t="s">
@@ -4695,10 +4684,10 @@
       <c r="U1" t="s">
         <v>13</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="W1" s="45" t="s">
         <v>15</v>
       </c>
       <c r="X1" s="2" t="s">
@@ -4742,10 +4731,10 @@
       <c r="G2" s="1">
         <v>1</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="45">
         <v>2</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="45">
         <v>6</v>
       </c>
       <c r="J2" s="3">
@@ -4784,10 +4773,10 @@
       <c r="U2">
         <v>3</v>
       </c>
-      <c r="V2" s="3">
+      <c r="V2" s="45">
         <v>8</v>
       </c>
-      <c r="W2" s="3">
+      <c r="W2" s="45">
         <v>25</v>
       </c>
       <c r="X2" s="2">
@@ -4832,10 +4821,10 @@
       <c r="G3" s="1">
         <v>1</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="45">
         <v>3</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="45">
         <v>12</v>
       </c>
       <c r="J3" s="3">
@@ -4874,10 +4863,10 @@
       <c r="U3">
         <v>3</v>
       </c>
-      <c r="V3" s="3">
+      <c r="V3" s="45">
         <v>12</v>
       </c>
-      <c r="W3" s="3">
+      <c r="W3" s="45">
         <v>25</v>
       </c>
       <c r="X3" s="2">
@@ -4922,10 +4911,10 @@
       <c r="G4" s="1">
         <v>1</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="45">
         <v>2</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="45">
         <v>7</v>
       </c>
       <c r="J4" s="3">
@@ -4964,10 +4953,10 @@
       <c r="U4">
         <v>4</v>
       </c>
-      <c r="V4" s="3">
+      <c r="V4" s="45">
         <v>17</v>
       </c>
-      <c r="W4" s="3">
+      <c r="W4" s="45">
         <v>45</v>
       </c>
       <c r="X4" s="2">
@@ -5012,10 +5001,10 @@
       <c r="G5" s="1">
         <v>1</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="45">
         <v>3</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="45">
         <v>10</v>
       </c>
       <c r="J5" s="3">
@@ -5054,10 +5043,10 @@
       <c r="U5">
         <v>3</v>
       </c>
-      <c r="V5" s="3">
+      <c r="V5" s="45">
         <v>12</v>
       </c>
-      <c r="W5" s="3">
+      <c r="W5" s="45">
         <v>25</v>
       </c>
       <c r="X5" s="2">
@@ -5102,10 +5091,10 @@
       <c r="G6" s="1">
         <v>1</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="45">
         <v>5</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="45">
         <v>20</v>
       </c>
       <c r="J6" s="3">
@@ -5144,10 +5133,10 @@
       <c r="U6">
         <v>4</v>
       </c>
-      <c r="V6" s="3">
+      <c r="V6" s="45">
         <v>18</v>
       </c>
-      <c r="W6" s="3">
+      <c r="W6" s="45">
         <v>40</v>
       </c>
       <c r="X6" s="2">
@@ -5192,10 +5181,10 @@
       <c r="G7" s="1">
         <v>0</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="45">
         <v>5</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="45">
         <v>20</v>
       </c>
       <c r="J7" s="3">
@@ -5207,16 +5196,16 @@
       <c r="L7" s="2">
         <v>100</v>
       </c>
-      <c r="M7" s="44">
+      <c r="M7">
         <v>1</v>
       </c>
-      <c r="N7" s="44">
+      <c r="N7">
         <v>6</v>
       </c>
-      <c r="O7" s="44">
+      <c r="O7">
         <v>13</v>
       </c>
-      <c r="P7" s="45">
+      <c r="P7" s="1">
         <v>25</v>
       </c>
       <c r="Q7">
@@ -5234,10 +5223,10 @@
       <c r="U7">
         <v>4</v>
       </c>
-      <c r="V7" s="3">
+      <c r="V7" s="45">
         <v>18</v>
       </c>
-      <c r="W7" s="3">
+      <c r="W7" s="45">
         <v>40</v>
       </c>
       <c r="X7" s="2">
@@ -5282,10 +5271,10 @@
       <c r="G8" s="1">
         <v>0</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="45">
         <v>4</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="45">
         <v>20</v>
       </c>
       <c r="J8" s="3">
@@ -5297,16 +5286,16 @@
       <c r="L8" s="2">
         <v>100</v>
       </c>
-      <c r="M8" s="44">
+      <c r="M8">
         <v>1</v>
       </c>
-      <c r="N8" s="44">
+      <c r="N8">
         <v>5</v>
       </c>
-      <c r="O8" s="44">
+      <c r="O8">
         <v>12</v>
       </c>
-      <c r="P8" s="45">
+      <c r="P8" s="1">
         <v>25</v>
       </c>
       <c r="Q8">
@@ -5324,10 +5313,10 @@
       <c r="U8">
         <v>3</v>
       </c>
-      <c r="V8" s="3">
+      <c r="V8" s="45">
         <v>12</v>
       </c>
-      <c r="W8" s="3">
+      <c r="W8" s="45">
         <v>40</v>
       </c>
       <c r="X8" s="2">
@@ -5372,10 +5361,10 @@
       <c r="G9" s="36">
         <v>0</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9" s="48">
         <v>1</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="48">
         <v>5</v>
       </c>
       <c r="J9" s="10">
@@ -5387,16 +5376,16 @@
       <c r="L9" s="4">
         <v>25</v>
       </c>
-      <c r="M9" s="46">
+      <c r="M9" s="31">
         <v>1</v>
       </c>
-      <c r="N9" s="46">
+      <c r="N9" s="31">
         <v>2</v>
       </c>
-      <c r="O9" s="46">
+      <c r="O9" s="31">
         <v>5</v>
       </c>
-      <c r="P9" s="47">
+      <c r="P9" s="35">
         <v>10</v>
       </c>
       <c r="Q9" s="31">
@@ -5414,10 +5403,10 @@
       <c r="U9" s="31">
         <v>1</v>
       </c>
-      <c r="V9" s="10">
+      <c r="V9" s="48">
         <v>3</v>
       </c>
-      <c r="W9" s="10">
+      <c r="W9" s="48">
         <v>10</v>
       </c>
       <c r="X9" s="4">
@@ -5501,11 +5490,11 @@
         <f t="shared" ref="U10" si="10">SUM(U2:U9)</f>
         <v>25</v>
       </c>
-      <c r="V10">
+      <c r="V10" s="45">
         <f t="shared" ref="V10" si="11">SUM(V2:V9)</f>
         <v>100</v>
       </c>
-      <c r="W10">
+      <c r="W10" s="45">
         <f t="shared" ref="W10" si="12">SUM(W2:W9)</f>
         <v>250</v>
       </c>
@@ -5604,7 +5593,7 @@
   <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6757,54 +6746,54 @@
       <c r="U1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="W1" s="43" t="s">
+      <c r="W1" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="X1" s="43"/>
-      <c r="Y1" s="43"/>
-      <c r="Z1" s="43"/>
-      <c r="AA1" s="43"/>
-      <c r="AB1" s="43"/>
-      <c r="AD1" s="43" t="s">
+      <c r="X1" s="44"/>
+      <c r="Y1" s="44"/>
+      <c r="Z1" s="44"/>
+      <c r="AA1" s="44"/>
+      <c r="AB1" s="44"/>
+      <c r="AD1" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="AE1" s="43"/>
-      <c r="AF1" s="43"/>
-      <c r="AG1" s="43"/>
-      <c r="AH1" s="43"/>
-      <c r="AI1" s="43"/>
-      <c r="AK1" s="43" t="s">
+      <c r="AE1" s="44"/>
+      <c r="AF1" s="44"/>
+      <c r="AG1" s="44"/>
+      <c r="AH1" s="44"/>
+      <c r="AI1" s="44"/>
+      <c r="AK1" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="AL1" s="43"/>
-      <c r="AM1" s="43"/>
-      <c r="AN1" s="43"/>
-      <c r="AO1" s="43"/>
-      <c r="AP1" s="43"/>
-      <c r="AR1" s="43" t="s">
+      <c r="AL1" s="44"/>
+      <c r="AM1" s="44"/>
+      <c r="AN1" s="44"/>
+      <c r="AO1" s="44"/>
+      <c r="AP1" s="44"/>
+      <c r="AR1" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="AS1" s="43"/>
-      <c r="AT1" s="43"/>
-      <c r="AU1" s="43"/>
-      <c r="AV1" s="43"/>
-      <c r="AW1" s="43"/>
-      <c r="AY1" s="43" t="s">
+      <c r="AS1" s="44"/>
+      <c r="AT1" s="44"/>
+      <c r="AU1" s="44"/>
+      <c r="AV1" s="44"/>
+      <c r="AW1" s="44"/>
+      <c r="AY1" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="AZ1" s="43"/>
-      <c r="BA1" s="43"/>
-      <c r="BB1" s="43"/>
-      <c r="BC1" s="43"/>
-      <c r="BD1" s="43"/>
-      <c r="BF1" s="43" t="s">
+      <c r="AZ1" s="44"/>
+      <c r="BA1" s="44"/>
+      <c r="BB1" s="44"/>
+      <c r="BC1" s="44"/>
+      <c r="BD1" s="44"/>
+      <c r="BF1" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="BG1" s="43"/>
-      <c r="BH1" s="43"/>
-      <c r="BI1" s="43"/>
-      <c r="BJ1" s="43"/>
-      <c r="BK1" s="43"/>
+      <c r="BG1" s="44"/>
+      <c r="BH1" s="44"/>
+      <c r="BI1" s="44"/>
+      <c r="BJ1" s="44"/>
+      <c r="BK1" s="44"/>
     </row>
     <row r="2" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
@@ -11722,9 +11711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD573711-C846-40DC-8629-19A685998D3E}">
   <dimension ref="A1:CW46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AC7" sqref="AC7"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11740,7 +11728,7 @@
     <col min="24" max="47" width="4" bestFit="1" customWidth="1"/>
     <col min="48" max="50" width="4" customWidth="1"/>
     <col min="51" max="51" width="16" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="54" max="94" width="4" bestFit="1" customWidth="1"/>
     <col min="95" max="100" width="4" customWidth="1"/>
@@ -11898,7 +11886,7 @@
       <c r="AY1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AZ1" s="52" t="s">
+      <c r="AZ1" s="37" t="s">
         <v>4</v>
       </c>
       <c r="BA1" s="3" t="s">
@@ -17084,7 +17072,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A33" s="31" t="s">
         <v>53</v>
       </c>
@@ -17155,7 +17143,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:52" x14ac:dyDescent="0.3">
       <c r="B34">
         <f>SUM(B26:B33)</f>
         <v>5</v>
@@ -17245,7 +17233,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:52" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>0</v>
       </c>
@@ -17303,17 +17291,104 @@
       <c r="T37" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="U37" s="3" t="s">
+      <c r="U37" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="V37" s="3" t="s">
+      <c r="V37" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="W37" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="X37" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y37" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z37" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA37" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB37" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC37" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD37" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE37" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF37" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG37" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH37" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="AI37" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="AJ37" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="AK37" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="AL37" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM37" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN37" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO37" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP37" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ37" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="AR37" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="AS37" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="AT37" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="AU37" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="AV37" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="AW37" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="AX37" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="AY37" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="W37" s="3" t="s">
+      <c r="AZ37" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>48</v>
       </c>
@@ -17377,14 +17452,101 @@
       <c r="U38">
         <v>8</v>
       </c>
-      <c r="V38" s="3">
+      <c r="V38">
+        <v>9</v>
+      </c>
+      <c r="W38">
+        <v>10</v>
+      </c>
+      <c r="X38">
+        <v>11</v>
+      </c>
+      <c r="Y38">
+        <v>12</v>
+      </c>
+      <c r="Z38">
+        <v>13</v>
+      </c>
+      <c r="AA38">
+        <v>14</v>
+      </c>
+      <c r="AB38">
+        <v>15</v>
+      </c>
+      <c r="AC38">
+        <v>16</v>
+      </c>
+      <c r="AD38">
+        <v>16</v>
+      </c>
+      <c r="AE38">
+        <v>17</v>
+      </c>
+      <c r="AF38">
+        <v>18</v>
+      </c>
+      <c r="AG38">
+        <v>18</v>
+      </c>
+      <c r="AH38">
+        <v>19</v>
+      </c>
+      <c r="AI38">
+        <v>19</v>
+      </c>
+      <c r="AJ38">
+        <v>20</v>
+      </c>
+      <c r="AK38">
+        <v>20</v>
+      </c>
+      <c r="AL38">
+        <v>21</v>
+      </c>
+      <c r="AM38">
+        <v>21</v>
+      </c>
+      <c r="AN38">
+        <v>21</v>
+      </c>
+      <c r="AO38">
+        <v>22</v>
+      </c>
+      <c r="AP38">
+        <v>22</v>
+      </c>
+      <c r="AQ38">
+        <v>22</v>
+      </c>
+      <c r="AR38">
+        <v>23</v>
+      </c>
+      <c r="AS38">
+        <v>23</v>
+      </c>
+      <c r="AT38">
+        <v>23</v>
+      </c>
+      <c r="AU38">
+        <v>24</v>
+      </c>
+      <c r="AV38">
+        <v>24</v>
+      </c>
+      <c r="AW38">
+        <v>24</v>
+      </c>
+      <c r="AX38">
         <v>25</v>
       </c>
-      <c r="W38" s="3">
+      <c r="AY38" s="45">
+        <v>25</v>
+      </c>
+      <c r="AZ38" s="3">
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>50</v>
       </c>
@@ -17448,14 +17610,101 @@
       <c r="U39">
         <v>12</v>
       </c>
-      <c r="V39" s="3">
+      <c r="V39">
+        <v>13</v>
+      </c>
+      <c r="W39">
+        <v>13</v>
+      </c>
+      <c r="X39">
+        <v>14</v>
+      </c>
+      <c r="Y39">
+        <v>14</v>
+      </c>
+      <c r="Z39">
+        <v>15</v>
+      </c>
+      <c r="AA39">
+        <v>15</v>
+      </c>
+      <c r="AB39">
+        <v>16</v>
+      </c>
+      <c r="AC39">
+        <v>16</v>
+      </c>
+      <c r="AD39">
+        <v>17</v>
+      </c>
+      <c r="AE39">
+        <v>17</v>
+      </c>
+      <c r="AF39">
+        <v>18</v>
+      </c>
+      <c r="AG39">
+        <v>19</v>
+      </c>
+      <c r="AH39">
+        <v>19</v>
+      </c>
+      <c r="AI39">
+        <v>20</v>
+      </c>
+      <c r="AJ39">
+        <v>20</v>
+      </c>
+      <c r="AK39">
+        <v>21</v>
+      </c>
+      <c r="AL39">
+        <v>21</v>
+      </c>
+      <c r="AM39">
+        <v>21</v>
+      </c>
+      <c r="AN39">
+        <v>22</v>
+      </c>
+      <c r="AO39">
+        <v>22</v>
+      </c>
+      <c r="AP39">
+        <v>22</v>
+      </c>
+      <c r="AQ39">
+        <v>23</v>
+      </c>
+      <c r="AR39">
+        <v>23</v>
+      </c>
+      <c r="AS39">
+        <v>23</v>
+      </c>
+      <c r="AT39">
+        <v>24</v>
+      </c>
+      <c r="AU39">
+        <v>24</v>
+      </c>
+      <c r="AV39">
+        <v>24</v>
+      </c>
+      <c r="AW39">
         <v>25</v>
       </c>
-      <c r="W39" s="3">
+      <c r="AX39">
+        <v>25</v>
+      </c>
+      <c r="AY39" s="45">
+        <v>25</v>
+      </c>
+      <c r="AZ39" s="3">
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>47</v>
       </c>
@@ -17519,14 +17768,101 @@
       <c r="U40">
         <v>17</v>
       </c>
-      <c r="V40" s="3">
+      <c r="V40">
+        <v>18</v>
+      </c>
+      <c r="W40">
+        <v>19</v>
+      </c>
+      <c r="X40">
+        <v>20</v>
+      </c>
+      <c r="Y40">
+        <v>21</v>
+      </c>
+      <c r="Z40">
+        <v>22</v>
+      </c>
+      <c r="AA40">
+        <v>23</v>
+      </c>
+      <c r="AB40">
+        <v>24</v>
+      </c>
+      <c r="AC40">
+        <v>25</v>
+      </c>
+      <c r="AD40">
+        <v>26</v>
+      </c>
+      <c r="AE40">
+        <v>27</v>
+      </c>
+      <c r="AF40">
+        <v>28</v>
+      </c>
+      <c r="AG40">
+        <v>29</v>
+      </c>
+      <c r="AH40">
+        <v>30</v>
+      </c>
+      <c r="AI40">
+        <v>31</v>
+      </c>
+      <c r="AJ40">
+        <v>32</v>
+      </c>
+      <c r="AK40">
+        <v>33</v>
+      </c>
+      <c r="AL40">
+        <v>34</v>
+      </c>
+      <c r="AM40">
+        <v>35</v>
+      </c>
+      <c r="AN40">
+        <v>36</v>
+      </c>
+      <c r="AO40">
+        <v>37</v>
+      </c>
+      <c r="AP40">
+        <v>38</v>
+      </c>
+      <c r="AQ40">
+        <v>39</v>
+      </c>
+      <c r="AR40">
+        <v>40</v>
+      </c>
+      <c r="AS40">
+        <v>41</v>
+      </c>
+      <c r="AT40">
+        <v>41</v>
+      </c>
+      <c r="AU40">
+        <v>41</v>
+      </c>
+      <c r="AV40">
+        <v>42</v>
+      </c>
+      <c r="AW40">
+        <v>43</v>
+      </c>
+      <c r="AX40">
+        <v>44</v>
+      </c>
+      <c r="AY40" s="45">
         <v>45</v>
       </c>
-      <c r="W40" s="3">
+      <c r="AZ40" s="3">
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -17590,14 +17926,101 @@
       <c r="U41">
         <v>12</v>
       </c>
-      <c r="V41" s="3">
+      <c r="V41">
+        <v>12</v>
+      </c>
+      <c r="W41">
+        <v>13</v>
+      </c>
+      <c r="X41">
+        <v>13</v>
+      </c>
+      <c r="Y41">
+        <v>14</v>
+      </c>
+      <c r="Z41">
+        <v>14</v>
+      </c>
+      <c r="AA41">
+        <v>15</v>
+      </c>
+      <c r="AB41">
+        <v>15</v>
+      </c>
+      <c r="AC41">
+        <v>16</v>
+      </c>
+      <c r="AD41">
+        <v>16</v>
+      </c>
+      <c r="AE41">
+        <v>17</v>
+      </c>
+      <c r="AF41">
+        <v>17</v>
+      </c>
+      <c r="AG41">
+        <v>18</v>
+      </c>
+      <c r="AH41">
+        <v>19</v>
+      </c>
+      <c r="AI41">
+        <v>19</v>
+      </c>
+      <c r="AJ41">
+        <v>20</v>
+      </c>
+      <c r="AK41">
+        <v>20</v>
+      </c>
+      <c r="AL41">
+        <v>20</v>
+      </c>
+      <c r="AM41">
+        <v>21</v>
+      </c>
+      <c r="AN41">
+        <v>21</v>
+      </c>
+      <c r="AO41">
+        <v>21</v>
+      </c>
+      <c r="AP41">
+        <v>22</v>
+      </c>
+      <c r="AQ41">
+        <v>22</v>
+      </c>
+      <c r="AR41">
+        <v>22</v>
+      </c>
+      <c r="AS41">
+        <v>23</v>
+      </c>
+      <c r="AT41">
+        <v>23</v>
+      </c>
+      <c r="AU41">
+        <v>23</v>
+      </c>
+      <c r="AV41">
+        <v>24</v>
+      </c>
+      <c r="AW41">
+        <v>24</v>
+      </c>
+      <c r="AX41">
+        <v>24</v>
+      </c>
+      <c r="AY41" s="45">
         <v>25</v>
       </c>
-      <c r="W41" s="3">
+      <c r="AZ41" s="3">
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>49</v>
       </c>
@@ -17661,14 +18084,101 @@
       <c r="U42">
         <v>18</v>
       </c>
-      <c r="V42" s="3">
+      <c r="V42">
+        <v>19</v>
+      </c>
+      <c r="W42">
+        <v>19</v>
+      </c>
+      <c r="X42">
+        <v>20</v>
+      </c>
+      <c r="Y42">
+        <v>20</v>
+      </c>
+      <c r="Z42">
+        <v>21</v>
+      </c>
+      <c r="AA42">
+        <v>21</v>
+      </c>
+      <c r="AB42">
+        <v>22</v>
+      </c>
+      <c r="AC42">
+        <v>22</v>
+      </c>
+      <c r="AD42">
+        <v>23</v>
+      </c>
+      <c r="AE42">
+        <v>23</v>
+      </c>
+      <c r="AF42">
+        <v>24</v>
+      </c>
+      <c r="AG42">
+        <v>24</v>
+      </c>
+      <c r="AH42">
+        <v>25</v>
+      </c>
+      <c r="AI42">
+        <v>25</v>
+      </c>
+      <c r="AJ42">
+        <v>26</v>
+      </c>
+      <c r="AK42">
+        <v>27</v>
+      </c>
+      <c r="AL42">
+        <v>28</v>
+      </c>
+      <c r="AM42">
+        <v>29</v>
+      </c>
+      <c r="AN42">
+        <v>30</v>
+      </c>
+      <c r="AO42">
+        <v>31</v>
+      </c>
+      <c r="AP42">
+        <v>32</v>
+      </c>
+      <c r="AQ42">
+        <v>33</v>
+      </c>
+      <c r="AR42">
+        <v>34</v>
+      </c>
+      <c r="AS42">
+        <v>35</v>
+      </c>
+      <c r="AT42">
+        <v>36</v>
+      </c>
+      <c r="AU42">
+        <v>37</v>
+      </c>
+      <c r="AV42">
+        <v>38</v>
+      </c>
+      <c r="AW42">
+        <v>39</v>
+      </c>
+      <c r="AX42">
+        <v>39</v>
+      </c>
+      <c r="AY42" s="45">
         <v>40</v>
       </c>
-      <c r="W42" s="3">
+      <c r="AZ42" s="3">
         <v>80</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>46</v>
       </c>
@@ -17732,14 +18242,101 @@
       <c r="U43">
         <v>18</v>
       </c>
-      <c r="V43" s="3">
+      <c r="V43">
+        <v>18</v>
+      </c>
+      <c r="W43">
+        <v>19</v>
+      </c>
+      <c r="X43">
+        <v>19</v>
+      </c>
+      <c r="Y43">
+        <v>20</v>
+      </c>
+      <c r="Z43">
+        <v>20</v>
+      </c>
+      <c r="AA43">
+        <v>21</v>
+      </c>
+      <c r="AB43">
+        <v>21</v>
+      </c>
+      <c r="AC43">
+        <v>22</v>
+      </c>
+      <c r="AD43">
+        <v>22</v>
+      </c>
+      <c r="AE43">
+        <v>23</v>
+      </c>
+      <c r="AF43">
+        <v>23</v>
+      </c>
+      <c r="AG43">
+        <v>24</v>
+      </c>
+      <c r="AH43">
+        <v>24</v>
+      </c>
+      <c r="AI43">
+        <v>25</v>
+      </c>
+      <c r="AJ43">
+        <v>26</v>
+      </c>
+      <c r="AK43">
+        <v>27</v>
+      </c>
+      <c r="AL43">
+        <v>28</v>
+      </c>
+      <c r="AM43">
+        <v>29</v>
+      </c>
+      <c r="AN43">
+        <v>30</v>
+      </c>
+      <c r="AO43">
+        <v>31</v>
+      </c>
+      <c r="AP43">
+        <v>32</v>
+      </c>
+      <c r="AQ43">
+        <v>33</v>
+      </c>
+      <c r="AR43">
+        <v>34</v>
+      </c>
+      <c r="AS43">
+        <v>35</v>
+      </c>
+      <c r="AT43">
+        <v>36</v>
+      </c>
+      <c r="AU43">
+        <v>37</v>
+      </c>
+      <c r="AV43">
+        <v>38</v>
+      </c>
+      <c r="AW43">
+        <v>38</v>
+      </c>
+      <c r="AX43">
+        <v>39</v>
+      </c>
+      <c r="AY43" s="45">
         <v>40</v>
       </c>
-      <c r="W43" s="3">
+      <c r="AZ43" s="3">
         <v>90</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>51</v>
       </c>
@@ -17803,14 +18400,101 @@
       <c r="U44">
         <v>12</v>
       </c>
-      <c r="V44" s="3">
+      <c r="V44">
+        <v>13</v>
+      </c>
+      <c r="W44">
+        <v>14</v>
+      </c>
+      <c r="X44">
+        <v>15</v>
+      </c>
+      <c r="Y44">
+        <v>16</v>
+      </c>
+      <c r="Z44">
+        <v>17</v>
+      </c>
+      <c r="AA44">
+        <v>18</v>
+      </c>
+      <c r="AB44">
+        <v>19</v>
+      </c>
+      <c r="AC44">
+        <v>20</v>
+      </c>
+      <c r="AD44">
+        <v>21</v>
+      </c>
+      <c r="AE44">
+        <v>22</v>
+      </c>
+      <c r="AF44">
+        <v>23</v>
+      </c>
+      <c r="AG44">
+        <v>24</v>
+      </c>
+      <c r="AH44">
+        <v>25</v>
+      </c>
+      <c r="AI44">
+        <v>26</v>
+      </c>
+      <c r="AJ44">
+        <v>26</v>
+      </c>
+      <c r="AK44">
+        <v>27</v>
+      </c>
+      <c r="AL44">
+        <v>28</v>
+      </c>
+      <c r="AM44">
+        <v>29</v>
+      </c>
+      <c r="AN44">
+        <v>30</v>
+      </c>
+      <c r="AO44">
+        <v>31</v>
+      </c>
+      <c r="AP44">
+        <v>32</v>
+      </c>
+      <c r="AQ44">
+        <v>33</v>
+      </c>
+      <c r="AR44">
+        <v>34</v>
+      </c>
+      <c r="AS44">
+        <v>35</v>
+      </c>
+      <c r="AT44">
+        <v>36</v>
+      </c>
+      <c r="AU44">
+        <v>37</v>
+      </c>
+      <c r="AV44">
+        <v>38</v>
+      </c>
+      <c r="AW44">
+        <v>39</v>
+      </c>
+      <c r="AX44">
         <v>40</v>
       </c>
-      <c r="W44" s="3">
+      <c r="AY44" s="45">
+        <v>40</v>
+      </c>
+      <c r="AZ44" s="3">
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A45" s="31" t="s">
         <v>53</v>
       </c>
@@ -17874,14 +18558,101 @@
       <c r="U45" s="31">
         <v>3</v>
       </c>
-      <c r="V45" s="10">
+      <c r="V45" s="31">
+        <v>3</v>
+      </c>
+      <c r="W45" s="31">
+        <v>3</v>
+      </c>
+      <c r="X45" s="31">
+        <v>3</v>
+      </c>
+      <c r="Y45" s="31">
+        <v>3</v>
+      </c>
+      <c r="Z45" s="31">
+        <v>3</v>
+      </c>
+      <c r="AA45" s="31">
+        <v>3</v>
+      </c>
+      <c r="AB45" s="31">
+        <v>3</v>
+      </c>
+      <c r="AC45" s="31">
+        <v>3</v>
+      </c>
+      <c r="AD45" s="31">
+        <v>4</v>
+      </c>
+      <c r="AE45" s="31">
+        <v>4</v>
+      </c>
+      <c r="AF45" s="31">
+        <v>4</v>
+      </c>
+      <c r="AG45" s="31">
+        <v>4</v>
+      </c>
+      <c r="AH45" s="31">
+        <v>4</v>
+      </c>
+      <c r="AI45" s="31">
+        <v>5</v>
+      </c>
+      <c r="AJ45" s="31">
+        <v>5</v>
+      </c>
+      <c r="AK45" s="31">
+        <v>5</v>
+      </c>
+      <c r="AL45" s="31">
+        <v>5</v>
+      </c>
+      <c r="AM45" s="31">
+        <v>5</v>
+      </c>
+      <c r="AN45" s="31">
+        <v>5</v>
+      </c>
+      <c r="AO45" s="31">
+        <v>5</v>
+      </c>
+      <c r="AP45" s="31">
+        <v>5</v>
+      </c>
+      <c r="AQ45" s="31">
+        <v>5</v>
+      </c>
+      <c r="AR45" s="31">
+        <v>5</v>
+      </c>
+      <c r="AS45" s="31">
+        <v>5</v>
+      </c>
+      <c r="AT45" s="31">
+        <v>6</v>
+      </c>
+      <c r="AU45" s="31">
+        <v>7</v>
+      </c>
+      <c r="AV45" s="31">
+        <v>7</v>
+      </c>
+      <c r="AW45" s="31">
+        <v>8</v>
+      </c>
+      <c r="AX45" s="31">
+        <v>9</v>
+      </c>
+      <c r="AY45" s="48">
         <v>10</v>
       </c>
-      <c r="W45" s="10">
+      <c r="AZ45" s="10">
         <v>25</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:52" x14ac:dyDescent="0.3">
       <c r="B46">
         <f>SUM(B38:B45)</f>
         <v>5</v>
@@ -17959,15 +18730,131 @@
         <v>95</v>
       </c>
       <c r="U46">
-        <f t="shared" ref="U46" si="24">SUM(U38:U45)</f>
+        <f t="shared" ref="U46:AX46" si="24">SUM(U38:U45)</f>
         <v>100</v>
       </c>
-      <c r="V46" s="3">
-        <f>SUM(V38:V45)</f>
+      <c r="V46">
+        <f t="shared" si="24"/>
+        <v>105</v>
+      </c>
+      <c r="W46">
+        <f t="shared" si="24"/>
+        <v>110</v>
+      </c>
+      <c r="X46">
+        <f t="shared" si="24"/>
+        <v>115</v>
+      </c>
+      <c r="Y46">
+        <f t="shared" si="24"/>
+        <v>120</v>
+      </c>
+      <c r="Z46">
+        <f t="shared" si="24"/>
+        <v>125</v>
+      </c>
+      <c r="AA46">
+        <f t="shared" si="24"/>
+        <v>130</v>
+      </c>
+      <c r="AB46">
+        <f t="shared" si="24"/>
+        <v>135</v>
+      </c>
+      <c r="AC46">
+        <f t="shared" si="24"/>
+        <v>140</v>
+      </c>
+      <c r="AD46">
+        <f t="shared" si="24"/>
+        <v>145</v>
+      </c>
+      <c r="AE46">
+        <f t="shared" si="24"/>
+        <v>150</v>
+      </c>
+      <c r="AF46">
+        <f t="shared" si="24"/>
+        <v>155</v>
+      </c>
+      <c r="AG46">
+        <f t="shared" si="24"/>
+        <v>160</v>
+      </c>
+      <c r="AH46">
+        <f t="shared" si="24"/>
+        <v>165</v>
+      </c>
+      <c r="AI46">
+        <f t="shared" si="24"/>
+        <v>170</v>
+      </c>
+      <c r="AJ46">
+        <f t="shared" si="24"/>
+        <v>175</v>
+      </c>
+      <c r="AK46">
+        <f t="shared" si="24"/>
+        <v>180</v>
+      </c>
+      <c r="AL46">
+        <f t="shared" si="24"/>
+        <v>185</v>
+      </c>
+      <c r="AM46">
+        <f t="shared" si="24"/>
+        <v>190</v>
+      </c>
+      <c r="AN46">
+        <f t="shared" si="24"/>
+        <v>195</v>
+      </c>
+      <c r="AO46">
+        <f t="shared" si="24"/>
+        <v>200</v>
+      </c>
+      <c r="AP46">
+        <f t="shared" si="24"/>
+        <v>205</v>
+      </c>
+      <c r="AQ46">
+        <f t="shared" si="24"/>
+        <v>210</v>
+      </c>
+      <c r="AR46">
+        <f t="shared" si="24"/>
+        <v>215</v>
+      </c>
+      <c r="AS46">
+        <f t="shared" si="24"/>
+        <v>220</v>
+      </c>
+      <c r="AT46">
+        <f t="shared" si="24"/>
+        <v>225</v>
+      </c>
+      <c r="AU46">
+        <f t="shared" si="24"/>
+        <v>230</v>
+      </c>
+      <c r="AV46">
+        <f t="shared" si="24"/>
+        <v>235</v>
+      </c>
+      <c r="AW46">
+        <f t="shared" si="24"/>
+        <v>240</v>
+      </c>
+      <c r="AX46">
+        <f t="shared" si="24"/>
+        <v>245</v>
+      </c>
+      <c r="AY46" s="45">
+        <f>SUM(AY38:AY45)</f>
         <v>250</v>
       </c>
-      <c r="W46" s="3">
-        <f>SUM(W38:W45)</f>
+      <c r="AZ46" s="3">
+        <f>SUM(AZ38:AZ45)</f>
         <v>500</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Introduce new SORCERER castes: - WITCHMASTER - AVATAR Sorcerer development path in the endurance test goes to AVATAR level now. Introduce new caste group (CLERIC) and caste (MONK). ClericEnduranceTest goes from ROGUE to MONK and further. Add the god GINDON to calculation tests. New NYMPH calculation test (sorcerer path instead of warrior).
</commit_message>
<xml_diff>
--- a/doc/caste_system.xlsx
+++ b/doc/caste_system.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/349dfb9748b30a92/Asztali gép/ataliasflame_2.0/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5854" documentId="8_{652F4476-B36F-42CD-831D-0D71B9923ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{114D89D3-C84B-4368-A896-4BC38E51C466}"/>
+  <xr:revisionPtr revIDLastSave="6478" documentId="8_{652F4476-B36F-42CD-831D-0D71B9923ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B4899D2-F2EA-4847-BEDB-4E3974DC746D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{CAF51EC3-63EC-48CD-AA7B-C21B3D5D222B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{CAF51EC3-63EC-48CD-AA7B-C21B3D5D222B}"/>
   </bookViews>
   <sheets>
     <sheet name="caste list" sheetId="1" r:id="rId1"/>
@@ -1557,7 +1557,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1246" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1325" uniqueCount="85">
   <si>
     <t>csavargó</t>
   </si>
@@ -2012,7 +2012,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2067,9 +2067,6 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2080,16 +2077,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2413,7 +2426,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E471BE-CB76-416C-8A0D-8BCD59B0033A}">
   <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P20" activeCellId="1" sqref="R20 P20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2545,7 +2560,7 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="37" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="28" t="s">
@@ -2601,7 +2616,7 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="39"/>
+      <c r="A4" s="38"/>
       <c r="B4" s="28" t="s">
         <v>2</v>
       </c>
@@ -2655,61 +2670,61 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="39"/>
-      <c r="B5" s="26" t="s">
+      <c r="A5" s="38"/>
+      <c r="B5" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="3" t="s">
+      <c r="C5" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="K5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q5" s="3" t="s">
+      <c r="K5" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="M5" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="N5" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="O5" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="P5" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q5" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="R5" s="2" t="s">
+      <c r="R5" s="43" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="39"/>
+      <c r="A6" s="38"/>
       <c r="B6" s="26" t="s">
         <v>21</v>
       </c>
@@ -2763,61 +2778,61 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="40"/>
-      <c r="B7" s="27" t="s">
+      <c r="A7" s="39"/>
+      <c r="B7" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="3" t="s">
+      <c r="C7" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="K7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="P7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q7" s="3" t="s">
+      <c r="K7" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="L7" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="M7" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="N7" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="O7" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="P7" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q7" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="R7" s="2" t="s">
+      <c r="R7" s="43" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="37" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="28" t="s">
@@ -2873,7 +2888,7 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="39"/>
+      <c r="A9" s="38"/>
       <c r="B9" s="28" t="s">
         <v>6</v>
       </c>
@@ -2927,7 +2942,7 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="39"/>
+      <c r="A10" s="38"/>
       <c r="B10" s="28" t="s">
         <v>7</v>
       </c>
@@ -2981,7 +2996,7 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="40"/>
+      <c r="A11" s="39"/>
       <c r="B11" s="25" t="s">
         <v>8</v>
       </c>
@@ -3035,7 +3050,7 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="37" t="s">
         <v>79</v>
       </c>
       <c r="B12" s="28" t="s">
@@ -3091,7 +3106,7 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="39"/>
+      <c r="A13" s="38"/>
       <c r="B13" s="26" t="s">
         <v>10</v>
       </c>
@@ -3145,7 +3160,7 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="39"/>
+      <c r="A14" s="38"/>
       <c r="B14" s="26" t="s">
         <v>11</v>
       </c>
@@ -3199,7 +3214,7 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="40"/>
+      <c r="A15" s="39"/>
       <c r="B15" s="27" t="s">
         <v>12</v>
       </c>
@@ -3253,7 +3268,7 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="37" t="s">
         <v>80</v>
       </c>
       <c r="B16" s="28" t="s">
@@ -3309,7 +3324,7 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="39"/>
+      <c r="A17" s="38"/>
       <c r="B17" s="28" t="s">
         <v>14</v>
       </c>
@@ -3363,7 +3378,7 @@
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" s="39"/>
+      <c r="A18" s="38"/>
       <c r="B18" s="28" t="s">
         <v>15</v>
       </c>
@@ -3417,7 +3432,7 @@
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" s="40"/>
+      <c r="A19" s="39"/>
       <c r="B19" s="27" t="s">
         <v>16</v>
       </c>
@@ -3471,63 +3486,63 @@
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="41" t="s">
+      <c r="A20" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I20" s="3" t="s">
+      <c r="C20" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="G20" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="H20" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="I20" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="J20" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="K20" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M20" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="N20" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="O20" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="P20" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q20" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="R20" s="2" t="s">
+      <c r="J20" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="K20" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="L20" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="M20" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="N20" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="O20" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="P20" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q20" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="R20" s="43" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21" s="42"/>
+      <c r="A21" s="48"/>
       <c r="B21" s="26" t="s">
         <v>18</v>
       </c>
@@ -3581,7 +3596,7 @@
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22" s="42"/>
+      <c r="A22" s="48"/>
       <c r="B22" s="26" t="s">
         <v>19</v>
       </c>
@@ -3635,7 +3650,7 @@
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23" s="43"/>
+      <c r="A23" s="49"/>
       <c r="B23" s="27" t="s">
         <v>20</v>
       </c>
@@ -3706,7 +3721,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D679E03F-D306-402E-AB27-0886D4533EB3}">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4321,7 +4338,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45FC8AA8-DC1F-4C97-8335-A619D1FCDEA7}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4576,7 +4595,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47799533-6B34-4949-9561-D6B03DB6E4FC}">
   <dimension ref="A1:AC10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2:AB9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4589,9 +4610,9 @@
     <col min="7" max="7" width="8.21875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16" style="41" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.21875" style="41" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="6.44140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.44140625" bestFit="1" customWidth="1"/>
@@ -4604,7 +4625,7 @@
     <col min="22" max="22" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.44140625" style="41" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="4" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="5.77734375" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="8.77734375" bestFit="1" customWidth="1"/>
@@ -4637,13 +4658,13 @@
       <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="41" t="s">
         <v>3</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="43" t="s">
         <v>4</v>
       </c>
       <c r="M1" t="s">
@@ -4682,7 +4703,7 @@
       <c r="X1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Y1" s="41" t="s">
         <v>17</v>
       </c>
       <c r="Z1" s="3" t="s">
@@ -4726,13 +4747,13 @@
       <c r="I2">
         <v>6</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="41">
         <v>18</v>
       </c>
       <c r="K2" s="3">
         <v>20</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="43">
         <v>40</v>
       </c>
       <c r="M2">
@@ -4771,7 +4792,7 @@
       <c r="X2" s="2">
         <v>45</v>
       </c>
-      <c r="Y2" s="3">
+      <c r="Y2" s="41">
         <v>3</v>
       </c>
       <c r="Z2" s="3">
@@ -4816,13 +4837,13 @@
       <c r="I3">
         <v>12</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="41">
         <v>25</v>
       </c>
       <c r="K3" s="3">
         <v>30</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="43">
         <v>45</v>
       </c>
       <c r="M3">
@@ -4861,7 +4882,7 @@
       <c r="X3" s="2">
         <v>50</v>
       </c>
-      <c r="Y3" s="3">
+      <c r="Y3" s="41">
         <v>3</v>
       </c>
       <c r="Z3" s="3">
@@ -4906,13 +4927,13 @@
       <c r="I4">
         <v>7</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="41">
         <v>20</v>
       </c>
       <c r="K4" s="3">
         <v>25</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="43">
         <v>45</v>
       </c>
       <c r="M4">
@@ -4951,7 +4972,7 @@
       <c r="X4" s="2">
         <v>70</v>
       </c>
-      <c r="Y4" s="3">
+      <c r="Y4" s="41">
         <v>2</v>
       </c>
       <c r="Z4" s="3">
@@ -4996,13 +5017,13 @@
       <c r="I5">
         <v>10</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="41">
         <v>22</v>
       </c>
       <c r="K5" s="3">
         <v>25</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="43">
         <v>45</v>
       </c>
       <c r="M5">
@@ -5041,7 +5062,7 @@
       <c r="X5" s="2">
         <v>50</v>
       </c>
-      <c r="Y5" s="3">
+      <c r="Y5" s="41">
         <v>3</v>
       </c>
       <c r="Z5" s="3">
@@ -5086,13 +5107,13 @@
       <c r="I6">
         <v>20</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="41">
         <v>50</v>
       </c>
       <c r="K6" s="3">
         <v>40</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6" s="43">
         <v>100</v>
       </c>
       <c r="M6">
@@ -5131,7 +5152,7 @@
       <c r="X6" s="2">
         <v>80</v>
       </c>
-      <c r="Y6" s="3">
+      <c r="Y6" s="41">
         <v>4</v>
       </c>
       <c r="Z6" s="3">
@@ -5176,13 +5197,13 @@
       <c r="I7">
         <v>20</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="41">
         <v>50</v>
       </c>
       <c r="K7" s="3">
         <v>60</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7" s="43">
         <v>100</v>
       </c>
       <c r="M7">
@@ -5221,7 +5242,7 @@
       <c r="X7" s="2">
         <v>90</v>
       </c>
-      <c r="Y7" s="3">
+      <c r="Y7" s="41">
         <v>5</v>
       </c>
       <c r="Z7" s="3">
@@ -5266,13 +5287,13 @@
       <c r="I8">
         <v>20</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="41">
         <v>50</v>
       </c>
       <c r="K8" s="3">
         <v>30</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L8" s="43">
         <v>100</v>
       </c>
       <c r="M8">
@@ -5311,7 +5332,7 @@
       <c r="X8" s="2">
         <v>90</v>
       </c>
-      <c r="Y8" s="3">
+      <c r="Y8" s="41">
         <v>4</v>
       </c>
       <c r="Z8" s="3">
@@ -5356,13 +5377,13 @@
       <c r="I9" s="30">
         <v>5</v>
       </c>
-      <c r="J9" s="10">
+      <c r="J9" s="42">
         <v>15</v>
       </c>
       <c r="K9" s="10">
         <v>20</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L9" s="46">
         <v>25</v>
       </c>
       <c r="M9" s="30">
@@ -5401,7 +5422,7 @@
       <c r="X9" s="4">
         <v>25</v>
       </c>
-      <c r="Y9" s="10">
+      <c r="Y9" s="42">
         <v>1</v>
       </c>
       <c r="Z9" s="10">
@@ -5413,7 +5434,7 @@
       <c r="AB9" s="4">
         <v>25</v>
       </c>
-      <c r="AC9" s="37">
+      <c r="AC9" s="36">
         <f>MAX(G9:AB9)</f>
         <v>100</v>
       </c>
@@ -5431,7 +5452,7 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="41">
         <f t="shared" si="1"/>
         <v>250</v>
       </c>
@@ -5439,7 +5460,7 @@
         <f t="shared" si="1"/>
         <v>250</v>
       </c>
-      <c r="L10" s="1">
+      <c r="L10" s="43">
         <f t="shared" si="1"/>
         <v>500</v>
       </c>
@@ -5491,7 +5512,7 @@
         <f t="shared" ref="X10" si="13">SUM(X2:X9)</f>
         <v>500</v>
       </c>
-      <c r="Y10">
+      <c r="Y10" s="41">
         <f t="shared" ref="Y10" si="14">SUM(Y2:Y9)</f>
         <v>25</v>
       </c>
@@ -6735,54 +6756,54 @@
       <c r="U1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="W1" s="44" t="s">
+      <c r="W1" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="X1" s="44"/>
-      <c r="Y1" s="44"/>
-      <c r="Z1" s="44"/>
-      <c r="AA1" s="44"/>
-      <c r="AB1" s="44"/>
-      <c r="AD1" s="44" t="s">
+      <c r="X1" s="40"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40"/>
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="40"/>
+      <c r="AD1" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="AE1" s="44"/>
-      <c r="AF1" s="44"/>
-      <c r="AG1" s="44"/>
-      <c r="AH1" s="44"/>
-      <c r="AI1" s="44"/>
-      <c r="AK1" s="44" t="s">
+      <c r="AE1" s="40"/>
+      <c r="AF1" s="40"/>
+      <c r="AG1" s="40"/>
+      <c r="AH1" s="40"/>
+      <c r="AI1" s="40"/>
+      <c r="AK1" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="AL1" s="44"/>
-      <c r="AM1" s="44"/>
-      <c r="AN1" s="44"/>
-      <c r="AO1" s="44"/>
-      <c r="AP1" s="44"/>
-      <c r="AR1" s="44" t="s">
+      <c r="AL1" s="40"/>
+      <c r="AM1" s="40"/>
+      <c r="AN1" s="40"/>
+      <c r="AO1" s="40"/>
+      <c r="AP1" s="40"/>
+      <c r="AR1" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="AS1" s="44"/>
-      <c r="AT1" s="44"/>
-      <c r="AU1" s="44"/>
-      <c r="AV1" s="44"/>
-      <c r="AW1" s="44"/>
-      <c r="AY1" s="44" t="s">
+      <c r="AS1" s="40"/>
+      <c r="AT1" s="40"/>
+      <c r="AU1" s="40"/>
+      <c r="AV1" s="40"/>
+      <c r="AW1" s="40"/>
+      <c r="AY1" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="AZ1" s="44"/>
-      <c r="BA1" s="44"/>
-      <c r="BB1" s="44"/>
-      <c r="BC1" s="44"/>
-      <c r="BD1" s="44"/>
-      <c r="BF1" s="44" t="s">
+      <c r="AZ1" s="40"/>
+      <c r="BA1" s="40"/>
+      <c r="BB1" s="40"/>
+      <c r="BC1" s="40"/>
+      <c r="BD1" s="40"/>
+      <c r="BF1" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="BG1" s="44"/>
-      <c r="BH1" s="44"/>
-      <c r="BI1" s="44"/>
-      <c r="BJ1" s="44"/>
-      <c r="BK1" s="44"/>
+      <c r="BG1" s="40"/>
+      <c r="BH1" s="40"/>
+      <c r="BI1" s="40"/>
+      <c r="BJ1" s="40"/>
+      <c r="BK1" s="40"/>
     </row>
     <row r="2" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
@@ -11698,10 +11719,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD573711-C846-40DC-8629-19A685998D3E}">
-  <dimension ref="A1:CW46"/>
+  <dimension ref="A1:DK58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="CK36" sqref="CK36"/>
+    <sheetView tabSelected="1" topLeftCell="CD22" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11717,13 +11738,14 @@
     <col min="24" max="47" width="4" bestFit="1" customWidth="1"/>
     <col min="48" max="50" width="4" customWidth="1"/>
     <col min="51" max="51" width="16" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="54" max="100" width="4" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="52" max="55" width="4" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="4" customWidth="1"/>
+    <col min="57" max="100" width="4" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="10.5546875" style="41" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="7.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:102" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -11871,17 +11893,164 @@
       <c r="AX1" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="AY1" s="3" t="s">
+      <c r="AY1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="AZ1" s="36" t="s">
+      <c r="AZ1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="BA1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="BB1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="BC1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="BD1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="BE1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="BF1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="BG1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="BH1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="BI1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="BJ1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="BK1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="BL1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="BM1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="BN1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="BO1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="BP1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="BQ1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="BR1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="BS1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="BT1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="BU1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="BV1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="BW1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="BX1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="BY1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="BZ1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="CA1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="CB1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="CC1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="CD1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="CE1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="CF1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="CG1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="CH1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="CI1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="CJ1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="CK1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="CL1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="CM1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="CN1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="CO1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="CP1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="CQ1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="CR1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="CS1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="CT1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="CU1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="CV1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="CW1" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="BA1" s="3" t="s">
+      <c r="CX1" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>48</v>
       </c>
@@ -12035,11 +12204,158 @@
       <c r="AY2">
         <v>18</v>
       </c>
-      <c r="AZ2" s="3">
+      <c r="AZ2">
+        <v>19</v>
+      </c>
+      <c r="BA2">
+        <v>20</v>
+      </c>
+      <c r="BB2">
+        <v>20</v>
+      </c>
+      <c r="BC2">
+        <v>21</v>
+      </c>
+      <c r="BD2">
+        <v>21</v>
+      </c>
+      <c r="BE2">
+        <v>22</v>
+      </c>
+      <c r="BF2">
+        <v>22</v>
+      </c>
+      <c r="BG2">
+        <v>23</v>
+      </c>
+      <c r="BH2">
+        <v>23</v>
+      </c>
+      <c r="BI2">
+        <v>24</v>
+      </c>
+      <c r="BJ2">
+        <v>25</v>
+      </c>
+      <c r="BK2">
+        <v>25</v>
+      </c>
+      <c r="BL2">
+        <v>25</v>
+      </c>
+      <c r="BM2">
+        <v>26</v>
+      </c>
+      <c r="BN2">
+        <v>26</v>
+      </c>
+      <c r="BO2">
+        <v>26</v>
+      </c>
+      <c r="BP2">
+        <v>27</v>
+      </c>
+      <c r="BQ2">
+        <v>28</v>
+      </c>
+      <c r="BR2">
+        <v>28</v>
+      </c>
+      <c r="BS2">
+        <v>29</v>
+      </c>
+      <c r="BT2">
+        <v>29</v>
+      </c>
+      <c r="BU2">
+        <v>30</v>
+      </c>
+      <c r="BV2">
+        <v>30</v>
+      </c>
+      <c r="BW2">
+        <v>31</v>
+      </c>
+      <c r="BX2">
+        <v>31</v>
+      </c>
+      <c r="BY2">
+        <v>31</v>
+      </c>
+      <c r="BZ2">
+        <v>32</v>
+      </c>
+      <c r="CA2">
+        <v>32</v>
+      </c>
+      <c r="CB2">
+        <v>33</v>
+      </c>
+      <c r="CC2">
+        <v>34</v>
+      </c>
+      <c r="CD2">
+        <v>35</v>
+      </c>
+      <c r="CE2">
+        <v>35</v>
+      </c>
+      <c r="CF2">
+        <v>35</v>
+      </c>
+      <c r="CG2">
+        <v>36</v>
+      </c>
+      <c r="CH2">
+        <v>36</v>
+      </c>
+      <c r="CI2">
+        <v>36</v>
+      </c>
+      <c r="CJ2">
+        <v>36</v>
+      </c>
+      <c r="CK2">
+        <v>37</v>
+      </c>
+      <c r="CL2">
+        <v>37</v>
+      </c>
+      <c r="CM2">
+        <v>37</v>
+      </c>
+      <c r="CN2">
+        <v>38</v>
+      </c>
+      <c r="CO2">
+        <v>39</v>
+      </c>
+      <c r="CP2">
+        <v>39</v>
+      </c>
+      <c r="CQ2">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:101" x14ac:dyDescent="0.3">
+      <c r="CR2">
+        <v>40</v>
+      </c>
+      <c r="CS2">
+        <v>40</v>
+      </c>
+      <c r="CT2">
+        <v>40</v>
+      </c>
+      <c r="CU2">
+        <v>40</v>
+      </c>
+      <c r="CV2">
+        <v>40</v>
+      </c>
+      <c r="CW2" s="41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -12193,11 +12509,158 @@
       <c r="AY3">
         <v>25</v>
       </c>
-      <c r="AZ3" s="3">
+      <c r="AZ3">
+        <v>25</v>
+      </c>
+      <c r="BA3">
+        <v>25</v>
+      </c>
+      <c r="BB3">
+        <v>25</v>
+      </c>
+      <c r="BC3">
+        <v>25</v>
+      </c>
+      <c r="BD3">
+        <v>25</v>
+      </c>
+      <c r="BE3">
+        <v>26</v>
+      </c>
+      <c r="BF3">
+        <v>26</v>
+      </c>
+      <c r="BG3">
+        <v>27</v>
+      </c>
+      <c r="BH3">
+        <v>27</v>
+      </c>
+      <c r="BI3">
+        <v>27</v>
+      </c>
+      <c r="BJ3">
+        <v>27</v>
+      </c>
+      <c r="BK3">
+        <v>28</v>
+      </c>
+      <c r="BL3">
+        <v>29</v>
+      </c>
+      <c r="BM3">
+        <v>29</v>
+      </c>
+      <c r="BN3">
+        <v>29</v>
+      </c>
+      <c r="BO3">
+        <v>30</v>
+      </c>
+      <c r="BP3">
+        <v>30</v>
+      </c>
+      <c r="BQ3">
+        <v>31</v>
+      </c>
+      <c r="BR3">
+        <v>31</v>
+      </c>
+      <c r="BS3">
+        <v>31</v>
+      </c>
+      <c r="BT3">
+        <v>32</v>
+      </c>
+      <c r="BU3">
+        <v>32</v>
+      </c>
+      <c r="BV3">
+        <v>33</v>
+      </c>
+      <c r="BW3">
+        <v>33</v>
+      </c>
+      <c r="BX3">
+        <v>33</v>
+      </c>
+      <c r="BY3">
+        <v>34</v>
+      </c>
+      <c r="BZ3">
+        <v>34</v>
+      </c>
+      <c r="CA3">
+        <v>35</v>
+      </c>
+      <c r="CB3">
+        <v>35</v>
+      </c>
+      <c r="CC3">
+        <v>35</v>
+      </c>
+      <c r="CD3">
+        <v>35</v>
+      </c>
+      <c r="CE3">
+        <v>36</v>
+      </c>
+      <c r="CF3">
+        <v>37</v>
+      </c>
+      <c r="CG3">
+        <v>37</v>
+      </c>
+      <c r="CH3">
+        <v>37</v>
+      </c>
+      <c r="CI3">
+        <v>38</v>
+      </c>
+      <c r="CJ3">
+        <v>39</v>
+      </c>
+      <c r="CK3">
+        <v>39</v>
+      </c>
+      <c r="CL3">
+        <v>40</v>
+      </c>
+      <c r="CM3">
+        <v>40</v>
+      </c>
+      <c r="CN3">
+        <v>40</v>
+      </c>
+      <c r="CO3">
+        <v>41</v>
+      </c>
+      <c r="CP3">
+        <v>41</v>
+      </c>
+      <c r="CQ3">
+        <v>42</v>
+      </c>
+      <c r="CR3">
+        <v>42</v>
+      </c>
+      <c r="CS3">
+        <v>43</v>
+      </c>
+      <c r="CT3">
+        <v>43</v>
+      </c>
+      <c r="CU3">
+        <v>44</v>
+      </c>
+      <c r="CV3">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="1:101" x14ac:dyDescent="0.3">
+      <c r="CW3" s="41">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -12351,11 +12814,158 @@
       <c r="AY4">
         <v>20</v>
       </c>
-      <c r="AZ4" s="3">
+      <c r="AZ4">
+        <v>21</v>
+      </c>
+      <c r="BA4">
+        <v>21</v>
+      </c>
+      <c r="BB4">
+        <v>22</v>
+      </c>
+      <c r="BC4">
+        <v>22</v>
+      </c>
+      <c r="BD4">
+        <v>23</v>
+      </c>
+      <c r="BE4">
+        <v>23</v>
+      </c>
+      <c r="BF4">
+        <v>24</v>
+      </c>
+      <c r="BG4">
+        <v>24</v>
+      </c>
+      <c r="BH4">
+        <v>25</v>
+      </c>
+      <c r="BI4">
+        <v>25</v>
+      </c>
+      <c r="BJ4">
+        <v>26</v>
+      </c>
+      <c r="BK4">
+        <v>26</v>
+      </c>
+      <c r="BL4">
+        <v>27</v>
+      </c>
+      <c r="BM4">
+        <v>27</v>
+      </c>
+      <c r="BN4">
+        <v>28</v>
+      </c>
+      <c r="BO4">
+        <v>28</v>
+      </c>
+      <c r="BP4">
+        <v>29</v>
+      </c>
+      <c r="BQ4">
+        <v>29</v>
+      </c>
+      <c r="BR4">
+        <v>30</v>
+      </c>
+      <c r="BS4">
+        <v>30</v>
+      </c>
+      <c r="BT4">
+        <v>31</v>
+      </c>
+      <c r="BU4">
+        <v>31</v>
+      </c>
+      <c r="BV4">
+        <v>32</v>
+      </c>
+      <c r="BW4">
+        <v>32</v>
+      </c>
+      <c r="BX4">
+        <v>33</v>
+      </c>
+      <c r="BY4">
+        <v>33</v>
+      </c>
+      <c r="BZ4">
+        <v>34</v>
+      </c>
+      <c r="CA4">
+        <v>34</v>
+      </c>
+      <c r="CB4">
+        <v>35</v>
+      </c>
+      <c r="CC4">
+        <v>35</v>
+      </c>
+      <c r="CD4">
+        <v>36</v>
+      </c>
+      <c r="CE4">
+        <v>36</v>
+      </c>
+      <c r="CF4">
+        <v>37</v>
+      </c>
+      <c r="CG4">
+        <v>37</v>
+      </c>
+      <c r="CH4">
+        <v>38</v>
+      </c>
+      <c r="CI4">
+        <v>38</v>
+      </c>
+      <c r="CJ4">
+        <v>39</v>
+      </c>
+      <c r="CK4">
+        <v>39</v>
+      </c>
+      <c r="CL4">
+        <v>40</v>
+      </c>
+      <c r="CM4">
+        <v>40</v>
+      </c>
+      <c r="CN4">
+        <v>41</v>
+      </c>
+      <c r="CO4">
+        <v>41</v>
+      </c>
+      <c r="CP4">
+        <v>42</v>
+      </c>
+      <c r="CQ4">
+        <v>42</v>
+      </c>
+      <c r="CR4">
+        <v>43</v>
+      </c>
+      <c r="CS4">
+        <v>43</v>
+      </c>
+      <c r="CT4">
+        <v>44</v>
+      </c>
+      <c r="CU4">
+        <v>44</v>
+      </c>
+      <c r="CV4">
         <v>45</v>
       </c>
-    </row>
-    <row r="5" spans="1:101" x14ac:dyDescent="0.3">
+      <c r="CW4" s="41">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -12509,11 +13119,158 @@
       <c r="AY5">
         <v>22</v>
       </c>
-      <c r="AZ5" s="3">
+      <c r="AZ5">
+        <v>22</v>
+      </c>
+      <c r="BA5">
+        <v>23</v>
+      </c>
+      <c r="BB5">
+        <v>24</v>
+      </c>
+      <c r="BC5">
+        <v>25</v>
+      </c>
+      <c r="BD5">
+        <v>25</v>
+      </c>
+      <c r="BE5">
+        <v>25</v>
+      </c>
+      <c r="BF5">
+        <v>26</v>
+      </c>
+      <c r="BG5">
+        <v>26</v>
+      </c>
+      <c r="BH5">
+        <v>27</v>
+      </c>
+      <c r="BI5">
+        <v>27</v>
+      </c>
+      <c r="BJ5">
+        <v>27</v>
+      </c>
+      <c r="BK5">
+        <v>28</v>
+      </c>
+      <c r="BL5">
+        <v>28</v>
+      </c>
+      <c r="BM5">
+        <v>29</v>
+      </c>
+      <c r="BN5">
+        <v>29</v>
+      </c>
+      <c r="BO5">
+        <v>30</v>
+      </c>
+      <c r="BP5">
+        <v>30</v>
+      </c>
+      <c r="BQ5">
+        <v>30</v>
+      </c>
+      <c r="BR5">
+        <v>31</v>
+      </c>
+      <c r="BS5">
+        <v>31</v>
+      </c>
+      <c r="BT5">
+        <v>31</v>
+      </c>
+      <c r="BU5">
+        <v>32</v>
+      </c>
+      <c r="BV5">
+        <v>32</v>
+      </c>
+      <c r="BW5">
+        <v>33</v>
+      </c>
+      <c r="BX5">
+        <v>33</v>
+      </c>
+      <c r="BY5">
+        <v>34</v>
+      </c>
+      <c r="BZ5">
+        <v>34</v>
+      </c>
+      <c r="CA5">
+        <v>35</v>
+      </c>
+      <c r="CB5">
+        <v>35</v>
+      </c>
+      <c r="CC5">
+        <v>35</v>
+      </c>
+      <c r="CD5">
+        <v>35</v>
+      </c>
+      <c r="CE5">
+        <v>36</v>
+      </c>
+      <c r="CF5">
+        <v>36</v>
+      </c>
+      <c r="CG5">
+        <v>37</v>
+      </c>
+      <c r="CH5">
+        <v>37</v>
+      </c>
+      <c r="CI5">
+        <v>38</v>
+      </c>
+      <c r="CJ5">
+        <v>38</v>
+      </c>
+      <c r="CK5">
+        <v>39</v>
+      </c>
+      <c r="CL5">
+        <v>39</v>
+      </c>
+      <c r="CM5">
+        <v>40</v>
+      </c>
+      <c r="CN5">
+        <v>40</v>
+      </c>
+      <c r="CO5">
+        <v>40</v>
+      </c>
+      <c r="CP5">
+        <v>41</v>
+      </c>
+      <c r="CQ5">
+        <v>41</v>
+      </c>
+      <c r="CR5">
+        <v>41</v>
+      </c>
+      <c r="CS5">
+        <v>42</v>
+      </c>
+      <c r="CT5">
+        <v>43</v>
+      </c>
+      <c r="CU5">
+        <v>44</v>
+      </c>
+      <c r="CV5">
+        <v>44</v>
+      </c>
+      <c r="CW5" s="41">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -12667,11 +13424,158 @@
       <c r="AY6">
         <v>50</v>
       </c>
-      <c r="AZ6" s="3">
+      <c r="AZ6">
+        <v>51</v>
+      </c>
+      <c r="BA6">
+        <v>52</v>
+      </c>
+      <c r="BB6">
+        <v>53</v>
+      </c>
+      <c r="BC6">
+        <v>54</v>
+      </c>
+      <c r="BD6">
+        <v>55</v>
+      </c>
+      <c r="BE6">
+        <v>56</v>
+      </c>
+      <c r="BF6">
+        <v>57</v>
+      </c>
+      <c r="BG6">
+        <v>58</v>
+      </c>
+      <c r="BH6">
+        <v>59</v>
+      </c>
+      <c r="BI6">
+        <v>60</v>
+      </c>
+      <c r="BJ6">
+        <v>61</v>
+      </c>
+      <c r="BK6">
+        <v>62</v>
+      </c>
+      <c r="BL6">
+        <v>63</v>
+      </c>
+      <c r="BM6">
+        <v>64</v>
+      </c>
+      <c r="BN6">
+        <v>65</v>
+      </c>
+      <c r="BO6">
+        <v>66</v>
+      </c>
+      <c r="BP6">
+        <v>67</v>
+      </c>
+      <c r="BQ6">
+        <v>68</v>
+      </c>
+      <c r="BR6">
+        <v>69</v>
+      </c>
+      <c r="BS6">
+        <v>70</v>
+      </c>
+      <c r="BT6">
+        <v>71</v>
+      </c>
+      <c r="BU6">
+        <v>72</v>
+      </c>
+      <c r="BV6">
+        <v>73</v>
+      </c>
+      <c r="BW6">
+        <v>74</v>
+      </c>
+      <c r="BX6">
+        <v>75</v>
+      </c>
+      <c r="BY6">
+        <v>76</v>
+      </c>
+      <c r="BZ6">
+        <v>77</v>
+      </c>
+      <c r="CA6">
+        <v>78</v>
+      </c>
+      <c r="CB6">
+        <v>79</v>
+      </c>
+      <c r="CC6">
+        <v>80</v>
+      </c>
+      <c r="CD6">
+        <v>81</v>
+      </c>
+      <c r="CE6">
+        <v>82</v>
+      </c>
+      <c r="CF6">
+        <v>83</v>
+      </c>
+      <c r="CG6">
+        <v>84</v>
+      </c>
+      <c r="CH6">
+        <v>85</v>
+      </c>
+      <c r="CI6">
+        <v>86</v>
+      </c>
+      <c r="CJ6">
+        <v>87</v>
+      </c>
+      <c r="CK6">
+        <v>88</v>
+      </c>
+      <c r="CL6">
+        <v>89</v>
+      </c>
+      <c r="CM6">
+        <v>90</v>
+      </c>
+      <c r="CN6">
+        <v>91</v>
+      </c>
+      <c r="CO6">
+        <v>92</v>
+      </c>
+      <c r="CP6">
+        <v>93</v>
+      </c>
+      <c r="CQ6">
+        <v>94</v>
+      </c>
+      <c r="CR6">
+        <v>95</v>
+      </c>
+      <c r="CS6">
+        <v>96</v>
+      </c>
+      <c r="CT6">
+        <v>97</v>
+      </c>
+      <c r="CU6">
+        <v>98</v>
+      </c>
+      <c r="CV6">
+        <v>99</v>
+      </c>
+      <c r="CW6" s="41">
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -12825,11 +13729,158 @@
       <c r="AY7">
         <v>50</v>
       </c>
-      <c r="AZ7" s="3">
+      <c r="AZ7">
+        <v>51</v>
+      </c>
+      <c r="BA7">
+        <v>52</v>
+      </c>
+      <c r="BB7">
+        <v>53</v>
+      </c>
+      <c r="BC7">
+        <v>54</v>
+      </c>
+      <c r="BD7">
+        <v>55</v>
+      </c>
+      <c r="BE7">
+        <v>56</v>
+      </c>
+      <c r="BF7">
+        <v>57</v>
+      </c>
+      <c r="BG7">
+        <v>58</v>
+      </c>
+      <c r="BH7">
+        <v>59</v>
+      </c>
+      <c r="BI7">
+        <v>60</v>
+      </c>
+      <c r="BJ7">
+        <v>61</v>
+      </c>
+      <c r="BK7">
+        <v>62</v>
+      </c>
+      <c r="BL7">
+        <v>63</v>
+      </c>
+      <c r="BM7">
+        <v>64</v>
+      </c>
+      <c r="BN7">
+        <v>65</v>
+      </c>
+      <c r="BO7">
+        <v>66</v>
+      </c>
+      <c r="BP7">
+        <v>67</v>
+      </c>
+      <c r="BQ7">
+        <v>68</v>
+      </c>
+      <c r="BR7">
+        <v>69</v>
+      </c>
+      <c r="BS7">
+        <v>70</v>
+      </c>
+      <c r="BT7">
+        <v>71</v>
+      </c>
+      <c r="BU7">
+        <v>72</v>
+      </c>
+      <c r="BV7">
+        <v>73</v>
+      </c>
+      <c r="BW7">
+        <v>74</v>
+      </c>
+      <c r="BX7">
+        <v>75</v>
+      </c>
+      <c r="BY7">
+        <v>76</v>
+      </c>
+      <c r="BZ7">
+        <v>77</v>
+      </c>
+      <c r="CA7">
+        <v>78</v>
+      </c>
+      <c r="CB7">
+        <v>79</v>
+      </c>
+      <c r="CC7">
+        <v>80</v>
+      </c>
+      <c r="CD7">
+        <v>81</v>
+      </c>
+      <c r="CE7">
+        <v>82</v>
+      </c>
+      <c r="CF7">
+        <v>83</v>
+      </c>
+      <c r="CG7">
+        <v>84</v>
+      </c>
+      <c r="CH7">
+        <v>85</v>
+      </c>
+      <c r="CI7">
+        <v>86</v>
+      </c>
+      <c r="CJ7">
+        <v>87</v>
+      </c>
+      <c r="CK7">
+        <v>88</v>
+      </c>
+      <c r="CL7">
+        <v>89</v>
+      </c>
+      <c r="CM7">
+        <v>90</v>
+      </c>
+      <c r="CN7">
+        <v>91</v>
+      </c>
+      <c r="CO7">
+        <v>92</v>
+      </c>
+      <c r="CP7">
+        <v>93</v>
+      </c>
+      <c r="CQ7">
+        <v>94</v>
+      </c>
+      <c r="CR7">
+        <v>95</v>
+      </c>
+      <c r="CS7">
+        <v>96</v>
+      </c>
+      <c r="CT7">
+        <v>97</v>
+      </c>
+      <c r="CU7">
+        <v>98</v>
+      </c>
+      <c r="CV7">
+        <v>99</v>
+      </c>
+      <c r="CW7" s="41">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -12983,11 +14034,158 @@
       <c r="AY8">
         <v>50</v>
       </c>
-      <c r="AZ8" s="3">
+      <c r="AZ8">
+        <v>51</v>
+      </c>
+      <c r="BA8">
+        <v>52</v>
+      </c>
+      <c r="BB8">
+        <v>53</v>
+      </c>
+      <c r="BC8">
+        <v>54</v>
+      </c>
+      <c r="BD8">
+        <v>55</v>
+      </c>
+      <c r="BE8">
+        <v>56</v>
+      </c>
+      <c r="BF8">
+        <v>57</v>
+      </c>
+      <c r="BG8">
+        <v>58</v>
+      </c>
+      <c r="BH8">
+        <v>59</v>
+      </c>
+      <c r="BI8">
+        <v>60</v>
+      </c>
+      <c r="BJ8">
+        <v>61</v>
+      </c>
+      <c r="BK8">
+        <v>62</v>
+      </c>
+      <c r="BL8">
+        <v>63</v>
+      </c>
+      <c r="BM8">
+        <v>64</v>
+      </c>
+      <c r="BN8">
+        <v>65</v>
+      </c>
+      <c r="BO8">
+        <v>66</v>
+      </c>
+      <c r="BP8">
+        <v>67</v>
+      </c>
+      <c r="BQ8">
+        <v>68</v>
+      </c>
+      <c r="BR8">
+        <v>69</v>
+      </c>
+      <c r="BS8">
+        <v>70</v>
+      </c>
+      <c r="BT8">
+        <v>71</v>
+      </c>
+      <c r="BU8">
+        <v>72</v>
+      </c>
+      <c r="BV8">
+        <v>73</v>
+      </c>
+      <c r="BW8">
+        <v>74</v>
+      </c>
+      <c r="BX8">
+        <v>75</v>
+      </c>
+      <c r="BY8">
+        <v>76</v>
+      </c>
+      <c r="BZ8">
+        <v>77</v>
+      </c>
+      <c r="CA8">
+        <v>78</v>
+      </c>
+      <c r="CB8">
+        <v>79</v>
+      </c>
+      <c r="CC8">
+        <v>80</v>
+      </c>
+      <c r="CD8">
+        <v>81</v>
+      </c>
+      <c r="CE8">
+        <v>82</v>
+      </c>
+      <c r="CF8">
+        <v>83</v>
+      </c>
+      <c r="CG8">
+        <v>84</v>
+      </c>
+      <c r="CH8">
+        <v>85</v>
+      </c>
+      <c r="CI8">
+        <v>86</v>
+      </c>
+      <c r="CJ8">
+        <v>87</v>
+      </c>
+      <c r="CK8">
+        <v>88</v>
+      </c>
+      <c r="CL8">
+        <v>89</v>
+      </c>
+      <c r="CM8">
+        <v>90</v>
+      </c>
+      <c r="CN8">
+        <v>91</v>
+      </c>
+      <c r="CO8">
+        <v>92</v>
+      </c>
+      <c r="CP8">
+        <v>93</v>
+      </c>
+      <c r="CQ8">
+        <v>94</v>
+      </c>
+      <c r="CR8">
+        <v>95</v>
+      </c>
+      <c r="CS8">
+        <v>96</v>
+      </c>
+      <c r="CT8">
+        <v>97</v>
+      </c>
+      <c r="CU8">
+        <v>98</v>
+      </c>
+      <c r="CV8">
+        <v>99</v>
+      </c>
+      <c r="CW8" s="41">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A9" s="30" t="s">
         <v>53</v>
       </c>
@@ -13141,17 +14339,164 @@
       <c r="AY9" s="30">
         <v>15</v>
       </c>
-      <c r="AZ9" s="10">
+      <c r="AZ9" s="30">
+        <v>15</v>
+      </c>
+      <c r="BA9" s="30">
+        <v>15</v>
+      </c>
+      <c r="BB9" s="30">
+        <v>15</v>
+      </c>
+      <c r="BC9" s="30">
+        <v>15</v>
+      </c>
+      <c r="BD9" s="30">
+        <v>16</v>
+      </c>
+      <c r="BE9" s="30">
+        <v>16</v>
+      </c>
+      <c r="BF9" s="30">
+        <v>16</v>
+      </c>
+      <c r="BG9" s="30">
+        <v>16</v>
+      </c>
+      <c r="BH9" s="30">
+        <v>16</v>
+      </c>
+      <c r="BI9" s="30">
+        <v>17</v>
+      </c>
+      <c r="BJ9" s="30">
+        <v>17</v>
+      </c>
+      <c r="BK9" s="30">
+        <v>17</v>
+      </c>
+      <c r="BL9" s="30">
+        <v>17</v>
+      </c>
+      <c r="BM9" s="30">
+        <v>17</v>
+      </c>
+      <c r="BN9" s="30">
+        <v>18</v>
+      </c>
+      <c r="BO9" s="30">
+        <v>18</v>
+      </c>
+      <c r="BP9" s="30">
+        <v>18</v>
+      </c>
+      <c r="BQ9" s="30">
+        <v>18</v>
+      </c>
+      <c r="BR9" s="30">
+        <v>18</v>
+      </c>
+      <c r="BS9" s="30">
+        <v>19</v>
+      </c>
+      <c r="BT9" s="30">
+        <v>19</v>
+      </c>
+      <c r="BU9" s="30">
+        <v>19</v>
+      </c>
+      <c r="BV9" s="30">
+        <v>19</v>
+      </c>
+      <c r="BW9" s="30">
+        <v>19</v>
+      </c>
+      <c r="BX9" s="30">
+        <v>20</v>
+      </c>
+      <c r="BY9" s="30">
+        <v>20</v>
+      </c>
+      <c r="BZ9" s="30">
+        <v>20</v>
+      </c>
+      <c r="CA9" s="30">
+        <v>20</v>
+      </c>
+      <c r="CB9" s="30">
+        <v>20</v>
+      </c>
+      <c r="CC9" s="30">
+        <v>21</v>
+      </c>
+      <c r="CD9" s="30">
+        <v>21</v>
+      </c>
+      <c r="CE9" s="30">
+        <v>21</v>
+      </c>
+      <c r="CF9" s="30">
+        <v>21</v>
+      </c>
+      <c r="CG9" s="30">
+        <v>21</v>
+      </c>
+      <c r="CH9" s="30">
+        <v>22</v>
+      </c>
+      <c r="CI9" s="30">
+        <v>22</v>
+      </c>
+      <c r="CJ9" s="30">
+        <v>22</v>
+      </c>
+      <c r="CK9" s="30">
+        <v>22</v>
+      </c>
+      <c r="CL9" s="30">
+        <v>22</v>
+      </c>
+      <c r="CM9" s="30">
+        <v>23</v>
+      </c>
+      <c r="CN9" s="30">
+        <v>23</v>
+      </c>
+      <c r="CO9" s="30">
+        <v>23</v>
+      </c>
+      <c r="CP9" s="30">
+        <v>23</v>
+      </c>
+      <c r="CQ9" s="30">
+        <v>23</v>
+      </c>
+      <c r="CR9" s="30">
+        <v>24</v>
+      </c>
+      <c r="CS9" s="30">
+        <v>24</v>
+      </c>
+      <c r="CT9" s="30">
+        <v>24</v>
+      </c>
+      <c r="CU9" s="30">
+        <v>24</v>
+      </c>
+      <c r="CV9" s="30">
+        <v>24</v>
+      </c>
+      <c r="CW9" s="42">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:102" x14ac:dyDescent="0.3">
       <c r="B10">
         <f>SUM(B2:B9)</f>
         <v>5</v>
       </c>
       <c r="C10">
-        <f t="shared" ref="C10:AZ10" si="0">SUM(C2:C9)</f>
+        <f t="shared" ref="C10:CW10" si="0">SUM(C2:C9)</f>
         <v>10</v>
       </c>
       <c r="D10">
@@ -13346,12 +14691,208 @@
         <f t="shared" si="0"/>
         <v>250</v>
       </c>
-      <c r="AZ10" s="3">
+      <c r="AZ10">
+        <f t="shared" si="0"/>
+        <v>255</v>
+      </c>
+      <c r="BA10">
+        <f t="shared" si="0"/>
+        <v>260</v>
+      </c>
+      <c r="BB10">
+        <f t="shared" si="0"/>
+        <v>265</v>
+      </c>
+      <c r="BC10">
+        <f t="shared" si="0"/>
+        <v>270</v>
+      </c>
+      <c r="BD10">
+        <f t="shared" si="0"/>
+        <v>275</v>
+      </c>
+      <c r="BE10">
+        <f t="shared" si="0"/>
+        <v>280</v>
+      </c>
+      <c r="BF10">
+        <f t="shared" si="0"/>
+        <v>285</v>
+      </c>
+      <c r="BG10">
+        <f t="shared" si="0"/>
+        <v>290</v>
+      </c>
+      <c r="BH10">
+        <f t="shared" si="0"/>
+        <v>295</v>
+      </c>
+      <c r="BI10">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="BJ10">
+        <f t="shared" si="0"/>
+        <v>305</v>
+      </c>
+      <c r="BK10">
+        <f t="shared" si="0"/>
+        <v>310</v>
+      </c>
+      <c r="BL10">
+        <f t="shared" si="0"/>
+        <v>315</v>
+      </c>
+      <c r="BM10">
+        <f t="shared" si="0"/>
+        <v>320</v>
+      </c>
+      <c r="BN10">
+        <f t="shared" si="0"/>
+        <v>325</v>
+      </c>
+      <c r="BO10">
+        <f t="shared" si="0"/>
+        <v>330</v>
+      </c>
+      <c r="BP10">
+        <f t="shared" si="0"/>
+        <v>335</v>
+      </c>
+      <c r="BQ10">
+        <f t="shared" si="0"/>
+        <v>340</v>
+      </c>
+      <c r="BR10">
+        <f t="shared" si="0"/>
+        <v>345</v>
+      </c>
+      <c r="BS10">
+        <f t="shared" si="0"/>
+        <v>350</v>
+      </c>
+      <c r="BT10">
+        <f t="shared" si="0"/>
+        <v>355</v>
+      </c>
+      <c r="BU10">
+        <f t="shared" si="0"/>
+        <v>360</v>
+      </c>
+      <c r="BV10">
+        <f t="shared" si="0"/>
+        <v>365</v>
+      </c>
+      <c r="BW10">
+        <f t="shared" si="0"/>
+        <v>370</v>
+      </c>
+      <c r="BX10">
+        <f t="shared" si="0"/>
+        <v>375</v>
+      </c>
+      <c r="BY10">
+        <f t="shared" si="0"/>
+        <v>380</v>
+      </c>
+      <c r="BZ10">
+        <f t="shared" si="0"/>
+        <v>385</v>
+      </c>
+      <c r="CA10">
+        <f t="shared" si="0"/>
+        <v>390</v>
+      </c>
+      <c r="CB10">
+        <f t="shared" si="0"/>
+        <v>395</v>
+      </c>
+      <c r="CC10">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="CD10">
+        <f t="shared" si="0"/>
+        <v>405</v>
+      </c>
+      <c r="CE10">
+        <f t="shared" si="0"/>
+        <v>410</v>
+      </c>
+      <c r="CF10">
+        <f t="shared" si="0"/>
+        <v>415</v>
+      </c>
+      <c r="CG10">
+        <f t="shared" si="0"/>
+        <v>420</v>
+      </c>
+      <c r="CH10">
+        <f t="shared" si="0"/>
+        <v>425</v>
+      </c>
+      <c r="CI10">
+        <f t="shared" si="0"/>
+        <v>430</v>
+      </c>
+      <c r="CJ10">
+        <f t="shared" si="0"/>
+        <v>435</v>
+      </c>
+      <c r="CK10">
+        <f t="shared" si="0"/>
+        <v>440</v>
+      </c>
+      <c r="CL10">
+        <f t="shared" si="0"/>
+        <v>445</v>
+      </c>
+      <c r="CM10">
+        <f t="shared" si="0"/>
+        <v>450</v>
+      </c>
+      <c r="CN10">
+        <f t="shared" si="0"/>
+        <v>455</v>
+      </c>
+      <c r="CO10">
+        <f t="shared" si="0"/>
+        <v>460</v>
+      </c>
+      <c r="CP10">
+        <f t="shared" si="0"/>
+        <v>465</v>
+      </c>
+      <c r="CQ10">
+        <f t="shared" si="0"/>
+        <v>470</v>
+      </c>
+      <c r="CR10">
+        <f>SUM(CR2:CR9)</f>
+        <v>475</v>
+      </c>
+      <c r="CS10">
+        <f t="shared" si="0"/>
+        <v>480</v>
+      </c>
+      <c r="CT10">
+        <f t="shared" si="0"/>
+        <v>485</v>
+      </c>
+      <c r="CU10">
+        <f t="shared" si="0"/>
+        <v>490</v>
+      </c>
+      <c r="CV10">
+        <f t="shared" si="0"/>
+        <v>495</v>
+      </c>
+      <c r="CW10" s="41">
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
     </row>
-    <row r="13" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:102" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>0</v>
       </c>
@@ -13649,11 +15190,11 @@
       <c r="CV13" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="CW13" t="s">
+      <c r="CW13" s="41" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>48</v>
       </c>
@@ -13954,11 +15495,11 @@
       <c r="CV14">
         <v>99</v>
       </c>
-      <c r="CW14">
+      <c r="CW14" s="41">
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -14259,11 +15800,11 @@
       <c r="CV15">
         <v>99</v>
       </c>
-      <c r="CW15">
+      <c r="CW15" s="41">
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:101" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -14564,7 +16105,7 @@
       <c r="CV16">
         <v>99</v>
       </c>
-      <c r="CW16">
+      <c r="CW16" s="41">
         <v>100</v>
       </c>
     </row>
@@ -14869,7 +16410,7 @@
       <c r="CV17">
         <v>99</v>
       </c>
-      <c r="CW17">
+      <c r="CW17" s="41">
         <v>100</v>
       </c>
     </row>
@@ -15174,7 +16715,7 @@
       <c r="CV18">
         <v>40</v>
       </c>
-      <c r="CW18">
+      <c r="CW18" s="41">
         <v>40</v>
       </c>
     </row>
@@ -15479,7 +17020,7 @@
       <c r="CV19">
         <v>25</v>
       </c>
-      <c r="CW19">
+      <c r="CW19" s="41">
         <v>25</v>
       </c>
     </row>
@@ -15784,7 +17325,7 @@
       <c r="CV20">
         <v>25</v>
       </c>
-      <c r="CW20">
+      <c r="CW20" s="41">
         <v>25</v>
       </c>
     </row>
@@ -16089,7 +17630,7 @@
       <c r="CV21" s="30">
         <v>9</v>
       </c>
-      <c r="CW21" s="30">
+      <c r="CW21" s="42">
         <v>10</v>
       </c>
     </row>
@@ -16490,7 +18031,7 @@
         <f t="shared" ref="CV22" si="16">SUM(CV14:CV21)</f>
         <v>495</v>
       </c>
-      <c r="CW22">
+      <c r="CW22" s="41">
         <f t="shared" ref="CW22" si="17">SUM(CW14:CW21)</f>
         <v>500</v>
       </c>
@@ -17824,7 +19365,7 @@
       <c r="CV38">
         <v>44</v>
       </c>
-      <c r="CW38">
+      <c r="CW38" s="41">
         <v>45</v>
       </c>
     </row>
@@ -18129,7 +19670,7 @@
       <c r="CV39">
         <v>50</v>
       </c>
-      <c r="CW39">
+      <c r="CW39" s="41">
         <v>50</v>
       </c>
     </row>
@@ -18434,7 +19975,7 @@
       <c r="CV40">
         <v>69</v>
       </c>
-      <c r="CW40">
+      <c r="CW40" s="41">
         <v>70</v>
       </c>
     </row>
@@ -18739,7 +20280,7 @@
       <c r="CV41">
         <v>50</v>
       </c>
-      <c r="CW41">
+      <c r="CW41" s="41">
         <v>50</v>
       </c>
     </row>
@@ -19044,7 +20585,7 @@
       <c r="CV42">
         <v>80</v>
       </c>
-      <c r="CW42">
+      <c r="CW42" s="41">
         <v>80</v>
       </c>
     </row>
@@ -19349,7 +20890,7 @@
       <c r="CV43">
         <v>89</v>
       </c>
-      <c r="CW43">
+      <c r="CW43" s="41">
         <v>90</v>
       </c>
     </row>
@@ -19654,7 +21195,7 @@
       <c r="CV44">
         <v>89</v>
       </c>
-      <c r="CW44">
+      <c r="CW44" s="41">
         <v>90</v>
       </c>
     </row>
@@ -19959,7 +21500,7 @@
       <c r="CV45" s="30">
         <v>24</v>
       </c>
-      <c r="CW45" s="30">
+      <c r="CW45" s="42">
         <v>25</v>
       </c>
     </row>
@@ -20360,10 +21901,756 @@
         <f t="shared" si="25"/>
         <v>495</v>
       </c>
-      <c r="CW46">
+      <c r="CW46" s="41">
         <f>SUM(CW38:CW45)</f>
         <v>500</v>
       </c>
+    </row>
+    <row r="49" spans="1:115" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="D49" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="E49" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="F49" t="s">
+        <v>17</v>
+      </c>
+      <c r="G49" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="H49" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="I49" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="J49" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="K49" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="L49" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="M49" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="N49" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="O49" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="P49" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q49" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="R49" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="S49" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="T49" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="U49" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="V49" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="W49" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="CW49"/>
+      <c r="DK49" s="41"/>
+    </row>
+    <row r="50" spans="1:115" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>48</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>2</v>
+      </c>
+      <c r="D50">
+        <v>2</v>
+      </c>
+      <c r="E50">
+        <v>3</v>
+      </c>
+      <c r="F50">
+        <v>3</v>
+      </c>
+      <c r="G50">
+        <v>3</v>
+      </c>
+      <c r="H50">
+        <v>3</v>
+      </c>
+      <c r="I50">
+        <v>4</v>
+      </c>
+      <c r="J50">
+        <v>4</v>
+      </c>
+      <c r="K50">
+        <v>5</v>
+      </c>
+      <c r="L50">
+        <v>6</v>
+      </c>
+      <c r="M50">
+        <v>6</v>
+      </c>
+      <c r="N50">
+        <v>6</v>
+      </c>
+      <c r="O50">
+        <v>6</v>
+      </c>
+      <c r="P50">
+        <v>7</v>
+      </c>
+      <c r="Q50">
+        <v>7</v>
+      </c>
+      <c r="R50">
+        <v>8</v>
+      </c>
+      <c r="S50">
+        <v>8</v>
+      </c>
+      <c r="T50">
+        <v>8</v>
+      </c>
+      <c r="U50" s="41">
+        <v>8</v>
+      </c>
+      <c r="V50" s="3">
+        <v>25</v>
+      </c>
+      <c r="W50" s="3">
+        <v>50</v>
+      </c>
+      <c r="CW50"/>
+      <c r="DK50" s="41"/>
+    </row>
+    <row r="51" spans="1:115" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>2</v>
+      </c>
+      <c r="E51">
+        <v>2</v>
+      </c>
+      <c r="F51">
+        <v>3</v>
+      </c>
+      <c r="G51">
+        <v>4</v>
+      </c>
+      <c r="H51">
+        <v>5</v>
+      </c>
+      <c r="I51">
+        <v>6</v>
+      </c>
+      <c r="J51">
+        <v>6</v>
+      </c>
+      <c r="K51">
+        <v>7</v>
+      </c>
+      <c r="L51">
+        <v>7</v>
+      </c>
+      <c r="M51">
+        <v>8</v>
+      </c>
+      <c r="N51">
+        <v>8</v>
+      </c>
+      <c r="O51">
+        <v>9</v>
+      </c>
+      <c r="P51">
+        <v>9</v>
+      </c>
+      <c r="Q51">
+        <v>10</v>
+      </c>
+      <c r="R51">
+        <v>10</v>
+      </c>
+      <c r="S51">
+        <v>11</v>
+      </c>
+      <c r="T51">
+        <v>11</v>
+      </c>
+      <c r="U51" s="41">
+        <v>12</v>
+      </c>
+      <c r="V51" s="3">
+        <v>27</v>
+      </c>
+      <c r="W51" s="3">
+        <v>55</v>
+      </c>
+      <c r="CW51"/>
+      <c r="DK51" s="41"/>
+    </row>
+    <row r="52" spans="1:115" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>47</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>2</v>
+      </c>
+      <c r="F52">
+        <v>2</v>
+      </c>
+      <c r="G52">
+        <v>3</v>
+      </c>
+      <c r="H52">
+        <v>4</v>
+      </c>
+      <c r="I52">
+        <v>4</v>
+      </c>
+      <c r="J52">
+        <v>5</v>
+      </c>
+      <c r="K52">
+        <v>6</v>
+      </c>
+      <c r="L52">
+        <v>6</v>
+      </c>
+      <c r="M52">
+        <v>7</v>
+      </c>
+      <c r="N52">
+        <v>8</v>
+      </c>
+      <c r="O52">
+        <v>8</v>
+      </c>
+      <c r="P52">
+        <v>9</v>
+      </c>
+      <c r="Q52">
+        <v>10</v>
+      </c>
+      <c r="R52">
+        <v>10</v>
+      </c>
+      <c r="S52">
+        <v>11</v>
+      </c>
+      <c r="T52">
+        <v>12</v>
+      </c>
+      <c r="U52" s="41">
+        <v>12</v>
+      </c>
+      <c r="V52" s="3">
+        <v>26</v>
+      </c>
+      <c r="W52" s="3">
+        <v>60</v>
+      </c>
+      <c r="CW52"/>
+      <c r="DK52" s="41"/>
+    </row>
+    <row r="53" spans="1:115" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>2</v>
+      </c>
+      <c r="E53">
+        <v>2</v>
+      </c>
+      <c r="F53">
+        <v>3</v>
+      </c>
+      <c r="G53">
+        <v>4</v>
+      </c>
+      <c r="H53">
+        <v>4</v>
+      </c>
+      <c r="I53">
+        <v>5</v>
+      </c>
+      <c r="J53">
+        <v>6</v>
+      </c>
+      <c r="K53">
+        <v>6</v>
+      </c>
+      <c r="L53">
+        <v>7</v>
+      </c>
+      <c r="M53">
+        <v>7</v>
+      </c>
+      <c r="N53">
+        <v>8</v>
+      </c>
+      <c r="O53">
+        <v>9</v>
+      </c>
+      <c r="P53">
+        <v>9</v>
+      </c>
+      <c r="Q53">
+        <v>9</v>
+      </c>
+      <c r="R53">
+        <v>10</v>
+      </c>
+      <c r="S53">
+        <v>10</v>
+      </c>
+      <c r="T53">
+        <v>11</v>
+      </c>
+      <c r="U53" s="41">
+        <v>12</v>
+      </c>
+      <c r="V53" s="3">
+        <v>27</v>
+      </c>
+      <c r="W53" s="3">
+        <v>50</v>
+      </c>
+      <c r="CW53"/>
+      <c r="DK53" s="41"/>
+    </row>
+    <row r="54" spans="1:115" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>49</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>2</v>
+      </c>
+      <c r="D54">
+        <v>3</v>
+      </c>
+      <c r="E54">
+        <v>4</v>
+      </c>
+      <c r="F54">
+        <v>4</v>
+      </c>
+      <c r="G54">
+        <v>4</v>
+      </c>
+      <c r="H54">
+        <v>5</v>
+      </c>
+      <c r="I54">
+        <v>5</v>
+      </c>
+      <c r="J54">
+        <v>6</v>
+      </c>
+      <c r="K54">
+        <v>6</v>
+      </c>
+      <c r="L54">
+        <v>7</v>
+      </c>
+      <c r="M54">
+        <v>8</v>
+      </c>
+      <c r="N54">
+        <v>9</v>
+      </c>
+      <c r="O54">
+        <v>10</v>
+      </c>
+      <c r="P54">
+        <v>11</v>
+      </c>
+      <c r="Q54">
+        <v>12</v>
+      </c>
+      <c r="R54">
+        <v>13</v>
+      </c>
+      <c r="S54">
+        <v>14</v>
+      </c>
+      <c r="T54">
+        <v>15</v>
+      </c>
+      <c r="U54" s="41">
+        <v>16</v>
+      </c>
+      <c r="V54" s="3">
+        <v>45</v>
+      </c>
+      <c r="W54" s="3">
+        <v>70</v>
+      </c>
+      <c r="CW54"/>
+      <c r="DK54" s="41"/>
+    </row>
+    <row r="55" spans="1:115" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>46</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+      <c r="C55">
+        <v>2</v>
+      </c>
+      <c r="D55">
+        <v>3</v>
+      </c>
+      <c r="E55">
+        <v>4</v>
+      </c>
+      <c r="F55">
+        <v>5</v>
+      </c>
+      <c r="G55">
+        <v>6</v>
+      </c>
+      <c r="H55">
+        <v>7</v>
+      </c>
+      <c r="I55">
+        <v>8</v>
+      </c>
+      <c r="J55">
+        <v>9</v>
+      </c>
+      <c r="K55">
+        <v>10</v>
+      </c>
+      <c r="L55">
+        <v>11</v>
+      </c>
+      <c r="M55">
+        <v>12</v>
+      </c>
+      <c r="N55">
+        <v>13</v>
+      </c>
+      <c r="O55">
+        <v>14</v>
+      </c>
+      <c r="P55">
+        <v>15</v>
+      </c>
+      <c r="Q55">
+        <v>16</v>
+      </c>
+      <c r="R55">
+        <v>17</v>
+      </c>
+      <c r="S55">
+        <v>18</v>
+      </c>
+      <c r="T55">
+        <v>19</v>
+      </c>
+      <c r="U55" s="41">
+        <v>20</v>
+      </c>
+      <c r="V55" s="3">
+        <v>50</v>
+      </c>
+      <c r="W55" s="3">
+        <v>100</v>
+      </c>
+      <c r="CW55"/>
+      <c r="DK55" s="41"/>
+    </row>
+    <row r="56" spans="1:115" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>51</v>
+      </c>
+      <c r="B56">
+        <v>0</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>2</v>
+      </c>
+      <c r="E56">
+        <v>3</v>
+      </c>
+      <c r="F56">
+        <v>4</v>
+      </c>
+      <c r="G56">
+        <v>5</v>
+      </c>
+      <c r="H56">
+        <v>6</v>
+      </c>
+      <c r="I56">
+        <v>7</v>
+      </c>
+      <c r="J56">
+        <v>8</v>
+      </c>
+      <c r="K56">
+        <v>9</v>
+      </c>
+      <c r="L56">
+        <v>10</v>
+      </c>
+      <c r="M56">
+        <v>11</v>
+      </c>
+      <c r="N56">
+        <v>12</v>
+      </c>
+      <c r="O56">
+        <v>13</v>
+      </c>
+      <c r="P56">
+        <v>14</v>
+      </c>
+      <c r="Q56">
+        <v>15</v>
+      </c>
+      <c r="R56">
+        <v>16</v>
+      </c>
+      <c r="S56">
+        <v>17</v>
+      </c>
+      <c r="T56">
+        <v>18</v>
+      </c>
+      <c r="U56" s="41">
+        <v>18</v>
+      </c>
+      <c r="V56" s="3">
+        <v>45</v>
+      </c>
+      <c r="W56" s="3">
+        <v>90</v>
+      </c>
+      <c r="CW56"/>
+      <c r="DK56" s="41"/>
+    </row>
+    <row r="57" spans="1:115" x14ac:dyDescent="0.3">
+      <c r="A57" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B57" s="30">
+        <v>0</v>
+      </c>
+      <c r="C57" s="30">
+        <v>0</v>
+      </c>
+      <c r="D57" s="30">
+        <v>0</v>
+      </c>
+      <c r="E57" s="30">
+        <v>0</v>
+      </c>
+      <c r="F57" s="30">
+        <v>1</v>
+      </c>
+      <c r="G57" s="30">
+        <v>1</v>
+      </c>
+      <c r="H57" s="30">
+        <v>1</v>
+      </c>
+      <c r="I57" s="30">
+        <v>1</v>
+      </c>
+      <c r="J57" s="30">
+        <v>1</v>
+      </c>
+      <c r="K57" s="30">
+        <v>1</v>
+      </c>
+      <c r="L57" s="30">
+        <v>1</v>
+      </c>
+      <c r="M57" s="30">
+        <v>1</v>
+      </c>
+      <c r="N57" s="30">
+        <v>1</v>
+      </c>
+      <c r="O57" s="30">
+        <v>1</v>
+      </c>
+      <c r="P57" s="30">
+        <v>1</v>
+      </c>
+      <c r="Q57" s="30">
+        <v>1</v>
+      </c>
+      <c r="R57" s="30">
+        <v>1</v>
+      </c>
+      <c r="S57" s="30">
+        <v>1</v>
+      </c>
+      <c r="T57" s="30">
+        <v>1</v>
+      </c>
+      <c r="U57" s="42">
+        <v>2</v>
+      </c>
+      <c r="V57" s="10">
+        <v>5</v>
+      </c>
+      <c r="W57" s="10">
+        <v>25</v>
+      </c>
+      <c r="CW57"/>
+      <c r="DK57" s="41"/>
+    </row>
+    <row r="58" spans="1:115" x14ac:dyDescent="0.3">
+      <c r="B58">
+        <f>SUM(B50:B57)</f>
+        <v>5</v>
+      </c>
+      <c r="C58">
+        <f t="shared" ref="C58:F58" si="26">SUM(C50:C57)</f>
+        <v>10</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="26"/>
+        <v>15</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="26"/>
+        <v>20</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="26"/>
+        <v>25</v>
+      </c>
+      <c r="G58">
+        <f t="shared" ref="G58" si="27">SUM(G50:G57)</f>
+        <v>30</v>
+      </c>
+      <c r="H58">
+        <f t="shared" ref="H58" si="28">SUM(H50:H57)</f>
+        <v>35</v>
+      </c>
+      <c r="I58">
+        <f t="shared" ref="I58" si="29">SUM(I50:I57)</f>
+        <v>40</v>
+      </c>
+      <c r="J58">
+        <f t="shared" ref="J58" si="30">SUM(J50:J57)</f>
+        <v>45</v>
+      </c>
+      <c r="K58">
+        <f t="shared" ref="K58" si="31">SUM(K50:K57)</f>
+        <v>50</v>
+      </c>
+      <c r="L58">
+        <f t="shared" ref="L58" si="32">SUM(L50:L57)</f>
+        <v>55</v>
+      </c>
+      <c r="M58">
+        <f t="shared" ref="M58" si="33">SUM(M50:M57)</f>
+        <v>60</v>
+      </c>
+      <c r="N58">
+        <f t="shared" ref="N58" si="34">SUM(N50:N57)</f>
+        <v>65</v>
+      </c>
+      <c r="O58">
+        <f t="shared" ref="O58" si="35">SUM(O50:O57)</f>
+        <v>70</v>
+      </c>
+      <c r="P58">
+        <f t="shared" ref="P58" si="36">SUM(P50:P57)</f>
+        <v>75</v>
+      </c>
+      <c r="Q58">
+        <f t="shared" ref="Q58" si="37">SUM(Q50:Q57)</f>
+        <v>80</v>
+      </c>
+      <c r="R58">
+        <f t="shared" ref="R58" si="38">SUM(R50:R57)</f>
+        <v>85</v>
+      </c>
+      <c r="S58">
+        <f t="shared" ref="S58" si="39">SUM(S50:S57)</f>
+        <v>90</v>
+      </c>
+      <c r="T58">
+        <f t="shared" ref="T58" si="40">SUM(T50:T57)</f>
+        <v>95</v>
+      </c>
+      <c r="U58">
+        <f t="shared" ref="U58" si="41">SUM(U50:U57)</f>
+        <v>100</v>
+      </c>
+      <c r="V58">
+        <f t="shared" ref="V58" si="42">SUM(V50:V57)</f>
+        <v>250</v>
+      </c>
+      <c r="W58">
+        <f t="shared" ref="W58" si="43">SUM(W50:W57)</f>
+        <v>500</v>
+      </c>
+      <c r="CW58"/>
+      <c r="DK58" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Introduce new CLERIC castes: - PRIEST - HIERARCH - ARCHANGEL Cleric development path in the endurance test goes to ARCHANGEL level now. PRIESTs and above can provide a code value to convert another character to their faith. (Changing defensive god.) These codes can be used once by a single character but there is no limitation to be converted many times with different codes.
</commit_message>
<xml_diff>
--- a/doc/caste_system.xlsx
+++ b/doc/caste_system.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/349dfb9748b30a92/Asztali gép/ataliasflame_2.0/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6652" documentId="8_{652F4476-B36F-42CD-831D-0D71B9923ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F17CFFB6-CA48-4264-AC04-DAC12A063A31}"/>
+  <xr:revisionPtr revIDLastSave="7618" documentId="8_{652F4476-B36F-42CD-831D-0D71B9923ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF92B959-0A93-4354-AC26-B19CB8EBFB5F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{CAF51EC3-63EC-48CD-AA7B-C21B3D5D222B}"/>
   </bookViews>
@@ -1557,7 +1557,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1403" uniqueCount="85">
   <si>
     <t>csavargó</t>
   </si>
@@ -2012,7 +2012,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2084,8 +2084,22 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -2407,7 +2421,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E471BE-CB76-416C-8A0D-8BCD59B0033A}">
   <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3522,163 +3538,163 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="38"/>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I21" s="3" t="s">
+      <c r="C21" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="H21" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="I21" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="J21" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M21" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="N21" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="O21" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="P21" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q21" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="R21" s="2" t="s">
+      <c r="J21" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="K21" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="L21" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="M21" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="N21" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="O21" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="P21" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q21" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="R21" s="44" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="38"/>
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I22" s="3" t="s">
+      <c r="C22" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="H22" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="I22" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="J22" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="K22" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M22" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="N22" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="O22" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="P22" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q22" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="R22" s="2" t="s">
+      <c r="J22" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="K22" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="L22" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="M22" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="N22" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="O22" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="P22" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q22" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="R22" s="44" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="39"/>
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I23" s="3" t="s">
+      <c r="C23" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="H23" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="I23" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="J23" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="K23" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M23" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="N23" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="O23" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="P23" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q23" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="R23" s="2" t="s">
+      <c r="J23" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="K23" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="L23" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="M23" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="N23" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="O23" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="P23" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q23" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="R23" s="44" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4574,9 +4590,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47799533-6B34-4949-9561-D6B03DB6E4FC}">
   <dimension ref="A1:AC10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4685,13 +4699,13 @@
       <c r="Y1" t="s">
         <v>17</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="Z1" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AA1" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AB1" s="44" t="s">
         <v>20</v>
       </c>
       <c r="AC1" t="s">
@@ -4774,13 +4788,13 @@
       <c r="Y2">
         <v>3</v>
       </c>
-      <c r="Z2" s="3">
+      <c r="Z2" s="43">
         <v>8</v>
       </c>
-      <c r="AA2" s="3">
+      <c r="AA2" s="43">
         <v>25</v>
       </c>
-      <c r="AB2" s="2">
+      <c r="AB2" s="44">
         <v>50</v>
       </c>
       <c r="AC2">
@@ -4864,13 +4878,13 @@
       <c r="Y3">
         <v>3</v>
       </c>
-      <c r="Z3" s="3">
+      <c r="Z3" s="43">
         <v>12</v>
       </c>
-      <c r="AA3" s="3">
+      <c r="AA3" s="43">
         <v>27</v>
       </c>
-      <c r="AB3" s="2">
+      <c r="AB3" s="44">
         <v>55</v>
       </c>
       <c r="AC3">
@@ -4954,13 +4968,13 @@
       <c r="Y4">
         <v>2</v>
       </c>
-      <c r="Z4" s="3">
+      <c r="Z4" s="43">
         <v>12</v>
       </c>
-      <c r="AA4" s="3">
+      <c r="AA4" s="43">
         <v>26</v>
       </c>
-      <c r="AB4" s="2">
+      <c r="AB4" s="44">
         <v>60</v>
       </c>
       <c r="AC4">
@@ -5044,13 +5058,13 @@
       <c r="Y5">
         <v>3</v>
       </c>
-      <c r="Z5" s="3">
+      <c r="Z5" s="43">
         <v>12</v>
       </c>
-      <c r="AA5" s="3">
+      <c r="AA5" s="43">
         <v>27</v>
       </c>
-      <c r="AB5" s="2">
+      <c r="AB5" s="44">
         <v>50</v>
       </c>
       <c r="AC5">
@@ -5134,13 +5148,13 @@
       <c r="Y6">
         <v>4</v>
       </c>
-      <c r="Z6" s="3">
+      <c r="Z6" s="43">
         <v>16</v>
       </c>
-      <c r="AA6" s="3">
+      <c r="AA6" s="43">
         <v>45</v>
       </c>
-      <c r="AB6" s="2">
+      <c r="AB6" s="44">
         <v>70</v>
       </c>
       <c r="AC6">
@@ -5224,13 +5238,13 @@
       <c r="Y7">
         <v>5</v>
       </c>
-      <c r="Z7" s="3">
+      <c r="Z7" s="43">
         <v>20</v>
       </c>
-      <c r="AA7" s="3">
+      <c r="AA7" s="43">
         <v>50</v>
       </c>
-      <c r="AB7" s="2">
+      <c r="AB7" s="44">
         <v>100</v>
       </c>
       <c r="AC7">
@@ -5314,13 +5328,13 @@
       <c r="Y8">
         <v>4</v>
       </c>
-      <c r="Z8" s="3">
+      <c r="Z8" s="43">
         <v>18</v>
       </c>
-      <c r="AA8" s="3">
+      <c r="AA8" s="43">
         <v>45</v>
       </c>
-      <c r="AB8" s="2">
+      <c r="AB8" s="44">
         <v>90</v>
       </c>
       <c r="AC8">
@@ -5404,13 +5418,13 @@
       <c r="Y9" s="27">
         <v>1</v>
       </c>
-      <c r="Z9" s="7">
+      <c r="Z9" s="45">
         <v>2</v>
       </c>
-      <c r="AA9" s="7">
+      <c r="AA9" s="45">
         <v>5</v>
       </c>
-      <c r="AB9" s="4">
+      <c r="AB9" s="46">
         <v>25</v>
       </c>
       <c r="AC9" s="33">
@@ -11700,8 +11714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD573711-C846-40DC-8629-19A685998D3E}">
   <dimension ref="A1:CX58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD40" workbookViewId="0">
-      <selection activeCell="AY59" sqref="AY59"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="CS49" sqref="CS49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11717,8 +11731,7 @@
     <col min="24" max="47" width="4" bestFit="1" customWidth="1"/>
     <col min="48" max="50" width="4" customWidth="1"/>
     <col min="51" max="51" width="16" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="53" max="55" width="4" bestFit="1" customWidth="1"/>
+    <col min="52" max="55" width="4" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="4" customWidth="1"/>
     <col min="57" max="100" width="4" bestFit="1" customWidth="1"/>
     <col min="101" max="101" width="10.5546875" bestFit="1" customWidth="1"/>
@@ -21886,7 +21899,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="49" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:101" x14ac:dyDescent="0.3">
       <c r="B49" s="36" t="s">
         <v>0</v>
       </c>
@@ -21944,7 +21957,7 @@
       <c r="T49" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="U49" s="34" t="s">
+      <c r="U49" s="47" t="s">
         <v>18</v>
       </c>
       <c r="V49" s="28" t="s">
@@ -22034,14 +22047,161 @@
       <c r="AX49" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="AY49" s="34" t="s">
+      <c r="AY49" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="AZ49" s="34" t="s">
+      <c r="AZ49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BA49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BB49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BC49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BD49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BE49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BF49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BG49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BH49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BI49" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="BJ49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BK49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BL49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BM49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BN49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BO49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BP49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BQ49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BR49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BS49" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="BT49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BU49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BV49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BW49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BX49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BY49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BZ49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CA49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CB49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CC49" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="CD49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CE49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CF49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CG49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CH49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CI49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CJ49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CK49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CL49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CM49" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="CN49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CO49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CP49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CQ49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CR49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CS49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CT49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CU49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CV49" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CW49" s="47" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -22192,14 +22352,161 @@
       <c r="AX50">
         <v>23</v>
       </c>
-      <c r="AY50" s="41">
+      <c r="AY50">
         <v>25</v>
       </c>
-      <c r="AZ50" s="3">
+      <c r="AZ50">
+        <v>26</v>
+      </c>
+      <c r="BA50">
+        <v>26</v>
+      </c>
+      <c r="BB50">
+        <v>27</v>
+      </c>
+      <c r="BC50">
+        <v>27</v>
+      </c>
+      <c r="BD50">
+        <v>28</v>
+      </c>
+      <c r="BE50">
+        <v>28</v>
+      </c>
+      <c r="BF50">
+        <v>29</v>
+      </c>
+      <c r="BG50">
+        <v>29</v>
+      </c>
+      <c r="BH50">
+        <v>30</v>
+      </c>
+      <c r="BI50">
+        <v>30</v>
+      </c>
+      <c r="BJ50">
+        <v>31</v>
+      </c>
+      <c r="BK50">
+        <v>31</v>
+      </c>
+      <c r="BL50">
+        <v>32</v>
+      </c>
+      <c r="BM50">
+        <v>32</v>
+      </c>
+      <c r="BN50">
+        <v>33</v>
+      </c>
+      <c r="BO50">
+        <v>33</v>
+      </c>
+      <c r="BP50">
+        <v>34</v>
+      </c>
+      <c r="BQ50">
+        <v>34</v>
+      </c>
+      <c r="BR50">
+        <v>35</v>
+      </c>
+      <c r="BS50">
+        <v>35</v>
+      </c>
+      <c r="BT50">
+        <v>36</v>
+      </c>
+      <c r="BU50">
+        <v>36</v>
+      </c>
+      <c r="BV50">
+        <v>37</v>
+      </c>
+      <c r="BW50">
+        <v>37</v>
+      </c>
+      <c r="BX50">
+        <v>38</v>
+      </c>
+      <c r="BY50">
+        <v>38</v>
+      </c>
+      <c r="BZ50">
+        <v>39</v>
+      </c>
+      <c r="CA50">
+        <v>39</v>
+      </c>
+      <c r="CB50">
+        <v>40</v>
+      </c>
+      <c r="CC50">
+        <v>40</v>
+      </c>
+      <c r="CD50">
+        <v>41</v>
+      </c>
+      <c r="CE50">
+        <v>41</v>
+      </c>
+      <c r="CF50">
+        <v>42</v>
+      </c>
+      <c r="CG50">
+        <v>42</v>
+      </c>
+      <c r="CH50">
+        <v>43</v>
+      </c>
+      <c r="CI50">
+        <v>43</v>
+      </c>
+      <c r="CJ50">
+        <v>44</v>
+      </c>
+      <c r="CK50">
+        <v>44</v>
+      </c>
+      <c r="CL50">
+        <v>45</v>
+      </c>
+      <c r="CM50">
+        <v>45</v>
+      </c>
+      <c r="CN50">
+        <v>46</v>
+      </c>
+      <c r="CO50">
+        <v>46</v>
+      </c>
+      <c r="CP50">
+        <v>47</v>
+      </c>
+      <c r="CQ50">
+        <v>47</v>
+      </c>
+      <c r="CR50">
+        <v>48</v>
+      </c>
+      <c r="CS50">
+        <v>48</v>
+      </c>
+      <c r="CT50">
+        <v>49</v>
+      </c>
+      <c r="CU50">
+        <v>49</v>
+      </c>
+      <c r="CV50">
         <v>50</v>
       </c>
-    </row>
-    <row r="51" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="CW50" s="43">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -22350,14 +22657,161 @@
       <c r="AX51">
         <v>27</v>
       </c>
-      <c r="AY51" s="41">
+      <c r="AY51">
         <v>27</v>
       </c>
-      <c r="AZ51" s="3">
+      <c r="AZ51">
+        <v>28</v>
+      </c>
+      <c r="BA51">
+        <v>29</v>
+      </c>
+      <c r="BB51">
+        <v>30</v>
+      </c>
+      <c r="BC51">
+        <v>30</v>
+      </c>
+      <c r="BD51">
+        <v>31</v>
+      </c>
+      <c r="BE51">
+        <v>32</v>
+      </c>
+      <c r="BF51">
+        <v>33</v>
+      </c>
+      <c r="BG51">
+        <v>34</v>
+      </c>
+      <c r="BH51">
+        <v>35</v>
+      </c>
+      <c r="BI51">
+        <v>35</v>
+      </c>
+      <c r="BJ51">
+        <v>36</v>
+      </c>
+      <c r="BK51">
+        <v>36</v>
+      </c>
+      <c r="BL51">
+        <v>37</v>
+      </c>
+      <c r="BM51">
+        <v>37</v>
+      </c>
+      <c r="BN51">
+        <v>38</v>
+      </c>
+      <c r="BO51">
+        <v>38</v>
+      </c>
+      <c r="BP51">
+        <v>39</v>
+      </c>
+      <c r="BQ51">
+        <v>39</v>
+      </c>
+      <c r="BR51">
+        <v>40</v>
+      </c>
+      <c r="BS51">
+        <v>40</v>
+      </c>
+      <c r="BT51">
+        <v>41</v>
+      </c>
+      <c r="BU51">
+        <v>41</v>
+      </c>
+      <c r="BV51">
+        <v>42</v>
+      </c>
+      <c r="BW51">
+        <v>42</v>
+      </c>
+      <c r="BX51">
+        <v>43</v>
+      </c>
+      <c r="BY51">
+        <v>43</v>
+      </c>
+      <c r="BZ51">
+        <v>44</v>
+      </c>
+      <c r="CA51">
+        <v>44</v>
+      </c>
+      <c r="CB51">
+        <v>45</v>
+      </c>
+      <c r="CC51">
+        <v>45</v>
+      </c>
+      <c r="CD51">
+        <v>46</v>
+      </c>
+      <c r="CE51">
+        <v>46</v>
+      </c>
+      <c r="CF51">
+        <v>47</v>
+      </c>
+      <c r="CG51">
+        <v>47</v>
+      </c>
+      <c r="CH51">
+        <v>48</v>
+      </c>
+      <c r="CI51">
+        <v>48</v>
+      </c>
+      <c r="CJ51">
+        <v>49</v>
+      </c>
+      <c r="CK51">
+        <v>49</v>
+      </c>
+      <c r="CL51">
+        <v>50</v>
+      </c>
+      <c r="CM51">
+        <v>50</v>
+      </c>
+      <c r="CN51">
+        <v>51</v>
+      </c>
+      <c r="CO51">
+        <v>51</v>
+      </c>
+      <c r="CP51">
+        <v>52</v>
+      </c>
+      <c r="CQ51">
+        <v>52</v>
+      </c>
+      <c r="CR51">
+        <v>53</v>
+      </c>
+      <c r="CS51">
+        <v>53</v>
+      </c>
+      <c r="CT51">
+        <v>54</v>
+      </c>
+      <c r="CU51">
+        <v>54</v>
+      </c>
+      <c r="CV51">
         <v>55</v>
       </c>
-    </row>
-    <row r="52" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="CW51" s="43">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>47</v>
       </c>
@@ -22508,14 +22962,161 @@
       <c r="AX52">
         <v>26</v>
       </c>
-      <c r="AY52" s="41">
+      <c r="AY52">
         <v>26</v>
       </c>
-      <c r="AZ52" s="3">
+      <c r="AZ52">
+        <v>27</v>
+      </c>
+      <c r="BA52">
+        <v>28</v>
+      </c>
+      <c r="BB52">
+        <v>29</v>
+      </c>
+      <c r="BC52">
+        <v>30</v>
+      </c>
+      <c r="BD52">
+        <v>31</v>
+      </c>
+      <c r="BE52">
+        <v>32</v>
+      </c>
+      <c r="BF52">
+        <v>32</v>
+      </c>
+      <c r="BG52">
+        <v>33</v>
+      </c>
+      <c r="BH52">
+        <v>34</v>
+      </c>
+      <c r="BI52">
+        <v>34</v>
+      </c>
+      <c r="BJ52">
+        <v>35</v>
+      </c>
+      <c r="BK52">
+        <v>36</v>
+      </c>
+      <c r="BL52">
+        <v>36</v>
+      </c>
+      <c r="BM52">
+        <v>37</v>
+      </c>
+      <c r="BN52">
+        <v>38</v>
+      </c>
+      <c r="BO52">
+        <v>38</v>
+      </c>
+      <c r="BP52">
+        <v>39</v>
+      </c>
+      <c r="BQ52">
+        <v>40</v>
+      </c>
+      <c r="BR52">
+        <v>40</v>
+      </c>
+      <c r="BS52">
+        <v>41</v>
+      </c>
+      <c r="BT52">
+        <v>42</v>
+      </c>
+      <c r="BU52">
+        <v>42</v>
+      </c>
+      <c r="BV52">
+        <v>43</v>
+      </c>
+      <c r="BW52">
+        <v>44</v>
+      </c>
+      <c r="BX52">
+        <v>44</v>
+      </c>
+      <c r="BY52">
+        <v>45</v>
+      </c>
+      <c r="BZ52">
+        <v>46</v>
+      </c>
+      <c r="CA52">
+        <v>46</v>
+      </c>
+      <c r="CB52">
+        <v>47</v>
+      </c>
+      <c r="CC52">
+        <v>48</v>
+      </c>
+      <c r="CD52">
+        <v>48</v>
+      </c>
+      <c r="CE52">
+        <v>49</v>
+      </c>
+      <c r="CF52">
+        <v>50</v>
+      </c>
+      <c r="CG52">
+        <v>50</v>
+      </c>
+      <c r="CH52">
+        <v>51</v>
+      </c>
+      <c r="CI52">
+        <v>52</v>
+      </c>
+      <c r="CJ52">
+        <v>52</v>
+      </c>
+      <c r="CK52">
+        <v>53</v>
+      </c>
+      <c r="CL52">
+        <v>54</v>
+      </c>
+      <c r="CM52">
+        <v>54</v>
+      </c>
+      <c r="CN52">
+        <v>55</v>
+      </c>
+      <c r="CO52">
+        <v>56</v>
+      </c>
+      <c r="CP52">
+        <v>56</v>
+      </c>
+      <c r="CQ52">
+        <v>57</v>
+      </c>
+      <c r="CR52">
+        <v>58</v>
+      </c>
+      <c r="CS52">
+        <v>58</v>
+      </c>
+      <c r="CT52">
+        <v>59</v>
+      </c>
+      <c r="CU52">
         <v>60</v>
       </c>
-    </row>
-    <row r="53" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="CV52">
+        <v>60</v>
+      </c>
+      <c r="CW52" s="43">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -22666,14 +23267,161 @@
       <c r="AX53">
         <v>26</v>
       </c>
-      <c r="AY53" s="41">
+      <c r="AY53">
         <v>27</v>
       </c>
-      <c r="AZ53" s="3">
+      <c r="AZ53">
+        <v>27</v>
+      </c>
+      <c r="BA53">
+        <v>27</v>
+      </c>
+      <c r="BB53">
+        <v>28</v>
+      </c>
+      <c r="BC53">
+        <v>28</v>
+      </c>
+      <c r="BD53">
+        <v>28</v>
+      </c>
+      <c r="BE53">
+        <v>29</v>
+      </c>
+      <c r="BF53">
+        <v>29</v>
+      </c>
+      <c r="BG53">
+        <v>29</v>
+      </c>
+      <c r="BH53">
+        <v>30</v>
+      </c>
+      <c r="BI53">
+        <v>30</v>
+      </c>
+      <c r="BJ53">
+        <v>31</v>
+      </c>
+      <c r="BK53">
+        <v>31</v>
+      </c>
+      <c r="BL53">
+        <v>32</v>
+      </c>
+      <c r="BM53">
+        <v>32</v>
+      </c>
+      <c r="BN53">
+        <v>33</v>
+      </c>
+      <c r="BO53">
+        <v>33</v>
+      </c>
+      <c r="BP53">
+        <v>34</v>
+      </c>
+      <c r="BQ53">
+        <v>34</v>
+      </c>
+      <c r="BR53">
+        <v>35</v>
+      </c>
+      <c r="BS53">
+        <v>35</v>
+      </c>
+      <c r="BT53">
+        <v>36</v>
+      </c>
+      <c r="BU53">
+        <v>36</v>
+      </c>
+      <c r="BV53">
+        <v>37</v>
+      </c>
+      <c r="BW53">
+        <v>37</v>
+      </c>
+      <c r="BX53">
+        <v>38</v>
+      </c>
+      <c r="BY53">
+        <v>38</v>
+      </c>
+      <c r="BZ53">
+        <v>39</v>
+      </c>
+      <c r="CA53">
+        <v>39</v>
+      </c>
+      <c r="CB53">
+        <v>40</v>
+      </c>
+      <c r="CC53">
+        <v>40</v>
+      </c>
+      <c r="CD53">
+        <v>41</v>
+      </c>
+      <c r="CE53">
+        <v>41</v>
+      </c>
+      <c r="CF53">
+        <v>42</v>
+      </c>
+      <c r="CG53">
+        <v>42</v>
+      </c>
+      <c r="CH53">
+        <v>43</v>
+      </c>
+      <c r="CI53">
+        <v>43</v>
+      </c>
+      <c r="CJ53">
+        <v>44</v>
+      </c>
+      <c r="CK53">
+        <v>44</v>
+      </c>
+      <c r="CL53">
+        <v>45</v>
+      </c>
+      <c r="CM53">
+        <v>45</v>
+      </c>
+      <c r="CN53">
+        <v>46</v>
+      </c>
+      <c r="CO53">
+        <v>46</v>
+      </c>
+      <c r="CP53">
+        <v>47</v>
+      </c>
+      <c r="CQ53">
+        <v>47</v>
+      </c>
+      <c r="CR53">
+        <v>48</v>
+      </c>
+      <c r="CS53">
+        <v>48</v>
+      </c>
+      <c r="CT53">
+        <v>49</v>
+      </c>
+      <c r="CU53">
+        <v>49</v>
+      </c>
+      <c r="CV53">
         <v>50</v>
       </c>
-    </row>
-    <row r="54" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="CW53" s="43">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>49</v>
       </c>
@@ -22824,14 +23572,161 @@
       <c r="AX54">
         <v>45</v>
       </c>
-      <c r="AY54" s="41">
+      <c r="AY54">
         <v>45</v>
       </c>
-      <c r="AZ54" s="3">
+      <c r="AZ54">
+        <v>45</v>
+      </c>
+      <c r="BA54">
+        <v>46</v>
+      </c>
+      <c r="BB54">
+        <v>46</v>
+      </c>
+      <c r="BC54">
+        <v>47</v>
+      </c>
+      <c r="BD54">
+        <v>47</v>
+      </c>
+      <c r="BE54">
+        <v>48</v>
+      </c>
+      <c r="BF54">
+        <v>48</v>
+      </c>
+      <c r="BG54">
+        <v>49</v>
+      </c>
+      <c r="BH54">
+        <v>49</v>
+      </c>
+      <c r="BI54">
+        <v>50</v>
+      </c>
+      <c r="BJ54">
+        <v>50</v>
+      </c>
+      <c r="BK54">
+        <v>51</v>
+      </c>
+      <c r="BL54">
+        <v>51</v>
+      </c>
+      <c r="BM54">
+        <v>52</v>
+      </c>
+      <c r="BN54">
+        <v>52</v>
+      </c>
+      <c r="BO54">
+        <v>53</v>
+      </c>
+      <c r="BP54">
+        <v>53</v>
+      </c>
+      <c r="BQ54">
+        <v>54</v>
+      </c>
+      <c r="BR54">
+        <v>54</v>
+      </c>
+      <c r="BS54">
+        <v>55</v>
+      </c>
+      <c r="BT54">
+        <v>55</v>
+      </c>
+      <c r="BU54">
+        <v>56</v>
+      </c>
+      <c r="BV54">
+        <v>56</v>
+      </c>
+      <c r="BW54">
+        <v>57</v>
+      </c>
+      <c r="BX54">
+        <v>57</v>
+      </c>
+      <c r="BY54">
+        <v>58</v>
+      </c>
+      <c r="BZ54">
+        <v>58</v>
+      </c>
+      <c r="CA54">
+        <v>59</v>
+      </c>
+      <c r="CB54">
+        <v>59</v>
+      </c>
+      <c r="CC54">
+        <v>60</v>
+      </c>
+      <c r="CD54">
+        <v>60</v>
+      </c>
+      <c r="CE54">
+        <v>61</v>
+      </c>
+      <c r="CF54">
+        <v>61</v>
+      </c>
+      <c r="CG54">
+        <v>62</v>
+      </c>
+      <c r="CH54">
+        <v>62</v>
+      </c>
+      <c r="CI54">
+        <v>63</v>
+      </c>
+      <c r="CJ54">
+        <v>63</v>
+      </c>
+      <c r="CK54">
+        <v>64</v>
+      </c>
+      <c r="CL54">
+        <v>64</v>
+      </c>
+      <c r="CM54">
+        <v>65</v>
+      </c>
+      <c r="CN54">
+        <v>65</v>
+      </c>
+      <c r="CO54">
+        <v>66</v>
+      </c>
+      <c r="CP54">
+        <v>66</v>
+      </c>
+      <c r="CQ54">
+        <v>67</v>
+      </c>
+      <c r="CR54">
+        <v>67</v>
+      </c>
+      <c r="CS54">
+        <v>68</v>
+      </c>
+      <c r="CT54">
+        <v>68</v>
+      </c>
+      <c r="CU54">
+        <v>69</v>
+      </c>
+      <c r="CV54">
+        <v>69</v>
+      </c>
+      <c r="CW54" s="43">
         <v>70</v>
       </c>
     </row>
-    <row r="55" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>46</v>
       </c>
@@ -22982,14 +23877,161 @@
       <c r="AX55">
         <v>49</v>
       </c>
-      <c r="AY55" s="41">
+      <c r="AY55">
         <v>50</v>
       </c>
-      <c r="AZ55" s="3">
+      <c r="AZ55">
+        <v>51</v>
+      </c>
+      <c r="BA55">
+        <v>52</v>
+      </c>
+      <c r="BB55">
+        <v>53</v>
+      </c>
+      <c r="BC55">
+        <v>54</v>
+      </c>
+      <c r="BD55">
+        <v>55</v>
+      </c>
+      <c r="BE55">
+        <v>56</v>
+      </c>
+      <c r="BF55">
+        <v>57</v>
+      </c>
+      <c r="BG55">
+        <v>58</v>
+      </c>
+      <c r="BH55">
+        <v>59</v>
+      </c>
+      <c r="BI55">
+        <v>60</v>
+      </c>
+      <c r="BJ55">
+        <v>61</v>
+      </c>
+      <c r="BK55">
+        <v>62</v>
+      </c>
+      <c r="BL55">
+        <v>63</v>
+      </c>
+      <c r="BM55">
+        <v>64</v>
+      </c>
+      <c r="BN55">
+        <v>65</v>
+      </c>
+      <c r="BO55">
+        <v>66</v>
+      </c>
+      <c r="BP55">
+        <v>67</v>
+      </c>
+      <c r="BQ55">
+        <v>68</v>
+      </c>
+      <c r="BR55">
+        <v>69</v>
+      </c>
+      <c r="BS55">
+        <v>70</v>
+      </c>
+      <c r="BT55">
+        <v>71</v>
+      </c>
+      <c r="BU55">
+        <v>72</v>
+      </c>
+      <c r="BV55">
+        <v>73</v>
+      </c>
+      <c r="BW55">
+        <v>74</v>
+      </c>
+      <c r="BX55">
+        <v>75</v>
+      </c>
+      <c r="BY55">
+        <v>76</v>
+      </c>
+      <c r="BZ55">
+        <v>77</v>
+      </c>
+      <c r="CA55">
+        <v>78</v>
+      </c>
+      <c r="CB55">
+        <v>79</v>
+      </c>
+      <c r="CC55">
+        <v>80</v>
+      </c>
+      <c r="CD55">
+        <v>81</v>
+      </c>
+      <c r="CE55">
+        <v>82</v>
+      </c>
+      <c r="CF55">
+        <v>83</v>
+      </c>
+      <c r="CG55">
+        <v>84</v>
+      </c>
+      <c r="CH55">
+        <v>85</v>
+      </c>
+      <c r="CI55">
+        <v>86</v>
+      </c>
+      <c r="CJ55">
+        <v>87</v>
+      </c>
+      <c r="CK55">
+        <v>88</v>
+      </c>
+      <c r="CL55">
+        <v>89</v>
+      </c>
+      <c r="CM55">
+        <v>90</v>
+      </c>
+      <c r="CN55">
+        <v>91</v>
+      </c>
+      <c r="CO55">
+        <v>92</v>
+      </c>
+      <c r="CP55">
+        <v>93</v>
+      </c>
+      <c r="CQ55">
+        <v>94</v>
+      </c>
+      <c r="CR55">
+        <v>95</v>
+      </c>
+      <c r="CS55">
+        <v>96</v>
+      </c>
+      <c r="CT55">
+        <v>97</v>
+      </c>
+      <c r="CU55">
+        <v>98</v>
+      </c>
+      <c r="CV55">
+        <v>99</v>
+      </c>
+      <c r="CW55" s="43">
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>51</v>
       </c>
@@ -23140,14 +24182,161 @@
       <c r="AX56">
         <v>45</v>
       </c>
-      <c r="AY56" s="41">
+      <c r="AY56">
         <v>45</v>
       </c>
-      <c r="AZ56" s="3">
+      <c r="AZ56">
+        <v>46</v>
+      </c>
+      <c r="BA56">
+        <v>47</v>
+      </c>
+      <c r="BB56">
+        <v>47</v>
+      </c>
+      <c r="BC56">
+        <v>48</v>
+      </c>
+      <c r="BD56">
+        <v>49</v>
+      </c>
+      <c r="BE56">
+        <v>49</v>
+      </c>
+      <c r="BF56">
+        <v>50</v>
+      </c>
+      <c r="BG56">
+        <v>51</v>
+      </c>
+      <c r="BH56">
+        <v>51</v>
+      </c>
+      <c r="BI56">
+        <v>54</v>
+      </c>
+      <c r="BJ56">
+        <v>54</v>
+      </c>
+      <c r="BK56">
+        <v>55</v>
+      </c>
+      <c r="BL56">
+        <v>56</v>
+      </c>
+      <c r="BM56">
+        <v>57</v>
+      </c>
+      <c r="BN56">
+        <v>57</v>
+      </c>
+      <c r="BO56">
+        <v>60</v>
+      </c>
+      <c r="BP56">
+        <v>60</v>
+      </c>
+      <c r="BQ56">
+        <v>61</v>
+      </c>
+      <c r="BR56">
+        <v>62</v>
+      </c>
+      <c r="BS56">
+        <v>63</v>
+      </c>
+      <c r="BT56">
+        <v>63</v>
+      </c>
+      <c r="BU56">
+        <v>66</v>
+      </c>
+      <c r="BV56">
+        <v>66</v>
+      </c>
+      <c r="BW56">
+        <v>67</v>
+      </c>
+      <c r="BX56">
+        <v>68</v>
+      </c>
+      <c r="BY56">
+        <v>69</v>
+      </c>
+      <c r="BZ56">
+        <v>69</v>
+      </c>
+      <c r="CA56">
+        <v>72</v>
+      </c>
+      <c r="CB56">
+        <v>72</v>
+      </c>
+      <c r="CC56">
+        <v>73</v>
+      </c>
+      <c r="CD56">
+        <v>74</v>
+      </c>
+      <c r="CE56">
+        <v>75</v>
+      </c>
+      <c r="CF56">
+        <v>75</v>
+      </c>
+      <c r="CG56">
+        <v>78</v>
+      </c>
+      <c r="CH56">
+        <v>78</v>
+      </c>
+      <c r="CI56">
+        <v>79</v>
+      </c>
+      <c r="CJ56">
+        <v>80</v>
+      </c>
+      <c r="CK56">
+        <v>81</v>
+      </c>
+      <c r="CL56">
+        <v>81</v>
+      </c>
+      <c r="CM56">
+        <v>84</v>
+      </c>
+      <c r="CN56">
+        <v>84</v>
+      </c>
+      <c r="CO56">
+        <v>85</v>
+      </c>
+      <c r="CP56">
+        <v>86</v>
+      </c>
+      <c r="CQ56">
+        <v>87</v>
+      </c>
+      <c r="CR56">
+        <v>87</v>
+      </c>
+      <c r="CS56">
         <v>90</v>
       </c>
-    </row>
-    <row r="57" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="CT56">
+        <v>90</v>
+      </c>
+      <c r="CU56">
+        <v>90</v>
+      </c>
+      <c r="CV56">
+        <v>90</v>
+      </c>
+      <c r="CW56" s="43">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="57" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A57" s="27" t="s">
         <v>53</v>
       </c>
@@ -23298,14 +24487,161 @@
       <c r="AX57" s="27">
         <v>4</v>
       </c>
-      <c r="AY57" s="42">
+      <c r="AY57" s="27">
         <v>5</v>
       </c>
-      <c r="AZ57" s="7">
+      <c r="AZ57" s="27">
+        <v>5</v>
+      </c>
+      <c r="BA57" s="27">
+        <v>5</v>
+      </c>
+      <c r="BB57" s="27">
+        <v>5</v>
+      </c>
+      <c r="BC57" s="27">
+        <v>6</v>
+      </c>
+      <c r="BD57" s="27">
+        <v>6</v>
+      </c>
+      <c r="BE57" s="27">
+        <v>6</v>
+      </c>
+      <c r="BF57" s="27">
+        <v>7</v>
+      </c>
+      <c r="BG57" s="27">
+        <v>7</v>
+      </c>
+      <c r="BH57" s="27">
+        <v>7</v>
+      </c>
+      <c r="BI57" s="27">
+        <v>7</v>
+      </c>
+      <c r="BJ57" s="27">
+        <v>7</v>
+      </c>
+      <c r="BK57" s="27">
+        <v>8</v>
+      </c>
+      <c r="BL57" s="27">
+        <v>8</v>
+      </c>
+      <c r="BM57" s="27">
+        <v>9</v>
+      </c>
+      <c r="BN57" s="27">
+        <v>9</v>
+      </c>
+      <c r="BO57" s="27">
+        <v>9</v>
+      </c>
+      <c r="BP57" s="27">
+        <v>9</v>
+      </c>
+      <c r="BQ57" s="27">
+        <v>10</v>
+      </c>
+      <c r="BR57" s="27">
+        <v>10</v>
+      </c>
+      <c r="BS57" s="27">
+        <v>11</v>
+      </c>
+      <c r="BT57" s="27">
+        <v>11</v>
+      </c>
+      <c r="BU57" s="27">
+        <v>11</v>
+      </c>
+      <c r="BV57" s="27">
+        <v>11</v>
+      </c>
+      <c r="BW57" s="27">
+        <v>12</v>
+      </c>
+      <c r="BX57" s="27">
+        <v>12</v>
+      </c>
+      <c r="BY57" s="27">
+        <v>13</v>
+      </c>
+      <c r="BZ57" s="27">
+        <v>13</v>
+      </c>
+      <c r="CA57" s="27">
+        <v>13</v>
+      </c>
+      <c r="CB57" s="27">
+        <v>13</v>
+      </c>
+      <c r="CC57" s="27">
+        <v>14</v>
+      </c>
+      <c r="CD57" s="27">
+        <v>14</v>
+      </c>
+      <c r="CE57" s="27">
+        <v>15</v>
+      </c>
+      <c r="CF57" s="27">
+        <v>15</v>
+      </c>
+      <c r="CG57" s="27">
+        <v>15</v>
+      </c>
+      <c r="CH57" s="27">
+        <v>15</v>
+      </c>
+      <c r="CI57" s="27">
+        <v>16</v>
+      </c>
+      <c r="CJ57" s="27">
+        <v>16</v>
+      </c>
+      <c r="CK57" s="27">
+        <v>17</v>
+      </c>
+      <c r="CL57" s="27">
+        <v>17</v>
+      </c>
+      <c r="CM57" s="27">
+        <v>17</v>
+      </c>
+      <c r="CN57" s="27">
+        <v>17</v>
+      </c>
+      <c r="CO57" s="27">
+        <v>18</v>
+      </c>
+      <c r="CP57" s="27">
+        <v>18</v>
+      </c>
+      <c r="CQ57" s="27">
+        <v>19</v>
+      </c>
+      <c r="CR57" s="27">
+        <v>19</v>
+      </c>
+      <c r="CS57" s="27">
+        <v>19</v>
+      </c>
+      <c r="CT57" s="27">
+        <v>19</v>
+      </c>
+      <c r="CU57" s="27">
+        <v>21</v>
+      </c>
+      <c r="CV57" s="27">
+        <v>22</v>
+      </c>
+      <c r="CW57" s="45">
         <v>25</v>
       </c>
     </row>
-    <row r="58" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:101" x14ac:dyDescent="0.3">
       <c r="B58">
         <f>SUM(B50:B57)</f>
         <v>5</v>
@@ -23383,7 +24719,7 @@
         <v>95</v>
       </c>
       <c r="U58">
-        <f t="shared" ref="U58:AY58" si="41">SUM(U50:U57)</f>
+        <f t="shared" ref="U58:CF58" si="41">SUM(U50:U57)</f>
         <v>100</v>
       </c>
       <c r="V58">
@@ -23507,7 +24843,203 @@
         <v>250</v>
       </c>
       <c r="AZ58">
-        <f t="shared" ref="AZ58" si="42">SUM(AZ50:AZ57)</f>
+        <f t="shared" si="41"/>
+        <v>255</v>
+      </c>
+      <c r="BA58">
+        <f t="shared" si="41"/>
+        <v>260</v>
+      </c>
+      <c r="BB58">
+        <f t="shared" si="41"/>
+        <v>265</v>
+      </c>
+      <c r="BC58">
+        <f t="shared" si="41"/>
+        <v>270</v>
+      </c>
+      <c r="BD58">
+        <f t="shared" si="41"/>
+        <v>275</v>
+      </c>
+      <c r="BE58">
+        <f t="shared" si="41"/>
+        <v>280</v>
+      </c>
+      <c r="BF58">
+        <f t="shared" si="41"/>
+        <v>285</v>
+      </c>
+      <c r="BG58">
+        <f t="shared" si="41"/>
+        <v>290</v>
+      </c>
+      <c r="BH58">
+        <f t="shared" si="41"/>
+        <v>295</v>
+      </c>
+      <c r="BI58">
+        <f t="shared" si="41"/>
+        <v>300</v>
+      </c>
+      <c r="BJ58">
+        <f t="shared" si="41"/>
+        <v>305</v>
+      </c>
+      <c r="BK58">
+        <f t="shared" si="41"/>
+        <v>310</v>
+      </c>
+      <c r="BL58">
+        <f t="shared" si="41"/>
+        <v>315</v>
+      </c>
+      <c r="BM58">
+        <f t="shared" si="41"/>
+        <v>320</v>
+      </c>
+      <c r="BN58">
+        <f t="shared" si="41"/>
+        <v>325</v>
+      </c>
+      <c r="BO58">
+        <f t="shared" si="41"/>
+        <v>330</v>
+      </c>
+      <c r="BP58">
+        <f t="shared" si="41"/>
+        <v>335</v>
+      </c>
+      <c r="BQ58">
+        <f t="shared" si="41"/>
+        <v>340</v>
+      </c>
+      <c r="BR58">
+        <f t="shared" si="41"/>
+        <v>345</v>
+      </c>
+      <c r="BS58">
+        <f t="shared" si="41"/>
+        <v>350</v>
+      </c>
+      <c r="BT58">
+        <f t="shared" si="41"/>
+        <v>355</v>
+      </c>
+      <c r="BU58">
+        <f t="shared" si="41"/>
+        <v>360</v>
+      </c>
+      <c r="BV58">
+        <f t="shared" si="41"/>
+        <v>365</v>
+      </c>
+      <c r="BW58">
+        <f t="shared" si="41"/>
+        <v>370</v>
+      </c>
+      <c r="BX58">
+        <f t="shared" si="41"/>
+        <v>375</v>
+      </c>
+      <c r="BY58">
+        <f t="shared" si="41"/>
+        <v>380</v>
+      </c>
+      <c r="BZ58">
+        <f t="shared" si="41"/>
+        <v>385</v>
+      </c>
+      <c r="CA58">
+        <f t="shared" si="41"/>
+        <v>390</v>
+      </c>
+      <c r="CB58">
+        <f t="shared" si="41"/>
+        <v>395</v>
+      </c>
+      <c r="CC58">
+        <f t="shared" si="41"/>
+        <v>400</v>
+      </c>
+      <c r="CD58">
+        <f t="shared" si="41"/>
+        <v>405</v>
+      </c>
+      <c r="CE58">
+        <f t="shared" si="41"/>
+        <v>410</v>
+      </c>
+      <c r="CF58">
+        <f t="shared" si="41"/>
+        <v>415</v>
+      </c>
+      <c r="CG58">
+        <f t="shared" ref="CG58:CV58" si="42">SUM(CG50:CG57)</f>
+        <v>420</v>
+      </c>
+      <c r="CH58">
+        <f t="shared" si="42"/>
+        <v>425</v>
+      </c>
+      <c r="CI58">
+        <f t="shared" si="42"/>
+        <v>430</v>
+      </c>
+      <c r="CJ58">
+        <f t="shared" si="42"/>
+        <v>435</v>
+      </c>
+      <c r="CK58">
+        <f t="shared" si="42"/>
+        <v>440</v>
+      </c>
+      <c r="CL58">
+        <f t="shared" si="42"/>
+        <v>445</v>
+      </c>
+      <c r="CM58">
+        <f t="shared" si="42"/>
+        <v>450</v>
+      </c>
+      <c r="CN58">
+        <f t="shared" si="42"/>
+        <v>455</v>
+      </c>
+      <c r="CO58">
+        <f t="shared" si="42"/>
+        <v>460</v>
+      </c>
+      <c r="CP58">
+        <f t="shared" si="42"/>
+        <v>465</v>
+      </c>
+      <c r="CQ58">
+        <f t="shared" si="42"/>
+        <v>470</v>
+      </c>
+      <c r="CR58">
+        <f t="shared" si="42"/>
+        <v>475</v>
+      </c>
+      <c r="CS58">
+        <f t="shared" si="42"/>
+        <v>480</v>
+      </c>
+      <c r="CT58">
+        <f t="shared" si="42"/>
+        <v>485</v>
+      </c>
+      <c r="CU58">
+        <f t="shared" si="42"/>
+        <v>490</v>
+      </c>
+      <c r="CV58">
+        <f t="shared" si="42"/>
+        <v>495</v>
+      </c>
+      <c r="CW58">
+        <f t="shared" ref="CW58" si="43">SUM(CW50:CW57)</f>
         <v>500</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Separate CharacterService logic into CharacterAdventureService and CharacterMaintenanceService. Wanderer development path in the endurance test goes to 50th level now. Introduce liquibase schema generation possibility (maven plugin) and replace schema sql with a yaml format.
Bugfix: Converting defensive god recalculates character properties so the effect of the god is now correctly replaced.
</commit_message>
<xml_diff>
--- a/doc/caste_system.xlsx
+++ b/doc/caste_system.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/349dfb9748b30a92/Asztali gép/ataliasflame_2.0/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7618" documentId="8_{652F4476-B36F-42CD-831D-0D71B9923ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF92B959-0A93-4354-AC26-B19CB8EBFB5F}"/>
+  <xr:revisionPtr revIDLastSave="7947" documentId="8_{652F4476-B36F-42CD-831D-0D71B9923ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7441BDF2-FCCA-4460-8DEA-2B2E46327A39}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{CAF51EC3-63EC-48CD-AA7B-C21B3D5D222B}"/>
   </bookViews>
@@ -1557,7 +1557,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1403" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="85">
   <si>
     <t>csavargó</t>
   </si>
@@ -2012,7 +2012,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2084,22 +2084,8 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -3538,163 +3524,163 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="38"/>
-      <c r="B21" s="41" t="s">
+      <c r="B21" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="E21" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="F21" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="G21" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="H21" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="I21" s="43" t="s">
+      <c r="C21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21" t="s">
+        <v>39</v>
+      </c>
+      <c r="H21" t="s">
+        <v>39</v>
+      </c>
+      <c r="I21" t="s">
         <v>40</v>
       </c>
-      <c r="J21" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="K21" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="L21" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="M21" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="N21" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="O21" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="P21" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q21" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="R21" s="44" t="s">
+      <c r="J21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M21" t="s">
+        <v>39</v>
+      </c>
+      <c r="N21" t="s">
+        <v>39</v>
+      </c>
+      <c r="O21" t="s">
+        <v>39</v>
+      </c>
+      <c r="P21" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>39</v>
+      </c>
+      <c r="R21" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="38"/>
-      <c r="B22" s="41" t="s">
+      <c r="B22" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="F22" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="G22" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="H22" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="I22" s="43" t="s">
+      <c r="C22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H22" t="s">
+        <v>39</v>
+      </c>
+      <c r="I22" t="s">
         <v>40</v>
       </c>
-      <c r="J22" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="K22" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="L22" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="M22" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="N22" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="O22" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="P22" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q22" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="R22" s="44" t="s">
+      <c r="J22" t="s">
+        <v>39</v>
+      </c>
+      <c r="K22" t="s">
+        <v>39</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M22" t="s">
+        <v>39</v>
+      </c>
+      <c r="N22" t="s">
+        <v>39</v>
+      </c>
+      <c r="O22" t="s">
+        <v>39</v>
+      </c>
+      <c r="P22" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>39</v>
+      </c>
+      <c r="R22" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="39"/>
-      <c r="B23" s="42" t="s">
+      <c r="B23" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="D23" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="E23" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="F23" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="G23" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="H23" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="I23" s="43" t="s">
+      <c r="C23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" t="s">
+        <v>39</v>
+      </c>
+      <c r="H23" t="s">
+        <v>39</v>
+      </c>
+      <c r="I23" t="s">
         <v>40</v>
       </c>
-      <c r="J23" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="K23" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="L23" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="M23" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="N23" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="O23" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="P23" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q23" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="R23" s="44" t="s">
+      <c r="J23" t="s">
+        <v>39</v>
+      </c>
+      <c r="K23" t="s">
+        <v>39</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M23" t="s">
+        <v>39</v>
+      </c>
+      <c r="N23" t="s">
+        <v>39</v>
+      </c>
+      <c r="O23" t="s">
+        <v>39</v>
+      </c>
+      <c r="P23" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>39</v>
+      </c>
+      <c r="R23" s="1" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4334,7 +4320,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4699,13 +4685,13 @@
       <c r="Y1" t="s">
         <v>17</v>
       </c>
-      <c r="Z1" s="43" t="s">
+      <c r="Z1" t="s">
         <v>18</v>
       </c>
-      <c r="AA1" s="43" t="s">
+      <c r="AA1" t="s">
         <v>19</v>
       </c>
-      <c r="AB1" s="44" t="s">
+      <c r="AB1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="AC1" t="s">
@@ -4788,13 +4774,13 @@
       <c r="Y2">
         <v>3</v>
       </c>
-      <c r="Z2" s="43">
+      <c r="Z2">
         <v>8</v>
       </c>
-      <c r="AA2" s="43">
+      <c r="AA2">
         <v>25</v>
       </c>
-      <c r="AB2" s="44">
+      <c r="AB2" s="1">
         <v>50</v>
       </c>
       <c r="AC2">
@@ -4878,13 +4864,13 @@
       <c r="Y3">
         <v>3</v>
       </c>
-      <c r="Z3" s="43">
+      <c r="Z3">
         <v>12</v>
       </c>
-      <c r="AA3" s="43">
+      <c r="AA3">
         <v>27</v>
       </c>
-      <c r="AB3" s="44">
+      <c r="AB3" s="1">
         <v>55</v>
       </c>
       <c r="AC3">
@@ -4968,13 +4954,13 @@
       <c r="Y4">
         <v>2</v>
       </c>
-      <c r="Z4" s="43">
+      <c r="Z4">
         <v>12</v>
       </c>
-      <c r="AA4" s="43">
+      <c r="AA4">
         <v>26</v>
       </c>
-      <c r="AB4" s="44">
+      <c r="AB4" s="1">
         <v>60</v>
       </c>
       <c r="AC4">
@@ -5058,13 +5044,13 @@
       <c r="Y5">
         <v>3</v>
       </c>
-      <c r="Z5" s="43">
+      <c r="Z5">
         <v>12</v>
       </c>
-      <c r="AA5" s="43">
+      <c r="AA5">
         <v>27</v>
       </c>
-      <c r="AB5" s="44">
+      <c r="AB5" s="1">
         <v>50</v>
       </c>
       <c r="AC5">
@@ -5148,13 +5134,13 @@
       <c r="Y6">
         <v>4</v>
       </c>
-      <c r="Z6" s="43">
+      <c r="Z6">
         <v>16</v>
       </c>
-      <c r="AA6" s="43">
+      <c r="AA6">
         <v>45</v>
       </c>
-      <c r="AB6" s="44">
+      <c r="AB6" s="1">
         <v>70</v>
       </c>
       <c r="AC6">
@@ -5238,13 +5224,13 @@
       <c r="Y7">
         <v>5</v>
       </c>
-      <c r="Z7" s="43">
+      <c r="Z7">
         <v>20</v>
       </c>
-      <c r="AA7" s="43">
+      <c r="AA7">
         <v>50</v>
       </c>
-      <c r="AB7" s="44">
+      <c r="AB7" s="1">
         <v>100</v>
       </c>
       <c r="AC7">
@@ -5328,13 +5314,13 @@
       <c r="Y8">
         <v>4</v>
       </c>
-      <c r="Z8" s="43">
+      <c r="Z8">
         <v>18</v>
       </c>
-      <c r="AA8" s="43">
+      <c r="AA8">
         <v>45</v>
       </c>
-      <c r="AB8" s="44">
+      <c r="AB8" s="1">
         <v>90</v>
       </c>
       <c r="AC8">
@@ -5418,13 +5404,13 @@
       <c r="Y9" s="27">
         <v>1</v>
       </c>
-      <c r="Z9" s="45">
+      <c r="Z9" s="27">
         <v>2</v>
       </c>
-      <c r="AA9" s="45">
+      <c r="AA9" s="27">
         <v>5</v>
       </c>
-      <c r="AB9" s="46">
+      <c r="AB9" s="31">
         <v>25</v>
       </c>
       <c r="AC9" s="33">
@@ -11714,8 +11700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD573711-C846-40DC-8629-19A685998D3E}">
   <dimension ref="A1:CX58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="CS49" sqref="CS49"/>
+    <sheetView tabSelected="1" topLeftCell="AA16" workbookViewId="0">
+      <selection activeCell="AY36" sqref="AY36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11726,12 +11712,11 @@
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="20" width="3" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="24" max="47" width="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="47" width="4" bestFit="1" customWidth="1"/>
     <col min="48" max="50" width="4" customWidth="1"/>
     <col min="51" max="51" width="16" bestFit="1" customWidth="1"/>
-    <col min="52" max="55" width="4" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="53" max="55" width="4" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="4" customWidth="1"/>
     <col min="57" max="100" width="4" bestFit="1" customWidth="1"/>
     <col min="101" max="101" width="10.5546875" bestFit="1" customWidth="1"/>
@@ -18090,10 +18075,97 @@
       <c r="U25" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="V25" s="34" t="s">
+      <c r="V25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="W25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="X25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="AI25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="AJ25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="AK25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="AL25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="AR25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="AS25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="AT25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="AU25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="AV25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="AW25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="AX25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="AY25" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="W25" s="34" t="s">
+      <c r="AZ25" s="34" t="s">
         <v>12</v>
       </c>
     </row>
@@ -18161,10 +18233,97 @@
       <c r="U26">
         <v>16</v>
       </c>
-      <c r="V26" s="3">
+      <c r="V26">
+        <v>17</v>
+      </c>
+      <c r="W26">
+        <v>18</v>
+      </c>
+      <c r="X26">
+        <v>18</v>
+      </c>
+      <c r="Y26">
+        <v>19</v>
+      </c>
+      <c r="Z26">
+        <v>20</v>
+      </c>
+      <c r="AA26">
+        <v>20</v>
+      </c>
+      <c r="AB26">
+        <v>21</v>
+      </c>
+      <c r="AC26">
+        <v>22</v>
+      </c>
+      <c r="AD26">
+        <v>22</v>
+      </c>
+      <c r="AE26">
+        <v>23</v>
+      </c>
+      <c r="AF26">
+        <v>24</v>
+      </c>
+      <c r="AG26">
+        <v>24</v>
+      </c>
+      <c r="AH26">
+        <v>25</v>
+      </c>
+      <c r="AI26">
+        <v>26</v>
+      </c>
+      <c r="AJ26">
+        <v>26</v>
+      </c>
+      <c r="AK26">
+        <v>27</v>
+      </c>
+      <c r="AL26">
+        <v>28</v>
+      </c>
+      <c r="AM26">
+        <v>28</v>
+      </c>
+      <c r="AN26">
+        <v>29</v>
+      </c>
+      <c r="AO26">
+        <v>30</v>
+      </c>
+      <c r="AP26">
+        <v>30</v>
+      </c>
+      <c r="AQ26">
+        <v>31</v>
+      </c>
+      <c r="AR26">
+        <v>32</v>
+      </c>
+      <c r="AS26">
+        <v>32</v>
+      </c>
+      <c r="AT26">
+        <v>33</v>
+      </c>
+      <c r="AU26">
+        <v>34</v>
+      </c>
+      <c r="AV26">
+        <v>34</v>
+      </c>
+      <c r="AW26">
         <v>35</v>
       </c>
-      <c r="W26" s="3">
+      <c r="AX26">
+        <v>35</v>
+      </c>
+      <c r="AY26" s="41">
+        <v>35</v>
+      </c>
+      <c r="AZ26" s="3">
         <v>75</v>
       </c>
     </row>
@@ -18232,10 +18391,97 @@
       <c r="U27">
         <v>18</v>
       </c>
-      <c r="V27" s="3">
+      <c r="V27">
+        <v>19</v>
+      </c>
+      <c r="W27">
+        <v>20</v>
+      </c>
+      <c r="X27">
+        <v>21</v>
+      </c>
+      <c r="Y27">
+        <v>22</v>
+      </c>
+      <c r="Z27">
+        <v>22</v>
+      </c>
+      <c r="AA27">
+        <v>23</v>
+      </c>
+      <c r="AB27">
+        <v>24</v>
+      </c>
+      <c r="AC27">
+        <v>25</v>
+      </c>
+      <c r="AD27">
+        <v>26</v>
+      </c>
+      <c r="AE27">
+        <v>26</v>
+      </c>
+      <c r="AF27">
+        <v>27</v>
+      </c>
+      <c r="AG27">
+        <v>28</v>
+      </c>
+      <c r="AH27">
+        <v>29</v>
+      </c>
+      <c r="AI27">
+        <v>30</v>
+      </c>
+      <c r="AJ27">
+        <v>30</v>
+      </c>
+      <c r="AK27">
+        <v>31</v>
+      </c>
+      <c r="AL27">
+        <v>32</v>
+      </c>
+      <c r="AM27">
+        <v>33</v>
+      </c>
+      <c r="AN27">
+        <v>34</v>
+      </c>
+      <c r="AO27">
+        <v>34</v>
+      </c>
+      <c r="AP27">
+        <v>35</v>
+      </c>
+      <c r="AQ27">
+        <v>36</v>
+      </c>
+      <c r="AR27">
+        <v>37</v>
+      </c>
+      <c r="AS27">
+        <v>38</v>
+      </c>
+      <c r="AT27">
+        <v>38</v>
+      </c>
+      <c r="AU27">
+        <v>39</v>
+      </c>
+      <c r="AV27">
+        <v>40</v>
+      </c>
+      <c r="AW27">
+        <v>41</v>
+      </c>
+      <c r="AX27">
         <v>42</v>
       </c>
-      <c r="W27" s="3">
+      <c r="AY27" s="41">
+        <v>42</v>
+      </c>
+      <c r="AZ27" s="3">
         <v>80</v>
       </c>
     </row>
@@ -18303,10 +18549,97 @@
       <c r="U28">
         <v>20</v>
       </c>
-      <c r="V28" s="3">
+      <c r="V28">
+        <v>21</v>
+      </c>
+      <c r="W28">
+        <v>22</v>
+      </c>
+      <c r="X28">
+        <v>23</v>
+      </c>
+      <c r="Y28">
+        <v>24</v>
+      </c>
+      <c r="Z28">
+        <v>24</v>
+      </c>
+      <c r="AA28">
+        <v>25</v>
+      </c>
+      <c r="AB28">
+        <v>26</v>
+      </c>
+      <c r="AC28">
+        <v>27</v>
+      </c>
+      <c r="AD28">
+        <v>28</v>
+      </c>
+      <c r="AE28">
+        <v>28</v>
+      </c>
+      <c r="AF28">
+        <v>29</v>
+      </c>
+      <c r="AG28">
+        <v>30</v>
+      </c>
+      <c r="AH28">
+        <v>31</v>
+      </c>
+      <c r="AI28">
+        <v>32</v>
+      </c>
+      <c r="AJ28">
+        <v>32</v>
+      </c>
+      <c r="AK28">
+        <v>33</v>
+      </c>
+      <c r="AL28">
+        <v>34</v>
+      </c>
+      <c r="AM28">
+        <v>35</v>
+      </c>
+      <c r="AN28">
+        <v>36</v>
+      </c>
+      <c r="AO28">
+        <v>36</v>
+      </c>
+      <c r="AP28">
+        <v>37</v>
+      </c>
+      <c r="AQ28">
+        <v>38</v>
+      </c>
+      <c r="AR28">
+        <v>39</v>
+      </c>
+      <c r="AS28">
+        <v>40</v>
+      </c>
+      <c r="AT28">
+        <v>40</v>
+      </c>
+      <c r="AU28">
+        <v>41</v>
+      </c>
+      <c r="AV28">
+        <v>42</v>
+      </c>
+      <c r="AW28">
+        <v>43</v>
+      </c>
+      <c r="AX28">
+        <v>44</v>
+      </c>
+      <c r="AY28" s="41">
         <v>45</v>
       </c>
-      <c r="W28" s="3">
+      <c r="AZ28" s="3">
         <v>85</v>
       </c>
     </row>
@@ -18374,10 +18707,97 @@
       <c r="U29">
         <v>18</v>
       </c>
-      <c r="V29" s="3">
+      <c r="V29">
+        <v>19</v>
+      </c>
+      <c r="W29">
+        <v>20</v>
+      </c>
+      <c r="X29">
+        <v>21</v>
+      </c>
+      <c r="Y29">
+        <v>22</v>
+      </c>
+      <c r="Z29">
+        <v>23</v>
+      </c>
+      <c r="AA29">
+        <v>24</v>
+      </c>
+      <c r="AB29">
+        <v>25</v>
+      </c>
+      <c r="AC29">
+        <v>26</v>
+      </c>
+      <c r="AD29">
+        <v>27</v>
+      </c>
+      <c r="AE29">
+        <v>28</v>
+      </c>
+      <c r="AF29">
+        <v>29</v>
+      </c>
+      <c r="AG29">
+        <v>30</v>
+      </c>
+      <c r="AH29">
+        <v>31</v>
+      </c>
+      <c r="AI29">
+        <v>32</v>
+      </c>
+      <c r="AJ29">
+        <v>33</v>
+      </c>
+      <c r="AK29">
+        <v>34</v>
+      </c>
+      <c r="AL29">
+        <v>35</v>
+      </c>
+      <c r="AM29">
+        <v>36</v>
+      </c>
+      <c r="AN29">
+        <v>37</v>
+      </c>
+      <c r="AO29">
+        <v>38</v>
+      </c>
+      <c r="AP29">
+        <v>39</v>
+      </c>
+      <c r="AQ29">
+        <v>40</v>
+      </c>
+      <c r="AR29">
+        <v>41</v>
+      </c>
+      <c r="AS29">
+        <v>42</v>
+      </c>
+      <c r="AT29">
+        <v>43</v>
+      </c>
+      <c r="AU29">
+        <v>44</v>
+      </c>
+      <c r="AV29">
         <v>45</v>
       </c>
-      <c r="W29" s="3">
+      <c r="AW29">
+        <v>45</v>
+      </c>
+      <c r="AX29">
+        <v>45</v>
+      </c>
+      <c r="AY29" s="41">
+        <v>45</v>
+      </c>
+      <c r="AZ29" s="3">
         <v>85</v>
       </c>
     </row>
@@ -18445,10 +18865,97 @@
       <c r="U30">
         <v>7</v>
       </c>
-      <c r="V30" s="3">
+      <c r="V30">
+        <v>7</v>
+      </c>
+      <c r="W30">
+        <v>7</v>
+      </c>
+      <c r="X30">
+        <v>7</v>
+      </c>
+      <c r="Y30">
+        <v>7</v>
+      </c>
+      <c r="Z30">
+        <v>8</v>
+      </c>
+      <c r="AA30">
+        <v>9</v>
+      </c>
+      <c r="AB30">
+        <v>9</v>
+      </c>
+      <c r="AC30">
+        <v>9</v>
+      </c>
+      <c r="AD30">
+        <v>9</v>
+      </c>
+      <c r="AE30">
+        <v>10</v>
+      </c>
+      <c r="AF30">
+        <v>10</v>
+      </c>
+      <c r="AG30">
+        <v>11</v>
+      </c>
+      <c r="AH30">
+        <v>11</v>
+      </c>
+      <c r="AI30">
+        <v>11</v>
+      </c>
+      <c r="AJ30">
+        <v>13</v>
+      </c>
+      <c r="AK30">
+        <v>13</v>
+      </c>
+      <c r="AL30">
+        <v>13</v>
+      </c>
+      <c r="AM30">
+        <v>13</v>
+      </c>
+      <c r="AN30">
+        <v>13</v>
+      </c>
+      <c r="AO30">
+        <v>14</v>
+      </c>
+      <c r="AP30">
+        <v>15</v>
+      </c>
+      <c r="AQ30">
+        <v>15</v>
+      </c>
+      <c r="AR30">
+        <v>15</v>
+      </c>
+      <c r="AS30">
+        <v>15</v>
+      </c>
+      <c r="AT30">
+        <v>16</v>
+      </c>
+      <c r="AU30">
+        <v>16</v>
+      </c>
+      <c r="AV30">
+        <v>17</v>
+      </c>
+      <c r="AW30">
+        <v>18</v>
+      </c>
+      <c r="AX30">
+        <v>19</v>
+      </c>
+      <c r="AY30" s="41">
         <v>20</v>
       </c>
-      <c r="W30" s="3">
+      <c r="AZ30" s="3">
         <v>40</v>
       </c>
     </row>
@@ -18516,10 +19023,97 @@
       <c r="U31">
         <v>7</v>
       </c>
-      <c r="V31" s="3">
+      <c r="V31">
+        <v>7</v>
+      </c>
+      <c r="W31">
+        <v>7</v>
+      </c>
+      <c r="X31">
+        <v>7</v>
+      </c>
+      <c r="Y31">
+        <v>7</v>
+      </c>
+      <c r="Z31">
+        <v>8</v>
+      </c>
+      <c r="AA31">
+        <v>8</v>
+      </c>
+      <c r="AB31">
+        <v>8</v>
+      </c>
+      <c r="AC31">
+        <v>8</v>
+      </c>
+      <c r="AD31">
+        <v>9</v>
+      </c>
+      <c r="AE31">
+        <v>10</v>
+      </c>
+      <c r="AF31">
+        <v>10</v>
+      </c>
+      <c r="AG31">
+        <v>10</v>
+      </c>
+      <c r="AH31">
+        <v>10</v>
+      </c>
+      <c r="AI31">
+        <v>10</v>
+      </c>
+      <c r="AJ31">
+        <v>11</v>
+      </c>
+      <c r="AK31">
+        <v>11</v>
+      </c>
+      <c r="AL31">
+        <v>11</v>
+      </c>
+      <c r="AM31">
+        <v>12</v>
+      </c>
+      <c r="AN31">
+        <v>12</v>
+      </c>
+      <c r="AO31">
+        <v>13</v>
+      </c>
+      <c r="AP31">
+        <v>13</v>
+      </c>
+      <c r="AQ31">
+        <v>13</v>
+      </c>
+      <c r="AR31">
+        <v>13</v>
+      </c>
+      <c r="AS31">
+        <v>14</v>
+      </c>
+      <c r="AT31">
+        <v>15</v>
+      </c>
+      <c r="AU31">
+        <v>15</v>
+      </c>
+      <c r="AV31">
+        <v>15</v>
+      </c>
+      <c r="AW31">
+        <v>15</v>
+      </c>
+      <c r="AX31">
+        <v>16</v>
+      </c>
+      <c r="AY31" s="41">
         <v>18</v>
       </c>
-      <c r="W31" s="3">
+      <c r="AZ31" s="3">
         <v>25</v>
       </c>
     </row>
@@ -18587,10 +19181,97 @@
       <c r="U32">
         <v>2</v>
       </c>
-      <c r="V32" s="3">
+      <c r="V32">
+        <v>3</v>
+      </c>
+      <c r="W32">
+        <v>4</v>
+      </c>
+      <c r="X32">
         <v>5</v>
       </c>
-      <c r="W32" s="3">
+      <c r="Y32">
+        <v>5</v>
+      </c>
+      <c r="Z32">
+        <v>5</v>
+      </c>
+      <c r="AA32">
+        <v>5</v>
+      </c>
+      <c r="AB32">
+        <v>5</v>
+      </c>
+      <c r="AC32">
+        <v>5</v>
+      </c>
+      <c r="AD32">
+        <v>5</v>
+      </c>
+      <c r="AE32">
+        <v>5</v>
+      </c>
+      <c r="AF32">
+        <v>5</v>
+      </c>
+      <c r="AG32">
+        <v>5</v>
+      </c>
+      <c r="AH32">
+        <v>5</v>
+      </c>
+      <c r="AI32">
+        <v>5</v>
+      </c>
+      <c r="AJ32">
+        <v>5</v>
+      </c>
+      <c r="AK32">
+        <v>5</v>
+      </c>
+      <c r="AL32">
+        <v>5</v>
+      </c>
+      <c r="AM32">
+        <v>5</v>
+      </c>
+      <c r="AN32">
+        <v>5</v>
+      </c>
+      <c r="AO32">
+        <v>5</v>
+      </c>
+      <c r="AP32">
+        <v>5</v>
+      </c>
+      <c r="AQ32">
+        <v>5</v>
+      </c>
+      <c r="AR32">
+        <v>5</v>
+      </c>
+      <c r="AS32">
+        <v>5</v>
+      </c>
+      <c r="AT32">
+        <v>5</v>
+      </c>
+      <c r="AU32">
+        <v>5</v>
+      </c>
+      <c r="AV32">
+        <v>5</v>
+      </c>
+      <c r="AW32">
+        <v>5</v>
+      </c>
+      <c r="AX32">
+        <v>5</v>
+      </c>
+      <c r="AY32" s="41">
+        <v>5</v>
+      </c>
+      <c r="AZ32" s="3">
         <v>10</v>
       </c>
     </row>
@@ -18658,10 +19339,97 @@
       <c r="U33" s="27">
         <v>12</v>
       </c>
-      <c r="V33" s="7">
+      <c r="V33" s="27">
+        <v>12</v>
+      </c>
+      <c r="W33" s="27">
+        <v>12</v>
+      </c>
+      <c r="X33" s="27">
+        <v>13</v>
+      </c>
+      <c r="Y33" s="27">
+        <v>14</v>
+      </c>
+      <c r="Z33" s="27">
+        <v>15</v>
+      </c>
+      <c r="AA33" s="27">
+        <v>16</v>
+      </c>
+      <c r="AB33" s="27">
+        <v>17</v>
+      </c>
+      <c r="AC33" s="27">
+        <v>18</v>
+      </c>
+      <c r="AD33" s="27">
+        <v>19</v>
+      </c>
+      <c r="AE33" s="27">
+        <v>20</v>
+      </c>
+      <c r="AF33" s="27">
+        <v>21</v>
+      </c>
+      <c r="AG33" s="27">
+        <v>22</v>
+      </c>
+      <c r="AH33" s="27">
+        <v>23</v>
+      </c>
+      <c r="AI33" s="27">
+        <v>24</v>
+      </c>
+      <c r="AJ33" s="27">
+        <v>25</v>
+      </c>
+      <c r="AK33" s="27">
+        <v>26</v>
+      </c>
+      <c r="AL33" s="27">
+        <v>27</v>
+      </c>
+      <c r="AM33" s="27">
+        <v>28</v>
+      </c>
+      <c r="AN33" s="27">
+        <v>29</v>
+      </c>
+      <c r="AO33" s="27">
+        <v>30</v>
+      </c>
+      <c r="AP33" s="27">
+        <v>31</v>
+      </c>
+      <c r="AQ33" s="27">
+        <v>32</v>
+      </c>
+      <c r="AR33" s="27">
+        <v>33</v>
+      </c>
+      <c r="AS33" s="27">
+        <v>34</v>
+      </c>
+      <c r="AT33" s="27">
+        <v>35</v>
+      </c>
+      <c r="AU33" s="27">
+        <v>36</v>
+      </c>
+      <c r="AV33" s="27">
+        <v>37</v>
+      </c>
+      <c r="AW33" s="27">
+        <v>38</v>
+      </c>
+      <c r="AX33" s="27">
+        <v>39</v>
+      </c>
+      <c r="AY33" s="42">
         <v>40</v>
       </c>
-      <c r="W33" s="7">
+      <c r="AZ33" s="7">
         <v>100</v>
       </c>
     </row>
@@ -18671,7 +19439,7 @@
         <v>5</v>
       </c>
       <c r="C34">
-        <f t="shared" ref="C34:U34" si="18">SUM(C26:C33)</f>
+        <f t="shared" ref="C34:AX34" si="18">SUM(C26:C33)</f>
         <v>10</v>
       </c>
       <c r="D34">
@@ -18746,12 +19514,128 @@
         <f t="shared" si="18"/>
         <v>100</v>
       </c>
-      <c r="V34" s="3">
-        <f>SUM(V26:V33)</f>
+      <c r="V34">
+        <f t="shared" si="18"/>
+        <v>105</v>
+      </c>
+      <c r="W34">
+        <f t="shared" si="18"/>
+        <v>110</v>
+      </c>
+      <c r="X34">
+        <f t="shared" si="18"/>
+        <v>115</v>
+      </c>
+      <c r="Y34">
+        <f t="shared" si="18"/>
+        <v>120</v>
+      </c>
+      <c r="Z34">
+        <f t="shared" si="18"/>
+        <v>125</v>
+      </c>
+      <c r="AA34">
+        <f t="shared" si="18"/>
+        <v>130</v>
+      </c>
+      <c r="AB34">
+        <f t="shared" si="18"/>
+        <v>135</v>
+      </c>
+      <c r="AC34">
+        <f t="shared" si="18"/>
+        <v>140</v>
+      </c>
+      <c r="AD34">
+        <f t="shared" si="18"/>
+        <v>145</v>
+      </c>
+      <c r="AE34">
+        <f t="shared" si="18"/>
+        <v>150</v>
+      </c>
+      <c r="AF34">
+        <f t="shared" si="18"/>
+        <v>155</v>
+      </c>
+      <c r="AG34">
+        <f t="shared" si="18"/>
+        <v>160</v>
+      </c>
+      <c r="AH34">
+        <f t="shared" si="18"/>
+        <v>165</v>
+      </c>
+      <c r="AI34">
+        <f t="shared" si="18"/>
+        <v>170</v>
+      </c>
+      <c r="AJ34">
+        <f t="shared" si="18"/>
+        <v>175</v>
+      </c>
+      <c r="AK34">
+        <f t="shared" si="18"/>
+        <v>180</v>
+      </c>
+      <c r="AL34">
+        <f t="shared" si="18"/>
+        <v>185</v>
+      </c>
+      <c r="AM34">
+        <f t="shared" si="18"/>
+        <v>190</v>
+      </c>
+      <c r="AN34">
+        <f t="shared" si="18"/>
+        <v>195</v>
+      </c>
+      <c r="AO34">
+        <f t="shared" si="18"/>
+        <v>200</v>
+      </c>
+      <c r="AP34">
+        <f t="shared" si="18"/>
+        <v>205</v>
+      </c>
+      <c r="AQ34">
+        <f t="shared" si="18"/>
+        <v>210</v>
+      </c>
+      <c r="AR34">
+        <f t="shared" si="18"/>
+        <v>215</v>
+      </c>
+      <c r="AS34">
+        <f t="shared" si="18"/>
+        <v>220</v>
+      </c>
+      <c r="AT34">
+        <f t="shared" si="18"/>
+        <v>225</v>
+      </c>
+      <c r="AU34">
+        <f t="shared" si="18"/>
+        <v>230</v>
+      </c>
+      <c r="AV34">
+        <f t="shared" si="18"/>
+        <v>235</v>
+      </c>
+      <c r="AW34">
+        <f t="shared" si="18"/>
+        <v>240</v>
+      </c>
+      <c r="AX34">
+        <f t="shared" si="18"/>
+        <v>245</v>
+      </c>
+      <c r="AY34" s="41">
+        <f>SUM(AY26:AY33)</f>
         <v>250</v>
       </c>
-      <c r="W34" s="3">
-        <f>SUM(W26:W33)</f>
+      <c r="AZ34" s="3">
+        <f>SUM(AZ26:AZ33)</f>
         <v>500</v>
       </c>
     </row>
@@ -21957,7 +22841,7 @@
       <c r="T49" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="U49" s="47" t="s">
+      <c r="U49" s="36" t="s">
         <v>18</v>
       </c>
       <c r="V49" s="28" t="s">
@@ -22047,7 +22931,7 @@
       <c r="AX49" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="AY49" s="47" t="s">
+      <c r="AY49" s="36" t="s">
         <v>19</v>
       </c>
       <c r="AZ49" s="28" t="s">
@@ -22077,7 +22961,7 @@
       <c r="BH49" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="BI49" s="48" t="s">
+      <c r="BI49" s="28" t="s">
         <v>82</v>
       </c>
       <c r="BJ49" s="28" t="s">
@@ -22107,7 +22991,7 @@
       <c r="BR49" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="BS49" s="48" t="s">
+      <c r="BS49" s="28" t="s">
         <v>82</v>
       </c>
       <c r="BT49" s="28" t="s">
@@ -22137,7 +23021,7 @@
       <c r="CB49" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="CC49" s="48" t="s">
+      <c r="CC49" s="28" t="s">
         <v>82</v>
       </c>
       <c r="CD49" s="28" t="s">
@@ -22167,7 +23051,7 @@
       <c r="CL49" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="CM49" s="48" t="s">
+      <c r="CM49" s="28" t="s">
         <v>82</v>
       </c>
       <c r="CN49" s="28" t="s">
@@ -22197,7 +23081,7 @@
       <c r="CV49" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="CW49" s="47" t="s">
+      <c r="CW49" s="36" t="s">
         <v>20</v>
       </c>
     </row>
@@ -22502,7 +23386,7 @@
       <c r="CV50">
         <v>50</v>
       </c>
-      <c r="CW50" s="43">
+      <c r="CW50">
         <v>50</v>
       </c>
     </row>
@@ -22807,7 +23691,7 @@
       <c r="CV51">
         <v>55</v>
       </c>
-      <c r="CW51" s="43">
+      <c r="CW51">
         <v>55</v>
       </c>
     </row>
@@ -23112,7 +23996,7 @@
       <c r="CV52">
         <v>60</v>
       </c>
-      <c r="CW52" s="43">
+      <c r="CW52">
         <v>60</v>
       </c>
     </row>
@@ -23417,7 +24301,7 @@
       <c r="CV53">
         <v>50</v>
       </c>
-      <c r="CW53" s="43">
+      <c r="CW53">
         <v>50</v>
       </c>
     </row>
@@ -23722,7 +24606,7 @@
       <c r="CV54">
         <v>69</v>
       </c>
-      <c r="CW54" s="43">
+      <c r="CW54">
         <v>70</v>
       </c>
     </row>
@@ -24027,7 +24911,7 @@
       <c r="CV55">
         <v>99</v>
       </c>
-      <c r="CW55" s="43">
+      <c r="CW55">
         <v>100</v>
       </c>
     </row>
@@ -24332,7 +25216,7 @@
       <c r="CV56">
         <v>90</v>
       </c>
-      <c r="CW56" s="43">
+      <c r="CW56">
         <v>90</v>
       </c>
     </row>
@@ -24637,7 +25521,7 @@
       <c r="CV57" s="27">
         <v>22</v>
       </c>
-      <c r="CW57" s="45">
+      <c r="CW57" s="27">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Introduce Energy class to centralize health and magic related functions. Add magic point assertions to calculation tests.
</commit_message>
<xml_diff>
--- a/doc/caste_system.xlsx
+++ b/doc/caste_system.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/349dfb9748b30a92/Asztali gép/ataliasflame_2.0/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7947" documentId="8_{652F4476-B36F-42CD-831D-0D71B9923ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7441BDF2-FCCA-4460-8DEA-2B2E46327A39}"/>
+  <xr:revisionPtr revIDLastSave="8332" documentId="8_{652F4476-B36F-42CD-831D-0D71B9923ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD120FA1-8182-4EAD-955F-AEC68DF05096}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{CAF51EC3-63EC-48CD-AA7B-C21B3D5D222B}"/>
   </bookViews>
@@ -1557,7 +1557,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1481" uniqueCount="85">
   <si>
     <t>csavargó</t>
   </si>
@@ -2012,7 +2012,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2084,8 +2084,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -11700,8 +11698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD573711-C846-40DC-8629-19A685998D3E}">
   <dimension ref="A1:CX58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA16" workbookViewId="0">
-      <selection activeCell="AY36" sqref="AY36"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="CS31" sqref="CS31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11715,11 +11713,10 @@
     <col min="22" max="47" width="4" bestFit="1" customWidth="1"/>
     <col min="48" max="50" width="4" customWidth="1"/>
     <col min="51" max="51" width="16" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="53" max="55" width="4" bestFit="1" customWidth="1"/>
+    <col min="52" max="55" width="4" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="4" customWidth="1"/>
     <col min="57" max="100" width="4" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="102" max="102" width="7.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -18165,7 +18162,154 @@
       <c r="AY25" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="AZ25" s="34" t="s">
+      <c r="AZ25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BA25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BB25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BC25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BD25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BE25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BF25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BG25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BH25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BI25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BJ25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BK25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BL25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BM25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BN25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BO25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BP25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BQ25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BR25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BS25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BT25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BU25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BV25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BW25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BX25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BY25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="BZ25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CA25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CB25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CC25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CD25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CE25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CF25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CG25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CH25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CI25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CJ25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CK25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CL25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CM25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CN25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CO25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CP25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CQ25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CR25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CS25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CT25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CU25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CV25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="CW25" s="34" t="s">
         <v>12</v>
       </c>
     </row>
@@ -18320,10 +18464,157 @@
       <c r="AX26">
         <v>35</v>
       </c>
-      <c r="AY26" s="41">
+      <c r="AY26">
         <v>35</v>
       </c>
-      <c r="AZ26" s="3">
+      <c r="AZ26">
+        <v>36</v>
+      </c>
+      <c r="BA26">
+        <v>37</v>
+      </c>
+      <c r="BB26">
+        <v>38</v>
+      </c>
+      <c r="BC26">
+        <v>39</v>
+      </c>
+      <c r="BD26">
+        <v>39</v>
+      </c>
+      <c r="BE26">
+        <v>40</v>
+      </c>
+      <c r="BF26">
+        <v>41</v>
+      </c>
+      <c r="BG26">
+        <v>42</v>
+      </c>
+      <c r="BH26">
+        <v>43</v>
+      </c>
+      <c r="BI26">
+        <v>43</v>
+      </c>
+      <c r="BJ26">
+        <v>44</v>
+      </c>
+      <c r="BK26">
+        <v>45</v>
+      </c>
+      <c r="BL26">
+        <v>46</v>
+      </c>
+      <c r="BM26">
+        <v>47</v>
+      </c>
+      <c r="BN26">
+        <v>47</v>
+      </c>
+      <c r="BO26">
+        <v>48</v>
+      </c>
+      <c r="BP26">
+        <v>49</v>
+      </c>
+      <c r="BQ26">
+        <v>50</v>
+      </c>
+      <c r="BR26">
+        <v>51</v>
+      </c>
+      <c r="BS26">
+        <v>51</v>
+      </c>
+      <c r="BT26">
+        <v>52</v>
+      </c>
+      <c r="BU26">
+        <v>53</v>
+      </c>
+      <c r="BV26">
+        <v>54</v>
+      </c>
+      <c r="BW26">
+        <v>55</v>
+      </c>
+      <c r="BX26">
+        <v>55</v>
+      </c>
+      <c r="BY26">
+        <v>56</v>
+      </c>
+      <c r="BZ26">
+        <v>57</v>
+      </c>
+      <c r="CA26">
+        <v>58</v>
+      </c>
+      <c r="CB26">
+        <v>59</v>
+      </c>
+      <c r="CC26">
+        <v>59</v>
+      </c>
+      <c r="CD26">
+        <v>60</v>
+      </c>
+      <c r="CE26">
+        <v>61</v>
+      </c>
+      <c r="CF26">
+        <v>62</v>
+      </c>
+      <c r="CG26">
+        <v>63</v>
+      </c>
+      <c r="CH26">
+        <v>63</v>
+      </c>
+      <c r="CI26">
+        <v>64</v>
+      </c>
+      <c r="CJ26">
+        <v>65</v>
+      </c>
+      <c r="CK26">
+        <v>66</v>
+      </c>
+      <c r="CL26">
+        <v>67</v>
+      </c>
+      <c r="CM26">
+        <v>67</v>
+      </c>
+      <c r="CN26">
+        <v>68</v>
+      </c>
+      <c r="CO26">
+        <v>69</v>
+      </c>
+      <c r="CP26">
+        <v>70</v>
+      </c>
+      <c r="CQ26">
+        <v>71</v>
+      </c>
+      <c r="CR26">
+        <v>71</v>
+      </c>
+      <c r="CS26">
+        <v>72</v>
+      </c>
+      <c r="CT26">
+        <v>73</v>
+      </c>
+      <c r="CU26">
+        <v>74</v>
+      </c>
+      <c r="CV26">
+        <v>75</v>
+      </c>
+      <c r="CW26" s="3">
         <v>75</v>
       </c>
     </row>
@@ -18478,10 +18769,157 @@
       <c r="AX27">
         <v>42</v>
       </c>
-      <c r="AY27" s="41">
+      <c r="AY27">
         <v>42</v>
       </c>
-      <c r="AZ27" s="3">
+      <c r="AZ27">
+        <v>42</v>
+      </c>
+      <c r="BA27">
+        <v>42</v>
+      </c>
+      <c r="BB27">
+        <v>42</v>
+      </c>
+      <c r="BC27">
+        <v>42</v>
+      </c>
+      <c r="BD27">
+        <v>43</v>
+      </c>
+      <c r="BE27">
+        <v>44</v>
+      </c>
+      <c r="BF27">
+        <v>45</v>
+      </c>
+      <c r="BG27">
+        <v>46</v>
+      </c>
+      <c r="BH27">
+        <v>47</v>
+      </c>
+      <c r="BI27">
+        <v>47</v>
+      </c>
+      <c r="BJ27">
+        <v>48</v>
+      </c>
+      <c r="BK27">
+        <v>49</v>
+      </c>
+      <c r="BL27">
+        <v>50</v>
+      </c>
+      <c r="BM27">
+        <v>51</v>
+      </c>
+      <c r="BN27">
+        <v>51</v>
+      </c>
+      <c r="BO27">
+        <v>52</v>
+      </c>
+      <c r="BP27">
+        <v>53</v>
+      </c>
+      <c r="BQ27">
+        <v>54</v>
+      </c>
+      <c r="BR27">
+        <v>55</v>
+      </c>
+      <c r="BS27">
+        <v>55</v>
+      </c>
+      <c r="BT27">
+        <v>56</v>
+      </c>
+      <c r="BU27">
+        <v>57</v>
+      </c>
+      <c r="BV27">
+        <v>58</v>
+      </c>
+      <c r="BW27">
+        <v>59</v>
+      </c>
+      <c r="BX27">
+        <v>59</v>
+      </c>
+      <c r="BY27">
+        <v>60</v>
+      </c>
+      <c r="BZ27">
+        <v>61</v>
+      </c>
+      <c r="CA27">
+        <v>62</v>
+      </c>
+      <c r="CB27">
+        <v>63</v>
+      </c>
+      <c r="CC27">
+        <v>63</v>
+      </c>
+      <c r="CD27">
+        <v>64</v>
+      </c>
+      <c r="CE27">
+        <v>65</v>
+      </c>
+      <c r="CF27">
+        <v>66</v>
+      </c>
+      <c r="CG27">
+        <v>67</v>
+      </c>
+      <c r="CH27">
+        <v>67</v>
+      </c>
+      <c r="CI27">
+        <v>68</v>
+      </c>
+      <c r="CJ27">
+        <v>69</v>
+      </c>
+      <c r="CK27">
+        <v>70</v>
+      </c>
+      <c r="CL27">
+        <v>71</v>
+      </c>
+      <c r="CM27">
+        <v>71</v>
+      </c>
+      <c r="CN27">
+        <v>72</v>
+      </c>
+      <c r="CO27">
+        <v>73</v>
+      </c>
+      <c r="CP27">
+        <v>74</v>
+      </c>
+      <c r="CQ27">
+        <v>75</v>
+      </c>
+      <c r="CR27">
+        <v>76</v>
+      </c>
+      <c r="CS27">
+        <v>77</v>
+      </c>
+      <c r="CT27">
+        <v>78</v>
+      </c>
+      <c r="CU27">
+        <v>79</v>
+      </c>
+      <c r="CV27">
+        <v>80</v>
+      </c>
+      <c r="CW27" s="3">
         <v>80</v>
       </c>
     </row>
@@ -18636,10 +19074,157 @@
       <c r="AX28">
         <v>44</v>
       </c>
-      <c r="AY28" s="41">
+      <c r="AY28">
         <v>45</v>
       </c>
-      <c r="AZ28" s="3">
+      <c r="AZ28">
+        <v>46</v>
+      </c>
+      <c r="BA28">
+        <v>47</v>
+      </c>
+      <c r="BB28">
+        <v>48</v>
+      </c>
+      <c r="BC28">
+        <v>49</v>
+      </c>
+      <c r="BD28">
+        <v>49</v>
+      </c>
+      <c r="BE28">
+        <v>50</v>
+      </c>
+      <c r="BF28">
+        <v>51</v>
+      </c>
+      <c r="BG28">
+        <v>52</v>
+      </c>
+      <c r="BH28">
+        <v>53</v>
+      </c>
+      <c r="BI28">
+        <v>53</v>
+      </c>
+      <c r="BJ28">
+        <v>54</v>
+      </c>
+      <c r="BK28">
+        <v>55</v>
+      </c>
+      <c r="BL28">
+        <v>56</v>
+      </c>
+      <c r="BM28">
+        <v>57</v>
+      </c>
+      <c r="BN28">
+        <v>57</v>
+      </c>
+      <c r="BO28">
+        <v>58</v>
+      </c>
+      <c r="BP28">
+        <v>59</v>
+      </c>
+      <c r="BQ28">
+        <v>60</v>
+      </c>
+      <c r="BR28">
+        <v>61</v>
+      </c>
+      <c r="BS28">
+        <v>61</v>
+      </c>
+      <c r="BT28">
+        <v>62</v>
+      </c>
+      <c r="BU28">
+        <v>63</v>
+      </c>
+      <c r="BV28">
+        <v>64</v>
+      </c>
+      <c r="BW28">
+        <v>65</v>
+      </c>
+      <c r="BX28">
+        <v>65</v>
+      </c>
+      <c r="BY28">
+        <v>66</v>
+      </c>
+      <c r="BZ28">
+        <v>67</v>
+      </c>
+      <c r="CA28">
+        <v>68</v>
+      </c>
+      <c r="CB28">
+        <v>69</v>
+      </c>
+      <c r="CC28">
+        <v>69</v>
+      </c>
+      <c r="CD28">
+        <v>70</v>
+      </c>
+      <c r="CE28">
+        <v>71</v>
+      </c>
+      <c r="CF28">
+        <v>72</v>
+      </c>
+      <c r="CG28">
+        <v>73</v>
+      </c>
+      <c r="CH28">
+        <v>73</v>
+      </c>
+      <c r="CI28">
+        <v>74</v>
+      </c>
+      <c r="CJ28">
+        <v>75</v>
+      </c>
+      <c r="CK28">
+        <v>76</v>
+      </c>
+      <c r="CL28">
+        <v>77</v>
+      </c>
+      <c r="CM28">
+        <v>77</v>
+      </c>
+      <c r="CN28">
+        <v>78</v>
+      </c>
+      <c r="CO28">
+        <v>79</v>
+      </c>
+      <c r="CP28">
+        <v>80</v>
+      </c>
+      <c r="CQ28">
+        <v>81</v>
+      </c>
+      <c r="CR28">
+        <v>81</v>
+      </c>
+      <c r="CS28">
+        <v>82</v>
+      </c>
+      <c r="CT28">
+        <v>83</v>
+      </c>
+      <c r="CU28">
+        <v>84</v>
+      </c>
+      <c r="CV28">
+        <v>85</v>
+      </c>
+      <c r="CW28" s="3">
         <v>85</v>
       </c>
     </row>
@@ -18794,10 +19379,157 @@
       <c r="AX29">
         <v>45</v>
       </c>
-      <c r="AY29" s="41">
+      <c r="AY29">
         <v>45</v>
       </c>
-      <c r="AZ29" s="3">
+      <c r="AZ29">
+        <v>46</v>
+      </c>
+      <c r="BA29">
+        <v>47</v>
+      </c>
+      <c r="BB29">
+        <v>48</v>
+      </c>
+      <c r="BC29">
+        <v>49</v>
+      </c>
+      <c r="BD29">
+        <v>49</v>
+      </c>
+      <c r="BE29">
+        <v>50</v>
+      </c>
+      <c r="BF29">
+        <v>51</v>
+      </c>
+      <c r="BG29">
+        <v>52</v>
+      </c>
+      <c r="BH29">
+        <v>53</v>
+      </c>
+      <c r="BI29">
+        <v>53</v>
+      </c>
+      <c r="BJ29">
+        <v>54</v>
+      </c>
+      <c r="BK29">
+        <v>55</v>
+      </c>
+      <c r="BL29">
+        <v>56</v>
+      </c>
+      <c r="BM29">
+        <v>57</v>
+      </c>
+      <c r="BN29">
+        <v>57</v>
+      </c>
+      <c r="BO29">
+        <v>58</v>
+      </c>
+      <c r="BP29">
+        <v>59</v>
+      </c>
+      <c r="BQ29">
+        <v>60</v>
+      </c>
+      <c r="BR29">
+        <v>61</v>
+      </c>
+      <c r="BS29">
+        <v>61</v>
+      </c>
+      <c r="BT29">
+        <v>62</v>
+      </c>
+      <c r="BU29">
+        <v>63</v>
+      </c>
+      <c r="BV29">
+        <v>64</v>
+      </c>
+      <c r="BW29">
+        <v>65</v>
+      </c>
+      <c r="BX29">
+        <v>65</v>
+      </c>
+      <c r="BY29">
+        <v>66</v>
+      </c>
+      <c r="BZ29">
+        <v>67</v>
+      </c>
+      <c r="CA29">
+        <v>68</v>
+      </c>
+      <c r="CB29">
+        <v>69</v>
+      </c>
+      <c r="CC29">
+        <v>69</v>
+      </c>
+      <c r="CD29">
+        <v>70</v>
+      </c>
+      <c r="CE29">
+        <v>71</v>
+      </c>
+      <c r="CF29">
+        <v>72</v>
+      </c>
+      <c r="CG29">
+        <v>73</v>
+      </c>
+      <c r="CH29">
+        <v>73</v>
+      </c>
+      <c r="CI29">
+        <v>74</v>
+      </c>
+      <c r="CJ29">
+        <v>75</v>
+      </c>
+      <c r="CK29">
+        <v>76</v>
+      </c>
+      <c r="CL29">
+        <v>77</v>
+      </c>
+      <c r="CM29">
+        <v>77</v>
+      </c>
+      <c r="CN29">
+        <v>78</v>
+      </c>
+      <c r="CO29">
+        <v>79</v>
+      </c>
+      <c r="CP29">
+        <v>80</v>
+      </c>
+      <c r="CQ29">
+        <v>81</v>
+      </c>
+      <c r="CR29">
+        <v>81</v>
+      </c>
+      <c r="CS29">
+        <v>82</v>
+      </c>
+      <c r="CT29">
+        <v>83</v>
+      </c>
+      <c r="CU29">
+        <v>84</v>
+      </c>
+      <c r="CV29">
+        <v>85</v>
+      </c>
+      <c r="CW29" s="3">
         <v>85</v>
       </c>
     </row>
@@ -18952,10 +19684,157 @@
       <c r="AX30">
         <v>19</v>
       </c>
-      <c r="AY30" s="41">
+      <c r="AY30">
         <v>20</v>
       </c>
-      <c r="AZ30" s="3">
+      <c r="AZ30">
+        <v>20</v>
+      </c>
+      <c r="BA30">
+        <v>20</v>
+      </c>
+      <c r="BB30">
+        <v>20</v>
+      </c>
+      <c r="BC30">
+        <v>20</v>
+      </c>
+      <c r="BD30">
+        <v>21</v>
+      </c>
+      <c r="BE30">
+        <v>21</v>
+      </c>
+      <c r="BF30">
+        <v>21</v>
+      </c>
+      <c r="BG30">
+        <v>21</v>
+      </c>
+      <c r="BH30">
+        <v>21</v>
+      </c>
+      <c r="BI30">
+        <v>23</v>
+      </c>
+      <c r="BJ30">
+        <v>23</v>
+      </c>
+      <c r="BK30">
+        <v>23</v>
+      </c>
+      <c r="BL30">
+        <v>23</v>
+      </c>
+      <c r="BM30">
+        <v>23</v>
+      </c>
+      <c r="BN30">
+        <v>25</v>
+      </c>
+      <c r="BO30">
+        <v>25</v>
+      </c>
+      <c r="BP30">
+        <v>25</v>
+      </c>
+      <c r="BQ30">
+        <v>25</v>
+      </c>
+      <c r="BR30">
+        <v>25</v>
+      </c>
+      <c r="BS30">
+        <v>27</v>
+      </c>
+      <c r="BT30">
+        <v>27</v>
+      </c>
+      <c r="BU30">
+        <v>27</v>
+      </c>
+      <c r="BV30">
+        <v>27</v>
+      </c>
+      <c r="BW30">
+        <v>27</v>
+      </c>
+      <c r="BX30">
+        <v>29</v>
+      </c>
+      <c r="BY30">
+        <v>29</v>
+      </c>
+      <c r="BZ30">
+        <v>29</v>
+      </c>
+      <c r="CA30">
+        <v>29</v>
+      </c>
+      <c r="CB30">
+        <v>29</v>
+      </c>
+      <c r="CC30">
+        <v>31</v>
+      </c>
+      <c r="CD30">
+        <v>31</v>
+      </c>
+      <c r="CE30">
+        <v>31</v>
+      </c>
+      <c r="CF30">
+        <v>31</v>
+      </c>
+      <c r="CG30">
+        <v>31</v>
+      </c>
+      <c r="CH30">
+        <v>33</v>
+      </c>
+      <c r="CI30">
+        <v>33</v>
+      </c>
+      <c r="CJ30">
+        <v>33</v>
+      </c>
+      <c r="CK30">
+        <v>33</v>
+      </c>
+      <c r="CL30">
+        <v>33</v>
+      </c>
+      <c r="CM30">
+        <v>35</v>
+      </c>
+      <c r="CN30">
+        <v>35</v>
+      </c>
+      <c r="CO30">
+        <v>35</v>
+      </c>
+      <c r="CP30">
+        <v>35</v>
+      </c>
+      <c r="CQ30">
+        <v>35</v>
+      </c>
+      <c r="CR30">
+        <v>37</v>
+      </c>
+      <c r="CS30">
+        <v>37</v>
+      </c>
+      <c r="CT30">
+        <v>37</v>
+      </c>
+      <c r="CU30">
+        <v>37</v>
+      </c>
+      <c r="CV30">
+        <v>37</v>
+      </c>
+      <c r="CW30" s="3">
         <v>40</v>
       </c>
     </row>
@@ -19110,10 +19989,157 @@
       <c r="AX31">
         <v>16</v>
       </c>
-      <c r="AY31" s="41">
+      <c r="AY31">
         <v>18</v>
       </c>
-      <c r="AZ31" s="3">
+      <c r="AZ31">
+        <v>18</v>
+      </c>
+      <c r="BA31">
+        <v>18</v>
+      </c>
+      <c r="BB31">
+        <v>18</v>
+      </c>
+      <c r="BC31">
+        <v>18</v>
+      </c>
+      <c r="BD31">
+        <v>18</v>
+      </c>
+      <c r="BE31">
+        <v>18</v>
+      </c>
+      <c r="BF31">
+        <v>18</v>
+      </c>
+      <c r="BG31">
+        <v>18</v>
+      </c>
+      <c r="BH31">
+        <v>18</v>
+      </c>
+      <c r="BI31">
+        <v>19</v>
+      </c>
+      <c r="BJ31">
+        <v>19</v>
+      </c>
+      <c r="BK31">
+        <v>19</v>
+      </c>
+      <c r="BL31">
+        <v>19</v>
+      </c>
+      <c r="BM31">
+        <v>19</v>
+      </c>
+      <c r="BN31">
+        <v>20</v>
+      </c>
+      <c r="BO31">
+        <v>20</v>
+      </c>
+      <c r="BP31">
+        <v>20</v>
+      </c>
+      <c r="BQ31">
+        <v>20</v>
+      </c>
+      <c r="BR31">
+        <v>20</v>
+      </c>
+      <c r="BS31">
+        <v>21</v>
+      </c>
+      <c r="BT31">
+        <v>21</v>
+      </c>
+      <c r="BU31">
+        <v>21</v>
+      </c>
+      <c r="BV31">
+        <v>21</v>
+      </c>
+      <c r="BW31">
+        <v>21</v>
+      </c>
+      <c r="BX31">
+        <v>22</v>
+      </c>
+      <c r="BY31">
+        <v>22</v>
+      </c>
+      <c r="BZ31">
+        <v>22</v>
+      </c>
+      <c r="CA31">
+        <v>22</v>
+      </c>
+      <c r="CB31">
+        <v>22</v>
+      </c>
+      <c r="CC31">
+        <v>23</v>
+      </c>
+      <c r="CD31">
+        <v>23</v>
+      </c>
+      <c r="CE31">
+        <v>23</v>
+      </c>
+      <c r="CF31">
+        <v>23</v>
+      </c>
+      <c r="CG31">
+        <v>23</v>
+      </c>
+      <c r="CH31">
+        <v>24</v>
+      </c>
+      <c r="CI31">
+        <v>24</v>
+      </c>
+      <c r="CJ31">
+        <v>24</v>
+      </c>
+      <c r="CK31">
+        <v>24</v>
+      </c>
+      <c r="CL31">
+        <v>24</v>
+      </c>
+      <c r="CM31">
+        <v>25</v>
+      </c>
+      <c r="CN31">
+        <v>25</v>
+      </c>
+      <c r="CO31">
+        <v>25</v>
+      </c>
+      <c r="CP31">
+        <v>25</v>
+      </c>
+      <c r="CQ31">
+        <v>25</v>
+      </c>
+      <c r="CR31">
+        <v>25</v>
+      </c>
+      <c r="CS31">
+        <v>25</v>
+      </c>
+      <c r="CT31">
+        <v>25</v>
+      </c>
+      <c r="CU31">
+        <v>25</v>
+      </c>
+      <c r="CV31">
+        <v>25</v>
+      </c>
+      <c r="CW31" s="3">
         <v>25</v>
       </c>
     </row>
@@ -19268,10 +20294,157 @@
       <c r="AX32">
         <v>5</v>
       </c>
-      <c r="AY32" s="41">
+      <c r="AY32">
         <v>5</v>
       </c>
-      <c r="AZ32" s="3">
+      <c r="AZ32">
+        <v>6</v>
+      </c>
+      <c r="BA32">
+        <v>7</v>
+      </c>
+      <c r="BB32">
+        <v>8</v>
+      </c>
+      <c r="BC32">
+        <v>9</v>
+      </c>
+      <c r="BD32">
+        <v>10</v>
+      </c>
+      <c r="BE32">
+        <v>10</v>
+      </c>
+      <c r="BF32">
+        <v>10</v>
+      </c>
+      <c r="BG32">
+        <v>10</v>
+      </c>
+      <c r="BH32">
+        <v>10</v>
+      </c>
+      <c r="BI32">
+        <v>10</v>
+      </c>
+      <c r="BJ32">
+        <v>10</v>
+      </c>
+      <c r="BK32">
+        <v>10</v>
+      </c>
+      <c r="BL32">
+        <v>10</v>
+      </c>
+      <c r="BM32">
+        <v>10</v>
+      </c>
+      <c r="BN32">
+        <v>10</v>
+      </c>
+      <c r="BO32">
+        <v>10</v>
+      </c>
+      <c r="BP32">
+        <v>10</v>
+      </c>
+      <c r="BQ32">
+        <v>10</v>
+      </c>
+      <c r="BR32">
+        <v>10</v>
+      </c>
+      <c r="BS32">
+        <v>10</v>
+      </c>
+      <c r="BT32">
+        <v>10</v>
+      </c>
+      <c r="BU32">
+        <v>10</v>
+      </c>
+      <c r="BV32">
+        <v>10</v>
+      </c>
+      <c r="BW32">
+        <v>10</v>
+      </c>
+      <c r="BX32">
+        <v>10</v>
+      </c>
+      <c r="BY32">
+        <v>10</v>
+      </c>
+      <c r="BZ32">
+        <v>10</v>
+      </c>
+      <c r="CA32">
+        <v>10</v>
+      </c>
+      <c r="CB32">
+        <v>10</v>
+      </c>
+      <c r="CC32">
+        <v>10</v>
+      </c>
+      <c r="CD32">
+        <v>10</v>
+      </c>
+      <c r="CE32">
+        <v>10</v>
+      </c>
+      <c r="CF32">
+        <v>10</v>
+      </c>
+      <c r="CG32">
+        <v>10</v>
+      </c>
+      <c r="CH32">
+        <v>10</v>
+      </c>
+      <c r="CI32">
+        <v>10</v>
+      </c>
+      <c r="CJ32">
+        <v>10</v>
+      </c>
+      <c r="CK32">
+        <v>10</v>
+      </c>
+      <c r="CL32">
+        <v>10</v>
+      </c>
+      <c r="CM32">
+        <v>10</v>
+      </c>
+      <c r="CN32">
+        <v>10</v>
+      </c>
+      <c r="CO32">
+        <v>10</v>
+      </c>
+      <c r="CP32">
+        <v>10</v>
+      </c>
+      <c r="CQ32">
+        <v>10</v>
+      </c>
+      <c r="CR32">
+        <v>10</v>
+      </c>
+      <c r="CS32">
+        <v>10</v>
+      </c>
+      <c r="CT32">
+        <v>10</v>
+      </c>
+      <c r="CU32">
+        <v>10</v>
+      </c>
+      <c r="CV32">
+        <v>10</v>
+      </c>
+      <c r="CW32" s="3">
         <v>10</v>
       </c>
     </row>
@@ -19426,10 +20599,157 @@
       <c r="AX33" s="27">
         <v>39</v>
       </c>
-      <c r="AY33" s="42">
+      <c r="AY33" s="27">
         <v>40</v>
       </c>
-      <c r="AZ33" s="7">
+      <c r="AZ33" s="27">
+        <v>41</v>
+      </c>
+      <c r="BA33" s="27">
+        <v>42</v>
+      </c>
+      <c r="BB33" s="27">
+        <v>43</v>
+      </c>
+      <c r="BC33" s="27">
+        <v>44</v>
+      </c>
+      <c r="BD33" s="27">
+        <v>46</v>
+      </c>
+      <c r="BE33" s="27">
+        <v>47</v>
+      </c>
+      <c r="BF33" s="27">
+        <v>48</v>
+      </c>
+      <c r="BG33" s="27">
+        <v>49</v>
+      </c>
+      <c r="BH33" s="27">
+        <v>50</v>
+      </c>
+      <c r="BI33" s="27">
+        <v>52</v>
+      </c>
+      <c r="BJ33" s="27">
+        <v>53</v>
+      </c>
+      <c r="BK33" s="27">
+        <v>54</v>
+      </c>
+      <c r="BL33" s="27">
+        <v>55</v>
+      </c>
+      <c r="BM33" s="27">
+        <v>56</v>
+      </c>
+      <c r="BN33" s="27">
+        <v>58</v>
+      </c>
+      <c r="BO33" s="27">
+        <v>59</v>
+      </c>
+      <c r="BP33" s="27">
+        <v>60</v>
+      </c>
+      <c r="BQ33" s="27">
+        <v>61</v>
+      </c>
+      <c r="BR33" s="27">
+        <v>62</v>
+      </c>
+      <c r="BS33" s="27">
+        <v>64</v>
+      </c>
+      <c r="BT33" s="27">
+        <v>65</v>
+      </c>
+      <c r="BU33" s="27">
+        <v>66</v>
+      </c>
+      <c r="BV33" s="27">
+        <v>67</v>
+      </c>
+      <c r="BW33" s="27">
+        <v>68</v>
+      </c>
+      <c r="BX33" s="27">
+        <v>70</v>
+      </c>
+      <c r="BY33" s="27">
+        <v>71</v>
+      </c>
+      <c r="BZ33" s="27">
+        <v>72</v>
+      </c>
+      <c r="CA33" s="27">
+        <v>73</v>
+      </c>
+      <c r="CB33" s="27">
+        <v>74</v>
+      </c>
+      <c r="CC33" s="27">
+        <v>76</v>
+      </c>
+      <c r="CD33" s="27">
+        <v>77</v>
+      </c>
+      <c r="CE33" s="27">
+        <v>78</v>
+      </c>
+      <c r="CF33" s="27">
+        <v>79</v>
+      </c>
+      <c r="CG33" s="27">
+        <v>80</v>
+      </c>
+      <c r="CH33" s="27">
+        <v>82</v>
+      </c>
+      <c r="CI33" s="27">
+        <v>83</v>
+      </c>
+      <c r="CJ33" s="27">
+        <v>84</v>
+      </c>
+      <c r="CK33" s="27">
+        <v>85</v>
+      </c>
+      <c r="CL33" s="27">
+        <v>86</v>
+      </c>
+      <c r="CM33" s="27">
+        <v>88</v>
+      </c>
+      <c r="CN33" s="27">
+        <v>89</v>
+      </c>
+      <c r="CO33" s="27">
+        <v>90</v>
+      </c>
+      <c r="CP33" s="27">
+        <v>91</v>
+      </c>
+      <c r="CQ33" s="27">
+        <v>92</v>
+      </c>
+      <c r="CR33" s="27">
+        <v>94</v>
+      </c>
+      <c r="CS33" s="27">
+        <v>95</v>
+      </c>
+      <c r="CT33" s="27">
+        <v>96</v>
+      </c>
+      <c r="CU33" s="27">
+        <v>97</v>
+      </c>
+      <c r="CV33" s="27">
+        <v>98</v>
+      </c>
+      <c r="CW33" s="7">
         <v>100</v>
       </c>
     </row>
@@ -19630,13 +20950,415 @@
         <f t="shared" si="18"/>
         <v>245</v>
       </c>
-      <c r="AY34" s="41">
+      <c r="AY34">
         <f>SUM(AY26:AY33)</f>
         <v>250</v>
       </c>
-      <c r="AZ34" s="3">
-        <f>SUM(AZ26:AZ33)</f>
+      <c r="AZ34">
+        <f t="shared" ref="AZ34:CW34" si="19">SUM(AZ26:AZ33)</f>
+        <v>255</v>
+      </c>
+      <c r="BA34">
+        <f t="shared" si="19"/>
+        <v>260</v>
+      </c>
+      <c r="BB34">
+        <f t="shared" si="19"/>
+        <v>265</v>
+      </c>
+      <c r="BC34">
+        <f t="shared" si="19"/>
+        <v>270</v>
+      </c>
+      <c r="BD34">
+        <f t="shared" si="19"/>
+        <v>275</v>
+      </c>
+      <c r="BE34">
+        <f t="shared" si="19"/>
+        <v>280</v>
+      </c>
+      <c r="BF34">
+        <f t="shared" si="19"/>
+        <v>285</v>
+      </c>
+      <c r="BG34">
+        <f t="shared" si="19"/>
+        <v>290</v>
+      </c>
+      <c r="BH34">
+        <f t="shared" si="19"/>
+        <v>295</v>
+      </c>
+      <c r="BI34">
+        <f t="shared" si="19"/>
+        <v>300</v>
+      </c>
+      <c r="BJ34">
+        <f t="shared" si="19"/>
+        <v>305</v>
+      </c>
+      <c r="BK34">
+        <f t="shared" si="19"/>
+        <v>310</v>
+      </c>
+      <c r="BL34">
+        <f t="shared" si="19"/>
+        <v>315</v>
+      </c>
+      <c r="BM34">
+        <f t="shared" si="19"/>
+        <v>320</v>
+      </c>
+      <c r="BN34">
+        <f t="shared" si="19"/>
+        <v>325</v>
+      </c>
+      <c r="BO34">
+        <f t="shared" si="19"/>
+        <v>330</v>
+      </c>
+      <c r="BP34">
+        <f t="shared" si="19"/>
+        <v>335</v>
+      </c>
+      <c r="BQ34">
+        <f t="shared" si="19"/>
+        <v>340</v>
+      </c>
+      <c r="BR34">
+        <f t="shared" si="19"/>
+        <v>345</v>
+      </c>
+      <c r="BS34">
+        <f t="shared" si="19"/>
+        <v>350</v>
+      </c>
+      <c r="BT34">
+        <f t="shared" si="19"/>
+        <v>355</v>
+      </c>
+      <c r="BU34">
+        <f t="shared" si="19"/>
+        <v>360</v>
+      </c>
+      <c r="BV34">
+        <f t="shared" si="19"/>
+        <v>365</v>
+      </c>
+      <c r="BW34">
+        <f t="shared" si="19"/>
+        <v>370</v>
+      </c>
+      <c r="BX34">
+        <f t="shared" si="19"/>
+        <v>375</v>
+      </c>
+      <c r="BY34">
+        <f t="shared" si="19"/>
+        <v>380</v>
+      </c>
+      <c r="BZ34">
+        <f t="shared" si="19"/>
+        <v>385</v>
+      </c>
+      <c r="CA34">
+        <f t="shared" si="19"/>
+        <v>390</v>
+      </c>
+      <c r="CB34">
+        <f t="shared" si="19"/>
+        <v>395</v>
+      </c>
+      <c r="CC34">
+        <f t="shared" si="19"/>
+        <v>400</v>
+      </c>
+      <c r="CD34">
+        <f t="shared" si="19"/>
+        <v>405</v>
+      </c>
+      <c r="CE34">
+        <f t="shared" si="19"/>
+        <v>410</v>
+      </c>
+      <c r="CF34">
+        <f t="shared" si="19"/>
+        <v>415</v>
+      </c>
+      <c r="CG34">
+        <f t="shared" si="19"/>
+        <v>420</v>
+      </c>
+      <c r="CH34">
+        <f t="shared" si="19"/>
+        <v>425</v>
+      </c>
+      <c r="CI34">
+        <f t="shared" si="19"/>
+        <v>430</v>
+      </c>
+      <c r="CJ34">
+        <f t="shared" si="19"/>
+        <v>435</v>
+      </c>
+      <c r="CK34">
+        <f t="shared" si="19"/>
+        <v>440</v>
+      </c>
+      <c r="CL34">
+        <f t="shared" si="19"/>
+        <v>445</v>
+      </c>
+      <c r="CM34">
+        <f t="shared" si="19"/>
+        <v>450</v>
+      </c>
+      <c r="CN34">
+        <f t="shared" si="19"/>
+        <v>455</v>
+      </c>
+      <c r="CO34">
+        <f t="shared" si="19"/>
+        <v>460</v>
+      </c>
+      <c r="CP34">
+        <f t="shared" si="19"/>
+        <v>465</v>
+      </c>
+      <c r="CQ34">
+        <f t="shared" si="19"/>
+        <v>470</v>
+      </c>
+      <c r="CR34">
+        <f t="shared" si="19"/>
+        <v>475</v>
+      </c>
+      <c r="CS34">
+        <f t="shared" si="19"/>
+        <v>480</v>
+      </c>
+      <c r="CT34">
+        <f t="shared" si="19"/>
+        <v>485</v>
+      </c>
+      <c r="CU34">
+        <f t="shared" si="19"/>
+        <v>490</v>
+      </c>
+      <c r="CV34">
+        <f t="shared" si="19"/>
+        <v>495</v>
+      </c>
+      <c r="CW34">
+        <f t="shared" si="19"/>
         <v>500</v>
+      </c>
+    </row>
+    <row r="35" spans="1:101" x14ac:dyDescent="0.3">
+      <c r="AY35">
+        <f>5*AY30+2*AY31+10*AY32+1*AY33</f>
+        <v>226</v>
+      </c>
+      <c r="AZ35">
+        <f t="shared" ref="AZ35:CW35" si="20">5*AZ30+2*AZ31+10*AZ32+1*AZ33</f>
+        <v>237</v>
+      </c>
+      <c r="BA35">
+        <f t="shared" si="20"/>
+        <v>248</v>
+      </c>
+      <c r="BB35">
+        <f t="shared" si="20"/>
+        <v>259</v>
+      </c>
+      <c r="BC35">
+        <f t="shared" si="20"/>
+        <v>270</v>
+      </c>
+      <c r="BD35">
+        <f t="shared" si="20"/>
+        <v>287</v>
+      </c>
+      <c r="BE35">
+        <f t="shared" si="20"/>
+        <v>288</v>
+      </c>
+      <c r="BF35">
+        <f t="shared" si="20"/>
+        <v>289</v>
+      </c>
+      <c r="BG35">
+        <f t="shared" si="20"/>
+        <v>290</v>
+      </c>
+      <c r="BH35">
+        <f t="shared" si="20"/>
+        <v>291</v>
+      </c>
+      <c r="BI35">
+        <f t="shared" si="20"/>
+        <v>305</v>
+      </c>
+      <c r="BJ35">
+        <f t="shared" si="20"/>
+        <v>306</v>
+      </c>
+      <c r="BK35">
+        <f t="shared" si="20"/>
+        <v>307</v>
+      </c>
+      <c r="BL35">
+        <f t="shared" si="20"/>
+        <v>308</v>
+      </c>
+      <c r="BM35">
+        <f t="shared" si="20"/>
+        <v>309</v>
+      </c>
+      <c r="BN35">
+        <f t="shared" si="20"/>
+        <v>323</v>
+      </c>
+      <c r="BO35">
+        <f t="shared" si="20"/>
+        <v>324</v>
+      </c>
+      <c r="BP35">
+        <f t="shared" si="20"/>
+        <v>325</v>
+      </c>
+      <c r="BQ35">
+        <f t="shared" si="20"/>
+        <v>326</v>
+      </c>
+      <c r="BR35">
+        <f t="shared" si="20"/>
+        <v>327</v>
+      </c>
+      <c r="BS35">
+        <f t="shared" si="20"/>
+        <v>341</v>
+      </c>
+      <c r="BT35">
+        <f t="shared" si="20"/>
+        <v>342</v>
+      </c>
+      <c r="BU35">
+        <f t="shared" si="20"/>
+        <v>343</v>
+      </c>
+      <c r="BV35">
+        <f t="shared" si="20"/>
+        <v>344</v>
+      </c>
+      <c r="BW35">
+        <f t="shared" si="20"/>
+        <v>345</v>
+      </c>
+      <c r="BX35">
+        <f t="shared" si="20"/>
+        <v>359</v>
+      </c>
+      <c r="BY35">
+        <f t="shared" si="20"/>
+        <v>360</v>
+      </c>
+      <c r="BZ35">
+        <f t="shared" si="20"/>
+        <v>361</v>
+      </c>
+      <c r="CA35">
+        <f t="shared" si="20"/>
+        <v>362</v>
+      </c>
+      <c r="CB35">
+        <f t="shared" si="20"/>
+        <v>363</v>
+      </c>
+      <c r="CC35">
+        <f t="shared" si="20"/>
+        <v>377</v>
+      </c>
+      <c r="CD35">
+        <f t="shared" si="20"/>
+        <v>378</v>
+      </c>
+      <c r="CE35">
+        <f t="shared" si="20"/>
+        <v>379</v>
+      </c>
+      <c r="CF35">
+        <f t="shared" si="20"/>
+        <v>380</v>
+      </c>
+      <c r="CG35">
+        <f t="shared" si="20"/>
+        <v>381</v>
+      </c>
+      <c r="CH35">
+        <f t="shared" si="20"/>
+        <v>395</v>
+      </c>
+      <c r="CI35">
+        <f t="shared" si="20"/>
+        <v>396</v>
+      </c>
+      <c r="CJ35">
+        <f t="shared" si="20"/>
+        <v>397</v>
+      </c>
+      <c r="CK35">
+        <f t="shared" si="20"/>
+        <v>398</v>
+      </c>
+      <c r="CL35">
+        <f t="shared" si="20"/>
+        <v>399</v>
+      </c>
+      <c r="CM35">
+        <f t="shared" si="20"/>
+        <v>413</v>
+      </c>
+      <c r="CN35">
+        <f t="shared" si="20"/>
+        <v>414</v>
+      </c>
+      <c r="CO35">
+        <f t="shared" si="20"/>
+        <v>415</v>
+      </c>
+      <c r="CP35">
+        <f t="shared" si="20"/>
+        <v>416</v>
+      </c>
+      <c r="CQ35">
+        <f t="shared" si="20"/>
+        <v>417</v>
+      </c>
+      <c r="CR35">
+        <f t="shared" si="20"/>
+        <v>429</v>
+      </c>
+      <c r="CS35">
+        <f t="shared" si="20"/>
+        <v>430</v>
+      </c>
+      <c r="CT35">
+        <f t="shared" si="20"/>
+        <v>431</v>
+      </c>
+      <c r="CU35">
+        <f t="shared" si="20"/>
+        <v>432</v>
+      </c>
+      <c r="CV35">
+        <f t="shared" si="20"/>
+        <v>433</v>
+      </c>
+      <c r="CW35">
+        <f t="shared" si="20"/>
+        <v>450</v>
       </c>
     </row>
     <row r="37" spans="1:101" x14ac:dyDescent="0.3">
@@ -22387,195 +24109,195 @@
         <v>5</v>
       </c>
       <c r="C46">
-        <f t="shared" ref="C46:P46" si="19">SUM(C38:C45)</f>
+        <f t="shared" ref="C46:P46" si="21">SUM(C38:C45)</f>
         <v>10</v>
       </c>
       <c r="D46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>15</v>
       </c>
       <c r="E46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>20</v>
       </c>
       <c r="F46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>25</v>
       </c>
       <c r="G46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>30</v>
       </c>
       <c r="H46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>35</v>
       </c>
       <c r="I46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>40</v>
       </c>
       <c r="J46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>45</v>
       </c>
       <c r="K46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>50</v>
       </c>
       <c r="L46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>55</v>
       </c>
       <c r="M46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>60</v>
       </c>
       <c r="N46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>65</v>
       </c>
       <c r="O46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>70</v>
       </c>
       <c r="P46">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>75</v>
       </c>
       <c r="Q46">
-        <f t="shared" ref="Q46" si="20">SUM(Q38:Q45)</f>
+        <f t="shared" ref="Q46" si="22">SUM(Q38:Q45)</f>
         <v>80</v>
       </c>
       <c r="R46">
-        <f t="shared" ref="R46" si="21">SUM(R38:R45)</f>
+        <f t="shared" ref="R46" si="23">SUM(R38:R45)</f>
         <v>85</v>
       </c>
       <c r="S46">
-        <f t="shared" ref="S46" si="22">SUM(S38:S45)</f>
+        <f t="shared" ref="S46" si="24">SUM(S38:S45)</f>
         <v>90</v>
       </c>
       <c r="T46">
-        <f t="shared" ref="T46" si="23">SUM(T38:T45)</f>
+        <f t="shared" ref="T46" si="25">SUM(T38:T45)</f>
         <v>95</v>
       </c>
       <c r="U46">
-        <f t="shared" ref="U46:AX46" si="24">SUM(U38:U45)</f>
+        <f t="shared" ref="U46:AX46" si="26">SUM(U38:U45)</f>
         <v>100</v>
       </c>
       <c r="V46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>105</v>
       </c>
       <c r="W46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>110</v>
       </c>
       <c r="X46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>115</v>
       </c>
       <c r="Y46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>120</v>
       </c>
       <c r="Z46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>125</v>
       </c>
       <c r="AA46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>130</v>
       </c>
       <c r="AB46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>135</v>
       </c>
       <c r="AC46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>140</v>
       </c>
       <c r="AD46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>145</v>
       </c>
       <c r="AE46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>150</v>
       </c>
       <c r="AF46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>155</v>
       </c>
       <c r="AG46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>160</v>
       </c>
       <c r="AH46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>165</v>
       </c>
       <c r="AI46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>170</v>
       </c>
       <c r="AJ46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>175</v>
       </c>
       <c r="AK46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>180</v>
       </c>
       <c r="AL46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>185</v>
       </c>
       <c r="AM46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>190</v>
       </c>
       <c r="AN46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>195</v>
       </c>
       <c r="AO46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>200</v>
       </c>
       <c r="AP46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>205</v>
       </c>
       <c r="AQ46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>210</v>
       </c>
       <c r="AR46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>215</v>
       </c>
       <c r="AS46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>220</v>
       </c>
       <c r="AT46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>225</v>
       </c>
       <c r="AU46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>230</v>
       </c>
       <c r="AV46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>235</v>
       </c>
       <c r="AW46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>240</v>
       </c>
       <c r="AX46">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>245</v>
       </c>
       <c r="AY46">
@@ -22583,19 +24305,19 @@
         <v>250</v>
       </c>
       <c r="AZ46">
-        <f t="shared" ref="AZ46:CV46" si="25">SUM(AZ38:AZ45)</f>
+        <f t="shared" ref="AZ46:CV46" si="27">SUM(AZ38:AZ45)</f>
         <v>255</v>
       </c>
       <c r="BA46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>260</v>
       </c>
       <c r="BB46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>265</v>
       </c>
       <c r="BC46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>270</v>
       </c>
       <c r="BD46">
@@ -22603,179 +24325,179 @@
         <v>275</v>
       </c>
       <c r="BE46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>280</v>
       </c>
       <c r="BF46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>285</v>
       </c>
       <c r="BG46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>290</v>
       </c>
       <c r="BH46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>295</v>
       </c>
       <c r="BI46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>300</v>
       </c>
       <c r="BJ46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>305</v>
       </c>
       <c r="BK46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>310</v>
       </c>
       <c r="BL46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>315</v>
       </c>
       <c r="BM46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>320</v>
       </c>
       <c r="BN46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>325</v>
       </c>
       <c r="BO46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>330</v>
       </c>
       <c r="BP46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>335</v>
       </c>
       <c r="BQ46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>340</v>
       </c>
       <c r="BR46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>345</v>
       </c>
       <c r="BS46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>350</v>
       </c>
       <c r="BT46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>355</v>
       </c>
       <c r="BU46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>360</v>
       </c>
       <c r="BV46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>365</v>
       </c>
       <c r="BW46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>370</v>
       </c>
       <c r="BX46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>375</v>
       </c>
       <c r="BY46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>380</v>
       </c>
       <c r="BZ46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>385</v>
       </c>
       <c r="CA46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>390</v>
       </c>
       <c r="CB46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>395</v>
       </c>
       <c r="CC46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>400</v>
       </c>
       <c r="CD46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>405</v>
       </c>
       <c r="CE46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>410</v>
       </c>
       <c r="CF46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>415</v>
       </c>
       <c r="CG46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>420</v>
       </c>
       <c r="CH46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>425</v>
       </c>
       <c r="CI46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>430</v>
       </c>
       <c r="CJ46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>435</v>
       </c>
       <c r="CK46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>440</v>
       </c>
       <c r="CL46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>445</v>
       </c>
       <c r="CM46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>450</v>
       </c>
       <c r="CN46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>455</v>
       </c>
       <c r="CO46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>460</v>
       </c>
       <c r="CP46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>465</v>
       </c>
       <c r="CQ46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>470</v>
       </c>
       <c r="CR46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>475</v>
       </c>
       <c r="CS46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>480</v>
       </c>
       <c r="CT46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>485</v>
       </c>
       <c r="CU46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>490</v>
       </c>
       <c r="CV46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>495</v>
       </c>
       <c r="CW46">
@@ -25531,399 +27253,399 @@
         <v>5</v>
       </c>
       <c r="C58">
-        <f t="shared" ref="C58:F58" si="26">SUM(C50:C57)</f>
+        <f t="shared" ref="C58:F58" si="28">SUM(C50:C57)</f>
         <v>10</v>
       </c>
       <c r="D58">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>15</v>
       </c>
       <c r="E58">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>20</v>
       </c>
       <c r="F58">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>25</v>
       </c>
       <c r="G58">
-        <f t="shared" ref="G58" si="27">SUM(G50:G57)</f>
+        <f t="shared" ref="G58" si="29">SUM(G50:G57)</f>
         <v>30</v>
       </c>
       <c r="H58">
-        <f t="shared" ref="H58" si="28">SUM(H50:H57)</f>
+        <f t="shared" ref="H58" si="30">SUM(H50:H57)</f>
         <v>35</v>
       </c>
       <c r="I58">
-        <f t="shared" ref="I58" si="29">SUM(I50:I57)</f>
+        <f t="shared" ref="I58" si="31">SUM(I50:I57)</f>
         <v>40</v>
       </c>
       <c r="J58">
-        <f t="shared" ref="J58" si="30">SUM(J50:J57)</f>
+        <f t="shared" ref="J58" si="32">SUM(J50:J57)</f>
         <v>45</v>
       </c>
       <c r="K58">
-        <f t="shared" ref="K58" si="31">SUM(K50:K57)</f>
+        <f t="shared" ref="K58" si="33">SUM(K50:K57)</f>
         <v>50</v>
       </c>
       <c r="L58">
-        <f t="shared" ref="L58" si="32">SUM(L50:L57)</f>
+        <f t="shared" ref="L58" si="34">SUM(L50:L57)</f>
         <v>55</v>
       </c>
       <c r="M58">
-        <f t="shared" ref="M58" si="33">SUM(M50:M57)</f>
+        <f t="shared" ref="M58" si="35">SUM(M50:M57)</f>
         <v>60</v>
       </c>
       <c r="N58">
-        <f t="shared" ref="N58" si="34">SUM(N50:N57)</f>
+        <f t="shared" ref="N58" si="36">SUM(N50:N57)</f>
         <v>65</v>
       </c>
       <c r="O58">
-        <f t="shared" ref="O58" si="35">SUM(O50:O57)</f>
+        <f t="shared" ref="O58" si="37">SUM(O50:O57)</f>
         <v>70</v>
       </c>
       <c r="P58">
-        <f t="shared" ref="P58" si="36">SUM(P50:P57)</f>
+        <f t="shared" ref="P58" si="38">SUM(P50:P57)</f>
         <v>75</v>
       </c>
       <c r="Q58">
-        <f t="shared" ref="Q58" si="37">SUM(Q50:Q57)</f>
+        <f t="shared" ref="Q58" si="39">SUM(Q50:Q57)</f>
         <v>80</v>
       </c>
       <c r="R58">
-        <f t="shared" ref="R58" si="38">SUM(R50:R57)</f>
+        <f t="shared" ref="R58" si="40">SUM(R50:R57)</f>
         <v>85</v>
       </c>
       <c r="S58">
-        <f t="shared" ref="S58" si="39">SUM(S50:S57)</f>
+        <f t="shared" ref="S58" si="41">SUM(S50:S57)</f>
         <v>90</v>
       </c>
       <c r="T58">
-        <f t="shared" ref="T58" si="40">SUM(T50:T57)</f>
+        <f t="shared" ref="T58" si="42">SUM(T50:T57)</f>
         <v>95</v>
       </c>
       <c r="U58">
-        <f t="shared" ref="U58:CF58" si="41">SUM(U50:U57)</f>
+        <f t="shared" ref="U58:CF58" si="43">SUM(U50:U57)</f>
         <v>100</v>
       </c>
       <c r="V58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>105</v>
       </c>
       <c r="W58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>110</v>
       </c>
       <c r="X58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>115</v>
       </c>
       <c r="Y58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>120</v>
       </c>
       <c r="Z58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>125</v>
       </c>
       <c r="AA58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>130</v>
       </c>
       <c r="AB58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>135</v>
       </c>
       <c r="AC58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>140</v>
       </c>
       <c r="AD58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>145</v>
       </c>
       <c r="AE58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>150</v>
       </c>
       <c r="AF58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>155</v>
       </c>
       <c r="AG58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>160</v>
       </c>
       <c r="AH58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>165</v>
       </c>
       <c r="AI58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>170</v>
       </c>
       <c r="AJ58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>175</v>
       </c>
       <c r="AK58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>180</v>
       </c>
       <c r="AL58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>185</v>
       </c>
       <c r="AM58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>190</v>
       </c>
       <c r="AN58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>195</v>
       </c>
       <c r="AO58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>200</v>
       </c>
       <c r="AP58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>205</v>
       </c>
       <c r="AQ58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>210</v>
       </c>
       <c r="AR58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>215</v>
       </c>
       <c r="AS58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>220</v>
       </c>
       <c r="AT58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>225</v>
       </c>
       <c r="AU58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>230</v>
       </c>
       <c r="AV58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>235</v>
       </c>
       <c r="AW58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>240</v>
       </c>
       <c r="AX58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>245</v>
       </c>
       <c r="AY58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>250</v>
       </c>
       <c r="AZ58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>255</v>
       </c>
       <c r="BA58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>260</v>
       </c>
       <c r="BB58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>265</v>
       </c>
       <c r="BC58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>270</v>
       </c>
       <c r="BD58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>275</v>
       </c>
       <c r="BE58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>280</v>
       </c>
       <c r="BF58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>285</v>
       </c>
       <c r="BG58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>290</v>
       </c>
       <c r="BH58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>295</v>
       </c>
       <c r="BI58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>300</v>
       </c>
       <c r="BJ58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>305</v>
       </c>
       <c r="BK58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>310</v>
       </c>
       <c r="BL58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>315</v>
       </c>
       <c r="BM58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>320</v>
       </c>
       <c r="BN58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>325</v>
       </c>
       <c r="BO58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>330</v>
       </c>
       <c r="BP58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>335</v>
       </c>
       <c r="BQ58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>340</v>
       </c>
       <c r="BR58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>345</v>
       </c>
       <c r="BS58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>350</v>
       </c>
       <c r="BT58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>355</v>
       </c>
       <c r="BU58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>360</v>
       </c>
       <c r="BV58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>365</v>
       </c>
       <c r="BW58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>370</v>
       </c>
       <c r="BX58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>375</v>
       </c>
       <c r="BY58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>380</v>
       </c>
       <c r="BZ58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>385</v>
       </c>
       <c r="CA58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>390</v>
       </c>
       <c r="CB58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>395</v>
       </c>
       <c r="CC58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>400</v>
       </c>
       <c r="CD58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>405</v>
       </c>
       <c r="CE58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>410</v>
       </c>
       <c r="CF58">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>415</v>
       </c>
       <c r="CG58">
-        <f t="shared" ref="CG58:CV58" si="42">SUM(CG50:CG57)</f>
+        <f t="shared" ref="CG58:CV58" si="44">SUM(CG50:CG57)</f>
         <v>420</v>
       </c>
       <c r="CH58">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>425</v>
       </c>
       <c r="CI58">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>430</v>
       </c>
       <c r="CJ58">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>435</v>
       </c>
       <c r="CK58">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>440</v>
       </c>
       <c r="CL58">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>445</v>
       </c>
       <c r="CM58">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>450</v>
       </c>
       <c r="CN58">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>455</v>
       </c>
       <c r="CO58">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>460</v>
       </c>
       <c r="CP58">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>465</v>
       </c>
       <c r="CQ58">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>470</v>
       </c>
       <c r="CR58">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>475</v>
       </c>
       <c r="CS58">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>480</v>
       </c>
       <c r="CT58">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>485</v>
       </c>
       <c r="CU58">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>490</v>
       </c>
       <c r="CV58">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>495</v>
       </c>
       <c r="CW58">
-        <f t="shared" ref="CW58" si="43">SUM(CW50:CW57)</f>
+        <f t="shared" ref="CW58" si="45">SUM(CW50:CW57)</f>
         <v>500</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Introduce grouping on spells: - GENERAL - ELEMENTAL - ENERGY - DIVINE - NATURE - SOUL Introduce new types of summoning spells (in addition to the CALLING_THE_SOULS): - CALLING_ANIMALS - SUMMON_GUARDIAN - PROJECTION_OF_ENERGY - FRIEND_IN_NEED Different summoning spells have different characteristics. CALLING_THE_SOULS: manifests one of the soul chips. CALLING_ANIMALS: summons a companion animal (FALCON, DOG, WOLF, BEAR). SUMMON_GUARDIAN: summons a guardian warrior (HUNTER, MILITIA, SWORDSMAN). PROJECTION_OF_ENERGY: projectiles the energy of the caster with its 80% properties (attack, defense, etc). FRIEND_IN_NEED: summons a divine guardian (KNIGHT, COMMANDER). May be unsuccessful. The automatism of casting summoning magic improved. Not only one summoning can be used whenever an opportunity arrives. However, there are limitations in the spell casting. E.g. a divine guardian can be called only when there are no other companions.
</commit_message>
<xml_diff>
--- a/doc/caste_system.xlsx
+++ b/doc/caste_system.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/349dfb9748b30a92/Asztali gép/ataliasflame_2.0/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8491" documentId="8_{652F4476-B36F-42CD-831D-0D71B9923ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF7D7D4A-0185-4387-A30A-9C058EC4EAA4}"/>
+  <xr:revisionPtr revIDLastSave="8562" documentId="8_{652F4476-B36F-42CD-831D-0D71B9923ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9510C17D-A269-4E8B-9F5F-AE777E450228}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="635" activeTab="7" xr2:uid="{CAF51EC3-63EC-48CD-AA7B-C21B3D5D222B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="635" activeTab="6" xr2:uid="{CAF51EC3-63EC-48CD-AA7B-C21B3D5D222B}"/>
   </bookViews>
   <sheets>
     <sheet name="caste list" sheetId="1" r:id="rId1"/>
@@ -2066,7 +2066,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2094,12 +2094,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2250,7 +2244,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2306,6 +2300,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2318,23 +2317,14 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -2351,6 +2341,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2786,7 +2780,7 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="40" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="23" t="s">
@@ -2842,7 +2836,7 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="36"/>
+      <c r="A4" s="41"/>
       <c r="B4" s="23" t="s">
         <v>2</v>
       </c>
@@ -2896,7 +2890,7 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="36"/>
+      <c r="A5" s="41"/>
       <c r="B5" s="23" t="s">
         <v>3</v>
       </c>
@@ -2950,7 +2944,7 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="36"/>
+      <c r="A6" s="41"/>
       <c r="B6" s="22" t="s">
         <v>21</v>
       </c>
@@ -3004,7 +2998,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="37"/>
+      <c r="A7" s="42"/>
       <c r="B7" s="21" t="s">
         <v>4</v>
       </c>
@@ -3058,7 +3052,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="40" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="23" t="s">
@@ -3114,7 +3108,7 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="36"/>
+      <c r="A9" s="41"/>
       <c r="B9" s="23" t="s">
         <v>6</v>
       </c>
@@ -3168,7 +3162,7 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="36"/>
+      <c r="A10" s="41"/>
       <c r="B10" s="23" t="s">
         <v>7</v>
       </c>
@@ -3222,7 +3216,7 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="37"/>
+      <c r="A11" s="42"/>
       <c r="B11" s="21" t="s">
         <v>8</v>
       </c>
@@ -3276,7 +3270,7 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="40" t="s">
         <v>79</v>
       </c>
       <c r="B12" s="23" t="s">
@@ -3332,7 +3326,7 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="36"/>
+      <c r="A13" s="41"/>
       <c r="B13" s="23" t="s">
         <v>10</v>
       </c>
@@ -3386,7 +3380,7 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="36"/>
+      <c r="A14" s="41"/>
       <c r="B14" s="23" t="s">
         <v>11</v>
       </c>
@@ -3440,7 +3434,7 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="37"/>
+      <c r="A15" s="42"/>
       <c r="B15" s="21" t="s">
         <v>12</v>
       </c>
@@ -3494,7 +3488,7 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="40" t="s">
         <v>80</v>
       </c>
       <c r="B16" s="23" t="s">
@@ -3550,7 +3544,7 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="36"/>
+      <c r="A17" s="41"/>
       <c r="B17" s="23" t="s">
         <v>14</v>
       </c>
@@ -3604,7 +3598,7 @@
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" s="36"/>
+      <c r="A18" s="41"/>
       <c r="B18" s="23" t="s">
         <v>15</v>
       </c>
@@ -3658,7 +3652,7 @@
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" s="37"/>
+      <c r="A19" s="42"/>
       <c r="B19" s="21" t="s">
         <v>16</v>
       </c>
@@ -3712,7 +3706,7 @@
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="40" t="s">
         <v>81</v>
       </c>
       <c r="B20" s="23" t="s">
@@ -3768,7 +3762,7 @@
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21" s="36"/>
+      <c r="A21" s="41"/>
       <c r="B21" s="23" t="s">
         <v>18</v>
       </c>
@@ -3822,7 +3816,7 @@
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22" s="36"/>
+      <c r="A22" s="41"/>
       <c r="B22" s="23" t="s">
         <v>19</v>
       </c>
@@ -3876,7 +3870,7 @@
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23" s="37"/>
+      <c r="A23" s="42"/>
       <c r="B23" s="21" t="s">
         <v>20</v>
       </c>
@@ -22604,23 +22598,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8F833C9-BBEE-43B5-917D-731D1CF064F0}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="60.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" style="34" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="44" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" style="32" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="10.33203125" style="32" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="32" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" style="34" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5546875" style="32" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" style="32" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="10.109375" style="32" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5546875" style="32" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="10.6640625" style="32" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="13.88671875" style="32" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" style="44" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5546875" style="44" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" style="44" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" style="44" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5546875" style="44" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" style="44" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" style="44" bestFit="1" customWidth="1"/>
     <col min="257" max="257" width="17.44140625" customWidth="1"/>
     <col min="258" max="258" width="63" customWidth="1"/>
     <col min="259" max="259" width="12.6640625" customWidth="1"/>
@@ -23443,7 +23439,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="44" t="s">
         <v>85</v>
       </c>
       <c r="D1" s="32" t="s">
@@ -23455,36 +23451,36 @@
       <c r="F1" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="44" t="s">
         <v>89</v>
       </c>
       <c r="H1" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="I1" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="J1" s="44" t="s">
         <v>92</v>
       </c>
-      <c r="K1" s="32" t="s">
+      <c r="K1" s="44" t="s">
         <v>93</v>
       </c>
-      <c r="L1" s="32" t="s">
+      <c r="L1" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="M1" s="32" t="s">
+      <c r="M1" s="44" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="35" t="s">
         <v>96</v>
       </c>
       <c r="B2" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="44" t="s">
         <v>39</v>
       </c>
       <c r="D2" s="32" t="s">
@@ -23496,36 +23492,36 @@
       <c r="F2" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="J2" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="K2" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="L2" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="M2" s="32" t="s">
+      <c r="G2" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" s="44" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="44" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="44" t="s">
         <v>39</v>
       </c>
       <c r="D3" s="32" t="s">
@@ -23537,36 +23533,36 @@
       <c r="F3" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="H3" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="I3" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="J3" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="K3" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="L3" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="M3" s="32" t="s">
+      <c r="G3" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="M3" s="44" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="44" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="45" t="s">
         <v>99</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="44" t="s">
         <v>39</v>
       </c>
       <c r="D4" s="32" t="s">
@@ -23578,36 +23574,36 @@
       <c r="F4" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="I4" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="J4" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="K4" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="L4" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="M4" s="32" t="s">
+      <c r="G4" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" s="44" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="44" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="45" t="s">
         <v>100</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="44" t="s">
         <v>39</v>
       </c>
       <c r="D5" s="32" t="s">
@@ -23619,36 +23615,36 @@
       <c r="F5" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G5" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="I5" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="J5" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="K5" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="L5" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="M5" s="32" t="s">
+      <c r="G5" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="L5" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="M5" s="44" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="44" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="44" t="s">
         <v>39</v>
       </c>
       <c r="D6" s="32" t="s">
@@ -23660,36 +23656,36 @@
       <c r="F6" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="J6" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="K6" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="L6" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="M6" s="32" t="s">
+      <c r="G6" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="M6" s="44" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="44" t="s">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="45" t="s">
         <v>102</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="44" t="s">
         <v>39</v>
       </c>
       <c r="D7" s="32" t="s">
@@ -23701,36 +23697,36 @@
       <c r="F7" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="H7" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="I7" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="J7" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="K7" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="L7" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="M7" s="32" t="s">
+      <c r="G7" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="J7" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="L7" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="M7" s="44" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="44" t="s">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="C8" s="45" t="s">
+      <c r="C8" s="44" t="s">
         <v>39</v>
       </c>
       <c r="D8" s="32" t="s">
@@ -23742,36 +23738,36 @@
       <c r="F8" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="I8" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="J8" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="K8" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="L8" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="M8" s="32" t="s">
+      <c r="G8" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="J8" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="K8" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="L8" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="M8" s="44" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="44" t="s">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="45" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="C9" s="44" t="s">
         <v>39</v>
       </c>
       <c r="D9" s="32" t="s">
@@ -23783,36 +23779,36 @@
       <c r="F9" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="H9" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="I9" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="J9" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="K9" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="L9" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="M9" s="32" t="s">
+      <c r="G9" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="J9" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="K9" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="L9" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="M9" s="44" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="44" t="s">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="45" t="s">
         <v>105</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="C10" s="45" t="s">
+      <c r="C10" s="44" t="s">
         <v>39</v>
       </c>
       <c r="D10" s="32" t="s">
@@ -23824,36 +23820,36 @@
       <c r="F10" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G10" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="H10" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="I10" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="J10" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="K10" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="L10" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="M10" s="32" t="s">
+      <c r="G10" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="J10" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="K10" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="L10" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="M10" s="44" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="46" t="s">
         <v>106</v>
       </c>
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="44" t="s">
         <v>39</v>
       </c>
       <c r="D11" s="32" t="s">
@@ -23865,30 +23861,30 @@
       <c r="F11" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G11" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="H11" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="I11" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="J11" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="K11" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="L11" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="M11" s="32" t="s">
+      <c r="G11" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="K11" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="L11" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="M11" s="44" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:13" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="37" t="s">
         <v>107</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -23906,7 +23902,7 @@
       <c r="F12" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G12" s="32" t="s">
+      <c r="G12" s="44" t="s">
         <v>40</v>
       </c>
       <c r="H12" s="32" t="s">
@@ -23947,7 +23943,7 @@
       <c r="F13" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G13" s="32" t="s">
+      <c r="G13" s="44" t="s">
         <v>40</v>
       </c>
       <c r="H13" s="32" t="s">
@@ -23988,7 +23984,7 @@
       <c r="F14" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G14" s="32" t="s">
+      <c r="G14" s="44" t="s">
         <v>40</v>
       </c>
       <c r="H14" s="32" t="s">
@@ -24029,7 +24025,7 @@
       <c r="F15" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G15" s="32" t="s">
+      <c r="G15" s="44" t="s">
         <v>40</v>
       </c>
       <c r="H15" s="32" t="s">
@@ -24070,7 +24066,7 @@
       <c r="F16" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G16" s="32" t="s">
+      <c r="G16" s="44" t="s">
         <v>40</v>
       </c>
       <c r="H16" s="32" t="s">
@@ -24111,7 +24107,7 @@
       <c r="F17" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G17" s="32" t="s">
+      <c r="G17" s="44" t="s">
         <v>40</v>
       </c>
       <c r="H17" s="32" t="s">
@@ -24152,7 +24148,7 @@
       <c r="F18" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G18" s="32" t="s">
+      <c r="G18" s="44" t="s">
         <v>40</v>
       </c>
       <c r="H18" s="32" t="s">
@@ -24193,7 +24189,7 @@
       <c r="F19" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G19" s="32" t="s">
+      <c r="G19" s="44" t="s">
         <v>40</v>
       </c>
       <c r="H19" s="32" t="s">
@@ -24234,7 +24230,7 @@
       <c r="F20" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="32" t="s">
+      <c r="G20" s="44" t="s">
         <v>40</v>
       </c>
       <c r="H20" s="32" t="s">
@@ -24257,7 +24253,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="42" t="s">
+      <c r="A21" s="38" t="s">
         <v>120</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -24275,7 +24271,7 @@
       <c r="F21" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="32" t="s">
+      <c r="G21" s="44" t="s">
         <v>40</v>
       </c>
       <c r="H21" s="32" t="s">
@@ -24298,7 +24294,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="37" t="s">
         <v>122</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -24316,7 +24312,7 @@
       <c r="F22" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G22" s="32" t="s">
+      <c r="G22" s="44" t="s">
         <v>40</v>
       </c>
       <c r="H22" s="32" t="s">
@@ -24357,7 +24353,7 @@
       <c r="F23" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G23" s="32" t="s">
+      <c r="G23" s="44" t="s">
         <v>40</v>
       </c>
       <c r="H23" s="32" t="s">
@@ -24398,7 +24394,7 @@
       <c r="F24" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G24" s="32" t="s">
+      <c r="G24" s="44" t="s">
         <v>40</v>
       </c>
       <c r="H24" s="32" t="s">
@@ -24439,7 +24435,7 @@
       <c r="F25" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G25" s="32" t="s">
+      <c r="G25" s="44" t="s">
         <v>40</v>
       </c>
       <c r="H25" s="32" t="s">
@@ -24462,7 +24458,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="42" t="s">
+      <c r="A26" s="38" t="s">
         <v>128</v>
       </c>
       <c r="B26" s="3" t="s">
@@ -24480,7 +24476,7 @@
       <c r="F26" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G26" s="32" t="s">
+      <c r="G26" s="44" t="s">
         <v>40</v>
       </c>
       <c r="H26" s="32" t="s">
@@ -24503,7 +24499,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="41" t="s">
+      <c r="A27" s="37" t="s">
         <v>130</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -24521,7 +24517,7 @@
       <c r="F27" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="G27" s="32" t="s">
+      <c r="G27" s="44" t="s">
         <v>40</v>
       </c>
       <c r="H27" s="32" t="s">
@@ -24562,7 +24558,7 @@
       <c r="F28" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="G28" s="32" t="s">
+      <c r="G28" s="44" t="s">
         <v>40</v>
       </c>
       <c r="H28" s="32" t="s">
@@ -24603,7 +24599,7 @@
       <c r="F29" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="G29" s="32" t="s">
+      <c r="G29" s="44" t="s">
         <v>40</v>
       </c>
       <c r="H29" s="32" t="s">
@@ -24644,7 +24640,7 @@
       <c r="F30" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="G30" s="32" t="s">
+      <c r="G30" s="44" t="s">
         <v>40</v>
       </c>
       <c r="H30" s="32" t="s">
@@ -24667,7 +24663,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="42" t="s">
+      <c r="A31" s="38" t="s">
         <v>137</v>
       </c>
       <c r="B31" s="3" t="s">
@@ -24685,7 +24681,7 @@
       <c r="F31" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="G31" s="32" t="s">
+      <c r="G31" s="44" t="s">
         <v>40</v>
       </c>
       <c r="H31" s="32" t="s">
@@ -24708,13 +24704,13 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32" s="39" t="s">
+      <c r="A32" s="35" t="s">
         <v>139</v>
       </c>
       <c r="B32" t="s">
         <v>140</v>
       </c>
-      <c r="C32" s="34" t="s">
+      <c r="C32" s="44" t="s">
         <v>40</v>
       </c>
       <c r="D32" s="32" t="s">
@@ -24726,189 +24722,189 @@
       <c r="F32" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G32" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="H32" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="I32" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="J32" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="K32" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="L32" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="M32" s="32" t="s">
+      <c r="G32" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="H32" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="I32" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="J32" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="K32" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="L32" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="M32" s="44" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="44" t="s">
+    <row r="33" spans="1:13" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="45" t="s">
         <v>141</v>
       </c>
-      <c r="B33" s="44" t="s">
+      <c r="B33" s="45" t="s">
         <v>142</v>
       </c>
-      <c r="C33" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="D33" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="E33" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="F33" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="G33" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="H33" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="I33" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="J33" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="K33" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="L33" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="M33" s="32" t="s">
+      <c r="C33" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="E33" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="F33" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="G33" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="H33" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="I33" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="J33" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="K33" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="L33" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="M33" s="44" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="44" t="s">
+    <row r="34" spans="1:13" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="B34" s="44" t="s">
+      <c r="B34" s="45" t="s">
         <v>144</v>
       </c>
-      <c r="C34" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="D34" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="E34" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="F34" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="G34" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="H34" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="I34" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="J34" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="K34" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="L34" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="M34" s="32" t="s">
+      <c r="C34" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="E34" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="F34" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="G34" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="H34" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="I34" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="J34" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="K34" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="L34" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="M34" s="44" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="44" t="s">
+    <row r="35" spans="1:13" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="45" t="s">
         <v>145</v>
       </c>
-      <c r="B35" s="44" t="s">
+      <c r="B35" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="C35" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="D35" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="E35" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="F35" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="G35" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="H35" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="I35" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="J35" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="K35" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="L35" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="M35" s="32" t="s">
+      <c r="C35" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="E35" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="F35" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="G35" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="H35" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="I35" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="J35" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="K35" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="L35" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="M35" s="44" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="B36" s="44" t="s">
+      <c r="B36" s="45" t="s">
         <v>148</v>
       </c>
-      <c r="C36" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="D36" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="E36" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="F36" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="G36" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="H36" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="I36" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="J36" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="K36" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="L36" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="M36" s="32" t="s">
+      <c r="C36" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="E36" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="F36" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="G36" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="H36" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="I36" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="J36" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="K36" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="L36" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="M36" s="44" t="s">
         <v>40</v>
       </c>
     </row>
@@ -24921,23 +24917,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA1C4ECE-D418-419E-9393-664BDA889D6E}">
   <dimension ref="A1:AJ35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AL10" sqref="AL10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.21875" style="49" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" style="49" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" style="49" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.109375" style="49" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" style="49" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" style="49" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" style="49" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.44140625" style="49" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11" style="49" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.88671875" style="3" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="13.5546875" style="3" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="4.5546875" style="3" hidden="1" customWidth="1"/>
@@ -24958,41 +24952,41 @@
     <col min="29" max="29" width="6.33203125" style="3" hidden="1" customWidth="1"/>
     <col min="30" max="30" width="11.33203125" style="3" hidden="1" customWidth="1"/>
     <col min="31" max="31" width="9.88671875" style="3" hidden="1" customWidth="1"/>
-    <col min="33" max="33" width="8.6640625" style="44" hidden="1" customWidth="1"/>
-    <col min="34" max="34" width="14.6640625" style="44" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="14.33203125" style="44" hidden="1" customWidth="1"/>
-    <col min="36" max="36" width="12.6640625" style="44" hidden="1" customWidth="1"/>
+    <col min="33" max="33" width="8.6640625" style="45" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.6640625" style="45" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.33203125" style="45" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.6640625" style="45" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.3">
       <c r="B1" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="E1" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="F1" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="G1" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="H1" s="48" t="s">
+      <c r="H1" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="I1" s="48" t="s">
+      <c r="I1" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="J1" s="48" t="s">
+      <c r="J1" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="K1" s="48" t="s">
+      <c r="K1" s="34" t="s">
         <v>106</v>
       </c>
       <c r="L1" s="32" t="s">
@@ -25058,51 +25052,51 @@
       <c r="AF1" s="34" t="s">
         <v>139</v>
       </c>
-      <c r="AG1" s="45" t="s">
+      <c r="AG1" s="44" t="s">
         <v>141</v>
       </c>
-      <c r="AH1" s="45" t="s">
+      <c r="AH1" s="44" t="s">
         <v>143</v>
       </c>
-      <c r="AI1" s="45" t="s">
+      <c r="AI1" s="44" t="s">
         <v>145</v>
       </c>
-      <c r="AJ1" s="45" t="s">
+      <c r="AJ1" s="44" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="39" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="J2" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="K2" s="48" t="s">
+      <c r="C2" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="34" t="s">
         <v>40</v>
       </c>
       <c r="L2" s="32" t="s">
@@ -25168,51 +25162,51 @@
       <c r="AF2" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AG2" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH2" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI2" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ2" s="45" t="s">
+      <c r="AG2" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH2" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI2" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ2" s="44" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="35" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="H3" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="I3" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="J3" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="K3" s="48" t="s">
+      <c r="C3" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" s="34" t="s">
         <v>40</v>
       </c>
       <c r="L3" s="32" t="s">
@@ -25278,16 +25272,16 @@
       <c r="AF3" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AG3" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH3" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI3" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ3" s="45" t="s">
+      <c r="AG3" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH3" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI3" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ3" s="44" t="s">
         <v>40</v>
       </c>
     </row>
@@ -25298,31 +25292,31 @@
       <c r="B4" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="I4" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="J4" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="K4" s="48" t="s">
+      <c r="C4" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" s="34" t="s">
         <v>40</v>
       </c>
       <c r="L4" s="32" t="s">
@@ -25388,16 +25382,16 @@
       <c r="AF4" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AG4" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH4" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI4" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ4" s="45" t="s">
+      <c r="AG4" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH4" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI4" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ4" s="44" t="s">
         <v>40</v>
       </c>
     </row>
@@ -25408,31 +25402,31 @@
       <c r="B5" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="I5" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="J5" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="K5" s="48" t="s">
+      <c r="C5" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" s="34" t="s">
         <v>40</v>
       </c>
       <c r="L5" s="32" t="s">
@@ -25498,51 +25492,51 @@
       <c r="AF5" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AG5" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH5" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI5" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ5" s="45" t="s">
+      <c r="AG5" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH5" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI5" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ5" s="44" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="36" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="I6" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="J6" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="K6" s="48" t="s">
+      <c r="C6" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" s="34" t="s">
         <v>40</v>
       </c>
       <c r="L6" s="32" t="s">
@@ -25608,51 +25602,51 @@
       <c r="AF6" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AG6" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH6" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI6" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ6" s="45" t="s">
+      <c r="AG6" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH6" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI6" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ6" s="44" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="35" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="H7" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="I7" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="J7" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="K7" s="48" t="s">
+      <c r="C7" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J7" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7" s="34" t="s">
         <v>40</v>
       </c>
       <c r="L7" s="32" t="s">
@@ -25718,16 +25712,16 @@
       <c r="AF7" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AG7" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH7" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI7" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ7" s="45" t="s">
+      <c r="AG7" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH7" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI7" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ7" s="44" t="s">
         <v>40</v>
       </c>
     </row>
@@ -25738,31 +25732,31 @@
       <c r="B8" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="H8" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="I8" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="J8" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="K8" s="48" t="s">
+      <c r="C8" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J8" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" s="34" t="s">
         <v>40</v>
       </c>
       <c r="L8" s="32" t="s">
@@ -25828,16 +25822,16 @@
       <c r="AF8" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AG8" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH8" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI8" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ8" s="45" t="s">
+      <c r="AG8" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH8" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI8" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ8" s="44" t="s">
         <v>40</v>
       </c>
     </row>
@@ -25848,31 +25842,31 @@
       <c r="B9" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="I9" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="J9" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="K9" s="48" t="s">
+      <c r="C9" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J9" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K9" s="34" t="s">
         <v>40</v>
       </c>
       <c r="L9" s="32" t="s">
@@ -25938,51 +25932,51 @@
       <c r="AF9" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AG9" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH9" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI9" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ9" s="45" t="s">
+      <c r="AG9" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH9" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI9" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ9" s="44" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="36" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="G10" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="H10" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="I10" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="J10" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="K10" s="48" t="s">
+      <c r="C10" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J10" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K10" s="34" t="s">
         <v>40</v>
       </c>
       <c r="L10" s="32" t="s">
@@ -26048,51 +26042,51 @@
       <c r="AF10" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AG10" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH10" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI10" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ10" s="45" t="s">
+      <c r="AG10" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH10" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI10" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ10" s="44" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="35" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="G11" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="H11" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="I11" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="J11" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="K11" s="48" t="s">
+      <c r="C11" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K11" s="34" t="s">
         <v>40</v>
       </c>
       <c r="L11" s="32" t="s">
@@ -26158,16 +26152,16 @@
       <c r="AF11" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AG11" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH11" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI11" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ11" s="45" t="s">
+      <c r="AG11" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH11" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI11" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ11" s="44" t="s">
         <v>40</v>
       </c>
     </row>
@@ -26178,31 +26172,31 @@
       <c r="B12" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="F12" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="H12" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="I12" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="J12" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="K12" s="48" t="s">
+      <c r="C12" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J12" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K12" s="34" t="s">
         <v>40</v>
       </c>
       <c r="L12" s="32" t="s">
@@ -26268,16 +26262,16 @@
       <c r="AF12" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AG12" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH12" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI12" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ12" s="45" t="s">
+      <c r="AG12" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH12" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI12" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ12" s="44" t="s">
         <v>40</v>
       </c>
     </row>
@@ -26288,31 +26282,31 @@
       <c r="B13" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="G13" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="H13" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="I13" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="J13" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="K13" s="48" t="s">
+      <c r="C13" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="I13" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J13" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K13" s="34" t="s">
         <v>40</v>
       </c>
       <c r="L13" s="32" t="s">
@@ -26378,51 +26372,51 @@
       <c r="AF13" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AG13" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH13" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI13" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ13" s="45" t="s">
+      <c r="AG13" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH13" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI13" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ13" s="44" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A14" s="40" t="s">
+      <c r="A14" s="36" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="H14" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="I14" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="J14" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="K14" s="48" t="s">
+      <c r="C14" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="I14" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J14" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K14" s="34" t="s">
         <v>40</v>
       </c>
       <c r="L14" s="32" t="s">
@@ -26488,51 +26482,51 @@
       <c r="AF14" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AG14" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH14" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI14" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ14" s="45" t="s">
+      <c r="AG14" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH14" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI14" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ14" s="44" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="35" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="G15" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="H15" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="I15" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="J15" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="K15" s="48" t="s">
+      <c r="C15" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I15" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J15" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="K15" s="34" t="s">
         <v>40</v>
       </c>
       <c r="L15" s="32" t="s">
@@ -26598,16 +26592,16 @@
       <c r="AF15" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AG15" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH15" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI15" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ15" s="45" t="s">
+      <c r="AG15" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH15" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI15" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ15" s="44" t="s">
         <v>40</v>
       </c>
     </row>
@@ -26618,31 +26612,31 @@
       <c r="B16" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="G16" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="H16" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="I16" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="J16" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="K16" s="48" t="s">
+      <c r="C16" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H16" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I16" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J16" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="K16" s="34" t="s">
         <v>40</v>
       </c>
       <c r="L16" s="32" t="s">
@@ -26708,16 +26702,16 @@
       <c r="AF16" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AG16" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH16" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI16" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ16" s="45" t="s">
+      <c r="AG16" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH16" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI16" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ16" s="44" t="s">
         <v>39</v>
       </c>
     </row>
@@ -26728,31 +26722,31 @@
       <c r="B17" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="F17" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="G17" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="H17" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="I17" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="J17" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="K17" s="48" t="s">
+      <c r="C17" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H17" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I17" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J17" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="K17" s="34" t="s">
         <v>40</v>
       </c>
       <c r="L17" s="32" t="s">
@@ -26818,51 +26812,51 @@
       <c r="AF17" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AG17" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH17" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI17" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ17" s="45" t="s">
+      <c r="AG17" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH17" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI17" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ17" s="44" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A18" s="40" t="s">
+      <c r="A18" s="36" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="G18" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="H18" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="I18" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="J18" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="K18" s="48" t="s">
+      <c r="C18" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H18" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I18" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J18" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="K18" s="34" t="s">
         <v>39</v>
       </c>
       <c r="L18" s="32" t="s">
@@ -26928,51 +26922,51 @@
       <c r="AF18" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AG18" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH18" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI18" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ18" s="45" t="s">
+      <c r="AG18" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH18" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI18" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ18" s="44" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="35" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="F19" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="G19" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="H19" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="I19" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="J19" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="K19" s="48" t="s">
+      <c r="C19" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H19" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I19" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J19" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="K19" s="34" t="s">
         <v>39</v>
       </c>
       <c r="L19" s="32" t="s">
@@ -27038,16 +27032,16 @@
       <c r="AF19" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AG19" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH19" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI19" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ19" s="45" t="s">
+      <c r="AG19" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH19" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI19" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ19" s="44" t="s">
         <v>39</v>
       </c>
     </row>
@@ -27058,31 +27052,31 @@
       <c r="B20" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="F20" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="G20" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="H20" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="I20" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="J20" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="K20" s="48" t="s">
+      <c r="C20" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="G20" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H20" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I20" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J20" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="K20" s="34" t="s">
         <v>39</v>
       </c>
       <c r="L20" s="32" t="s">
@@ -27148,16 +27142,16 @@
       <c r="AF20" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AG20" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH20" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI20" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ20" s="45" t="s">
+      <c r="AG20" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH20" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI20" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ20" s="44" t="s">
         <v>39</v>
       </c>
     </row>
@@ -27168,31 +27162,31 @@
       <c r="B21" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="E21" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="F21" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="G21" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="H21" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="I21" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="J21" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="K21" s="48" t="s">
+      <c r="C21" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H21" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I21" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J21" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="K21" s="34" t="s">
         <v>39</v>
       </c>
       <c r="L21" s="32" t="s">
@@ -27258,51 +27252,51 @@
       <c r="AF21" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AG21" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH21" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI21" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ21" s="45" t="s">
+      <c r="AG21" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH21" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI21" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ21" s="44" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A22" s="40" t="s">
+      <c r="A22" s="36" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="F22" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="G22" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="H22" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="I22" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="J22" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="K22" s="48" t="s">
+      <c r="C22" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H22" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I22" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J22" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="K22" s="34" t="s">
         <v>39</v>
       </c>
       <c r="L22" s="32" t="s">
@@ -27368,16 +27362,16 @@
       <c r="AF22" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AG22" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH22" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI22" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ22" s="45" t="s">
+      <c r="AG22" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH22" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI22" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ22" s="44" t="s">
         <v>39</v>
       </c>
     </row>
@@ -27385,31 +27379,31 @@
       <c r="B25" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="C25" s="48" t="s">
+      <c r="C25" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="D25" s="48" t="s">
+      <c r="D25" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="E25" s="48" t="s">
+      <c r="E25" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="F25" s="48" t="s">
+      <c r="F25" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="G25" s="48" t="s">
+      <c r="G25" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="H25" s="48" t="s">
+      <c r="H25" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="I25" s="48" t="s">
+      <c r="I25" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="J25" s="48" t="s">
+      <c r="J25" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="K25" s="48" t="s">
+      <c r="K25" s="34" t="s">
         <v>106</v>
       </c>
       <c r="L25" s="32" t="s">
@@ -27475,51 +27469,51 @@
       <c r="AF25" s="34" t="s">
         <v>139</v>
       </c>
-      <c r="AG25" s="45" t="s">
+      <c r="AG25" s="44" t="s">
         <v>141</v>
       </c>
-      <c r="AH25" s="45" t="s">
+      <c r="AH25" s="44" t="s">
         <v>143</v>
       </c>
-      <c r="AI25" s="45" t="s">
+      <c r="AI25" s="44" t="s">
         <v>145</v>
       </c>
-      <c r="AJ25" s="45" t="s">
+      <c r="AJ25" s="44" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="26" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A26" s="39" t="s">
+      <c r="A26" s="35" t="s">
         <v>22</v>
       </c>
       <c r="B26" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="E26" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="F26" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="G26" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="H26" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="I26" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="J26" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="K26" s="48" t="s">
+      <c r="C26" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="F26" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="G26" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H26" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="I26" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J26" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="K26" s="34" t="s">
         <v>39</v>
       </c>
       <c r="L26" s="32" t="s">
@@ -27585,16 +27579,16 @@
       <c r="AF26" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AG26" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH26" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI26" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ26" s="45" t="s">
+      <c r="AG26" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH26" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI26" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ26" s="44" t="s">
         <v>39</v>
       </c>
     </row>
@@ -27605,31 +27599,31 @@
       <c r="B27" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="D27" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="E27" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="F27" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="G27" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="H27" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="I27" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="J27" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="K27" s="48" t="s">
+      <c r="C27" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="F27" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="G27" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H27" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="I27" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J27" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="K27" s="34" t="s">
         <v>39</v>
       </c>
       <c r="L27" s="32" t="s">
@@ -27695,16 +27689,16 @@
       <c r="AF27" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AG27" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH27" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI27" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ27" s="45" t="s">
+      <c r="AG27" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH27" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI27" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ27" s="44" t="s">
         <v>39</v>
       </c>
     </row>
@@ -27715,31 +27709,31 @@
       <c r="B28" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="D28" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="E28" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="F28" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="G28" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="H28" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="I28" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="J28" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="K28" s="48" t="s">
+      <c r="C28" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="F28" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="G28" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H28" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="I28" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J28" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="K28" s="34" t="s">
         <v>39</v>
       </c>
       <c r="L28" s="32" t="s">
@@ -27805,16 +27799,16 @@
       <c r="AF28" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AG28" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH28" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI28" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ28" s="45" t="s">
+      <c r="AG28" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH28" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI28" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ28" s="44" t="s">
         <v>39</v>
       </c>
     </row>
@@ -27825,31 +27819,31 @@
       <c r="B29" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="D29" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="E29" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="F29" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="G29" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="H29" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="I29" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="J29" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="K29" s="48" t="s">
+      <c r="C29" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="F29" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="G29" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H29" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="I29" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J29" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="K29" s="34" t="s">
         <v>39</v>
       </c>
       <c r="L29" s="32" t="s">
@@ -27915,16 +27909,16 @@
       <c r="AF29" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AG29" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH29" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI29" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ29" s="45" t="s">
+      <c r="AG29" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH29" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI29" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ29" s="44" t="s">
         <v>39</v>
       </c>
     </row>
@@ -27935,31 +27929,31 @@
       <c r="B30" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="D30" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="E30" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="F30" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="G30" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="H30" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="I30" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="J30" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="K30" s="48" t="s">
+      <c r="C30" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E30" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="F30" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="G30" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H30" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="I30" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J30" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K30" s="34" t="s">
         <v>39</v>
       </c>
       <c r="L30" s="32" t="s">
@@ -28025,16 +28019,16 @@
       <c r="AF30" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AG30" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH30" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI30" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ30" s="45" t="s">
+      <c r="AG30" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH30" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI30" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ30" s="44" t="s">
         <v>40</v>
       </c>
     </row>
@@ -28045,31 +28039,31 @@
       <c r="B31" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C31" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="D31" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="E31" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="F31" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="G31" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="H31" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="I31" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="J31" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="K31" s="48" t="s">
+      <c r="C31" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="F31" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="G31" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H31" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="I31" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J31" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K31" s="34" t="s">
         <v>40</v>
       </c>
       <c r="L31" s="32" t="s">
@@ -28135,16 +28129,16 @@
       <c r="AF31" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AG31" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH31" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI31" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ31" s="45" t="s">
+      <c r="AG31" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH31" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI31" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ31" s="44" t="s">
         <v>40</v>
       </c>
     </row>
@@ -28155,31 +28149,31 @@
       <c r="B32" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="D32" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="E32" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="F32" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="G32" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="H32" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="I32" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="J32" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="K32" s="48" t="s">
+      <c r="C32" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E32" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="F32" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="G32" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H32" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="I32" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J32" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K32" s="34" t="s">
         <v>40</v>
       </c>
       <c r="L32" s="32" t="s">
@@ -28245,16 +28239,16 @@
       <c r="AF32" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AG32" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH32" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI32" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ32" s="45" t="s">
+      <c r="AG32" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH32" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI32" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ32" s="44" t="s">
         <v>40</v>
       </c>
     </row>
@@ -28265,31 +28259,31 @@
       <c r="B33" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C33" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="D33" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="E33" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="F33" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="G33" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="H33" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="I33" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="J33" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="K33" s="48" t="s">
+      <c r="C33" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E33" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="F33" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="G33" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H33" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="I33" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J33" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="K33" s="34" t="s">
         <v>39</v>
       </c>
       <c r="L33" s="32" t="s">
@@ -28355,16 +28349,16 @@
       <c r="AF33" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AG33" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH33" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI33" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ33" s="45" t="s">
+      <c r="AG33" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH33" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI33" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ33" s="44" t="s">
         <v>39</v>
       </c>
     </row>
@@ -28375,31 +28369,31 @@
       <c r="B34" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="D34" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="E34" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="F34" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="G34" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="H34" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="I34" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="J34" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="K34" s="48" t="s">
+      <c r="C34" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E34" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="F34" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="G34" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H34" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="I34" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J34" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="K34" s="34" t="s">
         <v>39</v>
       </c>
       <c r="L34" s="32" t="s">
@@ -28465,51 +28459,51 @@
       <c r="AF34" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AG34" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH34" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI34" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ34" s="45" t="s">
+      <c r="AG34" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH34" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI34" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ34" s="44" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A35" s="40" t="s">
+      <c r="A35" s="36" t="s">
         <v>31</v>
       </c>
       <c r="B35" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="D35" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="E35" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="F35" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="G35" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="H35" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="I35" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="J35" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="K35" s="48" t="s">
+      <c r="C35" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E35" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="F35" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="G35" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H35" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="I35" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J35" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="K35" s="34" t="s">
         <v>40</v>
       </c>
       <c r="L35" s="32" t="s">
@@ -28575,16 +28569,16 @@
       <c r="AF35" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AG35" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH35" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI35" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ35" s="45" t="s">
+      <c r="AG35" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH35" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI35" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ35" s="44" t="s">
         <v>39</v>
       </c>
     </row>
@@ -28730,54 +28724,54 @@
       <c r="U1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="W1" s="38" t="s">
+      <c r="W1" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="X1" s="38"/>
-      <c r="Y1" s="38"/>
-      <c r="Z1" s="38"/>
-      <c r="AA1" s="38"/>
-      <c r="AB1" s="38"/>
-      <c r="AD1" s="38" t="s">
+      <c r="X1" s="43"/>
+      <c r="Y1" s="43"/>
+      <c r="Z1" s="43"/>
+      <c r="AA1" s="43"/>
+      <c r="AB1" s="43"/>
+      <c r="AD1" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="AE1" s="38"/>
-      <c r="AF1" s="38"/>
-      <c r="AG1" s="38"/>
-      <c r="AH1" s="38"/>
-      <c r="AI1" s="38"/>
-      <c r="AK1" s="38" t="s">
+      <c r="AE1" s="43"/>
+      <c r="AF1" s="43"/>
+      <c r="AG1" s="43"/>
+      <c r="AH1" s="43"/>
+      <c r="AI1" s="43"/>
+      <c r="AK1" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="AL1" s="38"/>
-      <c r="AM1" s="38"/>
-      <c r="AN1" s="38"/>
-      <c r="AO1" s="38"/>
-      <c r="AP1" s="38"/>
-      <c r="AR1" s="38" t="s">
+      <c r="AL1" s="43"/>
+      <c r="AM1" s="43"/>
+      <c r="AN1" s="43"/>
+      <c r="AO1" s="43"/>
+      <c r="AP1" s="43"/>
+      <c r="AR1" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="AS1" s="38"/>
-      <c r="AT1" s="38"/>
-      <c r="AU1" s="38"/>
-      <c r="AV1" s="38"/>
-      <c r="AW1" s="38"/>
-      <c r="AY1" s="38" t="s">
+      <c r="AS1" s="43"/>
+      <c r="AT1" s="43"/>
+      <c r="AU1" s="43"/>
+      <c r="AV1" s="43"/>
+      <c r="AW1" s="43"/>
+      <c r="AY1" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="AZ1" s="38"/>
-      <c r="BA1" s="38"/>
-      <c r="BB1" s="38"/>
-      <c r="BC1" s="38"/>
-      <c r="BD1" s="38"/>
-      <c r="BF1" s="38" t="s">
+      <c r="AZ1" s="43"/>
+      <c r="BA1" s="43"/>
+      <c r="BB1" s="43"/>
+      <c r="BC1" s="43"/>
+      <c r="BD1" s="43"/>
+      <c r="BF1" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="BG1" s="38"/>
-      <c r="BH1" s="38"/>
-      <c r="BI1" s="38"/>
-      <c r="BJ1" s="38"/>
-      <c r="BK1" s="38"/>
+      <c r="BG1" s="43"/>
+      <c r="BH1" s="43"/>
+      <c r="BI1" s="43"/>
+      <c r="BJ1" s="43"/>
+      <c r="BK1" s="43"/>
     </row>
     <row r="2" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">

</xml_diff>

<commit_message>
Introduce BLESSING magic type. Introduce new types of blessing spells: - DIVINE_PROTECTION - STRENGTHENING - SOUL_CONNECTION - PROTECTIVE_HAND_OF_NATURE - ENERGY_SHIELD Blessing can be used before combat and can have booster effect on attributes. Food now can have a positive effect on magic points.
</commit_message>
<xml_diff>
--- a/doc/caste_system.xlsx
+++ b/doc/caste_system.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/349dfb9748b30a92/Asztali gép/ataliasflame_2.0/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8562" documentId="8_{652F4476-B36F-42CD-831D-0D71B9923ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9510C17D-A269-4E8B-9F5F-AE777E450228}"/>
+  <xr:revisionPtr revIDLastSave="8607" documentId="8_{652F4476-B36F-42CD-831D-0D71B9923ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0DE6EF51-7CC7-4043-8EDB-EFB9CA2B76C2}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="635" activeTab="6" xr2:uid="{CAF51EC3-63EC-48CD-AA7B-C21B3D5D222B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="635" activeTab="7" xr2:uid="{CAF51EC3-63EC-48CD-AA7B-C21B3D5D222B}"/>
   </bookViews>
   <sheets>
     <sheet name="caste list" sheetId="1" r:id="rId1"/>
@@ -2244,7 +2244,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2305,6 +2305,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2320,11 +2323,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -2780,7 +2781,7 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="41" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="23" t="s">
@@ -2836,7 +2837,7 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="41"/>
+      <c r="A4" s="42"/>
       <c r="B4" s="23" t="s">
         <v>2</v>
       </c>
@@ -2890,7 +2891,7 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="41"/>
+      <c r="A5" s="42"/>
       <c r="B5" s="23" t="s">
         <v>3</v>
       </c>
@@ -2944,7 +2945,7 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="41"/>
+      <c r="A6" s="42"/>
       <c r="B6" s="22" t="s">
         <v>21</v>
       </c>
@@ -2998,7 +2999,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="42"/>
+      <c r="A7" s="43"/>
       <c r="B7" s="21" t="s">
         <v>4</v>
       </c>
@@ -3052,7 +3053,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="41" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="23" t="s">
@@ -3108,7 +3109,7 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="41"/>
+      <c r="A9" s="42"/>
       <c r="B9" s="23" t="s">
         <v>6</v>
       </c>
@@ -3162,7 +3163,7 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="41"/>
+      <c r="A10" s="42"/>
       <c r="B10" s="23" t="s">
         <v>7</v>
       </c>
@@ -3216,7 +3217,7 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="42"/>
+      <c r="A11" s="43"/>
       <c r="B11" s="21" t="s">
         <v>8</v>
       </c>
@@ -3270,7 +3271,7 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="41" t="s">
         <v>79</v>
       </c>
       <c r="B12" s="23" t="s">
@@ -3326,7 +3327,7 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="41"/>
+      <c r="A13" s="42"/>
       <c r="B13" s="23" t="s">
         <v>10</v>
       </c>
@@ -3380,7 +3381,7 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="41"/>
+      <c r="A14" s="42"/>
       <c r="B14" s="23" t="s">
         <v>11</v>
       </c>
@@ -3434,7 +3435,7 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="42"/>
+      <c r="A15" s="43"/>
       <c r="B15" s="21" t="s">
         <v>12</v>
       </c>
@@ -3488,7 +3489,7 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="41" t="s">
         <v>80</v>
       </c>
       <c r="B16" s="23" t="s">
@@ -3544,7 +3545,7 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="41"/>
+      <c r="A17" s="42"/>
       <c r="B17" s="23" t="s">
         <v>14</v>
       </c>
@@ -3598,7 +3599,7 @@
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" s="41"/>
+      <c r="A18" s="42"/>
       <c r="B18" s="23" t="s">
         <v>15</v>
       </c>
@@ -3652,7 +3653,7 @@
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" s="42"/>
+      <c r="A19" s="43"/>
       <c r="B19" s="21" t="s">
         <v>16</v>
       </c>
@@ -3706,7 +3707,7 @@
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="40" t="s">
+      <c r="A20" s="41" t="s">
         <v>81</v>
       </c>
       <c r="B20" s="23" t="s">
@@ -3762,7 +3763,7 @@
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21" s="41"/>
+      <c r="A21" s="42"/>
       <c r="B21" s="23" t="s">
         <v>18</v>
       </c>
@@ -3816,7 +3817,7 @@
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22" s="41"/>
+      <c r="A22" s="42"/>
       <c r="B22" s="23" t="s">
         <v>19</v>
       </c>
@@ -3870,7 +3871,7 @@
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23" s="42"/>
+      <c r="A23" s="43"/>
       <c r="B23" s="21" t="s">
         <v>20</v>
       </c>
@@ -20572,7 +20573,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47799533-6B34-4949-9561-D6B03DB6E4FC}">
   <dimension ref="A1:AC10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -22598,25 +22601,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8F833C9-BBEE-43B5-917D-731D1CF064F0}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="60.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" style="44" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="34" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" style="32" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" style="32" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" style="45" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="32" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" style="44" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5546875" style="44" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" style="44" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.109375" style="44" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5546875" style="44" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.6640625" style="44" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.88671875" style="44" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" style="34" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5546875" style="34" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" style="34" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" style="34" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5546875" style="34" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" style="34" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" style="34" bestFit="1" customWidth="1"/>
     <col min="257" max="257" width="17.44140625" customWidth="1"/>
     <col min="258" max="258" width="63" customWidth="1"/>
     <col min="259" max="259" width="12.6640625" customWidth="1"/>
@@ -23439,37 +23440,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="34" t="s">
         <v>85</v>
       </c>
       <c r="D1" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="45" t="s">
         <v>87</v>
       </c>
       <c r="F1" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="G1" s="44" t="s">
+      <c r="G1" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="H1" s="47" t="s">
+      <c r="H1" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="I1" s="44" t="s">
+      <c r="I1" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="J1" s="44" t="s">
+      <c r="J1" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="K1" s="44" t="s">
+      <c r="K1" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="L1" s="44" t="s">
+      <c r="L1" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="M1" s="44" t="s">
+      <c r="M1" s="34" t="s">
         <v>95</v>
       </c>
     </row>
@@ -23480,406 +23481,406 @@
       <c r="B2" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="34" t="s">
         <v>39</v>
       </c>
       <c r="D2" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="45" t="s">
         <v>40</v>
       </c>
       <c r="F2" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="J2" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="K2" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="L2" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="M2" s="44" t="s">
+      <c r="G2" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" s="34" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="45" t="s">
+      <c r="A3" t="s">
         <v>98</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="34" t="s">
         <v>39</v>
       </c>
       <c r="D3" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="45" t="s">
         <v>40</v>
       </c>
       <c r="F3" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="H3" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="I3" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="J3" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="K3" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="L3" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="M3" s="44" t="s">
+      <c r="G3" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="M3" s="34" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="45" t="s">
+      <c r="A4" t="s">
         <v>99</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" t="s">
         <v>97</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="34" t="s">
         <v>39</v>
       </c>
       <c r="D4" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="45" t="s">
         <v>40</v>
       </c>
       <c r="F4" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="I4" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="J4" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="K4" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="L4" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="M4" s="44" t="s">
+      <c r="G4" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" s="34" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="45" t="s">
+      <c r="A5" t="s">
         <v>100</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" t="s">
         <v>97</v>
       </c>
-      <c r="C5" s="44" t="s">
+      <c r="C5" s="34" t="s">
         <v>39</v>
       </c>
       <c r="D5" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="45" t="s">
         <v>40</v>
       </c>
       <c r="F5" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G5" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="I5" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="J5" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="K5" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="L5" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="M5" s="44" t="s">
+      <c r="G5" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="L5" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="M5" s="34" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="45" t="s">
+      <c r="A6" t="s">
         <v>101</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B6" t="s">
         <v>97</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="C6" s="34" t="s">
         <v>39</v>
       </c>
       <c r="D6" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="E6" s="45" t="s">
         <v>40</v>
       </c>
       <c r="F6" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="J6" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="K6" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="L6" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="M6" s="44" t="s">
+      <c r="G6" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="M6" s="34" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="45" t="s">
+      <c r="A7" t="s">
         <v>102</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" t="s">
         <v>97</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="34" t="s">
         <v>39</v>
       </c>
       <c r="D7" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="32" t="s">
+      <c r="E7" s="45" t="s">
         <v>40</v>
       </c>
       <c r="F7" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="H7" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="I7" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="J7" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="K7" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="L7" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="M7" s="44" t="s">
+      <c r="G7" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J7" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="L7" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="M7" s="34" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="45" t="s">
+      <c r="A8" t="s">
         <v>103</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="B8" t="s">
         <v>97</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="34" t="s">
         <v>39</v>
       </c>
       <c r="D8" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="E8" s="45" t="s">
         <v>40</v>
       </c>
       <c r="F8" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="I8" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="J8" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="K8" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="L8" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="M8" s="44" t="s">
+      <c r="G8" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J8" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="K8" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="L8" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="M8" s="34" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="45" t="s">
+      <c r="A9" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" t="s">
         <v>97</v>
       </c>
-      <c r="C9" s="44" t="s">
+      <c r="C9" s="34" t="s">
         <v>39</v>
       </c>
       <c r="D9" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="32" t="s">
+      <c r="E9" s="45" t="s">
         <v>40</v>
       </c>
       <c r="F9" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="H9" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="I9" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="J9" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="K9" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="L9" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="M9" s="44" t="s">
+      <c r="G9" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J9" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K9" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="L9" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="M9" s="34" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="45" t="s">
+      <c r="A10" t="s">
         <v>105</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="B10" t="s">
         <v>97</v>
       </c>
-      <c r="C10" s="44" t="s">
+      <c r="C10" s="34" t="s">
         <v>39</v>
       </c>
       <c r="D10" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="32" t="s">
+      <c r="E10" s="45" t="s">
         <v>40</v>
       </c>
       <c r="F10" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G10" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="H10" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="I10" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="J10" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="K10" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="L10" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="M10" s="44" t="s">
+      <c r="G10" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J10" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K10" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="L10" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="M10" s="34" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="46" t="s">
+      <c r="A11" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="B11" s="45" t="s">
+      <c r="B11" t="s">
         <v>97</v>
       </c>
-      <c r="C11" s="44" t="s">
+      <c r="C11" s="34" t="s">
         <v>39</v>
       </c>
       <c r="D11" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="32" t="s">
+      <c r="E11" s="45" t="s">
         <v>40</v>
       </c>
       <c r="F11" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G11" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="H11" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="I11" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="J11" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="K11" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="L11" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="M11" s="44" t="s">
+      <c r="G11" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K11" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="L11" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M11" s="34" t="s">
         <v>40</v>
       </c>
     </row>
@@ -23896,13 +23897,13 @@
       <c r="D12" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="32" t="s">
+      <c r="E12" s="45" t="s">
         <v>40</v>
       </c>
       <c r="F12" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G12" s="44" t="s">
+      <c r="G12" s="32" t="s">
         <v>40</v>
       </c>
       <c r="H12" s="32" t="s">
@@ -23937,13 +23938,13 @@
       <c r="D13" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="32" t="s">
+      <c r="E13" s="45" t="s">
         <v>40</v>
       </c>
       <c r="F13" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G13" s="44" t="s">
+      <c r="G13" s="32" t="s">
         <v>40</v>
       </c>
       <c r="H13" s="32" t="s">
@@ -23978,13 +23979,13 @@
       <c r="D14" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="32" t="s">
+      <c r="E14" s="45" t="s">
         <v>40</v>
       </c>
       <c r="F14" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G14" s="44" t="s">
+      <c r="G14" s="32" t="s">
         <v>40</v>
       </c>
       <c r="H14" s="32" t="s">
@@ -24019,13 +24020,13 @@
       <c r="D15" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="E15" s="32" t="s">
+      <c r="E15" s="45" t="s">
         <v>40</v>
       </c>
       <c r="F15" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G15" s="44" t="s">
+      <c r="G15" s="32" t="s">
         <v>40</v>
       </c>
       <c r="H15" s="32" t="s">
@@ -24060,13 +24061,13 @@
       <c r="D16" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="32" t="s">
+      <c r="E16" s="45" t="s">
         <v>40</v>
       </c>
       <c r="F16" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G16" s="44" t="s">
+      <c r="G16" s="32" t="s">
         <v>40</v>
       </c>
       <c r="H16" s="32" t="s">
@@ -24101,13 +24102,13 @@
       <c r="D17" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="32" t="s">
+      <c r="E17" s="45" t="s">
         <v>40</v>
       </c>
       <c r="F17" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G17" s="44" t="s">
+      <c r="G17" s="32" t="s">
         <v>40</v>
       </c>
       <c r="H17" s="32" t="s">
@@ -24142,13 +24143,13 @@
       <c r="D18" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="E18" s="32" t="s">
+      <c r="E18" s="45" t="s">
         <v>40</v>
       </c>
       <c r="F18" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G18" s="44" t="s">
+      <c r="G18" s="32" t="s">
         <v>40</v>
       </c>
       <c r="H18" s="32" t="s">
@@ -24183,13 +24184,13 @@
       <c r="D19" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="E19" s="32" t="s">
+      <c r="E19" s="45" t="s">
         <v>40</v>
       </c>
       <c r="F19" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G19" s="44" t="s">
+      <c r="G19" s="32" t="s">
         <v>40</v>
       </c>
       <c r="H19" s="32" t="s">
@@ -24224,13 +24225,13 @@
       <c r="D20" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="E20" s="32" t="s">
+      <c r="E20" s="45" t="s">
         <v>40</v>
       </c>
       <c r="F20" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="44" t="s">
+      <c r="G20" s="32" t="s">
         <v>40</v>
       </c>
       <c r="H20" s="32" t="s">
@@ -24265,13 +24266,13 @@
       <c r="D21" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="E21" s="32" t="s">
+      <c r="E21" s="45" t="s">
         <v>40</v>
       </c>
       <c r="F21" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="44" t="s">
+      <c r="G21" s="32" t="s">
         <v>40</v>
       </c>
       <c r="H21" s="32" t="s">
@@ -24293,208 +24294,208 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="37" t="s">
+    <row r="22" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="46" t="s">
         <v>122</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="47" t="s">
         <v>123</v>
       </c>
-      <c r="C22" s="32" t="s">
+      <c r="C22" s="45" t="s">
         <v>40</v>
       </c>
       <c r="D22" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="E22" s="32" t="s">
+      <c r="E22" s="45" t="s">
         <v>39</v>
       </c>
       <c r="F22" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G22" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="H22" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="I22" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="J22" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="K22" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="L22" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="M22" s="32" t="s">
+      <c r="G22" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="H22" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="I22" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="J22" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="K22" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="L22" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="M22" s="45" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:13" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
+    <row r="23" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="47" t="s">
         <v>124</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="47" t="s">
         <v>123</v>
       </c>
-      <c r="C23" s="32" t="s">
+      <c r="C23" s="45" t="s">
         <v>40</v>
       </c>
       <c r="D23" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="E23" s="32" t="s">
+      <c r="E23" s="45" t="s">
         <v>39</v>
       </c>
       <c r="F23" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G23" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="H23" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="I23" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="J23" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="K23" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="L23" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="M23" s="32" t="s">
+      <c r="G23" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="H23" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="I23" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="J23" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="K23" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="L23" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="M23" s="45" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:13" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="47" t="s">
         <v>125</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="C24" s="32" t="s">
+      <c r="C24" s="45" t="s">
         <v>40</v>
       </c>
       <c r="D24" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="E24" s="32" t="s">
+      <c r="E24" s="45" t="s">
         <v>39</v>
       </c>
       <c r="F24" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G24" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="H24" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="I24" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="J24" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="K24" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="L24" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="M24" s="32" t="s">
+      <c r="G24" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="H24" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="I24" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="J24" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="K24" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="L24" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="M24" s="45" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:13" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
+    <row r="25" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="47" t="s">
         <v>127</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="47" t="s">
         <v>123</v>
       </c>
-      <c r="C25" s="32" t="s">
+      <c r="C25" s="45" t="s">
         <v>40</v>
       </c>
       <c r="D25" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="32" t="s">
+      <c r="E25" s="45" t="s">
         <v>39</v>
       </c>
       <c r="F25" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G25" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="H25" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="I25" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="J25" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="K25" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="L25" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="M25" s="32" t="s">
+      <c r="G25" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="H25" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="I25" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="J25" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="K25" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="L25" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="M25" s="45" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:13" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="38" t="s">
+    <row r="26" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="48" t="s">
         <v>128</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="47" t="s">
         <v>129</v>
       </c>
-      <c r="C26" s="32" t="s">
+      <c r="C26" s="45" t="s">
         <v>40</v>
       </c>
       <c r="D26" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="E26" s="32" t="s">
+      <c r="E26" s="45" t="s">
         <v>39</v>
       </c>
       <c r="F26" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G26" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="H26" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="I26" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="J26" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="K26" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="L26" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="M26" s="32" t="s">
+      <c r="G26" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="H26" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="I26" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="J26" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="K26" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="L26" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="M26" s="45" t="s">
         <v>40</v>
       </c>
     </row>
@@ -24511,13 +24512,13 @@
       <c r="D27" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="32" t="s">
+      <c r="E27" s="45" t="s">
         <v>40</v>
       </c>
       <c r="F27" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="G27" s="44" t="s">
+      <c r="G27" s="32" t="s">
         <v>40</v>
       </c>
       <c r="H27" s="32" t="s">
@@ -24552,13 +24553,13 @@
       <c r="D28" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="E28" s="32" t="s">
+      <c r="E28" s="45" t="s">
         <v>40</v>
       </c>
       <c r="F28" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="G28" s="44" t="s">
+      <c r="G28" s="32" t="s">
         <v>40</v>
       </c>
       <c r="H28" s="32" t="s">
@@ -24593,13 +24594,13 @@
       <c r="D29" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="E29" s="32" t="s">
+      <c r="E29" s="45" t="s">
         <v>40</v>
       </c>
       <c r="F29" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="G29" s="44" t="s">
+      <c r="G29" s="32" t="s">
         <v>40</v>
       </c>
       <c r="H29" s="32" t="s">
@@ -24634,13 +24635,13 @@
       <c r="D30" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="E30" s="32" t="s">
+      <c r="E30" s="45" t="s">
         <v>40</v>
       </c>
       <c r="F30" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="G30" s="44" t="s">
+      <c r="G30" s="32" t="s">
         <v>40</v>
       </c>
       <c r="H30" s="32" t="s">
@@ -24675,13 +24676,13 @@
       <c r="D31" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="E31" s="32" t="s">
+      <c r="E31" s="45" t="s">
         <v>40</v>
       </c>
       <c r="F31" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="G31" s="44" t="s">
+      <c r="G31" s="32" t="s">
         <v>40</v>
       </c>
       <c r="H31" s="32" t="s">
@@ -24710,201 +24711,201 @@
       <c r="B32" t="s">
         <v>140</v>
       </c>
-      <c r="C32" s="44" t="s">
+      <c r="C32" s="34" t="s">
         <v>40</v>
       </c>
       <c r="D32" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="E32" s="32" t="s">
+      <c r="E32" s="45" t="s">
         <v>40</v>
       </c>
       <c r="F32" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G32" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="H32" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="I32" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="J32" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="K32" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="L32" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="M32" s="44" t="s">
+      <c r="G32" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H32" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I32" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J32" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="K32" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="L32" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="M32" s="34" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:13" s="45" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="45" t="s">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>141</v>
       </c>
-      <c r="B33" s="45" t="s">
+      <c r="B33" t="s">
         <v>142</v>
       </c>
-      <c r="C33" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="D33" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="E33" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="F33" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="G33" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="H33" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="I33" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="J33" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="K33" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="L33" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="M33" s="44" t="s">
+      <c r="C33" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E33" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="F33" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="G33" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H33" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I33" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J33" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K33" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="L33" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="M33" s="34" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:13" s="45" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="45" t="s">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>143</v>
       </c>
-      <c r="B34" s="45" t="s">
+      <c r="B34" t="s">
         <v>144</v>
       </c>
-      <c r="C34" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="D34" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="E34" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="F34" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="G34" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="H34" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="I34" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="J34" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="K34" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="L34" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="M34" s="44" t="s">
+      <c r="C34" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E34" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="F34" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="G34" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H34" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I34" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J34" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K34" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="L34" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="M34" s="34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:13" s="45" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="45" t="s">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>145</v>
       </c>
-      <c r="B35" s="45" t="s">
+      <c r="B35" t="s">
         <v>146</v>
       </c>
-      <c r="C35" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="D35" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="E35" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="F35" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="G35" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="H35" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="I35" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="J35" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="K35" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="L35" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="M35" s="44" t="s">
+      <c r="C35" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E35" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="F35" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="G35" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H35" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I35" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J35" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K35" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="L35" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="M35" s="34" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:13" s="45" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="46" t="s">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" s="36" t="s">
         <v>147</v>
       </c>
-      <c r="B36" s="45" t="s">
+      <c r="B36" t="s">
         <v>148</v>
       </c>
-      <c r="C36" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="D36" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="E36" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="F36" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="G36" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="H36" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="I36" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="J36" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="K36" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="L36" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="M36" s="44" t="s">
+      <c r="C36" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E36" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="F36" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="G36" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H36" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I36" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J36" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K36" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="L36" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M36" s="34" t="s">
         <v>40</v>
       </c>
     </row>
@@ -24917,7 +24918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA1C4ECE-D418-419E-9393-664BDA889D6E}">
   <dimension ref="A1:AJ35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -24942,20 +24943,20 @@
     <col min="19" max="19" width="9.88671875" style="3" hidden="1" customWidth="1"/>
     <col min="20" max="20" width="13.88671875" style="3" hidden="1" customWidth="1"/>
     <col min="21" max="21" width="14.109375" style="3" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="12.6640625" style="3" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="7.44140625" style="3" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="12.6640625" style="3" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="16.88671875" style="3" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="12.33203125" style="3" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="12.6640625" style="47" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.44140625" style="47" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.6640625" style="47" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.88671875" style="47" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.33203125" style="47" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="10.21875" style="3" hidden="1" customWidth="1"/>
     <col min="28" max="28" width="8.5546875" style="3" hidden="1" customWidth="1"/>
     <col min="29" max="29" width="6.33203125" style="3" hidden="1" customWidth="1"/>
     <col min="30" max="30" width="11.33203125" style="3" hidden="1" customWidth="1"/>
     <col min="31" max="31" width="9.88671875" style="3" hidden="1" customWidth="1"/>
-    <col min="33" max="33" width="8.6640625" style="45" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="14.6640625" style="45" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.33203125" style="45" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.6640625" style="45" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.3">
@@ -25019,19 +25020,19 @@
       <c r="U1" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="V1" s="32" t="s">
+      <c r="V1" s="45" t="s">
         <v>122</v>
       </c>
-      <c r="W1" s="32" t="s">
+      <c r="W1" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="X1" s="32" t="s">
+      <c r="X1" s="45" t="s">
         <v>125</v>
       </c>
-      <c r="Y1" s="32" t="s">
+      <c r="Y1" s="45" t="s">
         <v>127</v>
       </c>
-      <c r="Z1" s="32" t="s">
+      <c r="Z1" s="45" t="s">
         <v>128</v>
       </c>
       <c r="AA1" s="32" t="s">
@@ -25052,16 +25053,16 @@
       <c r="AF1" s="34" t="s">
         <v>139</v>
       </c>
-      <c r="AG1" s="44" t="s">
+      <c r="AG1" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="AH1" s="44" t="s">
+      <c r="AH1" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="AI1" s="44" t="s">
+      <c r="AI1" s="34" t="s">
         <v>145</v>
       </c>
-      <c r="AJ1" s="44" t="s">
+      <c r="AJ1" s="34" t="s">
         <v>147</v>
       </c>
     </row>
@@ -25129,19 +25130,19 @@
       <c r="U2" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="V2" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="W2" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="X2" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y2" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z2" s="32" t="s">
+      <c r="V2" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="W2" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="X2" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y2" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z2" s="45" t="s">
         <v>40</v>
       </c>
       <c r="AA2" s="32" t="s">
@@ -25162,16 +25163,16 @@
       <c r="AF2" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AG2" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH2" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI2" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ2" s="44" t="s">
+      <c r="AG2" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH2" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI2" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ2" s="34" t="s">
         <v>40</v>
       </c>
     </row>
@@ -25239,19 +25240,19 @@
       <c r="U3" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="V3" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="W3" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="X3" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y3" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z3" s="32" t="s">
+      <c r="V3" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="W3" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="X3" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y3" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z3" s="45" t="s">
         <v>40</v>
       </c>
       <c r="AA3" s="32" t="s">
@@ -25272,16 +25273,16 @@
       <c r="AF3" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AG3" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH3" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI3" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ3" s="44" t="s">
+      <c r="AG3" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH3" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI3" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ3" s="34" t="s">
         <v>40</v>
       </c>
     </row>
@@ -25349,19 +25350,19 @@
       <c r="U4" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="W4" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="X4" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y4" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z4" s="32" t="s">
+      <c r="V4" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="W4" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="X4" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y4" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z4" s="45" t="s">
         <v>39</v>
       </c>
       <c r="AA4" s="32" t="s">
@@ -25382,16 +25383,16 @@
       <c r="AF4" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AG4" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH4" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI4" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ4" s="44" t="s">
+      <c r="AG4" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH4" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI4" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ4" s="34" t="s">
         <v>40</v>
       </c>
     </row>
@@ -25459,19 +25460,19 @@
       <c r="U5" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="V5" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="W5" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="X5" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y5" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z5" s="32" t="s">
+      <c r="V5" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="W5" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="X5" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y5" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z5" s="45" t="s">
         <v>39</v>
       </c>
       <c r="AA5" s="32" t="s">
@@ -25492,16 +25493,16 @@
       <c r="AF5" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AG5" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH5" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI5" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ5" s="44" t="s">
+      <c r="AG5" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH5" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI5" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ5" s="34" t="s">
         <v>39</v>
       </c>
     </row>
@@ -25569,19 +25570,19 @@
       <c r="U6" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="V6" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="W6" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="X6" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y6" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z6" s="32" t="s">
+      <c r="V6" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="W6" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="X6" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y6" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z6" s="45" t="s">
         <v>39</v>
       </c>
       <c r="AA6" s="32" t="s">
@@ -25602,16 +25603,16 @@
       <c r="AF6" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AG6" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH6" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI6" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ6" s="44" t="s">
+      <c r="AG6" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH6" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI6" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ6" s="34" t="s">
         <v>39</v>
       </c>
     </row>
@@ -25679,19 +25680,19 @@
       <c r="U7" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="V7" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="W7" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="X7" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y7" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z7" s="32" t="s">
+      <c r="V7" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="W7" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="X7" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y7" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z7" s="45" t="s">
         <v>40</v>
       </c>
       <c r="AA7" s="32" t="s">
@@ -25712,16 +25713,16 @@
       <c r="AF7" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AG7" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH7" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI7" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ7" s="44" t="s">
+      <c r="AG7" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH7" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI7" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ7" s="34" t="s">
         <v>40</v>
       </c>
     </row>
@@ -25789,19 +25790,19 @@
       <c r="U8" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="V8" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="W8" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="X8" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y8" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z8" s="32" t="s">
+      <c r="V8" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="W8" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="X8" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y8" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z8" s="45" t="s">
         <v>39</v>
       </c>
       <c r="AA8" s="32" t="s">
@@ -25822,16 +25823,16 @@
       <c r="AF8" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AG8" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH8" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI8" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ8" s="44" t="s">
+      <c r="AG8" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH8" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI8" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ8" s="34" t="s">
         <v>40</v>
       </c>
     </row>
@@ -25899,19 +25900,19 @@
       <c r="U9" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="V9" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="W9" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="X9" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y9" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z9" s="32" t="s">
+      <c r="V9" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="W9" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="X9" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y9" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z9" s="45" t="s">
         <v>39</v>
       </c>
       <c r="AA9" s="32" t="s">
@@ -25932,16 +25933,16 @@
       <c r="AF9" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AG9" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH9" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI9" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ9" s="44" t="s">
+      <c r="AG9" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH9" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI9" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ9" s="34" t="s">
         <v>40</v>
       </c>
     </row>
@@ -26009,19 +26010,19 @@
       <c r="U10" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="V10" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="W10" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="X10" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y10" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z10" s="32" t="s">
+      <c r="V10" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="W10" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="X10" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y10" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z10" s="45" t="s">
         <v>39</v>
       </c>
       <c r="AA10" s="32" t="s">
@@ -26042,16 +26043,16 @@
       <c r="AF10" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AG10" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH10" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI10" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ10" s="44" t="s">
+      <c r="AG10" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH10" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI10" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ10" s="34" t="s">
         <v>40</v>
       </c>
     </row>
@@ -26119,19 +26120,19 @@
       <c r="U11" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="V11" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="W11" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="X11" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y11" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z11" s="32" t="s">
+      <c r="V11" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="W11" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="X11" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y11" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z11" s="45" t="s">
         <v>40</v>
       </c>
       <c r="AA11" s="32" t="s">
@@ -26152,16 +26153,16 @@
       <c r="AF11" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AG11" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH11" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI11" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ11" s="44" t="s">
+      <c r="AG11" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH11" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI11" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ11" s="34" t="s">
         <v>40</v>
       </c>
     </row>
@@ -26229,19 +26230,19 @@
       <c r="U12" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="V12" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="W12" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="X12" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y12" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z12" s="32" t="s">
+      <c r="V12" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="W12" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="X12" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y12" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z12" s="45" t="s">
         <v>40</v>
       </c>
       <c r="AA12" s="32" t="s">
@@ -26262,16 +26263,16 @@
       <c r="AF12" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AG12" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH12" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI12" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ12" s="44" t="s">
+      <c r="AG12" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH12" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI12" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ12" s="34" t="s">
         <v>40</v>
       </c>
     </row>
@@ -26339,19 +26340,19 @@
       <c r="U13" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="V13" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="W13" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="X13" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y13" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z13" s="32" t="s">
+      <c r="V13" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="W13" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="X13" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y13" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z13" s="45" t="s">
         <v>39</v>
       </c>
       <c r="AA13" s="32" t="s">
@@ -26372,16 +26373,16 @@
       <c r="AF13" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AG13" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH13" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI13" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ13" s="44" t="s">
+      <c r="AG13" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH13" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI13" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ13" s="34" t="s">
         <v>40</v>
       </c>
     </row>
@@ -26449,19 +26450,19 @@
       <c r="U14" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="V14" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="W14" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="X14" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y14" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z14" s="32" t="s">
+      <c r="V14" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="W14" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="X14" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y14" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z14" s="45" t="s">
         <v>39</v>
       </c>
       <c r="AA14" s="32" t="s">
@@ -26482,16 +26483,16 @@
       <c r="AF14" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AG14" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH14" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI14" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ14" s="44" t="s">
+      <c r="AG14" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH14" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI14" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ14" s="34" t="s">
         <v>40</v>
       </c>
     </row>
@@ -26559,19 +26560,19 @@
       <c r="U15" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="V15" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="W15" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="X15" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y15" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z15" s="32" t="s">
+      <c r="V15" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="W15" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="X15" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y15" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z15" s="45" t="s">
         <v>40</v>
       </c>
       <c r="AA15" s="32" t="s">
@@ -26592,16 +26593,16 @@
       <c r="AF15" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AG15" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH15" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI15" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ15" s="44" t="s">
+      <c r="AG15" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH15" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI15" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ15" s="34" t="s">
         <v>40</v>
       </c>
     </row>
@@ -26669,19 +26670,19 @@
       <c r="U16" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="V16" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="W16" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="X16" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y16" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z16" s="32" t="s">
+      <c r="V16" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="W16" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="X16" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y16" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z16" s="45" t="s">
         <v>40</v>
       </c>
       <c r="AA16" s="32" t="s">
@@ -26702,16 +26703,16 @@
       <c r="AF16" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AG16" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH16" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI16" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ16" s="44" t="s">
+      <c r="AG16" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH16" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI16" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ16" s="34" t="s">
         <v>39</v>
       </c>
     </row>
@@ -26779,19 +26780,19 @@
       <c r="U17" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="V17" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="W17" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="X17" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y17" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z17" s="32" t="s">
+      <c r="V17" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="W17" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="X17" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y17" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z17" s="45" t="s">
         <v>39</v>
       </c>
       <c r="AA17" s="32" t="s">
@@ -26812,16 +26813,16 @@
       <c r="AF17" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AG17" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH17" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI17" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ17" s="44" t="s">
+      <c r="AG17" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH17" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI17" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ17" s="34" t="s">
         <v>39</v>
       </c>
     </row>
@@ -26889,19 +26890,19 @@
       <c r="U18" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="V18" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="W18" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="X18" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y18" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z18" s="32" t="s">
+      <c r="V18" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="W18" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="X18" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y18" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z18" s="45" t="s">
         <v>39</v>
       </c>
       <c r="AA18" s="32" t="s">
@@ -26922,16 +26923,16 @@
       <c r="AF18" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AG18" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH18" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI18" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ18" s="44" t="s">
+      <c r="AG18" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH18" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI18" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ18" s="34" t="s">
         <v>39</v>
       </c>
     </row>
@@ -26999,19 +27000,19 @@
       <c r="U19" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="V19" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="W19" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="X19" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y19" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z19" s="32" t="s">
+      <c r="V19" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="W19" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="X19" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y19" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z19" s="45" t="s">
         <v>40</v>
       </c>
       <c r="AA19" s="32" t="s">
@@ -27032,16 +27033,16 @@
       <c r="AF19" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AG19" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH19" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI19" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ19" s="44" t="s">
+      <c r="AG19" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH19" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI19" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ19" s="34" t="s">
         <v>39</v>
       </c>
     </row>
@@ -27109,19 +27110,19 @@
       <c r="U20" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="V20" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="W20" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="X20" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y20" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z20" s="32" t="s">
+      <c r="V20" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="W20" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="X20" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y20" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z20" s="45" t="s">
         <v>40</v>
       </c>
       <c r="AA20" s="32" t="s">
@@ -27142,16 +27143,16 @@
       <c r="AF20" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AG20" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH20" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI20" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ20" s="44" t="s">
+      <c r="AG20" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH20" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI20" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ20" s="34" t="s">
         <v>39</v>
       </c>
     </row>
@@ -27219,19 +27220,19 @@
       <c r="U21" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="V21" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="W21" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="X21" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y21" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z21" s="32" t="s">
+      <c r="V21" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="W21" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="X21" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y21" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z21" s="45" t="s">
         <v>39</v>
       </c>
       <c r="AA21" s="32" t="s">
@@ -27252,16 +27253,16 @@
       <c r="AF21" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AG21" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH21" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI21" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ21" s="44" t="s">
+      <c r="AG21" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH21" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI21" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ21" s="34" t="s">
         <v>39</v>
       </c>
     </row>
@@ -27329,19 +27330,19 @@
       <c r="U22" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="V22" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="W22" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="X22" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y22" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z22" s="32" t="s">
+      <c r="V22" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="W22" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="X22" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y22" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z22" s="45" t="s">
         <v>39</v>
       </c>
       <c r="AA22" s="32" t="s">
@@ -27362,16 +27363,16 @@
       <c r="AF22" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AG22" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH22" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI22" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ22" s="44" t="s">
+      <c r="AG22" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH22" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI22" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ22" s="34" t="s">
         <v>39</v>
       </c>
     </row>
@@ -27436,19 +27437,19 @@
       <c r="U25" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="V25" s="32" t="s">
+      <c r="V25" s="45" t="s">
         <v>122</v>
       </c>
-      <c r="W25" s="32" t="s">
+      <c r="W25" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="X25" s="32" t="s">
+      <c r="X25" s="45" t="s">
         <v>125</v>
       </c>
-      <c r="Y25" s="32" t="s">
+      <c r="Y25" s="45" t="s">
         <v>127</v>
       </c>
-      <c r="Z25" s="32" t="s">
+      <c r="Z25" s="45" t="s">
         <v>128</v>
       </c>
       <c r="AA25" s="32" t="s">
@@ -27469,16 +27470,16 @@
       <c r="AF25" s="34" t="s">
         <v>139</v>
       </c>
-      <c r="AG25" s="44" t="s">
+      <c r="AG25" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="AH25" s="44" t="s">
+      <c r="AH25" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="AI25" s="44" t="s">
+      <c r="AI25" s="34" t="s">
         <v>145</v>
       </c>
-      <c r="AJ25" s="44" t="s">
+      <c r="AJ25" s="34" t="s">
         <v>147</v>
       </c>
     </row>
@@ -27546,19 +27547,19 @@
       <c r="U26" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="V26" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="W26" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="X26" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y26" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z26" s="32" t="s">
+      <c r="V26" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="W26" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="X26" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y26" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z26" s="45" t="s">
         <v>39</v>
       </c>
       <c r="AA26" s="32" t="s">
@@ -27579,16 +27580,16 @@
       <c r="AF26" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AG26" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH26" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI26" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ26" s="44" t="s">
+      <c r="AG26" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH26" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI26" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ26" s="34" t="s">
         <v>39</v>
       </c>
     </row>
@@ -27656,19 +27657,19 @@
       <c r="U27" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="V27" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="W27" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="X27" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y27" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z27" s="32" t="s">
+      <c r="V27" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="W27" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="X27" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y27" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z27" s="45" t="s">
         <v>39</v>
       </c>
       <c r="AA27" s="32" t="s">
@@ -27689,16 +27690,16 @@
       <c r="AF27" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AG27" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH27" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI27" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ27" s="44" t="s">
+      <c r="AG27" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH27" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI27" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ27" s="34" t="s">
         <v>39</v>
       </c>
     </row>
@@ -27766,19 +27767,19 @@
       <c r="U28" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="V28" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="W28" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="X28" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y28" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z28" s="32" t="s">
+      <c r="V28" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="W28" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="X28" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y28" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z28" s="45" t="s">
         <v>39</v>
       </c>
       <c r="AA28" s="32" t="s">
@@ -27799,16 +27800,16 @@
       <c r="AF28" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AG28" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH28" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI28" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ28" s="44" t="s">
+      <c r="AG28" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH28" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI28" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ28" s="34" t="s">
         <v>39</v>
       </c>
     </row>
@@ -27876,19 +27877,19 @@
       <c r="U29" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="V29" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="W29" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="X29" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y29" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z29" s="32" t="s">
+      <c r="V29" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="W29" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="X29" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y29" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z29" s="45" t="s">
         <v>39</v>
       </c>
       <c r="AA29" s="32" t="s">
@@ -27909,16 +27910,16 @@
       <c r="AF29" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AG29" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH29" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI29" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ29" s="44" t="s">
+      <c r="AG29" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH29" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI29" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ29" s="34" t="s">
         <v>39</v>
       </c>
     </row>
@@ -27986,19 +27987,19 @@
       <c r="U30" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="V30" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="W30" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="X30" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y30" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z30" s="32" t="s">
+      <c r="V30" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="W30" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="X30" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y30" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z30" s="45" t="s">
         <v>39</v>
       </c>
       <c r="AA30" s="32" t="s">
@@ -28019,16 +28020,16 @@
       <c r="AF30" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AG30" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH30" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI30" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ30" s="44" t="s">
+      <c r="AG30" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH30" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI30" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ30" s="34" t="s">
         <v>40</v>
       </c>
     </row>
@@ -28096,19 +28097,19 @@
       <c r="U31" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="V31" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="W31" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="X31" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y31" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z31" s="32" t="s">
+      <c r="V31" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="W31" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="X31" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y31" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z31" s="45" t="s">
         <v>40</v>
       </c>
       <c r="AA31" s="32" t="s">
@@ -28129,16 +28130,16 @@
       <c r="AF31" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AG31" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH31" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI31" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ31" s="44" t="s">
+      <c r="AG31" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH31" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI31" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ31" s="34" t="s">
         <v>40</v>
       </c>
     </row>
@@ -28206,19 +28207,19 @@
       <c r="U32" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="V32" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="W32" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="X32" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y32" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z32" s="32" t="s">
+      <c r="V32" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="W32" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="X32" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y32" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z32" s="45" t="s">
         <v>39</v>
       </c>
       <c r="AA32" s="32" t="s">
@@ -28239,16 +28240,16 @@
       <c r="AF32" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AG32" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH32" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI32" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ32" s="44" t="s">
+      <c r="AG32" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH32" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI32" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ32" s="34" t="s">
         <v>40</v>
       </c>
     </row>
@@ -28316,19 +28317,19 @@
       <c r="U33" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="V33" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="W33" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="X33" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y33" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z33" s="32" t="s">
+      <c r="V33" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="W33" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="X33" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y33" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z33" s="45" t="s">
         <v>39</v>
       </c>
       <c r="AA33" s="32" t="s">
@@ -28349,16 +28350,16 @@
       <c r="AF33" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AG33" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH33" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI33" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ33" s="44" t="s">
+      <c r="AG33" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH33" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI33" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ33" s="34" t="s">
         <v>39</v>
       </c>
     </row>
@@ -28426,19 +28427,19 @@
       <c r="U34" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="V34" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="W34" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="X34" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y34" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z34" s="32" t="s">
+      <c r="V34" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="W34" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="X34" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y34" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z34" s="45" t="s">
         <v>39</v>
       </c>
       <c r="AA34" s="32" t="s">
@@ -28459,16 +28460,16 @@
       <c r="AF34" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AG34" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH34" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI34" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ34" s="44" t="s">
+      <c r="AG34" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH34" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI34" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ34" s="34" t="s">
         <v>39</v>
       </c>
     </row>
@@ -28536,19 +28537,19 @@
       <c r="U35" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="V35" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="W35" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="X35" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y35" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z35" s="32" t="s">
+      <c r="V35" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="W35" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="X35" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y35" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z35" s="45" t="s">
         <v>39</v>
       </c>
       <c r="AA35" s="32" t="s">
@@ -28569,16 +28570,16 @@
       <c r="AF35" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AG35" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH35" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI35" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ35" s="44" t="s">
+      <c r="AG35" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH35" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI35" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ35" s="34" t="s">
         <v>39</v>
       </c>
     </row>
@@ -28724,54 +28725,54 @@
       <c r="U1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="W1" s="43" t="s">
+      <c r="W1" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="X1" s="43"/>
-      <c r="Y1" s="43"/>
-      <c r="Z1" s="43"/>
-      <c r="AA1" s="43"/>
-      <c r="AB1" s="43"/>
-      <c r="AD1" s="43" t="s">
+      <c r="X1" s="44"/>
+      <c r="Y1" s="44"/>
+      <c r="Z1" s="44"/>
+      <c r="AA1" s="44"/>
+      <c r="AB1" s="44"/>
+      <c r="AD1" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="AE1" s="43"/>
-      <c r="AF1" s="43"/>
-      <c r="AG1" s="43"/>
-      <c r="AH1" s="43"/>
-      <c r="AI1" s="43"/>
-      <c r="AK1" s="43" t="s">
+      <c r="AE1" s="44"/>
+      <c r="AF1" s="44"/>
+      <c r="AG1" s="44"/>
+      <c r="AH1" s="44"/>
+      <c r="AI1" s="44"/>
+      <c r="AK1" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="AL1" s="43"/>
-      <c r="AM1" s="43"/>
-      <c r="AN1" s="43"/>
-      <c r="AO1" s="43"/>
-      <c r="AP1" s="43"/>
-      <c r="AR1" s="43" t="s">
+      <c r="AL1" s="44"/>
+      <c r="AM1" s="44"/>
+      <c r="AN1" s="44"/>
+      <c r="AO1" s="44"/>
+      <c r="AP1" s="44"/>
+      <c r="AR1" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="AS1" s="43"/>
-      <c r="AT1" s="43"/>
-      <c r="AU1" s="43"/>
-      <c r="AV1" s="43"/>
-      <c r="AW1" s="43"/>
-      <c r="AY1" s="43" t="s">
+      <c r="AS1" s="44"/>
+      <c r="AT1" s="44"/>
+      <c r="AU1" s="44"/>
+      <c r="AV1" s="44"/>
+      <c r="AW1" s="44"/>
+      <c r="AY1" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="AZ1" s="43"/>
-      <c r="BA1" s="43"/>
-      <c r="BB1" s="43"/>
-      <c r="BC1" s="43"/>
-      <c r="BD1" s="43"/>
-      <c r="BF1" s="43" t="s">
+      <c r="AZ1" s="44"/>
+      <c r="BA1" s="44"/>
+      <c r="BB1" s="44"/>
+      <c r="BC1" s="44"/>
+      <c r="BD1" s="44"/>
+      <c r="BF1" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="BG1" s="43"/>
-      <c r="BH1" s="43"/>
-      <c r="BI1" s="43"/>
-      <c r="BJ1" s="43"/>
-      <c r="BK1" s="43"/>
+      <c r="BG1" s="44"/>
+      <c r="BH1" s="44"/>
+      <c r="BI1" s="44"/>
+      <c r="BJ1" s="44"/>
+      <c r="BK1" s="44"/>
     </row>
     <row r="2" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">

</xml_diff>

<commit_message>
Introduce HEALING magic type. Introduce new types of healing spells: - WOUND_HEALING - HEALING_WORD - CURE - REGENERATION - BREATH_OF_GOD - POWER_OF_NATURE - SOUL_POWER - RECHARGING - HEALING_WAVE - ENERGY_ABSORPTION Healing can be used after combat if the character is seriously injured. HEALING_WAVE has area effect and heals companions as well. The effect of blessings ends after looting enemies and casting healing spells if any so dying because of it is less possible.
Bugfix: if there is no usable soul chip for blessing then spell cost is not paid now from magic.
</commit_message>
<xml_diff>
--- a/doc/caste_system.xlsx
+++ b/doc/caste_system.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/349dfb9748b30a92/Asztali gép/ataliasflame_2.0/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8607" documentId="8_{652F4476-B36F-42CD-831D-0D71B9923ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0DE6EF51-7CC7-4043-8EDB-EFB9CA2B76C2}"/>
+  <xr:revisionPtr revIDLastSave="8656" documentId="8_{652F4476-B36F-42CD-831D-0D71B9923ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B78D9428-5FCC-4794-9B97-39767000E2DB}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="635" activeTab="7" xr2:uid="{CAF51EC3-63EC-48CD-AA7B-C21B3D5D222B}"/>
   </bookViews>
@@ -22601,16 +22601,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8F833C9-BBEE-43B5-917D-731D1CF064F0}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="60.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" style="34" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="32" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" style="45" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" style="32" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="45" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" style="34" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="32" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.6640625" style="34" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.5546875" style="34" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.33203125" style="34" bestFit="1" customWidth="1"/>
@@ -23443,10 +23445,10 @@
       <c r="C1" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="34" t="s">
         <v>87</v>
       </c>
       <c r="F1" s="32" t="s">
@@ -23484,10 +23486,10 @@
       <c r="C2" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" s="45" t="s">
+      <c r="D2" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="34" t="s">
         <v>40</v>
       </c>
       <c r="F2" s="32" t="s">
@@ -23525,10 +23527,10 @@
       <c r="C3" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="45" t="s">
+      <c r="D3" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="34" t="s">
         <v>40</v>
       </c>
       <c r="F3" s="32" t="s">
@@ -23566,10 +23568,10 @@
       <c r="C4" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" s="45" t="s">
+      <c r="D4" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="34" t="s">
         <v>40</v>
       </c>
       <c r="F4" s="32" t="s">
@@ -23607,10 +23609,10 @@
       <c r="C5" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="45" t="s">
+      <c r="D5" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="34" t="s">
         <v>40</v>
       </c>
       <c r="F5" s="32" t="s">
@@ -23648,10 +23650,10 @@
       <c r="C6" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="45" t="s">
+      <c r="D6" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="34" t="s">
         <v>40</v>
       </c>
       <c r="F6" s="32" t="s">
@@ -23689,10 +23691,10 @@
       <c r="C7" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="45" t="s">
+      <c r="D7" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="34" t="s">
         <v>40</v>
       </c>
       <c r="F7" s="32" t="s">
@@ -23730,10 +23732,10 @@
       <c r="C8" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="45" t="s">
+      <c r="D8" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="34" t="s">
         <v>40</v>
       </c>
       <c r="F8" s="32" t="s">
@@ -23771,10 +23773,10 @@
       <c r="C9" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="45" t="s">
+      <c r="D9" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="34" t="s">
         <v>40</v>
       </c>
       <c r="F9" s="32" t="s">
@@ -23812,10 +23814,10 @@
       <c r="C10" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" s="45" t="s">
+      <c r="D10" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="34" t="s">
         <v>40</v>
       </c>
       <c r="F10" s="32" t="s">
@@ -23853,10 +23855,10 @@
       <c r="C11" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="45" t="s">
+      <c r="D11" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="34" t="s">
         <v>40</v>
       </c>
       <c r="F11" s="32" t="s">
@@ -23884,17 +23886,17 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="37" t="s">
+    <row r="12" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="C12" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" s="32" t="s">
+      <c r="C12" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="45" t="s">
         <v>39</v>
       </c>
       <c r="E12" s="45" t="s">
@@ -23903,39 +23905,39 @@
       <c r="F12" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G12" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="H12" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="I12" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="J12" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="K12" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="L12" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="M12" s="32" t="s">
+      <c r="G12" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="J12" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="K12" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="L12" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="M12" s="45" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="47" t="s">
         <v>110</v>
       </c>
-      <c r="C13" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="32" t="s">
+      <c r="C13" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="45" t="s">
         <v>39</v>
       </c>
       <c r="E13" s="45" t="s">
@@ -23944,39 +23946,39 @@
       <c r="F13" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G13" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="H13" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="I13" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="J13" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="K13" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="L13" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="M13" s="32" t="s">
+      <c r="G13" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="J13" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="K13" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="L13" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="M13" s="45" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="47" t="s">
         <v>110</v>
       </c>
-      <c r="C14" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="32" t="s">
+      <c r="C14" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="45" t="s">
         <v>39</v>
       </c>
       <c r="E14" s="45" t="s">
@@ -23985,39 +23987,39 @@
       <c r="F14" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G14" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="H14" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="I14" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="J14" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="K14" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="L14" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="M14" s="32" t="s">
+      <c r="G14" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="J14" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="K14" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="L14" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="M14" s="45" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="47" t="s">
         <v>113</v>
       </c>
-      <c r="C15" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="32" t="s">
+      <c r="C15" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="45" t="s">
         <v>39</v>
       </c>
       <c r="E15" s="45" t="s">
@@ -24026,39 +24028,39 @@
       <c r="F15" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G15" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="H15" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="I15" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="J15" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="K15" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="L15" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="M15" s="32" t="s">
+      <c r="G15" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="I15" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="J15" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="K15" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="L15" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="M15" s="45" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="47" t="s">
         <v>114</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="47" t="s">
         <v>110</v>
       </c>
-      <c r="C16" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="32" t="s">
+      <c r="C16" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="45" t="s">
         <v>39</v>
       </c>
       <c r="E16" s="45" t="s">
@@ -24067,39 +24069,39 @@
       <c r="F16" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G16" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="H16" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="I16" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="J16" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="K16" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="L16" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="M16" s="32" t="s">
+      <c r="G16" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="H16" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="I16" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="J16" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="K16" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="L16" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="M16" s="45" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="47" t="s">
         <v>115</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="47" t="s">
         <v>110</v>
       </c>
-      <c r="C17" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="32" t="s">
+      <c r="C17" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="45" t="s">
         <v>39</v>
       </c>
       <c r="E17" s="45" t="s">
@@ -24108,39 +24110,39 @@
       <c r="F17" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G17" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="H17" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="I17" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="J17" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="K17" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="L17" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="M17" s="32" t="s">
+      <c r="G17" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="H17" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="I17" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="J17" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="K17" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="L17" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="M17" s="45" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:13" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="47" t="s">
         <v>116</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="47" t="s">
         <v>110</v>
       </c>
-      <c r="C18" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="32" t="s">
+      <c r="C18" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="45" t="s">
         <v>39</v>
       </c>
       <c r="E18" s="45" t="s">
@@ -24149,39 +24151,39 @@
       <c r="F18" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G18" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="H18" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="I18" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="J18" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="K18" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="L18" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="M18" s="32" t="s">
+      <c r="G18" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="H18" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="I18" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="J18" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="K18" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="L18" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="M18" s="45" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="47" t="s">
         <v>117</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="47" t="s">
         <v>110</v>
       </c>
-      <c r="C19" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="32" t="s">
+      <c r="C19" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="45" t="s">
         <v>39</v>
       </c>
       <c r="E19" s="45" t="s">
@@ -24190,39 +24192,39 @@
       <c r="F19" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G19" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="H19" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="I19" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="J19" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="K19" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="L19" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="M19" s="32" t="s">
+      <c r="G19" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="H19" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="I19" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="J19" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="K19" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="L19" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="M19" s="45" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="47" t="s">
         <v>118</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="47" t="s">
         <v>119</v>
       </c>
-      <c r="C20" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" s="32" t="s">
+      <c r="C20" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="45" t="s">
         <v>39</v>
       </c>
       <c r="E20" s="45" t="s">
@@ -24231,39 +24233,39 @@
       <c r="F20" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="H20" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="I20" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="J20" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="K20" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="L20" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="M20" s="32" t="s">
+      <c r="G20" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="H20" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="I20" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="J20" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="K20" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="L20" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="M20" s="45" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="38" t="s">
+    <row r="21" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="48" t="s">
         <v>120</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="C21" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="32" t="s">
+      <c r="C21" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="45" t="s">
         <v>39</v>
       </c>
       <c r="E21" s="45" t="s">
@@ -24272,234 +24274,234 @@
       <c r="F21" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="H21" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="I21" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="J21" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="K21" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="L21" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="M21" s="32" t="s">
+      <c r="G21" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="H21" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="I21" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="J21" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="K21" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="L21" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="M21" s="45" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="46" t="s">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="B22" s="47" t="s">
+      <c r="B22" t="s">
         <v>123</v>
       </c>
-      <c r="C22" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="E22" s="45" t="s">
+      <c r="C22" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" s="34" t="s">
         <v>39</v>
       </c>
       <c r="F22" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G22" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="H22" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="I22" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="J22" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="K22" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="L22" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="M22" s="45" t="s">
+      <c r="G22" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H22" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I22" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J22" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K22" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="L22" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M22" s="34" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="47" t="s">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>124</v>
       </c>
-      <c r="B23" s="47" t="s">
+      <c r="B23" t="s">
         <v>123</v>
       </c>
-      <c r="C23" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" s="45" t="s">
+      <c r="C23" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="34" t="s">
         <v>39</v>
       </c>
       <c r="F23" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G23" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="H23" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="I23" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="J23" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="K23" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="L23" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="M23" s="45" t="s">
+      <c r="G23" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H23" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I23" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J23" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K23" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="L23" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="M23" s="34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="47" t="s">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>125</v>
       </c>
-      <c r="B24" s="47" t="s">
+      <c r="B24" t="s">
         <v>126</v>
       </c>
-      <c r="C24" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="D24" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" s="45" t="s">
+      <c r="C24" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="34" t="s">
         <v>39</v>
       </c>
       <c r="F24" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G24" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="H24" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="I24" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="J24" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="K24" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="L24" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="M24" s="45" t="s">
+      <c r="G24" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H24" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I24" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J24" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="K24" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="L24" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="M24" s="34" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="47" t="s">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>127</v>
       </c>
-      <c r="B25" s="47" t="s">
+      <c r="B25" t="s">
         <v>123</v>
       </c>
-      <c r="C25" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="D25" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="E25" s="45" t="s">
+      <c r="C25" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25" s="34" t="s">
         <v>39</v>
       </c>
       <c r="F25" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G25" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="H25" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="I25" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="J25" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="K25" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="L25" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="M25" s="45" t="s">
+      <c r="G25" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H25" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I25" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J25" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K25" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="L25" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="M25" s="34" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="48" t="s">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="36" t="s">
         <v>128</v>
       </c>
-      <c r="B26" s="47" t="s">
+      <c r="B26" t="s">
         <v>129</v>
       </c>
-      <c r="C26" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="D26" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="E26" s="45" t="s">
+      <c r="C26" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" s="34" t="s">
         <v>39</v>
       </c>
       <c r="F26" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G26" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="H26" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="I26" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="J26" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="K26" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="L26" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="M26" s="45" t="s">
+      <c r="G26" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H26" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I26" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J26" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K26" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="L26" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="M26" s="34" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:13" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="37" t="s">
         <v>130</v>
       </c>
@@ -24512,7 +24514,7 @@
       <c r="D27" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="45" t="s">
+      <c r="E27" s="32" t="s">
         <v>40</v>
       </c>
       <c r="F27" s="32" t="s">
@@ -24540,7 +24542,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>132</v>
       </c>
@@ -24553,7 +24555,7 @@
       <c r="D28" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="E28" s="45" t="s">
+      <c r="E28" s="32" t="s">
         <v>40</v>
       </c>
       <c r="F28" s="32" t="s">
@@ -24581,7 +24583,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:13" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>134</v>
       </c>
@@ -24594,7 +24596,7 @@
       <c r="D29" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="E29" s="45" t="s">
+      <c r="E29" s="32" t="s">
         <v>40</v>
       </c>
       <c r="F29" s="32" t="s">
@@ -24622,7 +24624,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:13" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>136</v>
       </c>
@@ -24635,7 +24637,7 @@
       <c r="D30" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="E30" s="45" t="s">
+      <c r="E30" s="32" t="s">
         <v>40</v>
       </c>
       <c r="F30" s="32" t="s">
@@ -24663,7 +24665,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:13" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="38" t="s">
         <v>137</v>
       </c>
@@ -24676,7 +24678,7 @@
       <c r="D31" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="E31" s="45" t="s">
+      <c r="E31" s="32" t="s">
         <v>40</v>
       </c>
       <c r="F31" s="32" t="s">
@@ -24714,10 +24716,10 @@
       <c r="C32" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="D32" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="E32" s="45" t="s">
+      <c r="D32" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="E32" s="34" t="s">
         <v>40</v>
       </c>
       <c r="F32" s="32" t="s">
@@ -24755,10 +24757,10 @@
       <c r="C33" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="E33" s="45" t="s">
+      <c r="D33" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="E33" s="34" t="s">
         <v>40</v>
       </c>
       <c r="F33" s="32" t="s">
@@ -24796,10 +24798,10 @@
       <c r="C34" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="D34" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="E34" s="45" t="s">
+      <c r="D34" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="E34" s="34" t="s">
         <v>40</v>
       </c>
       <c r="F34" s="32" t="s">
@@ -24837,10 +24839,10 @@
       <c r="C35" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="D35" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="E35" s="45" t="s">
+      <c r="D35" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="E35" s="34" t="s">
         <v>40</v>
       </c>
       <c r="F35" s="32" t="s">
@@ -24878,10 +24880,10 @@
       <c r="C36" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="D36" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="E36" s="45" t="s">
+      <c r="D36" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="E36" s="34" t="s">
         <v>40</v>
       </c>
       <c r="F36" s="32" t="s">
@@ -24918,7 +24920,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA1C4ECE-D418-419E-9393-664BDA889D6E}">
   <dimension ref="A1:AJ35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V15" sqref="V15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -24933,26 +24937,26 @@
     <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.88671875" style="3" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5546875" style="3" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="4.5546875" style="3" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="10.6640625" style="3" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="11.88671875" style="3" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="12.77734375" style="3" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="7.5546875" style="3" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="9.88671875" style="3" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="13.88671875" style="3" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="14.109375" style="3" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="12.6640625" style="47" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.44140625" style="47" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.6640625" style="47" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.88671875" style="47" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.33203125" style="47" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.21875" style="3" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="8.5546875" style="3" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="6.33203125" style="3" hidden="1" customWidth="1"/>
-    <col min="30" max="30" width="11.33203125" style="3" hidden="1" customWidth="1"/>
-    <col min="31" max="31" width="9.88671875" style="3" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="11.88671875" style="47" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5546875" style="47" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.5546875" style="47" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" style="47" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.88671875" style="47" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.77734375" style="47" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.5546875" style="47" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.88671875" style="47" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.88671875" style="47" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="6.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.88671875" style="3" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="14.33203125" bestFit="1" customWidth="1"/>
@@ -24990,49 +24994,49 @@
       <c r="K1" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="L1" s="32" t="s">
+      <c r="L1" s="45" t="s">
         <v>107</v>
       </c>
-      <c r="M1" s="32" t="s">
+      <c r="M1" s="45" t="s">
         <v>109</v>
       </c>
-      <c r="N1" s="32" t="s">
+      <c r="N1" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="O1" s="32" t="s">
+      <c r="O1" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="P1" s="32" t="s">
+      <c r="P1" s="45" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="32" t="s">
+      <c r="Q1" s="45" t="s">
         <v>115</v>
       </c>
-      <c r="R1" s="32" t="s">
+      <c r="R1" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="S1" s="32" t="s">
+      <c r="S1" s="45" t="s">
         <v>117</v>
       </c>
-      <c r="T1" s="32" t="s">
+      <c r="T1" s="45" t="s">
         <v>118</v>
       </c>
-      <c r="U1" s="32" t="s">
+      <c r="U1" s="45" t="s">
         <v>120</v>
       </c>
-      <c r="V1" s="45" t="s">
+      <c r="V1" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="W1" s="45" t="s">
+      <c r="W1" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="X1" s="45" t="s">
+      <c r="X1" s="34" t="s">
         <v>125</v>
       </c>
-      <c r="Y1" s="45" t="s">
+      <c r="Y1" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="Z1" s="45" t="s">
+      <c r="Z1" s="34" t="s">
         <v>128</v>
       </c>
       <c r="AA1" s="32" t="s">
@@ -25100,49 +25104,49 @@
       <c r="K2" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L2" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="M2" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="N2" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="O2" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="P2" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q2" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="R2" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="S2" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="T2" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="U2" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="V2" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="W2" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="X2" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y2" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z2" s="45" t="s">
+      <c r="L2" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="P2" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q2" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="R2" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="S2" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="T2" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="U2" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="V2" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="W2" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="X2" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y2" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z2" s="34" t="s">
         <v>40</v>
       </c>
       <c r="AA2" s="32" t="s">
@@ -25210,49 +25214,49 @@
       <c r="K3" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="M3" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="N3" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="O3" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="P3" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q3" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="R3" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="S3" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="T3" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="U3" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="V3" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="W3" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="X3" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y3" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z3" s="45" t="s">
+      <c r="L3" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="P3" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q3" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="R3" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="S3" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="T3" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="U3" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="V3" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="W3" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="X3" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y3" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z3" s="34" t="s">
         <v>40</v>
       </c>
       <c r="AA3" s="32" t="s">
@@ -25320,49 +25324,49 @@
       <c r="K4" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="M4" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="N4" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="O4" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="P4" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q4" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="R4" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="S4" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="T4" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="U4" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="V4" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="W4" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="X4" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y4" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z4" s="45" t="s">
+      <c r="L4" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="M4" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="O4" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="P4" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q4" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="R4" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="S4" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="T4" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="U4" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="V4" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="W4" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="X4" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y4" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z4" s="34" t="s">
         <v>39</v>
       </c>
       <c r="AA4" s="32" t="s">
@@ -25430,49 +25434,49 @@
       <c r="K5" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L5" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="M5" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="N5" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="O5" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="P5" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q5" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="R5" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="S5" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="T5" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="U5" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="V5" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="W5" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="X5" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y5" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z5" s="45" t="s">
+      <c r="L5" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="M5" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="N5" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="O5" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="P5" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q5" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="R5" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="S5" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="T5" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="U5" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="V5" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="W5" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="X5" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y5" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z5" s="34" t="s">
         <v>39</v>
       </c>
       <c r="AA5" s="32" t="s">
@@ -25540,49 +25544,49 @@
       <c r="K6" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L6" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="M6" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="N6" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="O6" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="P6" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q6" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="R6" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="S6" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="T6" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="U6" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="V6" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="W6" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="X6" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y6" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z6" s="45" t="s">
+      <c r="L6" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="M6" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="N6" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="O6" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="P6" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q6" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="R6" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="S6" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="T6" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="U6" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="V6" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="W6" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="X6" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y6" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z6" s="34" t="s">
         <v>39</v>
       </c>
       <c r="AA6" s="32" t="s">
@@ -25650,49 +25654,49 @@
       <c r="K7" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L7" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="M7" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="N7" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="O7" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="P7" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q7" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="R7" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="S7" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="T7" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="U7" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="V7" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="W7" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="X7" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y7" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z7" s="45" t="s">
+      <c r="L7" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="M7" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="N7" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="O7" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="P7" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q7" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="R7" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="S7" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="T7" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="U7" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="V7" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="W7" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="X7" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y7" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z7" s="34" t="s">
         <v>40</v>
       </c>
       <c r="AA7" s="32" t="s">
@@ -25760,49 +25764,49 @@
       <c r="K8" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L8" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="M8" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="N8" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="O8" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="P8" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q8" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="R8" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="S8" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="T8" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="U8" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="V8" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="W8" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="X8" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y8" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z8" s="45" t="s">
+      <c r="L8" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="M8" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="N8" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="O8" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="P8" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q8" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="R8" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="S8" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="T8" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="U8" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="V8" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="W8" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="X8" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y8" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z8" s="34" t="s">
         <v>39</v>
       </c>
       <c r="AA8" s="32" t="s">
@@ -25870,49 +25874,49 @@
       <c r="K9" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L9" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="M9" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="N9" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="O9" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="P9" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q9" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="R9" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="S9" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="T9" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="U9" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="V9" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="W9" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="X9" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y9" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z9" s="45" t="s">
+      <c r="L9" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="M9" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="N9" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="O9" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="P9" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q9" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="R9" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="S9" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="T9" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="U9" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="V9" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="W9" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="X9" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y9" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z9" s="34" t="s">
         <v>39</v>
       </c>
       <c r="AA9" s="32" t="s">
@@ -25980,49 +25984,49 @@
       <c r="K10" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L10" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="M10" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="N10" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="O10" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="P10" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q10" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="R10" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="S10" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="T10" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="U10" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="V10" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="W10" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="X10" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y10" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z10" s="45" t="s">
+      <c r="L10" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="M10" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="N10" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="O10" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="P10" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q10" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="R10" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="S10" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="T10" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="U10" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="V10" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="W10" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="X10" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y10" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z10" s="34" t="s">
         <v>39</v>
       </c>
       <c r="AA10" s="32" t="s">
@@ -26090,49 +26094,49 @@
       <c r="K11" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L11" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="M11" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="N11" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="O11" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="P11" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q11" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="R11" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="S11" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="T11" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="U11" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="V11" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="W11" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="X11" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y11" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z11" s="45" t="s">
+      <c r="L11" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="M11" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="N11" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="O11" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="P11" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q11" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="R11" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="S11" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="T11" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="U11" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="V11" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="W11" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="X11" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y11" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z11" s="34" t="s">
         <v>40</v>
       </c>
       <c r="AA11" s="32" t="s">
@@ -26200,49 +26204,49 @@
       <c r="K12" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L12" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="M12" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="N12" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="O12" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="P12" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q12" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="R12" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="S12" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="T12" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="U12" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="V12" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="W12" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="X12" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y12" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z12" s="45" t="s">
+      <c r="L12" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="M12" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="N12" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="O12" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="P12" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q12" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="R12" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="S12" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="T12" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="U12" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="V12" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="W12" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="X12" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y12" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z12" s="34" t="s">
         <v>40</v>
       </c>
       <c r="AA12" s="32" t="s">
@@ -26310,49 +26314,49 @@
       <c r="K13" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L13" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="M13" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="N13" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="O13" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="P13" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q13" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="R13" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="S13" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="T13" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="U13" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="V13" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="W13" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="X13" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y13" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z13" s="45" t="s">
+      <c r="L13" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="M13" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="N13" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="O13" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="P13" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q13" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="R13" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="S13" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="T13" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="U13" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="V13" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="W13" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="X13" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y13" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z13" s="34" t="s">
         <v>39</v>
       </c>
       <c r="AA13" s="32" t="s">
@@ -26420,49 +26424,49 @@
       <c r="K14" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L14" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="M14" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="N14" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="O14" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="P14" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q14" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="R14" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="S14" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="T14" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="U14" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="V14" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="W14" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="X14" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y14" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z14" s="45" t="s">
+      <c r="L14" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="M14" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="N14" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="O14" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="P14" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q14" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="R14" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="S14" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="T14" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="U14" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="V14" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="W14" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="X14" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y14" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z14" s="34" t="s">
         <v>39</v>
       </c>
       <c r="AA14" s="32" t="s">
@@ -26530,49 +26534,49 @@
       <c r="K15" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L15" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="M15" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="N15" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="O15" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="P15" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q15" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="R15" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="S15" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="T15" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="U15" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="V15" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="W15" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="X15" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y15" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z15" s="45" t="s">
+      <c r="L15" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="M15" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="N15" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="O15" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="P15" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q15" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="R15" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="S15" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="T15" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="U15" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="V15" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="W15" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="X15" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y15" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z15" s="34" t="s">
         <v>40</v>
       </c>
       <c r="AA15" s="32" t="s">
@@ -26640,49 +26644,49 @@
       <c r="K16" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L16" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="M16" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="N16" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="O16" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="P16" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q16" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="R16" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="S16" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="T16" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="U16" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="V16" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="W16" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="X16" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y16" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z16" s="45" t="s">
+      <c r="L16" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="M16" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="N16" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="O16" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="P16" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q16" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="R16" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="S16" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="T16" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="U16" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="V16" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="W16" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="X16" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y16" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z16" s="34" t="s">
         <v>40</v>
       </c>
       <c r="AA16" s="32" t="s">
@@ -26750,49 +26754,49 @@
       <c r="K17" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L17" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="M17" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="N17" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="O17" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="P17" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q17" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="R17" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="S17" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="T17" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="U17" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="V17" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="W17" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="X17" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y17" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z17" s="45" t="s">
+      <c r="L17" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="M17" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="N17" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="O17" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="P17" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q17" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="R17" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="S17" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="T17" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="U17" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="V17" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="W17" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="X17" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y17" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z17" s="34" t="s">
         <v>39</v>
       </c>
       <c r="AA17" s="32" t="s">
@@ -26860,49 +26864,49 @@
       <c r="K18" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="L18" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="M18" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="N18" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="O18" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="P18" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q18" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="R18" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="S18" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="T18" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="U18" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="V18" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="W18" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="X18" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y18" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z18" s="45" t="s">
+      <c r="L18" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="M18" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="N18" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="O18" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="P18" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q18" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="R18" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="S18" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="T18" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="U18" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="V18" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="W18" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="X18" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y18" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z18" s="34" t="s">
         <v>39</v>
       </c>
       <c r="AA18" s="32" t="s">
@@ -26970,49 +26974,49 @@
       <c r="K19" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="L19" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="M19" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="N19" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="O19" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="P19" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q19" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="R19" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="S19" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="T19" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="U19" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="V19" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="W19" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="X19" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y19" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z19" s="45" t="s">
+      <c r="L19" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="M19" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="N19" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="O19" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="P19" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q19" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="R19" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="S19" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="T19" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="U19" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="V19" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="W19" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="X19" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y19" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z19" s="34" t="s">
         <v>40</v>
       </c>
       <c r="AA19" s="32" t="s">
@@ -27080,49 +27084,49 @@
       <c r="K20" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="L20" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="M20" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="N20" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="O20" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="P20" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q20" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="R20" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="S20" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="T20" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="U20" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="V20" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="W20" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="X20" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y20" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z20" s="45" t="s">
+      <c r="L20" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="M20" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="N20" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="O20" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="P20" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q20" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="R20" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="S20" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="T20" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="U20" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="V20" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="W20" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="X20" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y20" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z20" s="34" t="s">
         <v>40</v>
       </c>
       <c r="AA20" s="32" t="s">
@@ -27190,49 +27194,49 @@
       <c r="K21" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="L21" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="M21" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="N21" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="O21" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="P21" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q21" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="R21" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="S21" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="T21" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="U21" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="V21" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="W21" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="X21" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y21" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z21" s="45" t="s">
+      <c r="L21" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="M21" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="N21" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="O21" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="P21" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q21" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="R21" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="S21" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="T21" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="U21" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="V21" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="W21" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="X21" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y21" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z21" s="34" t="s">
         <v>39</v>
       </c>
       <c r="AA21" s="32" t="s">
@@ -27300,49 +27304,49 @@
       <c r="K22" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="L22" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="M22" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="N22" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="O22" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="P22" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q22" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="R22" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="S22" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="T22" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="U22" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="V22" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="W22" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="X22" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y22" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z22" s="45" t="s">
+      <c r="L22" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="M22" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="N22" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="O22" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="P22" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q22" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="R22" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="S22" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="T22" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="U22" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="V22" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="W22" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="X22" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y22" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z22" s="34" t="s">
         <v>39</v>
       </c>
       <c r="AA22" s="32" t="s">
@@ -27407,49 +27411,49 @@
       <c r="K25" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="L25" s="32" t="s">
+      <c r="L25" s="45" t="s">
         <v>107</v>
       </c>
-      <c r="M25" s="32" t="s">
+      <c r="M25" s="45" t="s">
         <v>109</v>
       </c>
-      <c r="N25" s="32" t="s">
+      <c r="N25" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="O25" s="32" t="s">
+      <c r="O25" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="P25" s="32" t="s">
+      <c r="P25" s="45" t="s">
         <v>114</v>
       </c>
-      <c r="Q25" s="32" t="s">
+      <c r="Q25" s="45" t="s">
         <v>115</v>
       </c>
-      <c r="R25" s="32" t="s">
+      <c r="R25" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="S25" s="32" t="s">
+      <c r="S25" s="45" t="s">
         <v>117</v>
       </c>
-      <c r="T25" s="32" t="s">
+      <c r="T25" s="45" t="s">
         <v>118</v>
       </c>
-      <c r="U25" s="32" t="s">
+      <c r="U25" s="45" t="s">
         <v>120</v>
       </c>
-      <c r="V25" s="45" t="s">
+      <c r="V25" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="W25" s="45" t="s">
+      <c r="W25" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="X25" s="45" t="s">
+      <c r="X25" s="34" t="s">
         <v>125</v>
       </c>
-      <c r="Y25" s="45" t="s">
+      <c r="Y25" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="Z25" s="45" t="s">
+      <c r="Z25" s="34" t="s">
         <v>128</v>
       </c>
       <c r="AA25" s="32" t="s">
@@ -27517,49 +27521,49 @@
       <c r="K26" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="L26" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="M26" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="N26" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="O26" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="P26" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q26" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="R26" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="S26" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="T26" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="U26" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="V26" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="W26" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="X26" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y26" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z26" s="45" t="s">
+      <c r="L26" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="M26" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="N26" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="O26" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="P26" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q26" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="R26" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="S26" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="T26" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="U26" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="V26" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="W26" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="X26" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y26" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z26" s="34" t="s">
         <v>39</v>
       </c>
       <c r="AA26" s="32" t="s">
@@ -27627,49 +27631,49 @@
       <c r="K27" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="L27" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="M27" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="N27" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="O27" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="P27" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q27" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="R27" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="S27" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="T27" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="U27" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="V27" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="W27" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="X27" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y27" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z27" s="45" t="s">
+      <c r="L27" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="M27" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="N27" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="O27" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="P27" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q27" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="R27" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="S27" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="T27" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="U27" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="V27" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="W27" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="X27" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y27" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z27" s="34" t="s">
         <v>39</v>
       </c>
       <c r="AA27" s="32" t="s">
@@ -27737,49 +27741,49 @@
       <c r="K28" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="L28" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="M28" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="N28" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="O28" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="P28" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q28" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="R28" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="S28" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="T28" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="U28" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="V28" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="W28" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="X28" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y28" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z28" s="45" t="s">
+      <c r="L28" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="M28" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="N28" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="O28" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="P28" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q28" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="R28" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="S28" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="T28" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="U28" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="V28" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="W28" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="X28" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y28" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z28" s="34" t="s">
         <v>39</v>
       </c>
       <c r="AA28" s="32" t="s">
@@ -27847,49 +27851,49 @@
       <c r="K29" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="L29" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="M29" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="N29" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="O29" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="P29" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q29" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="R29" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="S29" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="T29" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="U29" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="V29" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="W29" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="X29" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y29" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z29" s="45" t="s">
+      <c r="L29" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="M29" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="N29" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="O29" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="P29" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q29" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="R29" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="S29" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="T29" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="U29" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="V29" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="W29" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="X29" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y29" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z29" s="34" t="s">
         <v>39</v>
       </c>
       <c r="AA29" s="32" t="s">
@@ -27957,49 +27961,49 @@
       <c r="K30" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="L30" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="M30" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="N30" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="O30" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="P30" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q30" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="R30" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="S30" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="T30" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="U30" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="V30" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="W30" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="X30" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y30" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z30" s="45" t="s">
+      <c r="L30" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="M30" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="N30" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="O30" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="P30" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q30" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="R30" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="S30" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="T30" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="U30" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="V30" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="W30" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="X30" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y30" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z30" s="34" t="s">
         <v>39</v>
       </c>
       <c r="AA30" s="32" t="s">
@@ -28067,49 +28071,49 @@
       <c r="K31" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L31" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="M31" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="N31" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="O31" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="P31" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q31" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="R31" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="S31" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="T31" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="U31" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="V31" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="W31" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="X31" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y31" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z31" s="45" t="s">
+      <c r="L31" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="M31" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="N31" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="O31" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="P31" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q31" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="R31" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="S31" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="T31" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="U31" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="V31" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="W31" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="X31" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y31" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z31" s="34" t="s">
         <v>40</v>
       </c>
       <c r="AA31" s="32" t="s">
@@ -28177,49 +28181,49 @@
       <c r="K32" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L32" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="M32" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="N32" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="O32" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="P32" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q32" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="R32" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="S32" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="T32" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="U32" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="V32" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="W32" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="X32" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y32" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z32" s="45" t="s">
+      <c r="L32" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="M32" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="N32" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="O32" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="P32" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q32" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="R32" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="S32" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="T32" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="U32" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="V32" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="W32" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="X32" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y32" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z32" s="34" t="s">
         <v>39</v>
       </c>
       <c r="AA32" s="32" t="s">
@@ -28287,49 +28291,49 @@
       <c r="K33" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="L33" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="M33" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="N33" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="O33" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="P33" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q33" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="R33" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="S33" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="T33" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="U33" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="V33" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="W33" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="X33" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y33" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z33" s="45" t="s">
+      <c r="L33" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="M33" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="N33" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="O33" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="P33" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q33" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="R33" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="S33" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="T33" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="U33" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="V33" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="W33" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="X33" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y33" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z33" s="34" t="s">
         <v>39</v>
       </c>
       <c r="AA33" s="32" t="s">
@@ -28397,49 +28401,49 @@
       <c r="K34" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="L34" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="M34" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="N34" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="O34" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="P34" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q34" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="R34" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="S34" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="T34" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="U34" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="V34" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="W34" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="X34" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y34" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z34" s="45" t="s">
+      <c r="L34" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="M34" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="N34" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="O34" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="P34" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q34" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="R34" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="S34" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="T34" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="U34" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="V34" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="W34" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="X34" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y34" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z34" s="34" t="s">
         <v>39</v>
       </c>
       <c r="AA34" s="32" t="s">
@@ -28507,49 +28511,49 @@
       <c r="K35" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L35" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="M35" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="N35" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="O35" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="P35" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q35" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="R35" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="S35" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="T35" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="U35" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="V35" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="W35" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="X35" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y35" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z35" s="45" t="s">
+      <c r="L35" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="M35" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="N35" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="O35" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="P35" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q35" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="R35" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="S35" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="T35" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="U35" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="V35" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="W35" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="X35" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y35" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z35" s="34" t="s">
         <v>39</v>
       </c>
       <c r="AA35" s="32" t="s">

</xml_diff>

<commit_message>
Generating defensive god conversion code now returns a detailed structure instead of a simple code string. Improve granularity of application service layer. Looting is now on locations in the first case instead of monsters (but still affects only the monsters on location). Combat is now only seizing the location. Magic casting and looting are independent decisions made in endurance tests now. (In the common base class in fact).
</commit_message>
<xml_diff>
--- a/doc/caste_system.xlsx
+++ b/doc/caste_system.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/349dfb9748b30a92/Asztali gép/ataliasflame_2.0/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8656" documentId="8_{652F4476-B36F-42CD-831D-0D71B9923ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B78D9428-5FCC-4794-9B97-39767000E2DB}"/>
+  <xr:revisionPtr revIDLastSave="8662" documentId="8_{652F4476-B36F-42CD-831D-0D71B9923ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{425D7C08-8F54-4FC4-B935-1C9BA55C6EF8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="635" activeTab="7" xr2:uid="{CAF51EC3-63EC-48CD-AA7B-C21B3D5D222B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="635" activeTab="5" xr2:uid="{CAF51EC3-63EC-48CD-AA7B-C21B3D5D222B}"/>
   </bookViews>
   <sheets>
     <sheet name="caste list" sheetId="1" r:id="rId1"/>
@@ -2244,7 +2244,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2320,12 +2320,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -2342,10 +2336,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -21580,8 +21570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E471D10E-602D-4E12-A93B-97B72309BCF6}">
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22610,7 +22600,7 @@
     <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="60.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" style="34" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="45" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="34" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.33203125" style="34" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="32" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.6640625" style="34" bestFit="1" customWidth="1"/>
@@ -23445,7 +23435,7 @@
       <c r="C1" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="34" t="s">
         <v>86</v>
       </c>
       <c r="E1" s="34" t="s">
@@ -23486,7 +23476,7 @@
       <c r="C2" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="34" t="s">
         <v>40</v>
       </c>
       <c r="E2" s="34" t="s">
@@ -23527,7 +23517,7 @@
       <c r="C3" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="34" t="s">
         <v>40</v>
       </c>
       <c r="E3" s="34" t="s">
@@ -23568,7 +23558,7 @@
       <c r="C4" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="D4" s="34" t="s">
         <v>40</v>
       </c>
       <c r="E4" s="34" t="s">
@@ -23609,7 +23599,7 @@
       <c r="C5" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="45" t="s">
+      <c r="D5" s="34" t="s">
         <v>40</v>
       </c>
       <c r="E5" s="34" t="s">
@@ -23650,7 +23640,7 @@
       <c r="C6" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="D6" s="34" t="s">
         <v>40</v>
       </c>
       <c r="E6" s="34" t="s">
@@ -23691,7 +23681,7 @@
       <c r="C7" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="45" t="s">
+      <c r="D7" s="34" t="s">
         <v>40</v>
       </c>
       <c r="E7" s="34" t="s">
@@ -23732,7 +23722,7 @@
       <c r="C8" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="45" t="s">
+      <c r="D8" s="34" t="s">
         <v>40</v>
       </c>
       <c r="E8" s="34" t="s">
@@ -23773,7 +23763,7 @@
       <c r="C9" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="45" t="s">
+      <c r="D9" s="34" t="s">
         <v>40</v>
       </c>
       <c r="E9" s="34" t="s">
@@ -23814,7 +23804,7 @@
       <c r="C10" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="45" t="s">
+      <c r="D10" s="34" t="s">
         <v>40</v>
       </c>
       <c r="E10" s="34" t="s">
@@ -23855,7 +23845,7 @@
       <c r="C11" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="45" t="s">
+      <c r="D11" s="34" t="s">
         <v>40</v>
       </c>
       <c r="E11" s="34" t="s">
@@ -23886,413 +23876,413 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="46" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="B12" s="47" t="s">
+      <c r="B12" t="s">
         <v>108</v>
       </c>
-      <c r="C12" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="45" t="s">
+      <c r="C12" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="34" t="s">
         <v>40</v>
       </c>
       <c r="F12" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G12" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="H12" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="I12" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="J12" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="K12" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="L12" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="M12" s="45" t="s">
+      <c r="G12" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J12" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K12" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="L12" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="M12" s="34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="47" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>109</v>
       </c>
-      <c r="B13" s="47" t="s">
+      <c r="B13" t="s">
         <v>110</v>
       </c>
-      <c r="C13" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="45" t="s">
+      <c r="C13" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="34" t="s">
         <v>40</v>
       </c>
       <c r="F13" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G13" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="H13" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="I13" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="J13" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="K13" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="L13" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="M13" s="45" t="s">
+      <c r="G13" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J13" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K13" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="L13" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M13" s="34" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="47" t="s">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>111</v>
       </c>
-      <c r="B14" s="47" t="s">
+      <c r="B14" t="s">
         <v>110</v>
       </c>
-      <c r="C14" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="45" t="s">
+      <c r="C14" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="34" t="s">
         <v>40</v>
       </c>
       <c r="F14" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G14" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="H14" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="I14" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="J14" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="K14" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="L14" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="M14" s="45" t="s">
+      <c r="G14" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J14" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K14" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="L14" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="M14" s="34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="47" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>112</v>
       </c>
-      <c r="B15" s="47" t="s">
+      <c r="B15" t="s">
         <v>113</v>
       </c>
-      <c r="C15" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="45" t="s">
+      <c r="C15" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="34" t="s">
         <v>40</v>
       </c>
       <c r="F15" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G15" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="H15" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="I15" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="J15" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="K15" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="L15" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="M15" s="45" t="s">
+      <c r="G15" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I15" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J15" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K15" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="L15" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="M15" s="34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="47" t="s">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>114</v>
       </c>
-      <c r="B16" s="47" t="s">
+      <c r="B16" t="s">
         <v>110</v>
       </c>
-      <c r="C16" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" s="45" t="s">
+      <c r="C16" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="34" t="s">
         <v>40</v>
       </c>
       <c r="F16" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G16" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="H16" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="I16" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="J16" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="K16" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="L16" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="M16" s="45" t="s">
+      <c r="G16" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H16" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I16" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J16" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K16" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="L16" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M16" s="34" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="47" t="s">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>115</v>
       </c>
-      <c r="B17" s="47" t="s">
+      <c r="B17" t="s">
         <v>110</v>
       </c>
-      <c r="C17" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="45" t="s">
+      <c r="C17" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="34" t="s">
         <v>40</v>
       </c>
       <c r="F17" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G17" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="H17" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="I17" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="J17" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="K17" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="L17" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="M17" s="45" t="s">
+      <c r="G17" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H17" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I17" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J17" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K17" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="L17" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="M17" s="34" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="47" t="s">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>116</v>
       </c>
-      <c r="B18" s="47" t="s">
+      <c r="B18" t="s">
         <v>110</v>
       </c>
-      <c r="C18" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" s="45" t="s">
+      <c r="C18" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="34" t="s">
         <v>40</v>
       </c>
       <c r="F18" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G18" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="H18" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="I18" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="J18" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="K18" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="L18" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="M18" s="45" t="s">
+      <c r="G18" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H18" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I18" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J18" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="K18" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="L18" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="M18" s="34" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="47" t="s">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>117</v>
       </c>
-      <c r="B19" s="47" t="s">
+      <c r="B19" t="s">
         <v>110</v>
       </c>
-      <c r="C19" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="E19" s="45" t="s">
+      <c r="C19" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="34" t="s">
         <v>40</v>
       </c>
       <c r="F19" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G19" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="H19" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="I19" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="J19" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="K19" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="L19" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="M19" s="45" t="s">
+      <c r="G19" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H19" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I19" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J19" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K19" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="L19" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="M19" s="34" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="47" t="s">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>118</v>
       </c>
-      <c r="B20" s="47" t="s">
+      <c r="B20" t="s">
         <v>119</v>
       </c>
-      <c r="C20" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" s="45" t="s">
+      <c r="C20" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="34" t="s">
         <v>40</v>
       </c>
       <c r="F20" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="H20" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="I20" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="J20" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="K20" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="L20" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="M20" s="45" t="s">
+      <c r="G20" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H20" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I20" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J20" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K20" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="L20" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="M20" s="34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="48" t="s">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="B21" s="47" t="s">
+      <c r="B21" t="s">
         <v>121</v>
       </c>
-      <c r="C21" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="E21" s="45" t="s">
+      <c r="C21" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" s="34" t="s">
         <v>40</v>
       </c>
       <c r="F21" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="H21" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="I21" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="J21" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="K21" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="L21" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="M21" s="45" t="s">
+      <c r="G21" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H21" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I21" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J21" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K21" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="L21" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="M21" s="34" t="s">
         <v>40</v>
       </c>
     </row>
@@ -24306,7 +24296,7 @@
       <c r="C22" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="45" t="s">
+      <c r="D22" s="34" t="s">
         <v>40</v>
       </c>
       <c r="E22" s="34" t="s">
@@ -24347,7 +24337,7 @@
       <c r="C23" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="45" t="s">
+      <c r="D23" s="34" t="s">
         <v>40</v>
       </c>
       <c r="E23" s="34" t="s">
@@ -24388,7 +24378,7 @@
       <c r="C24" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="45" t="s">
+      <c r="D24" s="34" t="s">
         <v>40</v>
       </c>
       <c r="E24" s="34" t="s">
@@ -24429,7 +24419,7 @@
       <c r="C25" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="D25" s="45" t="s">
+      <c r="D25" s="34" t="s">
         <v>40</v>
       </c>
       <c r="E25" s="34" t="s">
@@ -24470,7 +24460,7 @@
       <c r="C26" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="D26" s="45" t="s">
+      <c r="D26" s="34" t="s">
         <v>40</v>
       </c>
       <c r="E26" s="34" t="s">
@@ -24716,7 +24706,7 @@
       <c r="C32" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="D32" s="45" t="s">
+      <c r="D32" s="34" t="s">
         <v>40</v>
       </c>
       <c r="E32" s="34" t="s">
@@ -24757,7 +24747,7 @@
       <c r="C33" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="45" t="s">
+      <c r="D33" s="34" t="s">
         <v>40</v>
       </c>
       <c r="E33" s="34" t="s">
@@ -24798,7 +24788,7 @@
       <c r="C34" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="D34" s="45" t="s">
+      <c r="D34" s="34" t="s">
         <v>40</v>
       </c>
       <c r="E34" s="34" t="s">
@@ -24839,7 +24829,7 @@
       <c r="C35" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="D35" s="45" t="s">
+      <c r="D35" s="34" t="s">
         <v>40</v>
       </c>
       <c r="E35" s="34" t="s">
@@ -24880,7 +24870,7 @@
       <c r="C36" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="D36" s="45" t="s">
+      <c r="D36" s="34" t="s">
         <v>40</v>
       </c>
       <c r="E36" s="34" t="s">
@@ -24920,7 +24910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA1C4ECE-D418-419E-9393-664BDA889D6E}">
   <dimension ref="A1:AJ35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="V15" sqref="V15"/>
     </sheetView>
   </sheetViews>
@@ -24937,16 +24927,16 @@
     <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.88671875" style="47" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5546875" style="47" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.5546875" style="47" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.6640625" style="47" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.88671875" style="47" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.77734375" style="47" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.5546875" style="47" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.88671875" style="47" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.88671875" style="47" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="12.6640625" bestFit="1" customWidth="1"/>
@@ -24994,34 +24984,34 @@
       <c r="K1" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="M1" s="45" t="s">
+      <c r="M1" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="N1" s="45" t="s">
+      <c r="N1" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="O1" s="45" t="s">
+      <c r="O1" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="P1" s="45" t="s">
+      <c r="P1" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="45" t="s">
+      <c r="Q1" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="R1" s="45" t="s">
+      <c r="R1" s="34" t="s">
         <v>116</v>
       </c>
-      <c r="S1" s="45" t="s">
+      <c r="S1" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="T1" s="45" t="s">
+      <c r="T1" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="U1" s="45" t="s">
+      <c r="U1" s="34" t="s">
         <v>120</v>
       </c>
       <c r="V1" s="34" t="s">
@@ -25104,34 +25094,34 @@
       <c r="K2" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L2" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="M2" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="N2" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="O2" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="P2" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q2" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="R2" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="S2" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="T2" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="U2" s="45" t="s">
+      <c r="L2" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="P2" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q2" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="R2" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="S2" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="T2" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="U2" s="34" t="s">
         <v>40</v>
       </c>
       <c r="V2" s="34" t="s">
@@ -25214,34 +25204,34 @@
       <c r="K3" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="M3" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="N3" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="O3" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="P3" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q3" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="R3" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="S3" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="T3" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="U3" s="45" t="s">
+      <c r="L3" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="P3" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q3" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="R3" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="S3" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="T3" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="U3" s="34" t="s">
         <v>40</v>
       </c>
       <c r="V3" s="34" t="s">
@@ -25324,34 +25314,34 @@
       <c r="K4" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="M4" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="N4" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="O4" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="P4" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q4" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="R4" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="S4" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="T4" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="U4" s="45" t="s">
+      <c r="L4" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M4" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="O4" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="P4" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q4" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="R4" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="S4" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="T4" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="U4" s="34" t="s">
         <v>39</v>
       </c>
       <c r="V4" s="34" t="s">
@@ -25434,34 +25424,34 @@
       <c r="K5" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L5" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="M5" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="N5" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="O5" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="P5" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q5" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="R5" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="S5" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="T5" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="U5" s="45" t="s">
+      <c r="L5" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M5" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="N5" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="O5" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="P5" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q5" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="R5" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="S5" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="T5" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="U5" s="34" t="s">
         <v>39</v>
       </c>
       <c r="V5" s="34" t="s">
@@ -25544,34 +25534,34 @@
       <c r="K6" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L6" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="M6" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="N6" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="O6" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="P6" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q6" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="R6" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="S6" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="T6" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="U6" s="45" t="s">
+      <c r="L6" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M6" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="N6" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="O6" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="P6" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q6" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="R6" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="S6" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="T6" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="U6" s="34" t="s">
         <v>39</v>
       </c>
       <c r="V6" s="34" t="s">
@@ -25654,34 +25644,34 @@
       <c r="K7" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L7" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="M7" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="N7" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="O7" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="P7" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q7" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="R7" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="S7" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="T7" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="U7" s="45" t="s">
+      <c r="L7" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M7" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="N7" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="O7" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="P7" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q7" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="R7" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="S7" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="T7" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="U7" s="34" t="s">
         <v>40</v>
       </c>
       <c r="V7" s="34" t="s">
@@ -25764,34 +25754,34 @@
       <c r="K8" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L8" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="M8" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="N8" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="O8" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="P8" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q8" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="R8" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="S8" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="T8" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="U8" s="45" t="s">
+      <c r="L8" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M8" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="N8" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="O8" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="P8" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q8" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="R8" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="S8" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="T8" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="U8" s="34" t="s">
         <v>39</v>
       </c>
       <c r="V8" s="34" t="s">
@@ -25874,34 +25864,34 @@
       <c r="K9" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L9" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="M9" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="N9" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="O9" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="P9" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q9" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="R9" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="S9" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="T9" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="U9" s="45" t="s">
+      <c r="L9" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M9" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="N9" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="O9" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="P9" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q9" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="R9" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="S9" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="T9" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="U9" s="34" t="s">
         <v>39</v>
       </c>
       <c r="V9" s="34" t="s">
@@ -25984,34 +25974,34 @@
       <c r="K10" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L10" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="M10" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="N10" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="O10" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="P10" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q10" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="R10" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="S10" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="T10" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="U10" s="45" t="s">
+      <c r="L10" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M10" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="N10" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="O10" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="P10" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q10" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="R10" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="S10" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="T10" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="U10" s="34" t="s">
         <v>39</v>
       </c>
       <c r="V10" s="34" t="s">
@@ -26094,34 +26084,34 @@
       <c r="K11" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L11" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="M11" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="N11" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="O11" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="P11" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q11" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="R11" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="S11" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="T11" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="U11" s="45" t="s">
+      <c r="L11" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M11" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="N11" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="O11" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="P11" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q11" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="R11" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="S11" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="T11" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="U11" s="34" t="s">
         <v>40</v>
       </c>
       <c r="V11" s="34" t="s">
@@ -26204,34 +26194,34 @@
       <c r="K12" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L12" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="M12" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="N12" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="O12" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="P12" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q12" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="R12" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="S12" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="T12" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="U12" s="45" t="s">
+      <c r="L12" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M12" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="N12" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="O12" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="P12" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q12" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="R12" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="S12" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="T12" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="U12" s="34" t="s">
         <v>40</v>
       </c>
       <c r="V12" s="34" t="s">
@@ -26314,34 +26304,34 @@
       <c r="K13" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L13" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="M13" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="N13" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="O13" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="P13" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q13" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="R13" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="S13" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="T13" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="U13" s="45" t="s">
+      <c r="L13" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M13" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="N13" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="O13" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="P13" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q13" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="R13" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="S13" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="T13" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="U13" s="34" t="s">
         <v>39</v>
       </c>
       <c r="V13" s="34" t="s">
@@ -26424,34 +26414,34 @@
       <c r="K14" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L14" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="M14" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="N14" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="O14" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="P14" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q14" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="R14" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="S14" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="T14" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="U14" s="45" t="s">
+      <c r="L14" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M14" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="N14" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="O14" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="P14" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q14" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="R14" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="S14" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="T14" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="U14" s="34" t="s">
         <v>39</v>
       </c>
       <c r="V14" s="34" t="s">
@@ -26534,34 +26524,34 @@
       <c r="K15" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L15" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="M15" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="N15" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="O15" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="P15" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q15" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="R15" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="S15" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="T15" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="U15" s="45" t="s">
+      <c r="L15" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M15" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="N15" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="O15" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="P15" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q15" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="R15" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="S15" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="T15" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="U15" s="34" t="s">
         <v>40</v>
       </c>
       <c r="V15" s="34" t="s">
@@ -26644,34 +26634,34 @@
       <c r="K16" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L16" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="M16" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="N16" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="O16" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="P16" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q16" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="R16" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="S16" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="T16" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="U16" s="45" t="s">
+      <c r="L16" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M16" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="N16" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="O16" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="P16" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q16" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="R16" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="S16" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="T16" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="U16" s="34" t="s">
         <v>39</v>
       </c>
       <c r="V16" s="34" t="s">
@@ -26754,34 +26744,34 @@
       <c r="K17" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L17" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="M17" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="N17" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="O17" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="P17" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q17" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="R17" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="S17" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="T17" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="U17" s="45" t="s">
+      <c r="L17" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M17" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="N17" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="O17" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="P17" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q17" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="R17" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="S17" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="T17" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="U17" s="34" t="s">
         <v>39</v>
       </c>
       <c r="V17" s="34" t="s">
@@ -26864,34 +26854,34 @@
       <c r="K18" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="L18" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="M18" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="N18" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="O18" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="P18" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q18" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="R18" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="S18" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="T18" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="U18" s="45" t="s">
+      <c r="L18" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M18" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="N18" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="O18" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="P18" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q18" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="R18" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="S18" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="T18" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="U18" s="34" t="s">
         <v>39</v>
       </c>
       <c r="V18" s="34" t="s">
@@ -26974,34 +26964,34 @@
       <c r="K19" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="L19" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="M19" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="N19" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="O19" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="P19" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q19" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="R19" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="S19" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="T19" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="U19" s="45" t="s">
+      <c r="L19" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M19" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="N19" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="O19" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="P19" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q19" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="R19" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="S19" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="T19" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="U19" s="34" t="s">
         <v>40</v>
       </c>
       <c r="V19" s="34" t="s">
@@ -27084,34 +27074,34 @@
       <c r="K20" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="L20" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="M20" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="N20" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="O20" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="P20" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q20" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="R20" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="S20" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="T20" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="U20" s="45" t="s">
+      <c r="L20" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M20" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="N20" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="O20" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="P20" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q20" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="R20" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="S20" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="T20" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="U20" s="34" t="s">
         <v>40</v>
       </c>
       <c r="V20" s="34" t="s">
@@ -27194,34 +27184,34 @@
       <c r="K21" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="L21" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="M21" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="N21" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="O21" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="P21" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q21" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="R21" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="S21" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="T21" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="U21" s="45" t="s">
+      <c r="L21" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M21" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="N21" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="O21" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="P21" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q21" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="R21" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="S21" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="T21" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="U21" s="34" t="s">
         <v>39</v>
       </c>
       <c r="V21" s="34" t="s">
@@ -27304,34 +27294,34 @@
       <c r="K22" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="L22" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="M22" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="N22" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="O22" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="P22" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q22" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="R22" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="S22" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="T22" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="U22" s="45" t="s">
+      <c r="L22" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M22" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="N22" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="O22" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="P22" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q22" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="R22" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="S22" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="T22" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="U22" s="34" t="s">
         <v>39</v>
       </c>
       <c r="V22" s="34" t="s">
@@ -27411,34 +27401,34 @@
       <c r="K25" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="L25" s="45" t="s">
+      <c r="L25" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="M25" s="45" t="s">
+      <c r="M25" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="N25" s="45" t="s">
+      <c r="N25" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="O25" s="45" t="s">
+      <c r="O25" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="P25" s="45" t="s">
+      <c r="P25" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="Q25" s="45" t="s">
+      <c r="Q25" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="R25" s="45" t="s">
+      <c r="R25" s="34" t="s">
         <v>116</v>
       </c>
-      <c r="S25" s="45" t="s">
+      <c r="S25" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="T25" s="45" t="s">
+      <c r="T25" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="U25" s="45" t="s">
+      <c r="U25" s="34" t="s">
         <v>120</v>
       </c>
       <c r="V25" s="34" t="s">
@@ -27521,34 +27511,34 @@
       <c r="K26" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="L26" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="M26" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="N26" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="O26" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="P26" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q26" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="R26" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="S26" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="T26" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="U26" s="45" t="s">
+      <c r="L26" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M26" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="N26" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="O26" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="P26" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q26" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="R26" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="S26" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="T26" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="U26" s="34" t="s">
         <v>39</v>
       </c>
       <c r="V26" s="34" t="s">
@@ -27631,34 +27621,34 @@
       <c r="K27" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="L27" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="M27" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="N27" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="O27" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="P27" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q27" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="R27" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="S27" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="T27" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="U27" s="45" t="s">
+      <c r="L27" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M27" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="N27" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="O27" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="P27" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q27" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="R27" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="S27" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="T27" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="U27" s="34" t="s">
         <v>39</v>
       </c>
       <c r="V27" s="34" t="s">
@@ -27741,34 +27731,34 @@
       <c r="K28" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="L28" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="M28" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="N28" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="O28" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="P28" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q28" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="R28" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="S28" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="T28" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="U28" s="45" t="s">
+      <c r="L28" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M28" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="N28" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="O28" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="P28" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q28" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="R28" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="S28" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="T28" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="U28" s="34" t="s">
         <v>39</v>
       </c>
       <c r="V28" s="34" t="s">
@@ -27851,34 +27841,34 @@
       <c r="K29" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="L29" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="M29" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="N29" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="O29" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="P29" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q29" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="R29" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="S29" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="T29" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="U29" s="45" t="s">
+      <c r="L29" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M29" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="N29" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="O29" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="P29" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q29" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="R29" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="S29" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="T29" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="U29" s="34" t="s">
         <v>39</v>
       </c>
       <c r="V29" s="34" t="s">
@@ -27961,34 +27951,34 @@
       <c r="K30" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="L30" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="M30" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="N30" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="O30" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="P30" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q30" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="R30" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="S30" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="T30" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="U30" s="45" t="s">
+      <c r="L30" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M30" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="N30" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="O30" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="P30" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q30" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="R30" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="S30" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="T30" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="U30" s="34" t="s">
         <v>40</v>
       </c>
       <c r="V30" s="34" t="s">
@@ -28071,34 +28061,34 @@
       <c r="K31" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L31" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="M31" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="N31" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="O31" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="P31" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q31" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="R31" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="S31" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="T31" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="U31" s="45" t="s">
+      <c r="L31" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M31" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="N31" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="O31" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="P31" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q31" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="R31" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="S31" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="T31" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="U31" s="34" t="s">
         <v>40</v>
       </c>
       <c r="V31" s="34" t="s">
@@ -28181,34 +28171,34 @@
       <c r="K32" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L32" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="M32" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="N32" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="O32" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="P32" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q32" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="R32" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="S32" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="T32" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="U32" s="45" t="s">
+      <c r="L32" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M32" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="N32" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="O32" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="P32" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q32" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="R32" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="S32" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="T32" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="U32" s="34" t="s">
         <v>40</v>
       </c>
       <c r="V32" s="34" t="s">
@@ -28291,34 +28281,34 @@
       <c r="K33" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="L33" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="M33" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="N33" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="O33" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="P33" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q33" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="R33" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="S33" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="T33" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="U33" s="45" t="s">
+      <c r="L33" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M33" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="N33" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="O33" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="P33" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q33" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="R33" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="S33" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="T33" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="U33" s="34" t="s">
         <v>39</v>
       </c>
       <c r="V33" s="34" t="s">
@@ -28401,34 +28391,34 @@
       <c r="K34" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="L34" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="M34" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="N34" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="O34" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="P34" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q34" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="R34" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="S34" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="T34" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="U34" s="45" t="s">
+      <c r="L34" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M34" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="N34" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="O34" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="P34" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q34" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="R34" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="S34" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="T34" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="U34" s="34" t="s">
         <v>39</v>
       </c>
       <c r="V34" s="34" t="s">
@@ -28511,34 +28501,34 @@
       <c r="K35" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="L35" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="M35" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="N35" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="O35" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="P35" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q35" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="R35" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="S35" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="T35" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="U35" s="45" t="s">
+      <c r="L35" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M35" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="N35" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="O35" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="P35" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q35" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="R35" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="S35" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="T35" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="U35" s="34" t="s">
         <v>39</v>
       </c>
       <c r="V35" s="34" t="s">

</xml_diff>

<commit_message>
Introduce CURSE magic type. Introduce new types of curse spells: - SOUL_STRIKE - WEAKENING - SHACKLE - ENERGY_BLOCKING - POWER_DRAIN Curses can lower the enemy's attack, defense, damage and health.
</commit_message>
<xml_diff>
--- a/doc/caste_system.xlsx
+++ b/doc/caste_system.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/349dfb9748b30a92/Asztali gép/ataliasflame_2.0/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8938" documentId="8_{652F4476-B36F-42CD-831D-0D71B9923ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0AAD4D9E-F8A4-49D6-A71E-203DDABFB9B2}"/>
+  <xr:revisionPtr revIDLastSave="8973" documentId="8_{652F4476-B36F-42CD-831D-0D71B9923ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{237C751F-A45E-4C36-BCDE-991CA1048F40}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="696" activeTab="8" xr2:uid="{CAF51EC3-63EC-48CD-AA7B-C21B3D5D222B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="696" activeTab="7" xr2:uid="{CAF51EC3-63EC-48CD-AA7B-C21B3D5D222B}"/>
   </bookViews>
   <sheets>
     <sheet name="caste list" sheetId="1" r:id="rId1"/>
@@ -2552,29 +2552,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -2582,6 +2568,9 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2592,6 +2581,19 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2610,10 +2612,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3049,7 +3047,7 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="48" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="23" t="s">
@@ -3105,7 +3103,7 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="54"/>
+      <c r="A4" s="49"/>
       <c r="B4" s="23" t="s">
         <v>2</v>
       </c>
@@ -3159,7 +3157,7 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="54"/>
+      <c r="A5" s="49"/>
       <c r="B5" s="23" t="s">
         <v>3</v>
       </c>
@@ -3213,7 +3211,7 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="54"/>
+      <c r="A6" s="49"/>
       <c r="B6" s="22" t="s">
         <v>21</v>
       </c>
@@ -3267,7 +3265,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="55"/>
+      <c r="A7" s="50"/>
       <c r="B7" s="21" t="s">
         <v>4</v>
       </c>
@@ -3321,7 +3319,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="53" t="s">
+      <c r="A8" s="48" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="23" t="s">
@@ -3377,7 +3375,7 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="54"/>
+      <c r="A9" s="49"/>
       <c r="B9" s="23" t="s">
         <v>6</v>
       </c>
@@ -3431,7 +3429,7 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="54"/>
+      <c r="A10" s="49"/>
       <c r="B10" s="23" t="s">
         <v>7</v>
       </c>
@@ -3485,7 +3483,7 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="55"/>
+      <c r="A11" s="50"/>
       <c r="B11" s="21" t="s">
         <v>8</v>
       </c>
@@ -3539,7 +3537,7 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="53" t="s">
+      <c r="A12" s="48" t="s">
         <v>79</v>
       </c>
       <c r="B12" s="23" t="s">
@@ -3595,7 +3593,7 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="54"/>
+      <c r="A13" s="49"/>
       <c r="B13" s="23" t="s">
         <v>10</v>
       </c>
@@ -3649,7 +3647,7 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="54"/>
+      <c r="A14" s="49"/>
       <c r="B14" s="23" t="s">
         <v>11</v>
       </c>
@@ -3703,7 +3701,7 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="55"/>
+      <c r="A15" s="50"/>
       <c r="B15" s="21" t="s">
         <v>12</v>
       </c>
@@ -3757,7 +3755,7 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="53" t="s">
+      <c r="A16" s="48" t="s">
         <v>80</v>
       </c>
       <c r="B16" s="23" t="s">
@@ -3813,7 +3811,7 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="54"/>
+      <c r="A17" s="49"/>
       <c r="B17" s="23" t="s">
         <v>14</v>
       </c>
@@ -3867,7 +3865,7 @@
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" s="54"/>
+      <c r="A18" s="49"/>
       <c r="B18" s="23" t="s">
         <v>15</v>
       </c>
@@ -3921,7 +3919,7 @@
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" s="55"/>
+      <c r="A19" s="50"/>
       <c r="B19" s="21" t="s">
         <v>16</v>
       </c>
@@ -3975,7 +3973,7 @@
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="53" t="s">
+      <c r="A20" s="48" t="s">
         <v>81</v>
       </c>
       <c r="B20" s="23" t="s">
@@ -4031,7 +4029,7 @@
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21" s="54"/>
+      <c r="A21" s="49"/>
       <c r="B21" s="23" t="s">
         <v>18</v>
       </c>
@@ -4085,7 +4083,7 @@
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22" s="54"/>
+      <c r="A22" s="49"/>
       <c r="B22" s="23" t="s">
         <v>19</v>
       </c>
@@ -4139,7 +4137,7 @@
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23" s="55"/>
+      <c r="A23" s="50"/>
       <c r="B23" s="21" t="s">
         <v>20</v>
       </c>
@@ -4343,54 +4341,54 @@
       <c r="U1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="W1" s="56" t="s">
+      <c r="W1" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="56"/>
-      <c r="Z1" s="56"/>
-      <c r="AA1" s="56"/>
-      <c r="AB1" s="56"/>
-      <c r="AD1" s="56" t="s">
+      <c r="X1" s="51"/>
+      <c r="Y1" s="51"/>
+      <c r="Z1" s="51"/>
+      <c r="AA1" s="51"/>
+      <c r="AB1" s="51"/>
+      <c r="AD1" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="AE1" s="56"/>
-      <c r="AF1" s="56"/>
-      <c r="AG1" s="56"/>
-      <c r="AH1" s="56"/>
-      <c r="AI1" s="56"/>
-      <c r="AK1" s="56" t="s">
+      <c r="AE1" s="51"/>
+      <c r="AF1" s="51"/>
+      <c r="AG1" s="51"/>
+      <c r="AH1" s="51"/>
+      <c r="AI1" s="51"/>
+      <c r="AK1" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="AL1" s="56"/>
-      <c r="AM1" s="56"/>
-      <c r="AN1" s="56"/>
-      <c r="AO1" s="56"/>
-      <c r="AP1" s="56"/>
-      <c r="AR1" s="56" t="s">
+      <c r="AL1" s="51"/>
+      <c r="AM1" s="51"/>
+      <c r="AN1" s="51"/>
+      <c r="AO1" s="51"/>
+      <c r="AP1" s="51"/>
+      <c r="AR1" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="AS1" s="56"/>
-      <c r="AT1" s="56"/>
-      <c r="AU1" s="56"/>
-      <c r="AV1" s="56"/>
-      <c r="AW1" s="56"/>
-      <c r="AY1" s="56" t="s">
+      <c r="AS1" s="51"/>
+      <c r="AT1" s="51"/>
+      <c r="AU1" s="51"/>
+      <c r="AV1" s="51"/>
+      <c r="AW1" s="51"/>
+      <c r="AY1" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="AZ1" s="56"/>
-      <c r="BA1" s="56"/>
-      <c r="BB1" s="56"/>
-      <c r="BC1" s="56"/>
-      <c r="BD1" s="56"/>
-      <c r="BF1" s="56" t="s">
+      <c r="AZ1" s="51"/>
+      <c r="BA1" s="51"/>
+      <c r="BB1" s="51"/>
+      <c r="BC1" s="51"/>
+      <c r="BD1" s="51"/>
+      <c r="BF1" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="BG1" s="56"/>
-      <c r="BH1" s="56"/>
-      <c r="BI1" s="56"/>
-      <c r="BJ1" s="56"/>
-      <c r="BK1" s="56"/>
+      <c r="BG1" s="51"/>
+      <c r="BH1" s="51"/>
+      <c r="BI1" s="51"/>
+      <c r="BJ1" s="51"/>
+      <c r="BK1" s="51"/>
     </row>
     <row r="2" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
@@ -27968,7 +27966,7 @@
   <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A31" sqref="A31:XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27978,7 +27976,7 @@
     <col min="3" max="3" width="12.6640625" style="34" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" style="34" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.33203125" style="34" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" style="32" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="34" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.6640625" style="34" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.5546875" style="34" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.33203125" style="34" bestFit="1" customWidth="1"/>
@@ -28817,13 +28815,13 @@
       <c r="E1" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="34" t="s">
         <v>88</v>
       </c>
       <c r="G1" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="47" t="s">
         <v>90</v>
       </c>
       <c r="I1" s="34" t="s">
@@ -28858,7 +28856,7 @@
       <c r="E2" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="34" t="s">
         <v>40</v>
       </c>
       <c r="G2" s="34" t="s">
@@ -28899,7 +28897,7 @@
       <c r="E3" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="32" t="s">
+      <c r="F3" s="34" t="s">
         <v>40</v>
       </c>
       <c r="G3" s="34" t="s">
@@ -28940,7 +28938,7 @@
       <c r="E4" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="F4" s="34" t="s">
         <v>40</v>
       </c>
       <c r="G4" s="34" t="s">
@@ -28981,7 +28979,7 @@
       <c r="E5" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="32" t="s">
+      <c r="F5" s="34" t="s">
         <v>40</v>
       </c>
       <c r="G5" s="34" t="s">
@@ -29022,7 +29020,7 @@
       <c r="E6" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="32" t="s">
+      <c r="F6" s="34" t="s">
         <v>40</v>
       </c>
       <c r="G6" s="34" t="s">
@@ -29063,7 +29061,7 @@
       <c r="E7" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="32" t="s">
+      <c r="F7" s="34" t="s">
         <v>40</v>
       </c>
       <c r="G7" s="34" t="s">
@@ -29104,7 +29102,7 @@
       <c r="E8" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="32" t="s">
+      <c r="F8" s="34" t="s">
         <v>40</v>
       </c>
       <c r="G8" s="34" t="s">
@@ -29145,7 +29143,7 @@
       <c r="E9" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="32" t="s">
+      <c r="F9" s="34" t="s">
         <v>40</v>
       </c>
       <c r="G9" s="34" t="s">
@@ -29186,7 +29184,7 @@
       <c r="E10" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="32" t="s">
+      <c r="F10" s="34" t="s">
         <v>40</v>
       </c>
       <c r="G10" s="34" t="s">
@@ -29227,7 +29225,7 @@
       <c r="E11" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="32" t="s">
+      <c r="F11" s="34" t="s">
         <v>40</v>
       </c>
       <c r="G11" s="34" t="s">
@@ -29268,7 +29266,7 @@
       <c r="E12" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="32" t="s">
+      <c r="F12" s="34" t="s">
         <v>40</v>
       </c>
       <c r="G12" s="34" t="s">
@@ -29309,7 +29307,7 @@
       <c r="E13" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="32" t="s">
+      <c r="F13" s="34" t="s">
         <v>40</v>
       </c>
       <c r="G13" s="34" t="s">
@@ -29350,7 +29348,7 @@
       <c r="E14" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="32" t="s">
+      <c r="F14" s="34" t="s">
         <v>40</v>
       </c>
       <c r="G14" s="34" t="s">
@@ -29391,7 +29389,7 @@
       <c r="E15" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="F15" s="32" t="s">
+      <c r="F15" s="34" t="s">
         <v>40</v>
       </c>
       <c r="G15" s="34" t="s">
@@ -29432,7 +29430,7 @@
       <c r="E16" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="F16" s="32" t="s">
+      <c r="F16" s="34" t="s">
         <v>40</v>
       </c>
       <c r="G16" s="34" t="s">
@@ -29473,7 +29471,7 @@
       <c r="E17" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="F17" s="32" t="s">
+      <c r="F17" s="34" t="s">
         <v>40</v>
       </c>
       <c r="G17" s="34" t="s">
@@ -29514,7 +29512,7 @@
       <c r="E18" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="32" t="s">
+      <c r="F18" s="34" t="s">
         <v>40</v>
       </c>
       <c r="G18" s="34" t="s">
@@ -29555,7 +29553,7 @@
       <c r="E19" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="F19" s="32" t="s">
+      <c r="F19" s="34" t="s">
         <v>40</v>
       </c>
       <c r="G19" s="34" t="s">
@@ -29596,7 +29594,7 @@
       <c r="E20" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="F20" s="32" t="s">
+      <c r="F20" s="34" t="s">
         <v>40</v>
       </c>
       <c r="G20" s="34" t="s">
@@ -29637,7 +29635,7 @@
       <c r="E21" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="F21" s="32" t="s">
+      <c r="F21" s="34" t="s">
         <v>40</v>
       </c>
       <c r="G21" s="34" t="s">
@@ -29678,7 +29676,7 @@
       <c r="E22" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="F22" s="32" t="s">
+      <c r="F22" s="34" t="s">
         <v>40</v>
       </c>
       <c r="G22" s="34" t="s">
@@ -29719,7 +29717,7 @@
       <c r="E23" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="F23" s="32" t="s">
+      <c r="F23" s="34" t="s">
         <v>40</v>
       </c>
       <c r="G23" s="34" t="s">
@@ -29760,7 +29758,7 @@
       <c r="E24" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="F24" s="32" t="s">
+      <c r="F24" s="34" t="s">
         <v>40</v>
       </c>
       <c r="G24" s="34" t="s">
@@ -29801,7 +29799,7 @@
       <c r="E25" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="F25" s="32" t="s">
+      <c r="F25" s="34" t="s">
         <v>40</v>
       </c>
       <c r="G25" s="34" t="s">
@@ -29842,7 +29840,7 @@
       <c r="E26" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="F26" s="32" t="s">
+      <c r="F26" s="34" t="s">
         <v>40</v>
       </c>
       <c r="G26" s="34" t="s">
@@ -29867,208 +29865,208 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="37" t="s">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" t="s">
         <v>131</v>
       </c>
-      <c r="C27" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="D27" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="E27" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="F27" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="G27" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="H27" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="I27" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="J27" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="K27" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="L27" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="M27" s="32" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
+      <c r="C27" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="G27" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H27" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I27" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J27" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="K27" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="L27" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="M27" s="34" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>132</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" t="s">
         <v>133</v>
       </c>
-      <c r="C28" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="D28" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="E28" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="F28" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="G28" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="H28" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="I28" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="J28" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="K28" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="L28" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="M28" s="32" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
+      <c r="C28" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="G28" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H28" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I28" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J28" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K28" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="L28" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="M28" s="34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>134</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" t="s">
         <v>135</v>
       </c>
-      <c r="C29" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="D29" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="E29" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="F29" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="G29" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="H29" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="I29" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="J29" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="K29" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="L29" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="M29" s="32" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
+      <c r="C29" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="G29" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H29" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I29" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J29" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K29" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="L29" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="M29" s="34" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>136</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" t="s">
         <v>135</v>
       </c>
-      <c r="C30" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="D30" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="E30" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="F30" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="G30" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="H30" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="I30" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="J30" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="K30" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="L30" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="M30" s="32" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="38" t="s">
+      <c r="C30" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E30" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="F30" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="G30" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H30" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I30" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J30" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K30" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="L30" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="M30" s="34" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" t="s">
         <v>138</v>
       </c>
-      <c r="C31" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="D31" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="E31" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="F31" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="G31" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="H31" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="I31" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="J31" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="K31" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="L31" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="M31" s="32" t="s">
+      <c r="C31" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="F31" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="G31" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H31" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I31" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="J31" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K31" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="L31" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="M31" s="34" t="s">
         <v>39</v>
       </c>
     </row>
@@ -30088,7 +30086,7 @@
       <c r="E32" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="F32" s="32" t="s">
+      <c r="F32" s="34" t="s">
         <v>40</v>
       </c>
       <c r="G32" s="34" t="s">
@@ -30129,7 +30127,7 @@
       <c r="E33" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="F33" s="32" t="s">
+      <c r="F33" s="34" t="s">
         <v>40</v>
       </c>
       <c r="G33" s="34" t="s">
@@ -30170,7 +30168,7 @@
       <c r="E34" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="F34" s="32" t="s">
+      <c r="F34" s="34" t="s">
         <v>40</v>
       </c>
       <c r="G34" s="34" t="s">
@@ -30211,7 +30209,7 @@
       <c r="E35" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="F35" s="32" t="s">
+      <c r="F35" s="34" t="s">
         <v>40</v>
       </c>
       <c r="G35" s="34" t="s">
@@ -30252,7 +30250,7 @@
       <c r="E36" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="F36" s="32" t="s">
+      <c r="F36" s="34" t="s">
         <v>40</v>
       </c>
       <c r="G36" s="34" t="s">
@@ -30286,8 +30284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA1C4ECE-D418-419E-9393-664BDA889D6E}">
   <dimension ref="A1:AJ35"/>
   <sheetViews>
-    <sheetView topLeftCell="R13" workbookViewId="0">
-      <selection activeCell="AJ31" sqref="AJ31"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AG12" sqref="AG12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30318,11 +30316,11 @@
     <col min="24" max="24" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="6.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.88671875" style="52" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="14.33203125" bestFit="1" customWidth="1"/>
@@ -30405,19 +30403,19 @@
       <c r="Z1" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="AA1" s="32" t="s">
+      <c r="AA1" s="34" t="s">
         <v>130</v>
       </c>
-      <c r="AB1" s="32" t="s">
+      <c r="AB1" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="AC1" s="32" t="s">
+      <c r="AC1" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="AD1" s="32" t="s">
+      <c r="AD1" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="AE1" s="32" t="s">
+      <c r="AE1" s="53" t="s">
         <v>137</v>
       </c>
       <c r="AF1" s="34" t="s">
@@ -30437,222 +30435,222 @@
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="J2" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="K2" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="L2" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="M2" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="N2" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="O2" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="P2" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q2" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="R2" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="S2" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="T2" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="U2" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="V2" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="W2" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="X2" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y2" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z2" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA2" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB2" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC2" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="AD2" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE2" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="AF2" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="AG2" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH2" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI2" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ2" s="41" t="s">
+      <c r="B2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="P2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="R2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="S2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="T2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="U2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="V2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="W2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="X2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE2" s="56" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI2" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ2" s="38" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="H3" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="I3" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="J3" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="K3" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="L3" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="M3" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="N3" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="O3" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="P3" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q3" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="R3" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="S3" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="T3" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="U3" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="V3" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="W3" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="X3" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y3" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z3" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA3" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB3" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC3" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD3" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE3" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF3" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AG3" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH3" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI3" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ3" s="44" t="s">
+      <c r="B3" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="P3" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q3" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="R3" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="S3" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="T3" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="U3" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="V3" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="W3" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="X3" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y3" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z3" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA3" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB3" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC3" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD3" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE3" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF3" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG3" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH3" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI3" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ3" s="40" t="s">
         <v>40</v>
       </c>
     </row>
@@ -30735,19 +30733,19 @@
       <c r="Z4" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AA4" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB4" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC4" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD4" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE4" s="32" t="s">
+      <c r="AA4" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB4" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC4" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD4" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE4" s="53" t="s">
         <v>39</v>
       </c>
       <c r="AF4" s="34" t="s">
@@ -30845,19 +30843,19 @@
       <c r="Z5" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AA5" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB5" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC5" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD5" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE5" s="32" t="s">
+      <c r="AA5" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB5" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC5" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD5" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE5" s="53" t="s">
         <v>39</v>
       </c>
       <c r="AF5" s="34" t="s">
@@ -30880,219 +30878,219 @@
       <c r="A6" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="I6" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="J6" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="K6" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="L6" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="M6" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="N6" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="O6" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="P6" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q6" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="R6" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="S6" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="T6" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="U6" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="V6" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="W6" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="X6" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y6" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z6" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA6" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB6" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC6" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD6" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE6" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF6" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="AG6" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH6" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI6" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ6" s="46" t="s">
+      <c r="B6" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="M6" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="N6" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="O6" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="P6" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q6" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="R6" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="S6" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="T6" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="U6" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="V6" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="W6" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="X6" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y6" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z6" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA6" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB6" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC6" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD6" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE6" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF6" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG6" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH6" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI6" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ6" s="41" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="H7" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="I7" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="J7" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="K7" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="L7" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="M7" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="N7" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="O7" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="P7" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q7" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="R7" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="S7" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="T7" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="U7" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="V7" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="W7" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="X7" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y7" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z7" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA7" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB7" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC7" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AD7" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE7" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AF7" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AG7" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH7" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI7" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ7" s="44" t="s">
+      <c r="B7" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="J7" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="L7" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="M7" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="N7" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="O7" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="P7" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q7" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="R7" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="S7" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="T7" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="U7" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="V7" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="W7" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="X7" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y7" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z7" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA7" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB7" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC7" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD7" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE7" s="54" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF7" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG7" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH7" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI7" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ7" s="40" t="s">
         <v>40</v>
       </c>
     </row>
@@ -31175,19 +31173,19 @@
       <c r="Z8" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AA8" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB8" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC8" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="AD8" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE8" s="32" t="s">
+      <c r="AA8" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB8" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC8" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD8" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE8" s="53" t="s">
         <v>40</v>
       </c>
       <c r="AF8" s="34" t="s">
@@ -31285,19 +31283,19 @@
       <c r="Z9" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AA9" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB9" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC9" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD9" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE9" s="32" t="s">
+      <c r="AA9" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB9" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC9" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD9" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE9" s="53" t="s">
         <v>39</v>
       </c>
       <c r="AF9" s="34" t="s">
@@ -31320,219 +31318,219 @@
       <c r="A10" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="G10" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="H10" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="I10" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="J10" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="K10" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="L10" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="M10" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="N10" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="O10" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="P10" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q10" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="R10" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="S10" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="T10" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="U10" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="V10" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="W10" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="X10" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y10" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z10" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA10" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB10" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC10" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD10" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE10" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF10" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="AG10" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH10" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI10" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ10" s="46" t="s">
+      <c r="B10" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="J10" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="K10" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="L10" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="M10" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="N10" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="O10" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="P10" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q10" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="R10" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="S10" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="T10" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="U10" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="V10" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="W10" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="X10" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y10" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z10" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA10" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB10" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC10" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD10" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE10" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF10" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG10" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH10" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI10" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ10" s="41" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="G11" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="H11" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="I11" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="J11" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="K11" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="L11" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="M11" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="N11" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="O11" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="P11" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q11" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="R11" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="S11" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="T11" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="U11" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="V11" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="W11" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="X11" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y11" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z11" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA11" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB11" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC11" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD11" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE11" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AF11" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AG11" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH11" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI11" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ11" s="44" t="s">
+      <c r="B11" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="K11" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="L11" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="M11" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="N11" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="O11" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="P11" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q11" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="R11" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="S11" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="T11" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="U11" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="V11" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="W11" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="X11" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y11" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z11" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA11" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB11" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC11" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD11" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE11" s="54" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF11" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG11" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH11" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI11" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ11" s="40" t="s">
         <v>40</v>
       </c>
     </row>
@@ -31615,19 +31613,19 @@
       <c r="Z12" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AA12" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB12" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC12" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD12" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE12" s="32" t="s">
+      <c r="AA12" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB12" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC12" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD12" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE12" s="53" t="s">
         <v>40</v>
       </c>
       <c r="AF12" s="34" t="s">
@@ -31725,19 +31723,19 @@
       <c r="Z13" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AA13" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB13" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC13" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD13" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE13" s="32" t="s">
+      <c r="AA13" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB13" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC13" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD13" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE13" s="53" t="s">
         <v>40</v>
       </c>
       <c r="AF13" s="34" t="s">
@@ -31760,219 +31758,219 @@
       <c r="A14" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="H14" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="I14" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="J14" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="K14" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="L14" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="M14" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="N14" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="O14" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="P14" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q14" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="R14" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="S14" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="T14" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="U14" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="V14" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="W14" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="X14" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y14" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z14" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA14" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB14" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC14" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD14" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE14" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF14" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="AG14" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH14" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI14" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ14" s="46" t="s">
+      <c r="B14" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="I14" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="J14" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="K14" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="L14" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="M14" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="N14" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="O14" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="P14" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q14" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="R14" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="S14" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="T14" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="U14" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="V14" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="W14" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="X14" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y14" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z14" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA14" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB14" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC14" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD14" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE14" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF14" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG14" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH14" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI14" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ14" s="41" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="G15" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="H15" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="I15" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="J15" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="K15" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="L15" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="M15" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="N15" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="O15" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="P15" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q15" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="R15" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="S15" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="T15" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="U15" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="V15" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="W15" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="X15" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y15" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z15" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA15" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB15" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC15" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD15" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE15" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AF15" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AG15" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH15" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI15" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ15" s="44" t="s">
+      <c r="B15" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="I15" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="J15" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="K15" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="L15" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="M15" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="N15" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="O15" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="P15" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q15" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="R15" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="S15" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="T15" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="U15" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="V15" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="W15" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="X15" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y15" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z15" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA15" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB15" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC15" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD15" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE15" s="54" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF15" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG15" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH15" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI15" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ15" s="40" t="s">
         <v>40</v>
       </c>
     </row>
@@ -32055,19 +32053,19 @@
       <c r="Z16" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AA16" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB16" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC16" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD16" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE16" s="32" t="s">
+      <c r="AA16" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB16" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC16" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD16" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE16" s="53" t="s">
         <v>40</v>
       </c>
       <c r="AF16" s="34" t="s">
@@ -32165,19 +32163,19 @@
       <c r="Z17" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AA17" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB17" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC17" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD17" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE17" s="32" t="s">
+      <c r="AA17" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB17" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC17" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD17" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE17" s="53" t="s">
         <v>39</v>
       </c>
       <c r="AF17" s="34" t="s">
@@ -32200,219 +32198,219 @@
       <c r="A18" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="G18" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="H18" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="I18" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="J18" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="K18" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="L18" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="M18" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="N18" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="O18" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="P18" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q18" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="R18" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="S18" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="T18" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="U18" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="V18" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="W18" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="X18" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y18" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z18" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA18" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB18" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC18" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD18" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE18" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF18" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="AG18" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH18" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI18" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ18" s="46" t="s">
+      <c r="B18" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="H18" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="I18" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="J18" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="K18" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="L18" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="M18" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="N18" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="O18" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="P18" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q18" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="R18" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="S18" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="T18" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="U18" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="V18" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="W18" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="X18" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y18" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z18" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA18" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB18" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC18" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD18" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE18" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF18" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG18" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH18" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI18" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ18" s="41" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="F19" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="G19" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="H19" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="I19" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="J19" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="K19" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="L19" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="M19" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="N19" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="O19" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="P19" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q19" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="R19" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="S19" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="T19" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="U19" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="V19" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="W19" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="X19" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y19" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z19" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA19" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB19" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC19" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD19" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE19" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF19" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AG19" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH19" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI19" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ19" s="44" t="s">
+      <c r="B19" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="H19" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="I19" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="J19" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="K19" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="L19" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="M19" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="N19" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="O19" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="P19" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q19" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="R19" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="S19" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="T19" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="U19" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="V19" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="W19" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="X19" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y19" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z19" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA19" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB19" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC19" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD19" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE19" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF19" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG19" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH19" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI19" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ19" s="40" t="s">
         <v>39</v>
       </c>
     </row>
@@ -32495,19 +32493,19 @@
       <c r="Z20" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AA20" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB20" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC20" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD20" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE20" s="32" t="s">
+      <c r="AA20" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB20" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC20" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD20" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE20" s="53" t="s">
         <v>39</v>
       </c>
       <c r="AF20" s="34" t="s">
@@ -32605,19 +32603,19 @@
       <c r="Z21" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AA21" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB21" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC21" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD21" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE21" s="32" t="s">
+      <c r="AA21" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB21" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC21" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD21" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE21" s="53" t="s">
         <v>39</v>
       </c>
       <c r="AF21" s="34" t="s">
@@ -32640,109 +32638,109 @@
       <c r="A22" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="F22" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="G22" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="H22" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="I22" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="J22" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="K22" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="L22" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="M22" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="N22" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="O22" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="P22" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q22" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="R22" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="S22" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="T22" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="U22" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="V22" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="W22" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="X22" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y22" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z22" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA22" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB22" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC22" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD22" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE22" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF22" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="AG22" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH22" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI22" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ22" s="46" t="s">
+      <c r="B22" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="H22" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="I22" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="J22" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="K22" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="L22" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="M22" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="N22" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="O22" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="P22" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q22" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="R22" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="S22" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="T22" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="U22" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="V22" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="W22" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="X22" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y22" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z22" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA22" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB22" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC22" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD22" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE22" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF22" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG22" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH22" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI22" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ22" s="41" t="s">
         <v>39</v>
       </c>
     </row>
@@ -32822,19 +32820,19 @@
       <c r="Z25" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="AA25" s="32" t="s">
+      <c r="AA25" s="34" t="s">
         <v>130</v>
       </c>
-      <c r="AB25" s="32" t="s">
+      <c r="AB25" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="AC25" s="32" t="s">
+      <c r="AC25" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="AD25" s="32" t="s">
+      <c r="AD25" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="AE25" s="32" t="s">
+      <c r="AE25" s="53" t="s">
         <v>137</v>
       </c>
       <c r="AF25" s="34" t="s">
@@ -32854,112 +32852,112 @@
       </c>
     </row>
     <row r="26" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A26" s="43" t="s">
+      <c r="A26" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="E26" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="F26" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="G26" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="H26" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="I26" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="J26" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="K26" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="L26" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="M26" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="N26" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="O26" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="P26" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q26" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="R26" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="S26" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="T26" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="U26" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="V26" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="W26" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="X26" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y26" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z26" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA26" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB26" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC26" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD26" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE26" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF26" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AG26" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH26" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI26" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ26" s="44" t="s">
+      <c r="B26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="F26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="G26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="H26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="I26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="J26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="K26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="L26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="M26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="N26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="O26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="P26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="R26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="S26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="T26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="U26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="V26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="W26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="X26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE26" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ26" s="40" t="s">
         <v>39</v>
       </c>
     </row>
@@ -33042,19 +33040,19 @@
       <c r="Z27" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AA27" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB27" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC27" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD27" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE27" s="32" t="s">
+      <c r="AA27" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB27" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC27" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD27" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE27" s="53" t="s">
         <v>39</v>
       </c>
       <c r="AF27" s="34" t="s">
@@ -33152,19 +33150,19 @@
       <c r="Z28" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AA28" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB28" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC28" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD28" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE28" s="32" t="s">
+      <c r="AA28" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB28" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC28" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD28" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE28" s="53" t="s">
         <v>39</v>
       </c>
       <c r="AF28" s="34" t="s">
@@ -33262,19 +33260,19 @@
       <c r="Z29" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AA29" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB29" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC29" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD29" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE29" s="32" t="s">
+      <c r="AA29" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB29" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC29" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD29" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE29" s="53" t="s">
         <v>39</v>
       </c>
       <c r="AF29" s="34" t="s">
@@ -33372,19 +33370,19 @@
       <c r="Z30" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AA30" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB30" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC30" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD30" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE30" s="32" t="s">
+      <c r="AA30" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB30" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC30" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD30" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE30" s="53" t="s">
         <v>40</v>
       </c>
       <c r="AF30" s="34" t="s">
@@ -33482,19 +33480,19 @@
       <c r="Z31" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AA31" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB31" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC31" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD31" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE31" s="32" t="s">
+      <c r="AA31" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB31" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC31" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD31" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE31" s="53" t="s">
         <v>40</v>
       </c>
       <c r="AF31" s="34" t="s">
@@ -33592,19 +33590,19 @@
       <c r="Z32" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AA32" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB32" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC32" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD32" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE32" s="32" t="s">
+      <c r="AA32" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB32" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC32" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD32" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE32" s="53" t="s">
         <v>40</v>
       </c>
       <c r="AF32" s="34" t="s">
@@ -33702,19 +33700,19 @@
       <c r="Z33" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AA33" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB33" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC33" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD33" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE33" s="32" t="s">
+      <c r="AA33" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB33" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC33" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD33" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE33" s="53" t="s">
         <v>39</v>
       </c>
       <c r="AF33" s="34" t="s">
@@ -33812,19 +33810,19 @@
       <c r="Z34" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AA34" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB34" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC34" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD34" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE34" s="32" t="s">
+      <c r="AA34" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB34" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC34" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD34" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE34" s="53" t="s">
         <v>39</v>
       </c>
       <c r="AF34" s="34" t="s">
@@ -33847,109 +33845,109 @@
       <c r="A35" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="C35" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="D35" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="E35" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="F35" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="G35" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="H35" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="I35" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="J35" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="K35" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="L35" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="M35" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="N35" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="O35" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="P35" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q35" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="R35" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="S35" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="T35" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="U35" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="V35" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="W35" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="X35" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y35" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z35" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA35" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB35" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC35" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD35" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE35" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF35" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="AG35" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH35" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI35" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="AJ35" s="46" t="s">
+      <c r="B35" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="E35" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="F35" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="G35" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="H35" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="I35" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="J35" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="K35" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="L35" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="M35" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="N35" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="O35" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="P35" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q35" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="R35" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="S35" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="T35" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="U35" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="V35" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="W35" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="X35" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y35" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z35" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA35" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB35" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC35" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD35" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE35" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF35" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG35" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH35" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI35" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ35" s="41" t="s">
         <v>39</v>
       </c>
     </row>
@@ -33962,7 +33960,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F39E67B8-A1DC-45C6-A1D4-0073AA57C7BD}">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M20" sqref="M20:N20"/>
     </sheetView>
   </sheetViews>
@@ -34040,22 +34038,22 @@
       <c r="B6" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="51" t="s">
+      <c r="D6" s="45" t="s">
         <v>154</v>
       </c>
-      <c r="E6" s="51" t="s">
+      <c r="E6" s="45" t="s">
         <v>152</v>
       </c>
-      <c r="G6" s="52" t="s">
+      <c r="G6" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="H6" s="52" t="s">
+      <c r="H6" s="46" t="s">
         <v>165</v>
       </c>
-      <c r="J6" s="52" t="s">
+      <c r="J6" s="46" t="s">
         <v>162</v>
       </c>
-      <c r="K6" s="52" t="s">
+      <c r="K6" s="46" t="s">
         <v>166</v>
       </c>
       <c r="M6" t="s">
@@ -34083,16 +34081,16 @@
       <c r="B8" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="48" t="s">
+      <c r="D8" s="42" t="s">
         <v>153</v>
       </c>
-      <c r="E8" s="48" t="s">
+      <c r="E8" s="42" t="s">
         <v>151</v>
       </c>
-      <c r="G8" s="50" t="s">
+      <c r="G8" s="44" t="s">
         <v>160</v>
       </c>
-      <c r="H8" s="50" t="s">
+      <c r="H8" s="44" t="s">
         <v>164</v>
       </c>
       <c r="M8" t="s">
@@ -34126,8 +34124,8 @@
       <c r="B10" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
       <c r="M10" t="s">
         <v>160</v>
       </c>
@@ -34162,10 +34160,10 @@
       <c r="E12" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="G12" s="50" t="s">
+      <c r="G12" s="44" t="s">
         <v>155</v>
       </c>
-      <c r="H12" s="50" t="s">
+      <c r="H12" s="44" t="s">
         <v>156</v>
       </c>
     </row>
@@ -34203,10 +34201,10 @@
       <c r="E16" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="G16" s="50" t="s">
+      <c r="G16" s="44" t="s">
         <v>155</v>
       </c>
-      <c r="H16" s="50" t="s">
+      <c r="H16" s="44" t="s">
         <v>156</v>
       </c>
       <c r="M16" t="s">
@@ -34237,8 +34235,8 @@
       <c r="B18" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
       <c r="M18" t="s">
         <v>159</v>
       </c>
@@ -34317,10 +34315,10 @@
       <c r="E24" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="G24" s="50" t="s">
+      <c r="G24" s="44" t="s">
         <v>160</v>
       </c>
-      <c r="H24" s="50" t="s">
+      <c r="H24" s="44" t="s">
         <v>164</v>
       </c>
     </row>
@@ -34339,8 +34337,8 @@
       <c r="B26" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="49"/>
-      <c r="E26" s="49"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B27" t="s">

</xml_diff>

<commit_message>
Review spell prohibitions. Prohibitions can be made now on a spell group level. Healing spells are now cast until necessary and possible, there can be not only one spell per combat.
</commit_message>
<xml_diff>
--- a/doc/caste_system.xlsx
+++ b/doc/caste_system.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/349dfb9748b30a92/Asztali gép/ataliasflame_2.0/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8973" documentId="8_{652F4476-B36F-42CD-831D-0D71B9923ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{237C751F-A45E-4C36-BCDE-991CA1048F40}"/>
+  <xr:revisionPtr revIDLastSave="9590" documentId="8_{652F4476-B36F-42CD-831D-0D71B9923ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65C51AA8-7A2E-4CAB-925B-04EC196CD0E5}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="696" activeTab="7" xr2:uid="{CAF51EC3-63EC-48CD-AA7B-C21B3D5D222B}"/>
   </bookViews>
@@ -2494,7 +2494,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2583,18 +2583,8 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2612,6 +2602,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2914,7 +2908,7 @@
   <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27966,7 +27960,7 @@
   <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:XFD31"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30284,8 +30278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA1C4ECE-D418-419E-9393-664BDA889D6E}">
   <dimension ref="A1:AJ35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AG12" sqref="AG12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AJ19" sqref="AJ19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30320,7 +30314,7 @@
     <col min="28" max="28" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.88671875" style="52" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="14.33203125" bestFit="1" customWidth="1"/>
@@ -30415,7 +30409,7 @@
       <c r="AD1" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="AE1" s="53" t="s">
+      <c r="AE1" s="34" t="s">
         <v>137</v>
       </c>
       <c r="AF1" s="34" t="s">
@@ -30525,7 +30519,7 @@
       <c r="AD2" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="AE2" s="56" t="s">
+      <c r="AE2" s="38" t="s">
         <v>40</v>
       </c>
       <c r="AF2" s="38" t="s">
@@ -30552,19 +30546,19 @@
         <v>39</v>
       </c>
       <c r="C3" s="40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D3" s="40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E3" s="40" t="s">
         <v>40</v>
       </c>
       <c r="F3" s="40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G3" s="40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H3" s="40" t="s">
         <v>40</v>
@@ -30585,7 +30579,7 @@
         <v>40</v>
       </c>
       <c r="N3" s="40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O3" s="40" t="s">
         <v>39</v>
@@ -30600,10 +30594,10 @@
         <v>40</v>
       </c>
       <c r="S3" s="40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="T3" s="40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="U3" s="40" t="s">
         <v>40</v>
@@ -30612,7 +30606,7 @@
         <v>40</v>
       </c>
       <c r="W3" s="40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="X3" s="40" t="s">
         <v>40</v>
@@ -30621,7 +30615,7 @@
         <v>40</v>
       </c>
       <c r="Z3" s="40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AA3" s="40" t="s">
         <v>40</v>
@@ -30630,13 +30624,13 @@
         <v>39</v>
       </c>
       <c r="AC3" s="40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AD3" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="AE3" s="54" t="s">
-        <v>39</v>
+      <c r="AE3" s="40" t="s">
+        <v>40</v>
       </c>
       <c r="AF3" s="40" t="s">
         <v>40</v>
@@ -30645,7 +30639,7 @@
         <v>40</v>
       </c>
       <c r="AH3" s="40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AI3" s="40" t="s">
         <v>40</v>
@@ -30665,10 +30659,10 @@
         <v>39</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E4" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F4" s="34" t="s">
         <v>39</v>
@@ -30716,7 +30710,7 @@
         <v>39</v>
       </c>
       <c r="U4" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="V4" s="34" t="s">
         <v>40</v>
@@ -30740,19 +30734,19 @@
         <v>39</v>
       </c>
       <c r="AC4" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AD4" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AE4" s="53" t="s">
-        <v>39</v>
+      <c r="AE4" s="34" t="s">
+        <v>40</v>
       </c>
       <c r="AF4" s="34" t="s">
         <v>40</v>
       </c>
       <c r="AG4" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AH4" s="34" t="s">
         <v>39</v>
@@ -30778,7 +30772,7 @@
         <v>39</v>
       </c>
       <c r="E5" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F5" s="34" t="s">
         <v>39</v>
@@ -30790,7 +30784,7 @@
         <v>40</v>
       </c>
       <c r="I5" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J5" s="34" t="s">
         <v>39</v>
@@ -30838,7 +30832,7 @@
         <v>40</v>
       </c>
       <c r="Y5" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z5" s="34" t="s">
         <v>39</v>
@@ -30855,7 +30849,7 @@
       <c r="AD5" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AE5" s="53" t="s">
+      <c r="AE5" s="34" t="s">
         <v>39</v>
       </c>
       <c r="AF5" s="34" t="s">
@@ -30871,7 +30865,7 @@
         <v>39</v>
       </c>
       <c r="AJ5" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.3">
@@ -30906,13 +30900,13 @@
         <v>39</v>
       </c>
       <c r="K6" s="41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L6" s="41" t="s">
         <v>39</v>
       </c>
       <c r="M6" s="41" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N6" s="41" t="s">
         <v>39</v>
@@ -30921,7 +30915,7 @@
         <v>39</v>
       </c>
       <c r="P6" s="41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q6" s="41" t="s">
         <v>39</v>
@@ -30939,7 +30933,7 @@
         <v>39</v>
       </c>
       <c r="V6" s="41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="W6" s="41" t="s">
         <v>39</v>
@@ -30948,7 +30942,7 @@
         <v>40</v>
       </c>
       <c r="Y6" s="41" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z6" s="41" t="s">
         <v>39</v>
@@ -30965,7 +30959,7 @@
       <c r="AD6" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="AE6" s="55" t="s">
+      <c r="AE6" s="41" t="s">
         <v>39</v>
       </c>
       <c r="AF6" s="41" t="s">
@@ -30981,7 +30975,7 @@
         <v>39</v>
       </c>
       <c r="AJ6" s="41" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.3">
@@ -31025,10 +31019,10 @@
         <v>40</v>
       </c>
       <c r="N7" s="40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O7" s="40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P7" s="40" t="s">
         <v>40</v>
@@ -31043,7 +31037,7 @@
         <v>40</v>
       </c>
       <c r="T7" s="40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="U7" s="40" t="s">
         <v>40</v>
@@ -31061,13 +31055,13 @@
         <v>40</v>
       </c>
       <c r="Z7" s="40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AA7" s="40" t="s">
         <v>40</v>
       </c>
       <c r="AB7" s="40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AC7" s="40" t="s">
         <v>40</v>
@@ -31075,7 +31069,7 @@
       <c r="AD7" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="AE7" s="54" t="s">
+      <c r="AE7" s="40" t="s">
         <v>40</v>
       </c>
       <c r="AF7" s="40" t="s">
@@ -31099,7 +31093,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" s="34" t="s">
         <v>40</v>
@@ -31150,13 +31144,13 @@
         <v>40</v>
       </c>
       <c r="S8" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="T8" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="U8" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="V8" s="34" t="s">
         <v>40</v>
@@ -31177,7 +31171,7 @@
         <v>40</v>
       </c>
       <c r="AB8" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AC8" s="34" t="s">
         <v>40</v>
@@ -31185,7 +31179,7 @@
       <c r="AD8" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AE8" s="53" t="s">
+      <c r="AE8" s="34" t="s">
         <v>40</v>
       </c>
       <c r="AF8" s="34" t="s">
@@ -31212,7 +31206,7 @@
         <v>39</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D9" s="34" t="s">
         <v>40</v>
@@ -31266,7 +31260,7 @@
         <v>39</v>
       </c>
       <c r="U9" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="V9" s="34" t="s">
         <v>40</v>
@@ -31277,7 +31271,7 @@
       <c r="X9" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="Y9" s="34" t="s">
+      <c r="Y9" s="26" t="s">
         <v>40</v>
       </c>
       <c r="Z9" s="34" t="s">
@@ -31290,19 +31284,19 @@
         <v>39</v>
       </c>
       <c r="AC9" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AD9" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE9" s="53" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="AE9" s="34" t="s">
+        <v>40</v>
       </c>
       <c r="AF9" s="34" t="s">
         <v>40</v>
       </c>
       <c r="AG9" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AH9" s="34" t="s">
         <v>39</v>
@@ -31343,7 +31337,7 @@
         <v>40</v>
       </c>
       <c r="J10" s="41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K10" s="41" t="s">
         <v>40</v>
@@ -31405,14 +31399,14 @@
       <c r="AD10" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="AE10" s="55" t="s">
-        <v>39</v>
+      <c r="AE10" s="41" t="s">
+        <v>40</v>
       </c>
       <c r="AF10" s="41" t="s">
         <v>40</v>
       </c>
       <c r="AG10" s="41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AH10" s="41" t="s">
         <v>39</v>
@@ -31474,7 +31468,7 @@
         <v>40</v>
       </c>
       <c r="Q11" s="40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="R11" s="40" t="s">
         <v>40</v>
@@ -31498,7 +31492,7 @@
         <v>40</v>
       </c>
       <c r="Y11" s="40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Z11" s="40" t="s">
         <v>40</v>
@@ -31510,12 +31504,12 @@
         <v>40</v>
       </c>
       <c r="AC11" s="40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AD11" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="AE11" s="54" t="s">
+      <c r="AE11" s="40" t="s">
         <v>40</v>
       </c>
       <c r="AF11" s="40" t="s">
@@ -31539,7 +31533,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" s="34" t="s">
         <v>40</v>
@@ -31557,7 +31551,7 @@
         <v>40</v>
       </c>
       <c r="H12" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I12" s="34" t="s">
         <v>40</v>
@@ -31584,7 +31578,7 @@
         <v>40</v>
       </c>
       <c r="Q12" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="R12" s="34" t="s">
         <v>39</v>
@@ -31605,10 +31599,10 @@
         <v>40</v>
       </c>
       <c r="X12" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Y12" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Z12" s="34" t="s">
         <v>40</v>
@@ -31620,12 +31614,12 @@
         <v>40</v>
       </c>
       <c r="AC12" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AD12" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AE12" s="53" t="s">
+      <c r="AE12" s="34" t="s">
         <v>40</v>
       </c>
       <c r="AF12" s="34" t="s">
@@ -31649,10 +31643,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D13" s="34" t="s">
         <v>40</v>
@@ -31664,7 +31658,7 @@
         <v>40</v>
       </c>
       <c r="G13" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H13" s="34" t="s">
         <v>39</v>
@@ -31673,7 +31667,7 @@
         <v>40</v>
       </c>
       <c r="J13" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K13" s="34" t="s">
         <v>40</v>
@@ -31700,28 +31694,28 @@
         <v>39</v>
       </c>
       <c r="S13" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="T13" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="U13" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="V13" s="34" t="s">
         <v>40</v>
       </c>
       <c r="W13" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X13" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Y13" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Z13" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AA13" s="34" t="s">
         <v>39</v>
@@ -31735,7 +31729,7 @@
       <c r="AD13" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AE13" s="53" t="s">
+      <c r="AE13" s="34" t="s">
         <v>40</v>
       </c>
       <c r="AF13" s="34" t="s">
@@ -31748,7 +31742,7 @@
         <v>40</v>
       </c>
       <c r="AI13" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AJ13" s="34" t="s">
         <v>40</v>
@@ -31762,10 +31756,10 @@
         <v>39</v>
       </c>
       <c r="C14" s="41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D14" s="41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E14" s="41" t="s">
         <v>39</v>
@@ -31774,16 +31768,16 @@
         <v>40</v>
       </c>
       <c r="G14" s="41" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H14" s="41" t="s">
         <v>39</v>
       </c>
       <c r="I14" s="41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J14" s="41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K14" s="41" t="s">
         <v>40</v>
@@ -31810,13 +31804,13 @@
         <v>39</v>
       </c>
       <c r="S14" s="41" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="T14" s="41" t="s">
         <v>39</v>
       </c>
       <c r="U14" s="41" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="V14" s="41" t="s">
         <v>40</v>
@@ -31828,16 +31822,16 @@
         <v>39</v>
       </c>
       <c r="Y14" s="41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Z14" s="41" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AA14" s="41" t="s">
         <v>39</v>
       </c>
       <c r="AB14" s="41" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AC14" s="41" t="s">
         <v>39</v>
@@ -31845,8 +31839,8 @@
       <c r="AD14" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="AE14" s="55" t="s">
-        <v>39</v>
+      <c r="AE14" s="41" t="s">
+        <v>40</v>
       </c>
       <c r="AF14" s="41" t="s">
         <v>39</v>
@@ -31858,7 +31852,7 @@
         <v>39</v>
       </c>
       <c r="AI14" s="41" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AJ14" s="41" t="s">
         <v>40</v>
@@ -31869,10 +31863,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C15" s="40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D15" s="40" t="s">
         <v>40</v>
@@ -31881,7 +31875,7 @@
         <v>40</v>
       </c>
       <c r="F15" s="40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G15" s="40" t="s">
         <v>40</v>
@@ -31890,10 +31884,10 @@
         <v>40</v>
       </c>
       <c r="I15" s="40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J15" s="40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K15" s="40" t="s">
         <v>40</v>
@@ -31905,7 +31899,7 @@
         <v>40</v>
       </c>
       <c r="N15" s="40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O15" s="40" t="s">
         <v>39</v>
@@ -31923,7 +31917,7 @@
         <v>40</v>
       </c>
       <c r="T15" s="40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="U15" s="40" t="s">
         <v>40</v>
@@ -31938,7 +31932,7 @@
         <v>40</v>
       </c>
       <c r="Y15" s="40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z15" s="40" t="s">
         <v>40</v>
@@ -31950,12 +31944,12 @@
         <v>40</v>
       </c>
       <c r="AC15" s="40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AD15" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="AE15" s="54" t="s">
+      <c r="AE15" s="40" t="s">
         <v>40</v>
       </c>
       <c r="AF15" s="40" t="s">
@@ -31982,16 +31976,16 @@
         <v>39</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E16" s="34" t="s">
         <v>40</v>
       </c>
       <c r="F16" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G16" s="34" t="s">
         <v>39</v>
@@ -32000,7 +31994,7 @@
         <v>40</v>
       </c>
       <c r="I16" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J16" s="34" t="s">
         <v>39</v>
@@ -32033,16 +32027,16 @@
         <v>39</v>
       </c>
       <c r="T16" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="U16" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="V16" s="34" t="s">
         <v>40</v>
       </c>
       <c r="W16" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="X16" s="34" t="s">
         <v>40</v>
@@ -32051,7 +32045,7 @@
         <v>39</v>
       </c>
       <c r="Z16" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AA16" s="34" t="s">
         <v>40</v>
@@ -32065,7 +32059,7 @@
       <c r="AD16" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AE16" s="53" t="s">
+      <c r="AE16" s="34" t="s">
         <v>40</v>
       </c>
       <c r="AF16" s="34" t="s">
@@ -32081,7 +32075,7 @@
         <v>40</v>
       </c>
       <c r="AJ16" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:36" x14ac:dyDescent="0.3">
@@ -32095,7 +32089,7 @@
         <v>39</v>
       </c>
       <c r="D17" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E17" s="34" t="s">
         <v>40</v>
@@ -32122,7 +32116,7 @@
         <v>39</v>
       </c>
       <c r="M17" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N17" s="34" t="s">
         <v>39</v>
@@ -32152,7 +32146,7 @@
         <v>40</v>
       </c>
       <c r="W17" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="X17" s="34" t="s">
         <v>40</v>
@@ -32175,7 +32169,7 @@
       <c r="AD17" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AE17" s="53" t="s">
+      <c r="AE17" s="34" t="s">
         <v>39</v>
       </c>
       <c r="AF17" s="34" t="s">
@@ -32188,10 +32182,10 @@
         <v>39</v>
       </c>
       <c r="AI17" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AJ17" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.3">
@@ -32208,7 +32202,7 @@
         <v>39</v>
       </c>
       <c r="E18" s="41" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F18" s="41" t="s">
         <v>39</v>
@@ -32285,7 +32279,7 @@
       <c r="AD18" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="AE18" s="55" t="s">
+      <c r="AE18" s="41" t="s">
         <v>39</v>
       </c>
       <c r="AF18" s="41" t="s">
@@ -32301,7 +32295,7 @@
         <v>39</v>
       </c>
       <c r="AJ18" s="41" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:36" x14ac:dyDescent="0.3">
@@ -32309,10 +32303,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C19" s="40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D19" s="40" t="s">
         <v>40</v>
@@ -32321,7 +32315,7 @@
         <v>40</v>
       </c>
       <c r="F19" s="40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G19" s="40" t="s">
         <v>40</v>
@@ -32333,10 +32327,10 @@
         <v>40</v>
       </c>
       <c r="J19" s="40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K19" s="40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="L19" s="40" t="s">
         <v>39</v>
@@ -32345,13 +32339,13 @@
         <v>39</v>
       </c>
       <c r="N19" s="40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O19" s="40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P19" s="40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Q19" s="40" t="s">
         <v>40</v>
@@ -32368,11 +32362,11 @@
       <c r="U19" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="V19" s="40" t="s">
+      <c r="V19" s="34" t="s">
         <v>39</v>
       </c>
       <c r="W19" s="40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="X19" s="40" t="s">
         <v>40</v>
@@ -32387,16 +32381,16 @@
         <v>40</v>
       </c>
       <c r="AB19" s="40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AC19" s="40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AD19" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="AE19" s="54" t="s">
-        <v>39</v>
+      <c r="AE19" s="40" t="s">
+        <v>40</v>
       </c>
       <c r="AF19" s="40" t="s">
         <v>40</v>
@@ -32405,12 +32399,12 @@
         <v>40</v>
       </c>
       <c r="AH19" s="40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AI19" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="AJ19" s="40" t="s">
+      <c r="AJ19" s="34" t="s">
         <v>39</v>
       </c>
     </row>
@@ -32422,19 +32416,19 @@
         <v>39</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D20" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E20" s="34" t="s">
         <v>40</v>
       </c>
       <c r="F20" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G20" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H20" s="34" t="s">
         <v>40</v>
@@ -32464,13 +32458,13 @@
         <v>39</v>
       </c>
       <c r="Q20" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="R20" s="34" t="s">
         <v>40</v>
       </c>
       <c r="S20" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="T20" s="34" t="s">
         <v>39</v>
@@ -32491,13 +32485,13 @@
         <v>40</v>
       </c>
       <c r="Z20" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AA20" s="34" t="s">
         <v>40</v>
       </c>
       <c r="AB20" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AC20" s="34" t="s">
         <v>39</v>
@@ -32505,17 +32499,17 @@
       <c r="AD20" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AE20" s="53" t="s">
-        <v>39</v>
+      <c r="AE20" s="34" t="s">
+        <v>40</v>
       </c>
       <c r="AF20" s="34" t="s">
         <v>40</v>
       </c>
       <c r="AG20" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AH20" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AI20" s="34" t="s">
         <v>40</v>
@@ -32535,13 +32529,13 @@
         <v>39</v>
       </c>
       <c r="D21" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E21" s="34" t="s">
         <v>39</v>
       </c>
       <c r="F21" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G21" s="34" t="s">
         <v>39</v>
@@ -32574,7 +32568,7 @@
         <v>39</v>
       </c>
       <c r="Q21" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="R21" s="34" t="s">
         <v>40</v>
@@ -32586,7 +32580,7 @@
         <v>39</v>
       </c>
       <c r="U21" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="V21" s="34" t="s">
         <v>39</v>
@@ -32598,7 +32592,7 @@
         <v>40</v>
       </c>
       <c r="Y21" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Z21" s="34" t="s">
         <v>39</v>
@@ -32615,14 +32609,14 @@
       <c r="AD21" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AE21" s="53" t="s">
-        <v>39</v>
+      <c r="AE21" s="34" t="s">
+        <v>40</v>
       </c>
       <c r="AF21" s="34" t="s">
         <v>40</v>
       </c>
       <c r="AG21" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AH21" s="34" t="s">
         <v>39</v>
@@ -32660,7 +32654,7 @@
         <v>40</v>
       </c>
       <c r="I22" s="41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J22" s="41" t="s">
         <v>39</v>
@@ -32684,7 +32678,7 @@
         <v>39</v>
       </c>
       <c r="Q22" s="41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="R22" s="41" t="s">
         <v>40</v>
@@ -32696,7 +32690,7 @@
         <v>39</v>
       </c>
       <c r="U22" s="41" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="V22" s="41" t="s">
         <v>39</v>
@@ -32708,7 +32702,7 @@
         <v>40</v>
       </c>
       <c r="Y22" s="41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Z22" s="41" t="s">
         <v>39</v>
@@ -32725,14 +32719,14 @@
       <c r="AD22" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="AE22" s="55" t="s">
-        <v>39</v>
+      <c r="AE22" s="41" t="s">
+        <v>40</v>
       </c>
       <c r="AF22" s="41" t="s">
         <v>40</v>
       </c>
       <c r="AG22" s="41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AH22" s="41" t="s">
         <v>39</v>
@@ -32832,7 +32826,7 @@
       <c r="AD25" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="AE25" s="53" t="s">
+      <c r="AE25" s="34" t="s">
         <v>137</v>
       </c>
       <c r="AF25" s="34" t="s">
@@ -32942,7 +32936,7 @@
       <c r="AD26" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="AE26" s="54" t="s">
+      <c r="AE26" s="40" t="s">
         <v>39</v>
       </c>
       <c r="AF26" s="40" t="s">
@@ -33052,7 +33046,7 @@
       <c r="AD27" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AE27" s="53" t="s">
+      <c r="AE27" s="34" t="s">
         <v>39</v>
       </c>
       <c r="AF27" s="34" t="s">
@@ -33162,7 +33156,7 @@
       <c r="AD28" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AE28" s="53" t="s">
+      <c r="AE28" s="34" t="s">
         <v>39</v>
       </c>
       <c r="AF28" s="34" t="s">
@@ -33272,7 +33266,7 @@
       <c r="AD29" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AE29" s="53" t="s">
+      <c r="AE29" s="34" t="s">
         <v>39</v>
       </c>
       <c r="AF29" s="34" t="s">
@@ -33299,16 +33293,16 @@
         <v>39</v>
       </c>
       <c r="C30" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D30" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E30" s="34" t="s">
         <v>39</v>
       </c>
       <c r="F30" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G30" s="34" t="s">
         <v>40</v>
@@ -33320,7 +33314,7 @@
         <v>39</v>
       </c>
       <c r="J30" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K30" s="34" t="s">
         <v>39</v>
@@ -33329,16 +33323,16 @@
         <v>39</v>
       </c>
       <c r="M30" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N30" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O30" s="34" t="s">
         <v>39</v>
       </c>
       <c r="P30" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q30" s="34" t="s">
         <v>39</v>
@@ -33350,13 +33344,13 @@
         <v>40</v>
       </c>
       <c r="T30" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="U30" s="34" t="s">
         <v>40</v>
       </c>
       <c r="V30" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="W30" s="34" t="s">
         <v>39</v>
@@ -33368,13 +33362,13 @@
         <v>39</v>
       </c>
       <c r="Z30" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AA30" s="34" t="s">
         <v>39</v>
       </c>
       <c r="AB30" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AC30" s="34" t="s">
         <v>39</v>
@@ -33382,8 +33376,8 @@
       <c r="AD30" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AE30" s="53" t="s">
-        <v>40</v>
+      <c r="AE30" s="34" t="s">
+        <v>39</v>
       </c>
       <c r="AF30" s="34" t="s">
         <v>39</v>
@@ -33409,16 +33403,16 @@
         <v>39</v>
       </c>
       <c r="C31" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D31" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E31" s="34" t="s">
         <v>39</v>
       </c>
       <c r="F31" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G31" s="34" t="s">
         <v>40</v>
@@ -33430,7 +33424,7 @@
         <v>39</v>
       </c>
       <c r="J31" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K31" s="34" t="s">
         <v>40</v>
@@ -33442,7 +33436,7 @@
         <v>40</v>
       </c>
       <c r="N31" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O31" s="34" t="s">
         <v>39</v>
@@ -33460,7 +33454,7 @@
         <v>40</v>
       </c>
       <c r="T31" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="U31" s="34" t="s">
         <v>40</v>
@@ -33492,8 +33486,8 @@
       <c r="AD31" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="AE31" s="53" t="s">
-        <v>40</v>
+      <c r="AE31" s="34" t="s">
+        <v>39</v>
       </c>
       <c r="AF31" s="34" t="s">
         <v>39</v>
@@ -33502,7 +33496,7 @@
         <v>39</v>
       </c>
       <c r="AH31" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AI31" s="34" t="s">
         <v>40</v>
@@ -33519,7 +33513,7 @@
         <v>39</v>
       </c>
       <c r="C32" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D32" s="34" t="s">
         <v>39</v>
@@ -33528,10 +33522,10 @@
         <v>39</v>
       </c>
       <c r="F32" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G32" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H32" s="34" t="s">
         <v>39</v>
@@ -33540,25 +33534,25 @@
         <v>39</v>
       </c>
       <c r="J32" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K32" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L32" s="34" t="s">
         <v>39</v>
       </c>
       <c r="M32" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N32" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O32" s="34" t="s">
         <v>39</v>
       </c>
       <c r="P32" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q32" s="34" t="s">
         <v>39</v>
@@ -33567,16 +33561,16 @@
         <v>39</v>
       </c>
       <c r="S32" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T32" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="U32" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="V32" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="W32" s="34" t="s">
         <v>39</v>
@@ -33602,20 +33596,20 @@
       <c r="AD32" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AE32" s="53" t="s">
-        <v>40</v>
+      <c r="AE32" s="34" t="s">
+        <v>39</v>
       </c>
       <c r="AF32" s="34" t="s">
         <v>39</v>
       </c>
       <c r="AG32" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AH32" s="34" t="s">
         <v>39</v>
       </c>
       <c r="AI32" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AJ32" s="34" t="s">
         <v>39</v>
@@ -33653,13 +33647,13 @@
         <v>39</v>
       </c>
       <c r="K33" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="L33" s="34" t="s">
         <v>39</v>
       </c>
       <c r="M33" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N33" s="34" t="s">
         <v>39</v>
@@ -33668,7 +33662,7 @@
         <v>39</v>
       </c>
       <c r="P33" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Q33" s="34" t="s">
         <v>39</v>
@@ -33686,7 +33680,7 @@
         <v>39</v>
       </c>
       <c r="V33" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="W33" s="34" t="s">
         <v>39</v>
@@ -33712,7 +33706,7 @@
       <c r="AD33" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AE33" s="53" t="s">
+      <c r="AE33" s="34" t="s">
         <v>39</v>
       </c>
       <c r="AF33" s="34" t="s">
@@ -33728,7 +33722,7 @@
         <v>39</v>
       </c>
       <c r="AJ33" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:36" x14ac:dyDescent="0.3">
@@ -33822,7 +33816,7 @@
       <c r="AD34" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AE34" s="53" t="s">
+      <c r="AE34" s="34" t="s">
         <v>39</v>
       </c>
       <c r="AF34" s="34" t="s">
@@ -33861,7 +33855,7 @@
         <v>39</v>
       </c>
       <c r="G35" s="41" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H35" s="41" t="s">
         <v>39</v>
@@ -33897,13 +33891,13 @@
         <v>39</v>
       </c>
       <c r="S35" s="41" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="T35" s="41" t="s">
         <v>39</v>
       </c>
       <c r="U35" s="41" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="V35" s="41" t="s">
         <v>39</v>
@@ -33918,7 +33912,7 @@
         <v>39</v>
       </c>
       <c r="Z35" s="41" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AA35" s="41" t="s">
         <v>39</v>
@@ -33930,9 +33924,9 @@
         <v>39</v>
       </c>
       <c r="AD35" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE35" s="55" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE35" s="41" t="s">
         <v>39</v>
       </c>
       <c r="AF35" s="41" t="s">
@@ -33945,7 +33939,7 @@
         <v>39</v>
       </c>
       <c r="AI35" s="41" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AJ35" s="41" t="s">
         <v>39</v>
@@ -33958,20 +33952,21 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F39E67B8-A1DC-45C6-A1D4-0073AA57C7BD}">
-  <dimension ref="A1:P27"/>
+  <dimension ref="A1:P35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M20" sqref="M20:N20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.21875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.77734375" bestFit="1" customWidth="1"/>
@@ -34345,6 +34340,7 @@
         <v>20</v>
       </c>
     </row>
+    <row r="35" s="52" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Lower the cost of SOUL magic. Do some more adventuring after reaching 100 level.
Bugfix: reverse preferences of curse magic.
</commit_message>
<xml_diff>
--- a/doc/caste_system.xlsx
+++ b/doc/caste_system.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/349dfb9748b30a92/Asztali gép/ataliasflame_2.0/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9590" documentId="8_{652F4476-B36F-42CD-831D-0D71B9923ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65C51AA8-7A2E-4CAB-925B-04EC196CD0E5}"/>
+  <xr:revisionPtr revIDLastSave="9601" documentId="8_{652F4476-B36F-42CD-831D-0D71B9923ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2FA7F17-D9C5-4D4E-B9D6-5BC86FEE74C8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="696" activeTab="7" xr2:uid="{CAF51EC3-63EC-48CD-AA7B-C21B3D5D222B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="696" activeTab="8" xr2:uid="{CAF51EC3-63EC-48CD-AA7B-C21B3D5D222B}"/>
   </bookViews>
   <sheets>
     <sheet name="caste list" sheetId="1" r:id="rId1"/>
@@ -1680,7 +1680,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3235" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3245" uniqueCount="197">
   <si>
     <t>csavargó</t>
   </si>
@@ -2242,6 +2242,36 @@
   <si>
     <t>summonings (animal)</t>
   </si>
+  <si>
+    <t>pásztor</t>
+  </si>
+  <si>
+    <t>shepherd</t>
+  </si>
+  <si>
+    <t>guide</t>
+  </si>
+  <si>
+    <t>escort</t>
+  </si>
+  <si>
+    <t>usher</t>
+  </si>
+  <si>
+    <t>ajtónálló</t>
+  </si>
+  <si>
+    <t>kísérő</t>
+  </si>
+  <si>
+    <t>vezető</t>
+  </si>
+  <si>
+    <t>scout</t>
+  </si>
+  <si>
+    <t>felderítő</t>
+  </si>
 </sst>
 </file>
 
@@ -2571,6 +2601,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2582,9 +2615,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3041,7 +3071,7 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="23" t="s">
@@ -3097,7 +3127,7 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="49"/>
+      <c r="A4" s="50"/>
       <c r="B4" s="23" t="s">
         <v>2</v>
       </c>
@@ -3151,7 +3181,7 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="49"/>
+      <c r="A5" s="50"/>
       <c r="B5" s="23" t="s">
         <v>3</v>
       </c>
@@ -3205,7 +3235,7 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="49"/>
+      <c r="A6" s="50"/>
       <c r="B6" s="22" t="s">
         <v>21</v>
       </c>
@@ -3259,7 +3289,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="50"/>
+      <c r="A7" s="51"/>
       <c r="B7" s="21" t="s">
         <v>4</v>
       </c>
@@ -3313,7 +3343,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="49" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="23" t="s">
@@ -3369,7 +3399,7 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="49"/>
+      <c r="A9" s="50"/>
       <c r="B9" s="23" t="s">
         <v>6</v>
       </c>
@@ -3423,7 +3453,7 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="49"/>
+      <c r="A10" s="50"/>
       <c r="B10" s="23" t="s">
         <v>7</v>
       </c>
@@ -3477,7 +3507,7 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="50"/>
+      <c r="A11" s="51"/>
       <c r="B11" s="21" t="s">
         <v>8</v>
       </c>
@@ -3531,7 +3561,7 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="48" t="s">
+      <c r="A12" s="49" t="s">
         <v>79</v>
       </c>
       <c r="B12" s="23" t="s">
@@ -3587,7 +3617,7 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="49"/>
+      <c r="A13" s="50"/>
       <c r="B13" s="23" t="s">
         <v>10</v>
       </c>
@@ -3641,7 +3671,7 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="49"/>
+      <c r="A14" s="50"/>
       <c r="B14" s="23" t="s">
         <v>11</v>
       </c>
@@ -3695,7 +3725,7 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="50"/>
+      <c r="A15" s="51"/>
       <c r="B15" s="21" t="s">
         <v>12</v>
       </c>
@@ -3749,7 +3779,7 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="48" t="s">
+      <c r="A16" s="49" t="s">
         <v>80</v>
       </c>
       <c r="B16" s="23" t="s">
@@ -3805,7 +3835,7 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="49"/>
+      <c r="A17" s="50"/>
       <c r="B17" s="23" t="s">
         <v>14</v>
       </c>
@@ -3859,7 +3889,7 @@
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" s="49"/>
+      <c r="A18" s="50"/>
       <c r="B18" s="23" t="s">
         <v>15</v>
       </c>
@@ -3913,7 +3943,7 @@
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" s="50"/>
+      <c r="A19" s="51"/>
       <c r="B19" s="21" t="s">
         <v>16</v>
       </c>
@@ -3967,7 +3997,7 @@
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="48" t="s">
+      <c r="A20" s="49" t="s">
         <v>81</v>
       </c>
       <c r="B20" s="23" t="s">
@@ -4023,7 +4053,7 @@
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21" s="49"/>
+      <c r="A21" s="50"/>
       <c r="B21" s="23" t="s">
         <v>18</v>
       </c>
@@ -4077,7 +4107,7 @@
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22" s="49"/>
+      <c r="A22" s="50"/>
       <c r="B22" s="23" t="s">
         <v>19</v>
       </c>
@@ -4131,7 +4161,7 @@
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23" s="50"/>
+      <c r="A23" s="51"/>
       <c r="B23" s="21" t="s">
         <v>20</v>
       </c>
@@ -4335,54 +4365,54 @@
       <c r="U1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="W1" s="51" t="s">
+      <c r="W1" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="X1" s="51"/>
-      <c r="Y1" s="51"/>
-      <c r="Z1" s="51"/>
-      <c r="AA1" s="51"/>
-      <c r="AB1" s="51"/>
-      <c r="AD1" s="51" t="s">
+      <c r="X1" s="52"/>
+      <c r="Y1" s="52"/>
+      <c r="Z1" s="52"/>
+      <c r="AA1" s="52"/>
+      <c r="AB1" s="52"/>
+      <c r="AD1" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="AE1" s="51"/>
-      <c r="AF1" s="51"/>
-      <c r="AG1" s="51"/>
-      <c r="AH1" s="51"/>
-      <c r="AI1" s="51"/>
-      <c r="AK1" s="51" t="s">
+      <c r="AE1" s="52"/>
+      <c r="AF1" s="52"/>
+      <c r="AG1" s="52"/>
+      <c r="AH1" s="52"/>
+      <c r="AI1" s="52"/>
+      <c r="AK1" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="AL1" s="51"/>
-      <c r="AM1" s="51"/>
-      <c r="AN1" s="51"/>
-      <c r="AO1" s="51"/>
-      <c r="AP1" s="51"/>
-      <c r="AR1" s="51" t="s">
+      <c r="AL1" s="52"/>
+      <c r="AM1" s="52"/>
+      <c r="AN1" s="52"/>
+      <c r="AO1" s="52"/>
+      <c r="AP1" s="52"/>
+      <c r="AR1" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="AS1" s="51"/>
-      <c r="AT1" s="51"/>
-      <c r="AU1" s="51"/>
-      <c r="AV1" s="51"/>
-      <c r="AW1" s="51"/>
-      <c r="AY1" s="51" t="s">
+      <c r="AS1" s="52"/>
+      <c r="AT1" s="52"/>
+      <c r="AU1" s="52"/>
+      <c r="AV1" s="52"/>
+      <c r="AW1" s="52"/>
+      <c r="AY1" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="AZ1" s="51"/>
-      <c r="BA1" s="51"/>
-      <c r="BB1" s="51"/>
-      <c r="BC1" s="51"/>
-      <c r="BD1" s="51"/>
-      <c r="BF1" s="51" t="s">
+      <c r="AZ1" s="52"/>
+      <c r="BA1" s="52"/>
+      <c r="BB1" s="52"/>
+      <c r="BC1" s="52"/>
+      <c r="BD1" s="52"/>
+      <c r="BF1" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="BG1" s="51"/>
-      <c r="BH1" s="51"/>
-      <c r="BI1" s="51"/>
-      <c r="BJ1" s="51"/>
-      <c r="BK1" s="51"/>
+      <c r="BG1" s="52"/>
+      <c r="BH1" s="52"/>
+      <c r="BI1" s="52"/>
+      <c r="BJ1" s="52"/>
+      <c r="BK1" s="52"/>
     </row>
     <row r="2" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
@@ -30278,7 +30308,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA1C4ECE-D418-419E-9393-664BDA889D6E}">
   <dimension ref="A1:AJ35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AJ19" sqref="AJ19"/>
     </sheetView>
   </sheetViews>
@@ -33954,7 +33984,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F39E67B8-A1DC-45C6-A1D4-0073AA57C7BD}">
   <dimension ref="A1:P35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -34286,16 +34318,34 @@
       <c r="E21" s="3" t="s">
         <v>169</v>
       </c>
+      <c r="M21" t="s">
+        <v>187</v>
+      </c>
+      <c r="N21" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>15</v>
       </c>
+      <c r="M22" t="s">
+        <v>194</v>
+      </c>
+      <c r="N22" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>16</v>
       </c>
+      <c r="M23" t="s">
+        <v>193</v>
+      </c>
+      <c r="N23" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
@@ -34316,6 +34366,12 @@
       <c r="H24" s="44" t="s">
         <v>164</v>
       </c>
+      <c r="M24" t="s">
+        <v>192</v>
+      </c>
+      <c r="N24" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
@@ -34327,6 +34383,12 @@
       <c r="E25" s="3" t="s">
         <v>149</v>
       </c>
+      <c r="M25" t="s">
+        <v>196</v>
+      </c>
+      <c r="N25" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
@@ -34340,7 +34402,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" s="52" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="35" s="48" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>